<commit_message>
Lode Runner - progress
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43A2B210-8300-4AC1-B999-ECD01DA4E8DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD32AE11-ABF6-44E4-B3B4-86B7E66D24C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32415" yWindow="2235" windowWidth="20670" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40785" yWindow="1365" windowWidth="18585" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V3" sheetId="1" r:id="rId1"/>
@@ -658,7 +658,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,9 +799,15 @@
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="D9" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B9" s="3">
+        <v>23845</v>
+      </c>
+      <c r="C9" s="3">
+        <v>28099</v>
+      </c>
+      <c r="D9" s="4">
+        <f t="shared" si="1"/>
+        <v>4254</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -809,9 +815,15 @@
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="D10" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B10" s="3">
+        <v>27369</v>
+      </c>
+      <c r="C10" s="3">
+        <v>32036</v>
+      </c>
+      <c r="D10" s="4">
+        <f t="shared" si="1"/>
+        <v>4667</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -819,9 +831,15 @@
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="D11" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B11" s="3">
+        <v>32334</v>
+      </c>
+      <c r="C11" s="3">
+        <v>37877</v>
+      </c>
+      <c r="D11" s="4">
+        <f t="shared" si="1"/>
+        <v>5543</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -829,9 +847,15 @@
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="D12" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B12" s="3">
+        <v>35635</v>
+      </c>
+      <c r="C12" s="3">
+        <v>41646</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="1"/>
+        <v>6011</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -839,9 +863,15 @@
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="D13" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B13" s="3">
+        <v>38350</v>
+      </c>
+      <c r="C13" s="3">
+        <v>45474</v>
+      </c>
+      <c r="D13" s="4">
+        <f t="shared" si="1"/>
+        <v>7124</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -849,9 +879,15 @@
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="D14" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B14" s="3">
+        <v>41932</v>
+      </c>
+      <c r="C14" s="3">
+        <v>50990</v>
+      </c>
+      <c r="D14" s="4">
+        <f t="shared" si="1"/>
+        <v>9058</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
LodeRunner - v2 progress
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD32AE11-ABF6-44E4-B3B4-86B7E66D24C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA5AF3B-9C55-48AA-B18B-C01A2D860CF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40785" yWindow="1365" windowWidth="18585" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35175" yWindow="1305" windowWidth="18585" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V3" sheetId="1" r:id="rId1"/>
@@ -232,12 +232,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -316,25 +323,26 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -658,7 +666,7 @@
   <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,9 +903,15 @@
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="D15" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B15" s="3">
+        <v>45855</v>
+      </c>
+      <c r="C15" s="3">
+        <v>55415</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="1"/>
+        <v>9560</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -905,9 +919,15 @@
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="D16" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B16" s="3">
+        <v>50630</v>
+      </c>
+      <c r="C16" s="3">
+        <v>60540</v>
+      </c>
+      <c r="D16" s="4">
+        <f t="shared" si="1"/>
+        <v>9910</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -915,9 +935,15 @@
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="D17" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B17" s="5">
+        <v>55302</v>
+      </c>
+      <c r="C17" s="3">
+        <v>65410</v>
+      </c>
+      <c r="D17" s="4">
+        <f t="shared" si="1"/>
+        <v>10108</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -925,9 +951,15 @@
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="D18" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B18" s="3">
+        <v>58398</v>
+      </c>
+      <c r="C18" s="3">
+        <v>68919</v>
+      </c>
+      <c r="D18" s="4">
+        <f t="shared" si="1"/>
+        <v>10521</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -935,9 +967,15 @@
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="D19" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B19" s="3">
+        <v>63243</v>
+      </c>
+      <c r="C19" s="3">
+        <v>74902</v>
+      </c>
+      <c r="D19" s="4">
+        <f t="shared" si="1"/>
+        <v>11659</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -945,9 +983,15 @@
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="D20" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B20" s="3">
+        <v>68698</v>
+      </c>
+      <c r="C20" s="3">
+        <v>82072</v>
+      </c>
+      <c r="D20" s="4">
+        <f t="shared" si="1"/>
+        <v>13374</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -955,9 +999,15 @@
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="D21" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B21" s="3">
+        <v>71616</v>
+      </c>
+      <c r="C21" s="3">
+        <v>85866</v>
+      </c>
+      <c r="D21" s="4">
+        <f t="shared" si="1"/>
+        <v>14250</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -965,9 +1015,15 @@
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="D22" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B22" s="3">
+        <v>76434</v>
+      </c>
+      <c r="C22" s="3">
+        <v>90752</v>
+      </c>
+      <c r="D22" s="4">
+        <f t="shared" si="1"/>
+        <v>14318</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lode runner v3 - lv 1-2 done
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF00A7F5-D6B4-4E9A-B8E1-89BC2D520F62}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC455E0-CFA0-4ED9-B111-8A42DD8C9ECE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40680" yWindow="1230" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
   <si>
     <t>Place</t>
   </si>
@@ -187,6 +187,45 @@
   </si>
   <si>
     <t>end = black screen after level (1st lag frame after existing the level, tastudio perspective)</t>
+  </si>
+  <si>
+    <t>Lv1 End</t>
+  </si>
+  <si>
+    <t>Lv1 Start</t>
+  </si>
+  <si>
+    <t>Lv2 Start</t>
+  </si>
+  <si>
+    <t>1st Kill</t>
+  </si>
+  <si>
+    <t>883 - earliest - X 27</t>
+  </si>
+  <si>
+    <t>Frame</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Ideal</t>
+  </si>
+  <si>
+    <t>(3 ideal, 0-3 acceptable)</t>
+  </si>
+  <si>
+    <t>743 - dig</t>
+  </si>
+  <si>
+    <t>but drops too soon</t>
+  </si>
+  <si>
+    <t>Lv2 End</t>
+  </si>
+  <si>
+    <t>Lv3 Start</t>
   </si>
 </sst>
 </file>
@@ -639,15 +678,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2A8891-531F-43A4-B044-6C02F070C564}">
-  <dimension ref="A1:F45"/>
+  <dimension ref="A1:I278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -661,287 +700,1739 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>53</v>
       </c>
       <c r="B2" s="2">
-        <v>347</v>
+        <v>427</v>
       </c>
       <c r="C2" s="2">
         <v>347</v>
       </c>
-      <c r="D2" s="2">
-        <f t="shared" ref="D2:D45" si="0">IF(B2="","-",IF(C2="","-",B2-C2))</f>
-        <v>0</v>
+      <c r="D2" s="3">
+        <f>IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <v>-80</v>
       </c>
       <c r="F2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D3" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="2">
+        <v>902</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="3"/>
       <c r="F3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1062</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1973</v>
+      </c>
+      <c r="D4" s="3">
+        <f>IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
+        <v>911</v>
+      </c>
+      <c r="F4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D4" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D5" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D7" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D8" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D9" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D10" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D11" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D12" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D13" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D14" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D15" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="D16" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="17" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D17" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="18" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="19" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D19" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="20" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D20" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="21" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D21" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="22" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D22" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="23" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D23" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="24" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D24" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="25" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D25" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="26" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D26" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="27" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D27" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="28" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D28" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="29" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D29" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="30" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D30" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="31" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D31" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="32" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D32" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="33" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D34" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="35" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D35" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="36" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D36" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="37" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D37" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="38" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D38" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="39" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D39" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="40" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D40" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="41" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D41" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="42" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D42" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="43" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D43" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="44" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D44" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="45" spans="4:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="D45" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1408</v>
+      </c>
+      <c r="C5" s="7">
+        <v>3042</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" ref="D5:D68" si="0">IF(C5&lt;&gt;"",IF(B5&lt;&gt;"",C5-B5,"-"), "-")</f>
+        <v>1634</v>
+      </c>
+      <c r="G5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="7">
+        <v>2336</v>
+      </c>
+      <c r="C6" s="7">
+        <v>5594</v>
+      </c>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>3258</v>
+      </c>
+      <c r="G6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2679</v>
+      </c>
+      <c r="C7" s="7">
+        <v>6660</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>3981</v>
+      </c>
+      <c r="G7">
+        <v>883</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="G8">
+        <v>888</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="G13">
+        <v>902</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="7"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="7"/>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="7"/>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="7"/>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="7"/>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="3" t="str">
+        <f t="shared" ref="D69:D132" si="1">IF(C69&lt;&gt;"",IF(B69&lt;&gt;"",C69-B69,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="7"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="7"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="7"/>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="7"/>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="7"/>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="7"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="7"/>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="7"/>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="7"/>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="7"/>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="7"/>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="7"/>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="7"/>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="7"/>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="7"/>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="7"/>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="7"/>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="7"/>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="7"/>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="7"/>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="7"/>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="7"/>
+      <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="7"/>
+      <c r="B95" s="7"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="7"/>
+      <c r="B96" s="7"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="7"/>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="7"/>
+      <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="7"/>
+      <c r="B99" s="7"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="7"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="7"/>
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="7"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="7"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="7"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="7"/>
+      <c r="B107" s="7"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="7"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="7"/>
+      <c r="B109" s="7"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="7"/>
+      <c r="B110" s="7"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111" s="7"/>
+      <c r="B111" s="7"/>
+      <c r="C111" s="7"/>
+      <c r="D111" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="7"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="7"/>
+      <c r="D112" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="7"/>
+      <c r="B113" s="7"/>
+      <c r="C113" s="7"/>
+      <c r="D113" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="7"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="7"/>
+      <c r="D114" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A115" s="7"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="7"/>
+      <c r="D115" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A116" s="7"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="7"/>
+      <c r="D116" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A117" s="7"/>
+      <c r="B117" s="7"/>
+      <c r="C117" s="7"/>
+      <c r="D117" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A118" s="7"/>
+      <c r="B118" s="7"/>
+      <c r="C118" s="7"/>
+      <c r="D118" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A119" s="7"/>
+      <c r="B119" s="7"/>
+      <c r="C119" s="7"/>
+      <c r="D119" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A120" s="7"/>
+      <c r="B120" s="7"/>
+      <c r="C120" s="7"/>
+      <c r="D120" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A121" s="7"/>
+      <c r="B121" s="7"/>
+      <c r="C121" s="7"/>
+      <c r="D121" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A122" s="7"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="7"/>
+      <c r="D122" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A123" s="7"/>
+      <c r="B123" s="7"/>
+      <c r="C123" s="7"/>
+      <c r="D123" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A124" s="7"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="7"/>
+      <c r="D124" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A125" s="7"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="7"/>
+      <c r="D125" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A126" s="7"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="7"/>
+      <c r="D126" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A127" s="7"/>
+      <c r="B127" s="7"/>
+      <c r="C127" s="7"/>
+      <c r="D127" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A128" s="7"/>
+      <c r="B128" s="7"/>
+      <c r="C128" s="7"/>
+      <c r="D128" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A129" s="7"/>
+      <c r="B129" s="7"/>
+      <c r="C129" s="7"/>
+      <c r="D129" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A130" s="7"/>
+      <c r="B130" s="7"/>
+      <c r="C130" s="7"/>
+      <c r="D130" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A131" s="7"/>
+      <c r="B131" s="7"/>
+      <c r="C131" s="7"/>
+      <c r="D131" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A132" s="7"/>
+      <c r="B132" s="7"/>
+      <c r="C132" s="7"/>
+      <c r="D132" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A133" s="7"/>
+      <c r="B133" s="7"/>
+      <c r="C133" s="7"/>
+      <c r="D133" s="3" t="str">
+        <f t="shared" ref="D133:D137" si="2">IF(C133&lt;&gt;"",IF(B133&lt;&gt;"",C133-B133,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A134" s="7"/>
+      <c r="B134" s="7"/>
+      <c r="C134" s="7"/>
+      <c r="D134" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A135" s="7"/>
+      <c r="B135" s="7"/>
+      <c r="C135" s="7"/>
+      <c r="D135" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A136" s="7"/>
+      <c r="B136" s="7"/>
+      <c r="D136" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A137" s="7"/>
+      <c r="B137" s="7"/>
+      <c r="D137" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A138" s="7"/>
+      <c r="B138" s="7"/>
+      <c r="D138" s="3" t="str">
+        <f t="shared" ref="D138:D139" si="3">IF(C138&lt;&gt;"",IF(B138&lt;&gt;"",B138-C138,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A139" s="7"/>
+      <c r="B139" s="7"/>
+      <c r="D139" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A140" s="7"/>
+      <c r="B140" s="7"/>
+    </row>
+    <row r="141" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A141" s="7"/>
+      <c r="B141" s="7"/>
+    </row>
+    <row r="142" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B142" s="7"/>
+    </row>
+    <row r="143" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B143" s="7"/>
+    </row>
+    <row r="144" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B144" s="7"/>
+    </row>
+    <row r="145" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B145" s="7"/>
+    </row>
+    <row r="146" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B146" s="7"/>
+    </row>
+    <row r="147" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B147" s="7"/>
+    </row>
+    <row r="148" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B148" s="7"/>
+    </row>
+    <row r="149" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B149" s="7"/>
+    </row>
+    <row r="150" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B150" s="7"/>
+    </row>
+    <row r="151" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B151" s="7"/>
+    </row>
+    <row r="152" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B152" s="7"/>
+    </row>
+    <row r="153" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B153" s="7"/>
+    </row>
+    <row r="154" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B154" s="7"/>
+    </row>
+    <row r="155" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B155" s="7"/>
+    </row>
+    <row r="156" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B156" s="7"/>
+    </row>
+    <row r="157" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B157" s="7"/>
+    </row>
+    <row r="158" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B158" s="7"/>
+    </row>
+    <row r="159" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B159" s="7"/>
+    </row>
+    <row r="160" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B160" s="7"/>
+    </row>
+    <row r="161" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B161" s="7"/>
+    </row>
+    <row r="162" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B162" s="7"/>
+    </row>
+    <row r="163" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B163" s="7"/>
+    </row>
+    <row r="164" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B164" s="7"/>
+    </row>
+    <row r="165" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B165" s="7"/>
+    </row>
+    <row r="166" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B166" s="7"/>
+    </row>
+    <row r="167" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B167" s="7"/>
+    </row>
+    <row r="168" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B168" s="7"/>
+    </row>
+    <row r="169" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B169" s="7"/>
+    </row>
+    <row r="170" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B170" s="7"/>
+    </row>
+    <row r="171" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B171" s="7"/>
+    </row>
+    <row r="172" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B172" s="7"/>
+    </row>
+    <row r="173" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B173" s="7"/>
+    </row>
+    <row r="174" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B174" s="7"/>
+    </row>
+    <row r="175" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B175" s="7"/>
+    </row>
+    <row r="176" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B176" s="7"/>
+    </row>
+    <row r="177" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B177" s="7"/>
+    </row>
+    <row r="178" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B178" s="7"/>
+    </row>
+    <row r="179" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B179" s="7"/>
+    </row>
+    <row r="180" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B180" s="7"/>
+    </row>
+    <row r="181" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B181" s="7"/>
+    </row>
+    <row r="182" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B182" s="7"/>
+    </row>
+    <row r="183" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B183" s="7"/>
+    </row>
+    <row r="184" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B184" s="7"/>
+    </row>
+    <row r="185" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B185" s="7"/>
+    </row>
+    <row r="186" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B186" s="7"/>
+    </row>
+    <row r="187" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B187" s="7"/>
+    </row>
+    <row r="188" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B188" s="7"/>
+    </row>
+    <row r="189" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B189" s="7"/>
+    </row>
+    <row r="190" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B190" s="7"/>
+    </row>
+    <row r="191" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B191" s="7"/>
+    </row>
+    <row r="192" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B192" s="7"/>
+    </row>
+    <row r="193" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B193" s="7"/>
+    </row>
+    <row r="194" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B194" s="7"/>
+    </row>
+    <row r="195" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B195" s="7"/>
+    </row>
+    <row r="196" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B196" s="7"/>
+    </row>
+    <row r="197" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B197" s="7"/>
+    </row>
+    <row r="198" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B198" s="7"/>
+    </row>
+    <row r="199" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B199" s="7"/>
+    </row>
+    <row r="200" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B200" s="7"/>
+    </row>
+    <row r="201" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B201" s="7"/>
+    </row>
+    <row r="202" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B202" s="7"/>
+    </row>
+    <row r="203" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B203" s="7"/>
+    </row>
+    <row r="204" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B204" s="7"/>
+    </row>
+    <row r="205" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B205" s="7"/>
+    </row>
+    <row r="206" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B206" s="7"/>
+    </row>
+    <row r="207" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B207" s="7"/>
+    </row>
+    <row r="208" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B208" s="7"/>
+    </row>
+    <row r="209" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B209" s="7"/>
+    </row>
+    <row r="210" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B210" s="7"/>
+    </row>
+    <row r="211" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B211" s="7"/>
+    </row>
+    <row r="212" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B212" s="7"/>
+    </row>
+    <row r="213" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B213" s="7"/>
+    </row>
+    <row r="214" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B214" s="7"/>
+    </row>
+    <row r="215" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B215" s="7"/>
+    </row>
+    <row r="216" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B216" s="7"/>
+    </row>
+    <row r="217" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B217" s="7"/>
+    </row>
+    <row r="218" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B218" s="7"/>
+    </row>
+    <row r="219" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B219" s="7"/>
+    </row>
+    <row r="220" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B220" s="7"/>
+    </row>
+    <row r="221" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B221" s="7"/>
+    </row>
+    <row r="222" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B222" s="7"/>
+    </row>
+    <row r="223" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B223" s="7"/>
+    </row>
+    <row r="224" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B224" s="7"/>
+    </row>
+    <row r="225" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B225" s="7"/>
+    </row>
+    <row r="226" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B226" s="7"/>
+    </row>
+    <row r="227" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B227" s="7"/>
+    </row>
+    <row r="228" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B228" s="7"/>
+    </row>
+    <row r="229" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B229" s="7"/>
+    </row>
+    <row r="230" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B230" s="7"/>
+    </row>
+    <row r="231" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B231" s="7"/>
+    </row>
+    <row r="232" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B232" s="7"/>
+    </row>
+    <row r="233" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B233" s="7"/>
+    </row>
+    <row r="234" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B234" s="7"/>
+    </row>
+    <row r="235" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B235" s="7"/>
+    </row>
+    <row r="236" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B236" s="7"/>
+    </row>
+    <row r="237" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B237" s="7"/>
+    </row>
+    <row r="238" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B238" s="7"/>
+    </row>
+    <row r="239" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B239" s="7"/>
+    </row>
+    <row r="240" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B240" s="7"/>
+    </row>
+    <row r="241" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B241" s="7"/>
+    </row>
+    <row r="242" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B242" s="7"/>
+    </row>
+    <row r="243" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B243" s="7"/>
+    </row>
+    <row r="244" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B244" s="7"/>
+    </row>
+    <row r="245" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B245" s="7"/>
+    </row>
+    <row r="246" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B246" s="7"/>
+    </row>
+    <row r="247" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B247" s="7"/>
+    </row>
+    <row r="248" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B248" s="7"/>
+    </row>
+    <row r="249" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B249" s="7"/>
+    </row>
+    <row r="250" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B250" s="7"/>
+    </row>
+    <row r="251" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B251" s="7"/>
+    </row>
+    <row r="252" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B252" s="7"/>
+    </row>
+    <row r="253" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B253" s="7"/>
+    </row>
+    <row r="254" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B254" s="7"/>
+    </row>
+    <row r="255" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B255" s="7"/>
+    </row>
+    <row r="256" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B256" s="7"/>
+    </row>
+    <row r="257" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B257" s="7"/>
+    </row>
+    <row r="258" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B258" s="7"/>
+    </row>
+    <row r="259" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B259" s="7"/>
+    </row>
+    <row r="260" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B260" s="7"/>
+    </row>
+    <row r="261" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B261" s="7"/>
+    </row>
+    <row r="262" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B262" s="7"/>
+    </row>
+    <row r="263" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B263" s="7"/>
+    </row>
+    <row r="264" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B264" s="7"/>
+    </row>
+    <row r="265" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B265" s="7"/>
+    </row>
+    <row r="266" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B266" s="7"/>
+    </row>
+    <row r="267" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B267" s="7"/>
+    </row>
+    <row r="268" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B268" s="7"/>
+    </row>
+    <row r="269" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B269" s="7"/>
+    </row>
+    <row r="270" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B270" s="7"/>
+    </row>
+    <row r="271" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B271" s="7"/>
+    </row>
+    <row r="272" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B272" s="7"/>
+    </row>
+    <row r="273" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B273" s="7"/>
+    </row>
+    <row r="274" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B274" s="7"/>
+    </row>
+    <row r="275" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B275" s="7"/>
+    </row>
+    <row r="276" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B276" s="7"/>
+    </row>
+    <row r="277" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B277" s="7"/>
+    </row>
+    <row r="278" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B278" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -950,7 +2441,7 @@
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,8 +2477,8 @@
       <c r="C2" s="2">
         <v>347</v>
       </c>
-      <c r="D2" s="2">
-        <f t="shared" ref="D2" si="0">IF(B2="","-",IF(C2="","-",B2-C2))</f>
+      <c r="D2" s="3">
+        <f t="shared" ref="D2:D70" si="0">IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
         <v>0</v>
       </c>
     </row>
@@ -1002,7 +2493,7 @@
         <v>2256</v>
       </c>
       <c r="D3" s="3">
-        <f t="shared" ref="D3:D70" si="1">IF(C3&lt;&gt;"",IF(B3&lt;&gt;"",C3-B3,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>283</v>
       </c>
     </row>
@@ -1018,13 +2509,13 @@
         <v>6039</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>445</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <f t="shared" ref="A5:A31" si="2">A4+1</f>
+        <f t="shared" ref="A5:A31" si="1">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5" s="2">
@@ -1034,13 +2525,13 @@
         <v>9778</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>570</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="B6" s="2">
@@ -1050,13 +2541,13 @@
         <v>13996</v>
       </c>
       <c r="D6" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1328</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="B7" s="2">
@@ -1066,13 +2557,13 @@
         <v>18801</v>
       </c>
       <c r="D7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3343</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="B8" s="2">
@@ -1082,13 +2573,13 @@
         <v>24011</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3791</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B9" s="2">
@@ -1098,13 +2589,13 @@
         <v>28099</v>
       </c>
       <c r="D9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4254</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B10" s="2">
@@ -1114,13 +2605,13 @@
         <v>32036</v>
       </c>
       <c r="D10" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4667</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B11" s="2">
@@ -1130,13 +2621,13 @@
         <v>37877</v>
       </c>
       <c r="D11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5543</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B12" s="2">
@@ -1146,13 +2637,13 @@
         <v>41646</v>
       </c>
       <c r="D12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6011</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="B13" s="2">
@@ -1162,13 +2653,13 @@
         <v>45474</v>
       </c>
       <c r="D13" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>7124</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="B14" s="2">
@@ -1178,13 +2669,13 @@
         <v>50990</v>
       </c>
       <c r="D14" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9058</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="B15" s="2">
@@ -1194,13 +2685,13 @@
         <v>55415</v>
       </c>
       <c r="D15" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9560</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="B16" s="2">
@@ -1210,13 +2701,13 @@
         <v>60540</v>
       </c>
       <c r="D16" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9910</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="B17" s="4">
@@ -1226,13 +2717,13 @@
         <v>65410</v>
       </c>
       <c r="D17" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10108</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="B18" s="2">
@@ -1242,13 +2733,13 @@
         <v>68919</v>
       </c>
       <c r="D18" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>10521</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="B19" s="2">
@@ -1258,7 +2749,7 @@
         <v>74902</v>
       </c>
       <c r="D19" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>11659</v>
       </c>
       <c r="I19" s="2">
@@ -1267,7 +2758,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="B20" s="2">
@@ -1277,7 +2768,7 @@
         <v>82072</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13374</v>
       </c>
       <c r="I20" s="2">
@@ -1286,7 +2777,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="B21" s="2">
@@ -1296,7 +2787,7 @@
         <v>85866</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14250</v>
       </c>
       <c r="I21" s="2">
@@ -1306,7 +2797,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="B22" s="2">
@@ -1316,13 +2807,13 @@
         <v>90752</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>14318</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>21</v>
       </c>
       <c r="B23" s="2">
@@ -1332,13 +2823,13 @@
         <v>97300</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>16037</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>22</v>
       </c>
       <c r="B24" s="2">
@@ -1348,13 +2839,13 @@
         <v>102904</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>17343</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="B25" s="2">
@@ -1364,13 +2855,13 @@
         <v>112456</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20871</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>24</v>
       </c>
       <c r="B26" s="2">
@@ -1380,7 +2871,7 @@
         <v>116217</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21764</v>
       </c>
     </row>
@@ -1392,7 +2883,7 @@
         <v>118434</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>21822</v>
       </c>
     </row>
@@ -1408,13 +2899,13 @@
         <v>120804</v>
       </c>
       <c r="D28" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22245</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>26</v>
       </c>
       <c r="B29" s="2">
@@ -1424,13 +2915,13 @@
         <v>125924</v>
       </c>
       <c r="D29" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22539</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>27</v>
       </c>
       <c r="B30" s="2">
@@ -1440,17 +2931,17 @@
         <v>134560</v>
       </c>
       <c r="D30" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>24785</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>28</v>
       </c>
       <c r="D31" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
@@ -1465,7 +2956,7 @@
         <v>141048</v>
       </c>
       <c r="D32" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>26891</v>
       </c>
     </row>
@@ -1480,7 +2971,7 @@
         <v>145397</v>
       </c>
       <c r="D33" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>27493</v>
       </c>
     </row>
@@ -1495,7 +2986,7 @@
         <v>146464</v>
       </c>
       <c r="D34" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28207</v>
       </c>
     </row>
@@ -1510,7 +3001,7 @@
         <v>150524</v>
       </c>
       <c r="D35" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>28667</v>
       </c>
     </row>
@@ -1525,7 +3016,7 @@
         <v>151592</v>
       </c>
       <c r="D36" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>29374</v>
       </c>
     </row>
@@ -1540,7 +3031,7 @@
         <v>153052</v>
       </c>
       <c r="D37" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>29578</v>
       </c>
     </row>
@@ -1555,7 +3046,7 @@
         <v>154119</v>
       </c>
       <c r="D38" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30302</v>
       </c>
     </row>
@@ -1570,7 +3061,7 @@
         <v>158045</v>
       </c>
       <c r="D39" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>30907</v>
       </c>
     </row>
@@ -1585,7 +3076,7 @@
         <v>159112</v>
       </c>
       <c r="D40" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>31631</v>
       </c>
     </row>
@@ -1600,7 +3091,7 @@
         <v>162453</v>
       </c>
       <c r="D41" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32187</v>
       </c>
     </row>
@@ -1615,7 +3106,7 @@
         <v>163519</v>
       </c>
       <c r="D42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>32907</v>
       </c>
     </row>
@@ -1630,7 +3121,7 @@
         <v>167634</v>
       </c>
       <c r="D43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>33604</v>
       </c>
     </row>
@@ -1645,7 +3136,7 @@
         <v>168700</v>
       </c>
       <c r="D44" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>34324</v>
       </c>
     </row>
@@ -1660,7 +3151,7 @@
         <v>172230</v>
       </c>
       <c r="D45" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>34508</v>
       </c>
     </row>
@@ -1675,7 +3166,7 @@
         <v>173296</v>
       </c>
       <c r="D46" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>35231</v>
       </c>
     </row>
@@ -1690,7 +3181,7 @@
         <v>177203</v>
       </c>
       <c r="D47" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>36501</v>
       </c>
     </row>
@@ -1705,7 +3196,7 @@
         <v>178269</v>
       </c>
       <c r="D48" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>37223</v>
       </c>
     </row>
@@ -1720,7 +3211,7 @@
         <v>182363</v>
       </c>
       <c r="D49" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>38031</v>
       </c>
     </row>
@@ -1735,7 +3226,7 @@
         <v>183431</v>
       </c>
       <c r="D50" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>38755</v>
       </c>
     </row>
@@ -1750,7 +3241,7 @@
         <v>187810</v>
       </c>
       <c r="D51" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>39370</v>
       </c>
     </row>
@@ -1765,7 +3256,7 @@
         <v>188877</v>
       </c>
       <c r="D52" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>40094</v>
       </c>
     </row>
@@ -1780,7 +3271,7 @@
         <v>190986</v>
       </c>
       <c r="D53" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>40336</v>
       </c>
     </row>
@@ -1795,7 +3286,7 @@
         <v>192052</v>
       </c>
       <c r="D54" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>41059</v>
       </c>
     </row>
@@ -1810,7 +3301,7 @@
         <v>198298</v>
       </c>
       <c r="D55" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>42932</v>
       </c>
     </row>
@@ -1825,7 +3316,7 @@
         <v>199364</v>
       </c>
       <c r="D56" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>43655</v>
       </c>
     </row>
@@ -1840,7 +3331,7 @@
         <v>203725</v>
       </c>
       <c r="D57" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44034</v>
       </c>
     </row>
@@ -1855,7 +3346,7 @@
         <v>204792</v>
       </c>
       <c r="D58" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>44758</v>
       </c>
     </row>
@@ -1870,7 +3361,7 @@
         <v>209869</v>
       </c>
       <c r="D59" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>45550</v>
       </c>
     </row>
@@ -1885,7 +3376,7 @@
         <v>210935</v>
       </c>
       <c r="D60" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>46273</v>
       </c>
     </row>
@@ -1900,7 +3391,7 @@
         <v>213616</v>
       </c>
       <c r="D61" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>46967</v>
       </c>
     </row>
@@ -1915,7 +3406,7 @@
         <v>214683</v>
       </c>
       <c r="D62" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>47683</v>
       </c>
     </row>
@@ -1930,7 +3421,7 @@
         <v>218068</v>
       </c>
       <c r="D63" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>48621</v>
       </c>
     </row>
@@ -1945,7 +3436,7 @@
         <v>219136</v>
       </c>
       <c r="D64" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>49345</v>
       </c>
     </row>
@@ -1960,7 +3451,7 @@
         <v>223225</v>
       </c>
       <c r="D65" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>49886</v>
       </c>
     </row>
@@ -1975,7 +3466,7 @@
         <v>224293</v>
       </c>
       <c r="D66" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>50610</v>
       </c>
     </row>
@@ -1990,7 +3481,7 @@
         <v>227656</v>
       </c>
       <c r="D67" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>51123</v>
       </c>
     </row>
@@ -2005,7 +3496,7 @@
         <v>228723</v>
       </c>
       <c r="D68" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>51847</v>
       </c>
     </row>
@@ -2020,7 +3511,7 @@
         <v>232919</v>
       </c>
       <c r="D69" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>52461</v>
       </c>
     </row>
@@ -2035,7 +3526,7 @@
         <v>233985</v>
       </c>
       <c r="D70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>53183</v>
       </c>
     </row>
@@ -2050,7 +3541,7 @@
         <v>238403</v>
       </c>
       <c r="D71" s="3">
-        <f t="shared" ref="D71:D75" si="3">IF(C71&lt;&gt;"",IF(B71&lt;&gt;"",C71-B71,"-"), "-")</f>
+        <f t="shared" ref="D71:D75" si="2">IF(C71&lt;&gt;"",IF(B71&lt;&gt;"",C71-B71,"-"), "-")</f>
         <v>54330</v>
       </c>
     </row>
@@ -2065,7 +3556,7 @@
         <v>239469</v>
       </c>
       <c r="D72" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>55052</v>
       </c>
     </row>
@@ -2080,7 +3571,7 @@
         <v>243523</v>
       </c>
       <c r="D73" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>55863</v>
       </c>
     </row>
@@ -2095,7 +3586,7 @@
         <v>244589</v>
       </c>
       <c r="D74" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>56585</v>
       </c>
     </row>
@@ -2110,7 +3601,7 @@
         <v>248070</v>
       </c>
       <c r="D75" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>56869</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Lode Runner v3 - fast mode - up to level level 6
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC455E0-CFA0-4ED9-B111-8A42DD8C9ECE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46247DFF-ECBC-477D-BFF4-50FDF1B07858}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40680" yWindow="1230" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
   <si>
     <t>Place</t>
   </si>
@@ -226,6 +226,27 @@
   </si>
   <si>
     <t>Lv3 Start</t>
+  </si>
+  <si>
+    <t>Lv3 End</t>
+  </si>
+  <si>
+    <t>Lv4 Start</t>
+  </si>
+  <si>
+    <t>Lv4 End</t>
+  </si>
+  <si>
+    <t>Lv5 Start</t>
+  </si>
+  <si>
+    <t>Lv5 End</t>
+  </si>
+  <si>
+    <t>Lv6 Start</t>
+  </si>
+  <si>
+    <t>Lv6 End</t>
   </si>
 </sst>
 </file>
@@ -681,7 +702,7 @@
   <dimension ref="A1:I278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -810,12 +831,18 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A8" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="7">
+        <v>3469</v>
+      </c>
+      <c r="C8" s="7">
+        <v>9208</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>5739</v>
       </c>
       <c r="G8">
         <v>888</v>
@@ -828,48 +855,78 @@
       </c>
     </row>
     <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="7">
+        <v>3814</v>
+      </c>
+      <c r="C9" s="7">
+        <v>10274</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>6460</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A10" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="7">
+        <v>4647</v>
+      </c>
+      <c r="C10" s="7">
+        <v>12668</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>8021</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A11" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B11" s="7">
+        <v>4991</v>
+      </c>
+      <c r="C11" s="7">
+        <v>13734</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>8743</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="7">
+        <v>5667</v>
+      </c>
+      <c r="C12" s="7">
+        <v>15458</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>9791</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A13" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="7">
+        <v>6010</v>
+      </c>
+      <c r="C13" s="7">
+        <v>16526</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>10516</v>
       </c>
       <c r="G13">
         <v>902</v>
@@ -882,9 +939,13 @@
       </c>
     </row>
     <row r="14" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
+      <c r="A14" s="7" t="s">
+        <v>71</v>
+      </c>
       <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
+      <c r="C14" s="7">
+        <v>20220</v>
+      </c>
       <c r="D14" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>

</xml_diff>

<commit_message>
lode runner - v3 - lv 8 done
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46247DFF-ECBC-477D-BFF4-50FDF1B07858}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C76CCC-2870-4D5D-BF68-3997A4DB843C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40680" yWindow="1230" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
   <si>
     <t>Place</t>
   </si>
@@ -247,6 +247,21 @@
   </si>
   <si>
     <t>Lv6 End</t>
+  </si>
+  <si>
+    <t>Lv7 Start</t>
+  </si>
+  <si>
+    <t>Lv7 End</t>
+  </si>
+  <si>
+    <t>Lv8 Start</t>
+  </si>
+  <si>
+    <t>Lv8 End</t>
+  </si>
+  <si>
+    <t>Lv9 Start</t>
   </si>
 </sst>
 </file>
@@ -702,7 +717,7 @@
   <dimension ref="A1:I278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -942,58 +957,90 @@
       <c r="A14" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="7">
+        <v>7418</v>
+      </c>
       <c r="C14" s="7">
         <v>20220</v>
       </c>
-      <c r="D14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>12802</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A15" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="7">
+        <v>7761</v>
+      </c>
+      <c r="C15" s="7">
+        <v>21286</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>13525</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A16" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="7">
+        <v>8558</v>
+      </c>
+      <c r="C16" s="7">
+        <v>23845</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>15287</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A17" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="7">
+        <v>8902</v>
+      </c>
+      <c r="C17" s="7">
+        <v>24912</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>16010</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A18" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" s="7">
+        <v>9676</v>
+      </c>
+      <c r="C18" s="7">
+        <v>27369</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>17693</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A19" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B19" s="7">
+        <v>10028</v>
+      </c>
+      <c r="C19" s="7">
+        <v>28435</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>18407</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lode runner v3 - up to level 13
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C76CCC-2870-4D5D-BF68-3997A4DB843C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6058794E-1F16-4ABB-928A-D47B1BC0E354}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40680" yWindow="1230" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
   <si>
     <t>Place</t>
   </si>
@@ -262,6 +262,27 @@
   </si>
   <si>
     <t>Lv9 Start</t>
+  </si>
+  <si>
+    <t>Lv9 End</t>
+  </si>
+  <si>
+    <t>Lv10 Start</t>
+  </si>
+  <si>
+    <t>Lv10 End</t>
+  </si>
+  <si>
+    <t>Lv11 Start</t>
+  </si>
+  <si>
+    <t>Lv12 Start</t>
+  </si>
+  <si>
+    <t>Lv12 End</t>
+  </si>
+  <si>
+    <t>Lv13 Start</t>
   </si>
 </sst>
 </file>
@@ -716,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2A8891-531F-43A4-B044-6C02F070C564}">
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1044,66 +1065,108 @@
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A20" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20" s="7">
+        <v>11437</v>
+      </c>
+      <c r="C20" s="7">
+        <v>32334</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>20897</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="7">
+        <v>11780</v>
+      </c>
+      <c r="C21" s="7">
+        <v>33403</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>21623</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A22" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B22" s="7">
+        <v>12700</v>
+      </c>
+      <c r="C22" s="7">
+        <v>35643</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>22943</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A23" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="7">
+        <v>13043</v>
+      </c>
+      <c r="C23" s="7">
+        <v>36710</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>23667</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A24" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="7">
+        <v>14041</v>
+      </c>
+      <c r="C24" s="7">
+        <v>39416</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>25375</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A25" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="7">
+        <v>15026</v>
+      </c>
+      <c r="C25" s="7">
+        <v>41934</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>26908</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A26" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="7">
+        <v>15369</v>
+      </c>
+      <c r="C26" s="7">
+        <v>43001</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>27632</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lode runner v3 - up to lv20
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6058794E-1F16-4ABB-928A-D47B1BC0E354}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D7D53D-97CD-44E7-8597-F79DC148C1CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40680" yWindow="1230" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
   <si>
     <t>Place</t>
   </si>
@@ -283,6 +283,48 @@
   </si>
   <si>
     <t>Lv13 Start</t>
+  </si>
+  <si>
+    <t>Lv13 End</t>
+  </si>
+  <si>
+    <t>Lv14 Start</t>
+  </si>
+  <si>
+    <t>Lv14 End</t>
+  </si>
+  <si>
+    <t>Lv15 Start</t>
+  </si>
+  <si>
+    <t>Lv15 End</t>
+  </si>
+  <si>
+    <t>Lv16 Start</t>
+  </si>
+  <si>
+    <t>Lv16 End</t>
+  </si>
+  <si>
+    <t>Lv17 Start</t>
+  </si>
+  <si>
+    <t>Lv17 End</t>
+  </si>
+  <si>
+    <t>Lv18 Start</t>
+  </si>
+  <si>
+    <t>Lv18 End</t>
+  </si>
+  <si>
+    <t>Lv19 Start</t>
+  </si>
+  <si>
+    <t>Lv19 End</t>
+  </si>
+  <si>
+    <t>Lv20 Start</t>
   </si>
 </sst>
 </file>
@@ -737,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2A8891-531F-43A4-B044-6C02F070C564}">
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1170,129 +1212,213 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A27" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="7">
+        <v>16257</v>
+      </c>
+      <c r="C27" s="7">
+        <v>45855</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="0"/>
+        <v>29598</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A28" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="7">
+        <v>16601</v>
+      </c>
+      <c r="C28" s="7">
+        <v>46921</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>30320</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A29" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="7">
+        <v>17482</v>
+      </c>
+      <c r="C29" s="7">
+        <v>50630</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>33148</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A30" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="7">
+        <v>17826</v>
+      </c>
+      <c r="C30" s="7">
+        <v>51696</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>33870</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A31" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="7">
+        <v>18918</v>
+      </c>
+      <c r="C31" s="7">
+        <v>55302</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
+        <v>36384</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A32" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="7">
+        <v>19261</v>
+      </c>
+      <c r="C32" s="7">
+        <v>56368</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="0"/>
+        <v>37107</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A33" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="7">
+        <v>19995</v>
+      </c>
+      <c r="C33" s="7">
+        <v>58398</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="0"/>
+        <v>38403</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A34" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="7">
+        <v>20338</v>
+      </c>
+      <c r="C34" s="7">
+        <v>59464</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="0"/>
+        <v>39126</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="7"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A35" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="7">
+        <v>21653</v>
+      </c>
+      <c r="C35" s="7">
+        <v>63242</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="0"/>
+        <v>41589</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="7"/>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A36" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="7">
+        <v>21996</v>
+      </c>
+      <c r="C36" s="7">
+        <v>64308</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="0"/>
+        <v>42312</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="7"/>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A37" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="7">
+        <v>23337</v>
+      </c>
+      <c r="C37" s="7">
+        <v>68785</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="0"/>
+        <v>45448</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="7"/>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A38" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="7">
+        <v>23681</v>
+      </c>
+      <c r="C38" s="7">
+        <v>69851</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="0"/>
+        <v>46170</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="7"/>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A39" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="7">
+        <v>24335</v>
+      </c>
+      <c r="C39" s="7">
+        <v>71616</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="0"/>
+        <v>47281</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="7"/>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A40" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="7">
+        <v>24677</v>
+      </c>
+      <c r="C40" s="7">
+        <v>72682</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="0"/>
+        <v>48005</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lode runner v3 - up to level 22
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D7D53D-97CD-44E7-8597-F79DC148C1CC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC83BB7-EDAD-4355-904C-A588188C5742}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40680" yWindow="1230" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="102">
   <si>
     <t>Place</t>
   </si>
@@ -325,6 +325,18 @@
   </si>
   <si>
     <t>Lv20 Start</t>
+  </si>
+  <si>
+    <t>Lv20 End</t>
+  </si>
+  <si>
+    <t>Lv21 Start</t>
+  </si>
+  <si>
+    <t>Lv21 End</t>
+  </si>
+  <si>
+    <t>Lv22 Start</t>
   </si>
 </sst>
 </file>
@@ -780,7 +792,7 @@
   <dimension ref="A1:I278"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1422,39 +1434,63 @@
       </c>
     </row>
     <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="7"/>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A41" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="7">
+        <v>25622</v>
+      </c>
+      <c r="C41" s="7">
+        <v>76247</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="0"/>
+        <v>50625</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="7"/>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A42" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="7">
+        <v>25966</v>
+      </c>
+      <c r="C42" s="7">
+        <v>77314</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="0"/>
+        <v>51348</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A43" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="7">
+        <v>27212</v>
+      </c>
+      <c r="C43" s="7">
+        <v>81264</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="0"/>
+        <v>54052</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A44" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="7">
+        <v>27564</v>
+      </c>
+      <c r="C44" s="7">
+        <v>82330</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="0"/>
+        <v>54766</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2737,8 +2773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Lode Runner v3 - up to lv 29
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC83BB7-EDAD-4355-904C-A588188C5742}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAB58B2-3A71-430C-87E0-BB0C8797967A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40680" yWindow="1230" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33105" yWindow="1260" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V3" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="125">
   <si>
     <t>Place</t>
   </si>
@@ -337,6 +337,75 @@
   </si>
   <si>
     <t>Lv22 Start</t>
+  </si>
+  <si>
+    <t>Lv22 End</t>
+  </si>
+  <si>
+    <t>Lv23 Start</t>
+  </si>
+  <si>
+    <t>Lv23 End</t>
+  </si>
+  <si>
+    <t>Lv24 Start</t>
+  </si>
+  <si>
+    <t>Lv24 End</t>
+  </si>
+  <si>
+    <t>Lv25 Start</t>
+  </si>
+  <si>
+    <t>Lv25 End</t>
+  </si>
+  <si>
+    <t>Lv26 Start</t>
+  </si>
+  <si>
+    <t>Lv26 End</t>
+  </si>
+  <si>
+    <t>Lv27 Start</t>
+  </si>
+  <si>
+    <t>Lv27 End</t>
+  </si>
+  <si>
+    <t>Lv28 Start</t>
+  </si>
+  <si>
+    <t>Lv29 End</t>
+  </si>
+  <si>
+    <t>Lv28 End</t>
+  </si>
+  <si>
+    <t>Lv29 Start</t>
+  </si>
+  <si>
+    <t>Lv30 Start</t>
+  </si>
+  <si>
+    <t>Lv30 End</t>
+  </si>
+  <si>
+    <t>Lv31 Start</t>
+  </si>
+  <si>
+    <t>Lv31 End</t>
+  </si>
+  <si>
+    <t>Lv32 Start</t>
+  </si>
+  <si>
+    <t>Lv32 End</t>
+  </si>
+  <si>
+    <t>33 Start</t>
+  </si>
+  <si>
+    <t>33 End</t>
   </si>
 </sst>
 </file>
@@ -791,11 +860,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2A8891-531F-43A4-B044-6C02F070C564}">
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1494,513 +1566,769 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A45" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="7">
+        <v>28524</v>
+      </c>
+      <c r="C45" s="7">
+        <v>85561</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="0"/>
+        <v>57037</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="7"/>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A46" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="7">
+        <v>28858</v>
+      </c>
+      <c r="C46" s="7">
+        <v>86638</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="0"/>
+        <v>57780</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="7"/>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A47" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="7">
+        <v>30371</v>
+      </c>
+      <c r="C47" s="7">
+        <v>91585</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="0"/>
+        <v>61214</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="7"/>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A48" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48" s="7">
+        <v>30715</v>
+      </c>
+      <c r="C48" s="7">
+        <v>92653</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="0"/>
+        <v>61938</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A49" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="7">
+        <v>31295</v>
+      </c>
+      <c r="C49" s="7">
+        <v>94453</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="0"/>
+        <v>63158</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A50" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" s="7">
+        <v>31638</v>
+      </c>
+      <c r="C50" s="7">
+        <v>95520</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="0"/>
+        <v>63882</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A51" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" s="7">
+        <v>32598</v>
+      </c>
+      <c r="C51" s="7">
+        <v>98559</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="0"/>
+        <v>65961</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A52" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="7">
+        <v>32943</v>
+      </c>
+      <c r="C52" s="7">
+        <v>99625</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="0"/>
+        <v>66682</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A53" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" s="7">
+        <v>34210</v>
+      </c>
+      <c r="C53" s="7">
+        <v>103385</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="0"/>
+        <v>69175</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="7"/>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A54" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="7">
+        <v>34554</v>
+      </c>
+      <c r="C54" s="7">
+        <v>104452</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="0"/>
+        <v>69898</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A55" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" s="7">
+        <v>36007</v>
+      </c>
+      <c r="C55" s="7">
+        <v>109774</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="0"/>
+        <v>73767</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A56" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" s="7">
+        <v>36350</v>
+      </c>
+      <c r="C56" s="7">
+        <v>110117</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" si="0"/>
+        <v>73767</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A57" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" s="7">
+        <v>37554</v>
+      </c>
+      <c r="C57" s="7">
+        <v>113806</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" si="0"/>
+        <v>76252</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="7"/>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A58" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="7">
+        <v>37897</v>
+      </c>
+      <c r="C58" s="2">
+        <v>114157</v>
+      </c>
+      <c r="D58" s="3">
+        <f t="shared" si="0"/>
+        <v>76260</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="7"/>
+      <c r="A59" s="7" t="s">
+        <v>114</v>
+      </c>
       <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
+      <c r="C59" s="2">
+        <v>117904</v>
+      </c>
       <c r="D59" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="7"/>
+      <c r="A60" s="7" t="s">
+        <v>117</v>
+      </c>
       <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
+      <c r="C60" s="2">
+        <v>118257</v>
+      </c>
       <c r="D60" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
+      <c r="A61" s="7" t="s">
+        <v>118</v>
+      </c>
       <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
+      <c r="C61" s="2">
+        <v>121857</v>
+      </c>
       <c r="D61" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
+      <c r="A62" s="7" t="s">
+        <v>119</v>
+      </c>
       <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
+      <c r="C62" s="2">
+        <v>122218</v>
+      </c>
       <c r="D62" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
+      <c r="A63" s="7" t="s">
+        <v>120</v>
+      </c>
       <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
+      <c r="C63" s="2">
+        <v>123474</v>
+      </c>
       <c r="D63" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="7"/>
+      <c r="A64" s="7" t="s">
+        <v>121</v>
+      </c>
       <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
+      <c r="C64" s="2">
+        <v>123817</v>
+      </c>
       <c r="D64" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="7"/>
+      <c r="A65" s="7" t="s">
+        <v>122</v>
+      </c>
       <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
+      <c r="C65" s="2">
+        <v>127138</v>
+      </c>
       <c r="D65" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="7"/>
+      <c r="A66" s="7" t="s">
+        <v>123</v>
+      </c>
       <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
+      <c r="C66" s="2">
+        <v>127481</v>
+      </c>
       <c r="D66" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="7"/>
+      <c r="A67" s="7" t="s">
+        <v>124</v>
+      </c>
       <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
+      <c r="C67" s="2">
+        <v>130266</v>
+      </c>
       <c r="D67" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="7"/>
+      <c r="A68" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
+      <c r="C68" s="2">
+        <v>130612</v>
+      </c>
       <c r="D68" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="7"/>
+      <c r="A69" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
+      <c r="C69" s="2">
+        <v>134030</v>
+      </c>
       <c r="D69" s="3" t="str">
         <f t="shared" ref="D69:D132" si="1">IF(C69&lt;&gt;"",IF(B69&lt;&gt;"",C69-B69,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="7"/>
+      <c r="A70" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
+      <c r="C70" s="2">
+        <v>134376</v>
+      </c>
       <c r="D70" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="7"/>
+      <c r="A71" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
+      <c r="C71" s="2">
+        <v>137722</v>
+      </c>
       <c r="D71" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="7"/>
+      <c r="A72" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
+      <c r="C72" s="2">
+        <v>138065</v>
+      </c>
       <c r="D72" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="7"/>
+      <c r="A73" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
+      <c r="C73" s="2">
+        <v>140702</v>
+      </c>
       <c r="D73" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="7"/>
+      <c r="A74" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
+      <c r="C74" s="2">
+        <v>141046</v>
+      </c>
       <c r="D74" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="7"/>
+      <c r="A75" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
+      <c r="C75" s="2">
+        <v>144332</v>
+      </c>
       <c r="D75" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="7"/>
+      <c r="A76" s="7" t="s">
+        <v>48</v>
+      </c>
       <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
+      <c r="C76" s="2">
+        <v>144676</v>
+      </c>
       <c r="D76" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
+      <c r="A77" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
+      <c r="C77" s="2">
+        <v>148440</v>
+      </c>
       <c r="D77" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="7"/>
+      <c r="A78" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
+      <c r="C78" s="2">
+        <v>148783</v>
+      </c>
       <c r="D78" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="7"/>
+      <c r="A79" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
+      <c r="C79" s="2">
+        <v>150650</v>
+      </c>
       <c r="D79" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="7"/>
+      <c r="A80" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
+      <c r="C80" s="2">
+        <v>150993</v>
+      </c>
       <c r="D80" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="7"/>
+      <c r="A81" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
+      <c r="C81" s="2">
+        <v>155366</v>
+      </c>
       <c r="D81" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="7"/>
+      <c r="A82" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
+      <c r="C82" s="2">
+        <v>155709</v>
+      </c>
       <c r="D82" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="7"/>
+      <c r="A83" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="B83" s="7"/>
-      <c r="C83" s="7"/>
+      <c r="C83" s="7">
+        <v>159691</v>
+      </c>
       <c r="D83" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="7"/>
+      <c r="A84" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="B84" s="7"/>
-      <c r="C84" s="7"/>
+      <c r="C84" s="2">
+        <v>160034</v>
+      </c>
       <c r="D84" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="7"/>
+      <c r="A85" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="B85" s="7"/>
-      <c r="C85" s="7"/>
+      <c r="C85" s="2">
+        <v>164319</v>
+      </c>
       <c r="D85" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="7"/>
+      <c r="A86" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="B86" s="7"/>
-      <c r="C86" s="7"/>
+      <c r="C86" s="2">
+        <v>164662</v>
+      </c>
       <c r="D86" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="7"/>
+      <c r="A87" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
+      <c r="C87" s="2">
+        <v>166649</v>
+      </c>
       <c r="D87" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="7"/>
+      <c r="A88" s="5" t="s">
+        <v>19</v>
+      </c>
       <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
+      <c r="C88" s="2">
+        <v>167000</v>
+      </c>
       <c r="D88" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="7"/>
+      <c r="A89" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="B89" s="7"/>
-      <c r="C89" s="7"/>
+      <c r="C89" s="2">
+        <v>169447</v>
+      </c>
       <c r="D89" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="7"/>
+      <c r="A90" s="5" t="s">
+        <v>20</v>
+      </c>
       <c r="B90" s="7"/>
-      <c r="C90" s="7"/>
+      <c r="C90" s="2">
+        <v>169791</v>
+      </c>
       <c r="D90" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="7"/>
+      <c r="A91" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
+      <c r="C91" s="2">
+        <v>173339</v>
+      </c>
       <c r="D91" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="7"/>
+      <c r="A92" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="B92" s="7"/>
-      <c r="C92" s="7"/>
+      <c r="C92" s="2">
+        <v>173683</v>
+      </c>
       <c r="D92" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="7"/>
+      <c r="A93" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="B93" s="7"/>
-      <c r="C93" s="7"/>
+      <c r="C93" s="2">
+        <v>176533</v>
+      </c>
       <c r="D93" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="7"/>
+      <c r="A94" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="B94" s="7"/>
-      <c r="C94" s="7"/>
+      <c r="C94" s="2">
+        <v>176876</v>
+      </c>
       <c r="D94" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="7"/>
+      <c r="A95" s="5" t="s">
+        <v>42</v>
+      </c>
       <c r="B95" s="7"/>
-      <c r="C95" s="7"/>
+      <c r="C95" s="2">
+        <v>180458</v>
+      </c>
       <c r="D95" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="7"/>
+      <c r="A96" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
+      <c r="C96" s="2">
+        <v>180802</v>
+      </c>
       <c r="D96" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="7"/>
+      <c r="A97" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="B97" s="7"/>
-      <c r="C97" s="7"/>
+      <c r="C97" s="2">
+        <v>184073</v>
+      </c>
       <c r="D97" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="7"/>
+      <c r="A98" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="B98" s="7"/>
-      <c r="C98" s="7"/>
+      <c r="C98" s="2">
+        <v>184417</v>
+      </c>
       <c r="D98" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99" s="7"/>
+      <c r="A99" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="B99" s="7"/>
-      <c r="C99" s="7"/>
+      <c r="C99" s="2">
+        <v>187660</v>
+      </c>
       <c r="D99" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="7"/>
+      <c r="A100" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="B100" s="7"/>
-      <c r="C100" s="7"/>
+      <c r="C100" s="2">
+        <v>188004</v>
+      </c>
       <c r="D100" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="7"/>
+      <c r="A101" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B101" s="7"/>
-      <c r="C101" s="7"/>
+      <c r="C101" s="2">
+        <v>191201</v>
+      </c>
       <c r="D101" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>
@@ -2773,8 +3101,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42:A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
lode runner v3 - up to lv 32
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CAB58B2-3A71-430C-87E0-BB0C8797967A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229E3DFF-8511-4AA4-8A15-268B6DCA1ACF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33105" yWindow="1260" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2A8891-531F-43A4-B044-6C02F070C564}">
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1779,78 +1779,90 @@
       <c r="A59" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B59" s="7"/>
+      <c r="B59" s="7">
+        <v>39284</v>
+      </c>
       <c r="C59" s="2">
         <v>117904</v>
       </c>
-      <c r="D59" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D59" s="3">
+        <f t="shared" si="0"/>
+        <v>78620</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B60" s="7"/>
+      <c r="B60" s="7">
+        <v>39630</v>
+      </c>
       <c r="C60" s="2">
         <v>118257</v>
       </c>
-      <c r="D60" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D60" s="3">
+        <f t="shared" si="0"/>
+        <v>78627</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B61" s="7"/>
+      <c r="B61" s="7">
+        <v>40613</v>
+      </c>
       <c r="C61" s="2">
         <v>121857</v>
       </c>
-      <c r="D61" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D61" s="3">
+        <f t="shared" si="0"/>
+        <v>81244</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B62" s="7"/>
+      <c r="B62" s="7">
+        <v>40936</v>
+      </c>
       <c r="C62" s="2">
         <v>122218</v>
       </c>
-      <c r="D62" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D62" s="3">
+        <f t="shared" si="0"/>
+        <v>81282</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B63" s="7"/>
+      <c r="B63" s="7">
+        <v>41401</v>
+      </c>
       <c r="C63" s="2">
         <v>123474</v>
       </c>
-      <c r="D63" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D63" s="3">
+        <f t="shared" si="0"/>
+        <v>82073</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B64" s="7"/>
+      <c r="B64" s="7">
+        <v>41746</v>
+      </c>
       <c r="C64" s="2">
         <v>123817</v>
       </c>
-      <c r="D64" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D64" s="3">
+        <f t="shared" si="0"/>
+        <v>82071</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lode runner v3 - up to Lv35
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{229E3DFF-8511-4AA4-8A15-268B6DCA1ACF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD42A33F-F65B-4328-968C-9B3A324CF0FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33105" yWindow="1260" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2A8891-531F-43A4-B044-6C02F070C564}">
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1869,91 +1869,105 @@
       <c r="A65" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B65" s="7"/>
+      <c r="B65" s="7">
+        <v>42744</v>
+      </c>
       <c r="C65" s="2">
         <v>127138</v>
       </c>
-      <c r="D65" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D65" s="3">
+        <f t="shared" si="0"/>
+        <v>84394</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B66" s="7"/>
+      <c r="B66" s="7">
+        <v>43088</v>
+      </c>
       <c r="C66" s="2">
         <v>127481</v>
       </c>
-      <c r="D66" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D66" s="3">
+        <f t="shared" si="0"/>
+        <v>84393</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B67" s="7"/>
+      <c r="B67" s="7">
+        <v>44004</v>
+      </c>
       <c r="C67" s="2">
         <v>130266</v>
       </c>
-      <c r="D67" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D67" s="3">
+        <f t="shared" si="0"/>
+        <v>86262</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B68" s="7"/>
+      <c r="B68" s="7">
+        <v>44352</v>
+      </c>
       <c r="C68" s="2">
         <v>130612</v>
       </c>
-      <c r="D68" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D68" s="3">
+        <f t="shared" si="0"/>
+        <v>86260</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B69" s="7"/>
+      <c r="B69" s="7">
+        <v>45313</v>
+      </c>
       <c r="C69" s="2">
         <v>134030</v>
       </c>
-      <c r="D69" s="3" t="str">
+      <c r="D69" s="3">
         <f t="shared" ref="D69:D132" si="1">IF(C69&lt;&gt;"",IF(B69&lt;&gt;"",C69-B69,"-"), "-")</f>
-        <v>-</v>
+        <v>88717</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B70" s="7"/>
+      <c r="B70" s="7">
+        <v>45657</v>
+      </c>
       <c r="C70" s="2">
         <v>134376</v>
       </c>
-      <c r="D70" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D70" s="3">
+        <f t="shared" si="1"/>
+        <v>88719</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B71" s="7"/>
+      <c r="B71" s="7">
+        <v>46614</v>
+      </c>
       <c r="C71" s="2">
         <v>137722</v>
       </c>
-      <c r="D71" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D71" s="3">
+        <f t="shared" si="1"/>
+        <v>91108</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lode runner v3 - up to lv 45
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD42A33F-F65B-4328-968C-9B3A324CF0FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5485AC1-E524-4CA8-BE9F-690DEBFBFC32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33105" yWindow="1260" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2A8891-531F-43A4-B044-6C02F070C564}">
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="B72" sqref="B72"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="B90" sqref="B90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1974,234 +1974,270 @@
       <c r="A72" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B72" s="7"/>
+      <c r="B72" s="7">
+        <v>46958</v>
+      </c>
       <c r="C72" s="2">
         <v>138065</v>
       </c>
-      <c r="D72" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D72" s="3">
+        <f t="shared" si="1"/>
+        <v>91107</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B73" s="7"/>
+      <c r="B73" s="7">
+        <v>47930</v>
+      </c>
       <c r="C73" s="2">
         <v>140702</v>
       </c>
-      <c r="D73" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D73" s="3">
+        <f t="shared" si="1"/>
+        <v>92772</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B74" s="7"/>
+      <c r="B74" s="7">
+        <v>48273</v>
+      </c>
       <c r="C74" s="2">
         <v>141046</v>
       </c>
-      <c r="D74" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D74" s="3">
+        <f t="shared" si="1"/>
+        <v>92773</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B75" s="7"/>
+      <c r="B75" s="7">
+        <v>49356</v>
+      </c>
       <c r="C75" s="2">
         <v>144332</v>
       </c>
-      <c r="D75" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D75" s="3">
+        <f t="shared" si="1"/>
+        <v>94976</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B76" s="7"/>
+      <c r="B76" s="7">
+        <v>49699</v>
+      </c>
       <c r="C76" s="2">
         <v>144676</v>
       </c>
-      <c r="D76" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D76" s="3">
+        <f t="shared" si="1"/>
+        <v>94977</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B77" s="7"/>
+      <c r="B77" s="7">
+        <v>50839</v>
+      </c>
       <c r="C77" s="2">
         <v>148440</v>
       </c>
-      <c r="D77" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D77" s="3">
+        <f t="shared" si="1"/>
+        <v>97601</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B78" s="7"/>
+      <c r="B78" s="7">
+        <v>51182</v>
+      </c>
       <c r="C78" s="2">
         <v>148783</v>
       </c>
-      <c r="D78" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D78" s="3">
+        <f t="shared" si="1"/>
+        <v>97601</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B79" s="7"/>
+      <c r="B79" s="7">
+        <v>51882</v>
+      </c>
       <c r="C79" s="2">
         <v>150650</v>
       </c>
-      <c r="D79" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D79" s="3">
+        <f t="shared" si="1"/>
+        <v>98768</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B80" s="7"/>
+      <c r="B80" s="7">
+        <v>52225</v>
+      </c>
       <c r="C80" s="2">
         <v>150993</v>
       </c>
-      <c r="D80" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D80" s="3">
+        <f t="shared" si="1"/>
+        <v>98768</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B81" s="7"/>
+      <c r="B81" s="7">
+        <v>53516</v>
+      </c>
       <c r="C81" s="2">
         <v>155366</v>
       </c>
-      <c r="D81" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D81" s="3">
+        <f t="shared" si="1"/>
+        <v>101850</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B82" s="7"/>
+      <c r="B82" s="7">
+        <v>53860</v>
+      </c>
       <c r="C82" s="2">
         <v>155709</v>
       </c>
-      <c r="D82" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D82" s="3">
+        <f t="shared" si="1"/>
+        <v>101849</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B83" s="7"/>
+      <c r="B83" s="7">
+        <v>55029</v>
+      </c>
       <c r="C83" s="7">
         <v>159691</v>
       </c>
-      <c r="D83" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D83" s="3">
+        <f t="shared" si="1"/>
+        <v>104662</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B84" s="7"/>
+      <c r="B84" s="7">
+        <v>55373</v>
+      </c>
       <c r="C84" s="2">
         <v>160034</v>
       </c>
-      <c r="D84" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D84" s="3">
+        <f t="shared" si="1"/>
+        <v>104661</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B85" s="7"/>
+      <c r="B85" s="7">
+        <v>56774</v>
+      </c>
       <c r="C85" s="2">
         <v>164319</v>
       </c>
-      <c r="D85" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D85" s="3">
+        <f t="shared" si="1"/>
+        <v>107545</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B86" s="7"/>
+      <c r="B86" s="7">
+        <v>57118</v>
+      </c>
       <c r="C86" s="2">
         <v>164662</v>
       </c>
-      <c r="D86" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D86" s="3">
+        <f t="shared" si="1"/>
+        <v>107544</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B87" s="7"/>
+      <c r="B87" s="7">
+        <v>57747</v>
+      </c>
       <c r="C87" s="2">
         <v>166649</v>
       </c>
-      <c r="D87" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D87" s="3">
+        <f t="shared" si="1"/>
+        <v>108902</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B88" s="7"/>
+      <c r="B88" s="7">
+        <v>58090</v>
+      </c>
       <c r="C88" s="2">
         <v>167000</v>
       </c>
-      <c r="D88" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D88" s="3">
+        <f t="shared" si="1"/>
+        <v>108910</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B89" s="7"/>
+      <c r="B89" s="7">
+        <v>59219</v>
+      </c>
       <c r="C89" s="2">
         <v>169447</v>
       </c>
-      <c r="D89" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D89" s="3">
+        <f t="shared" si="1"/>
+        <v>110228</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3127,8 +3163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42:A75"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
lode runner v3 - up to lv 47
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5485AC1-E524-4CA8-BE9F-690DEBFBFC32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282833BF-F005-46B2-8F45-B579BF89468D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33105" yWindow="1260" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32670" yWindow="1005" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V3" sheetId="3" r:id="rId1"/>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2A8891-531F-43A4-B044-6C02F070C564}">
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B90" sqref="B90"/>
+    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2105,7 +2105,7 @@
         <v>98768</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>35</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>101850</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>16</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>101849</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>36</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>104662</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>17</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>104661</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>37</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>107545</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>18</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>107544</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>38</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>108902</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>19</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>108910</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>39</v>
       </c>
@@ -2240,59 +2240,70 @@
         <v>110228</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B90" s="7"/>
+      <c r="B90" s="7">
+        <v>59562</v>
+      </c>
       <c r="C90" s="2">
         <v>169791</v>
       </c>
-      <c r="D90" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D90" s="3">
+        <f t="shared" si="1"/>
+        <v>110229</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B91" s="7"/>
+      <c r="B91" s="7">
+        <v>60447</v>
+      </c>
       <c r="C91" s="2">
         <v>173339</v>
       </c>
-      <c r="D91" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D91" s="3">
+        <f t="shared" si="1"/>
+        <v>112892</v>
+      </c>
+      <c r="E91">
+        <v>60489</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B92" s="7"/>
+      <c r="B92" s="7">
+        <v>60833</v>
+      </c>
       <c r="C92" s="2">
         <v>173683</v>
       </c>
-      <c r="D92" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D92" s="3">
+        <f t="shared" si="1"/>
+        <v>112850</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B93" s="7"/>
+      <c r="B93" s="7">
+        <v>61723</v>
+      </c>
       <c r="C93" s="2">
         <v>176533</v>
       </c>
-      <c r="D93" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="D93" s="3">
+        <f t="shared" si="1"/>
+        <v>114810</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>22</v>
       </c>
@@ -2305,7 +2316,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>42</v>
       </c>
@@ -2318,7 +2329,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>23</v>
       </c>

</xml_diff>

<commit_message>
lode runner - v3 finished, 67116 frames
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282833BF-F005-46B2-8F45-B579BF89468D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD59441C-9FD5-400C-978F-7FFEA4B0E094}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32670" yWindow="1005" windowWidth="15555" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41880" yWindow="4335" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V3" sheetId="3" r:id="rId1"/>
@@ -860,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2A8891-531F-43A4-B044-6C02F070C564}">
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2105,7 +2105,7 @@
         <v>98768</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>35</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>101850</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>16</v>
       </c>
@@ -2135,7 +2135,7 @@
         <v>101849</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>36</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>104662</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>17</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>104661</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>37</v>
       </c>
@@ -2180,7 +2180,7 @@
         <v>107545</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
         <v>18</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>107544</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
         <v>38</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>108902</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
         <v>19</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>108910</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>39</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>110228</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>20</v>
       </c>
@@ -2255,7 +2255,7 @@
         <v>110229</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>40</v>
       </c>
@@ -2269,11 +2269,8 @@
         <f t="shared" si="1"/>
         <v>112892</v>
       </c>
-      <c r="E91">
-        <v>60489</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>21</v>
       </c>
@@ -2288,7 +2285,7 @@
         <v>112850</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>41</v>
       </c>
@@ -2303,108 +2300,124 @@
         <v>114810</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B94" s="7"/>
+      <c r="B94" s="7">
+        <v>62069</v>
+      </c>
       <c r="C94" s="2">
         <v>176876</v>
       </c>
-      <c r="D94" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D94" s="3">
+        <f t="shared" si="1"/>
+        <v>114807</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B95" s="7"/>
+      <c r="B95" s="7">
+        <v>63206</v>
+      </c>
       <c r="C95" s="2">
         <v>180458</v>
       </c>
-      <c r="D95" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="D95" s="3">
+        <f t="shared" si="1"/>
+        <v>117252</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B96" s="7"/>
+      <c r="B96" s="7">
+        <v>63549</v>
+      </c>
       <c r="C96" s="2">
         <v>180802</v>
       </c>
-      <c r="D96" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D96" s="3">
+        <f t="shared" si="1"/>
+        <v>117253</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B97" s="7"/>
+      <c r="B97" s="7">
+        <v>64475</v>
+      </c>
       <c r="C97" s="2">
         <v>184073</v>
       </c>
-      <c r="D97" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D97" s="3">
+        <f t="shared" si="1"/>
+        <v>119598</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B98" s="7"/>
+      <c r="B98" s="7">
+        <v>64818</v>
+      </c>
       <c r="C98" s="2">
         <v>184417</v>
       </c>
-      <c r="D98" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D98" s="3">
+        <f t="shared" si="1"/>
+        <v>119599</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B99" s="7"/>
+      <c r="B99" s="7">
+        <v>65880</v>
+      </c>
       <c r="C99" s="2">
         <v>187660</v>
       </c>
-      <c r="D99" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D99" s="3">
+        <f t="shared" si="1"/>
+        <v>121780</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B100" s="7"/>
+      <c r="B100" s="7">
+        <v>66223</v>
+      </c>
       <c r="C100" s="2">
         <v>188004</v>
       </c>
-      <c r="D100" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D100" s="3">
+        <f t="shared" si="1"/>
+        <v>121781</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B101" s="7"/>
+      <c r="B101" s="7">
+        <v>67116</v>
+      </c>
       <c r="C101" s="2">
         <v>191201</v>
       </c>
-      <c r="D101" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="D101" s="3">
+        <f t="shared" si="1"/>
+        <v>124085</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
start lode runner v4 - up to level 3, 46 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD59441C-9FD5-400C-978F-7FFEA4B0E094}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DB18BE-902E-40F5-BD05-8CDC904F7E68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41880" yWindow="4335" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43650" yWindow="3900" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="V3" sheetId="3" r:id="rId1"/>
-    <sheet name="V2" sheetId="1" r:id="rId2"/>
+    <sheet name="V4" sheetId="4" r:id="rId1"/>
+    <sheet name="V3" sheetId="3" r:id="rId2"/>
+    <sheet name="V2" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="128">
   <si>
     <t>Place</t>
   </si>
@@ -406,6 +407,15 @@
   </si>
   <si>
     <t>33 End</t>
+  </si>
+  <si>
+    <t>v4</t>
+  </si>
+  <si>
+    <t>end = frame S is pressed</t>
+  </si>
+  <si>
+    <t>Lv11 End</t>
   </si>
 </sst>
 </file>
@@ -415,12 +425,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -518,25 +535,26 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
@@ -857,11 +875,1934 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06DA051-0308-42D5-B7F7-51E79FAF1C31}">
+  <dimension ref="A1:F278"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2">
+        <v>444</v>
+      </c>
+      <c r="D2" s="3" t="str">
+        <f>IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="F2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="7">
+        <v>1052</v>
+      </c>
+      <c r="C3" s="7">
+        <v>1068</v>
+      </c>
+      <c r="D3" s="3">
+        <f>IF(C3&lt;&gt;"",IF(B3&lt;&gt;"",C3-B3,"-"), "-")</f>
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1389</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1408</v>
+      </c>
+      <c r="D4" s="3">
+        <f t="shared" ref="D4:D68" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="7">
+        <v>2296</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2342</v>
+      </c>
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7">
+        <v>2679</v>
+      </c>
+      <c r="D6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7">
+        <v>3814</v>
+      </c>
+      <c r="D8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7">
+        <v>4991</v>
+      </c>
+      <c r="D10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7">
+        <v>6010</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7">
+        <v>7761</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7">
+        <v>8902</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7">
+        <v>10028</v>
+      </c>
+      <c r="D18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7">
+        <v>11780</v>
+      </c>
+      <c r="D20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B28" s="7"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B30" s="7"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A32" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B47" s="7"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B48" s="7"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" s="7"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" s="7"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" s="7"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B57" s="7"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B62" s="7"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B63" s="7"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B65" s="7"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B66" s="7"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="3" t="str">
+        <f t="shared" ref="D69:D132" si="1">IF(C69&lt;&gt;"",IF(B69&lt;&gt;"",C69-B69,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B75" s="7"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B78" s="7"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B79" s="7"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B80" s="7"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B82" s="7"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B83" s="7"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B84" s="7"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B85" s="7"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B86" s="7"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B87" s="7"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B88" s="7"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B89" s="7"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B90" s="7"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B91" s="7"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B92" s="7"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B93" s="7"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B94" s="7"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B95" s="7"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B96" s="7"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B97" s="7"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B98" s="7"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B99" s="7"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="7"/>
+      <c r="B102" s="7"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="7"/>
+      <c r="B103" s="7"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="7"/>
+      <c r="B104" s="7"/>
+      <c r="C104" s="7"/>
+      <c r="D104" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="7"/>
+      <c r="B105" s="7"/>
+      <c r="C105" s="7"/>
+      <c r="D105" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="7"/>
+      <c r="B106" s="7"/>
+      <c r="C106" s="7"/>
+      <c r="D106" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="7"/>
+      <c r="B107" s="7"/>
+      <c r="C107" s="7"/>
+      <c r="D107" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="7"/>
+      <c r="B108" s="7"/>
+      <c r="C108" s="7"/>
+      <c r="D108" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="7"/>
+      <c r="B109" s="7"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="7"/>
+      <c r="B110" s="7"/>
+      <c r="C110" s="7"/>
+      <c r="D110" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111" s="7"/>
+      <c r="B111" s="7"/>
+      <c r="C111" s="7"/>
+      <c r="D111" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="7"/>
+      <c r="B112" s="7"/>
+      <c r="C112" s="7"/>
+      <c r="D112" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A113" s="7"/>
+      <c r="B113" s="7"/>
+      <c r="C113" s="7"/>
+      <c r="D113" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A114" s="7"/>
+      <c r="B114" s="7"/>
+      <c r="C114" s="7"/>
+      <c r="D114" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A115" s="7"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="7"/>
+      <c r="D115" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A116" s="7"/>
+      <c r="B116" s="7"/>
+      <c r="C116" s="7"/>
+      <c r="D116" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A117" s="7"/>
+      <c r="B117" s="7"/>
+      <c r="C117" s="7"/>
+      <c r="D117" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A118" s="7"/>
+      <c r="B118" s="7"/>
+      <c r="C118" s="7"/>
+      <c r="D118" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A119" s="7"/>
+      <c r="B119" s="7"/>
+      <c r="C119" s="7"/>
+      <c r="D119" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A120" s="7"/>
+      <c r="B120" s="7"/>
+      <c r="C120" s="7"/>
+      <c r="D120" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A121" s="7"/>
+      <c r="B121" s="7"/>
+      <c r="C121" s="7"/>
+      <c r="D121" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A122" s="7"/>
+      <c r="B122" s="7"/>
+      <c r="C122" s="7"/>
+      <c r="D122" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A123" s="7"/>
+      <c r="B123" s="7"/>
+      <c r="C123" s="7"/>
+      <c r="D123" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A124" s="7"/>
+      <c r="B124" s="7"/>
+      <c r="C124" s="7"/>
+      <c r="D124" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A125" s="7"/>
+      <c r="B125" s="7"/>
+      <c r="C125" s="7"/>
+      <c r="D125" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A126" s="7"/>
+      <c r="B126" s="7"/>
+      <c r="C126" s="7"/>
+      <c r="D126" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A127" s="7"/>
+      <c r="B127" s="7"/>
+      <c r="C127" s="7"/>
+      <c r="D127" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A128" s="7"/>
+      <c r="B128" s="7"/>
+      <c r="C128" s="7"/>
+      <c r="D128" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A129" s="7"/>
+      <c r="B129" s="7"/>
+      <c r="C129" s="7"/>
+      <c r="D129" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A130" s="7"/>
+      <c r="B130" s="7"/>
+      <c r="C130" s="7"/>
+      <c r="D130" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A131" s="7"/>
+      <c r="B131" s="7"/>
+      <c r="C131" s="7"/>
+      <c r="D131" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A132" s="7"/>
+      <c r="B132" s="7"/>
+      <c r="C132" s="7"/>
+      <c r="D132" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A133" s="7"/>
+      <c r="B133" s="7"/>
+      <c r="C133" s="7"/>
+      <c r="D133" s="3" t="str">
+        <f t="shared" ref="D133:D137" si="2">IF(C133&lt;&gt;"",IF(B133&lt;&gt;"",C133-B133,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A134" s="7"/>
+      <c r="B134" s="7"/>
+      <c r="C134" s="7"/>
+      <c r="D134" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A135" s="7"/>
+      <c r="B135" s="7"/>
+      <c r="C135" s="7"/>
+      <c r="D135" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A136" s="7"/>
+      <c r="B136" s="7"/>
+      <c r="D136" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A137" s="7"/>
+      <c r="B137" s="7"/>
+      <c r="D137" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A138" s="7"/>
+      <c r="B138" s="7"/>
+      <c r="D138" s="3" t="str">
+        <f t="shared" ref="D138:D139" si="3">IF(C138&lt;&gt;"",IF(B138&lt;&gt;"",B138-C138,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A139" s="7"/>
+      <c r="B139" s="7"/>
+      <c r="D139" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A140" s="7"/>
+      <c r="B140" s="7"/>
+    </row>
+    <row r="141" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A141" s="7"/>
+      <c r="B141" s="7"/>
+    </row>
+    <row r="142" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B142" s="7"/>
+    </row>
+    <row r="143" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B143" s="7"/>
+    </row>
+    <row r="144" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B144" s="7"/>
+    </row>
+    <row r="145" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B145" s="7"/>
+    </row>
+    <row r="146" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B146" s="7"/>
+    </row>
+    <row r="147" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B147" s="7"/>
+    </row>
+    <row r="148" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B148" s="7"/>
+    </row>
+    <row r="149" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B149" s="7"/>
+    </row>
+    <row r="150" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B150" s="7"/>
+    </row>
+    <row r="151" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B151" s="7"/>
+    </row>
+    <row r="152" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B152" s="7"/>
+    </row>
+    <row r="153" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B153" s="7"/>
+    </row>
+    <row r="154" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B154" s="7"/>
+    </row>
+    <row r="155" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B155" s="7"/>
+    </row>
+    <row r="156" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B156" s="7"/>
+    </row>
+    <row r="157" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B157" s="7"/>
+    </row>
+    <row r="158" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B158" s="7"/>
+    </row>
+    <row r="159" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B159" s="7"/>
+    </row>
+    <row r="160" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B160" s="7"/>
+    </row>
+    <row r="161" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B161" s="7"/>
+    </row>
+    <row r="162" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B162" s="7"/>
+    </row>
+    <row r="163" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B163" s="7"/>
+    </row>
+    <row r="164" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B164" s="7"/>
+    </row>
+    <row r="165" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B165" s="7"/>
+    </row>
+    <row r="166" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B166" s="7"/>
+    </row>
+    <row r="167" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B167" s="7"/>
+    </row>
+    <row r="168" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B168" s="7"/>
+    </row>
+    <row r="169" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B169" s="7"/>
+    </row>
+    <row r="170" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B170" s="7"/>
+    </row>
+    <row r="171" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B171" s="7"/>
+    </row>
+    <row r="172" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B172" s="7"/>
+    </row>
+    <row r="173" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B173" s="7"/>
+    </row>
+    <row r="174" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B174" s="7"/>
+    </row>
+    <row r="175" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B175" s="7"/>
+    </row>
+    <row r="176" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B176" s="7"/>
+    </row>
+    <row r="177" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B177" s="7"/>
+    </row>
+    <row r="178" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B178" s="7"/>
+    </row>
+    <row r="179" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B179" s="7"/>
+    </row>
+    <row r="180" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B180" s="7"/>
+    </row>
+    <row r="181" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B181" s="7"/>
+    </row>
+    <row r="182" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B182" s="7"/>
+    </row>
+    <row r="183" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B183" s="7"/>
+    </row>
+    <row r="184" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B184" s="7"/>
+    </row>
+    <row r="185" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B185" s="7"/>
+    </row>
+    <row r="186" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B186" s="7"/>
+    </row>
+    <row r="187" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B187" s="7"/>
+    </row>
+    <row r="188" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B188" s="7"/>
+    </row>
+    <row r="189" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B189" s="7"/>
+    </row>
+    <row r="190" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B190" s="7"/>
+    </row>
+    <row r="191" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B191" s="7"/>
+    </row>
+    <row r="192" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B192" s="7"/>
+    </row>
+    <row r="193" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B193" s="7"/>
+    </row>
+    <row r="194" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B194" s="7"/>
+    </row>
+    <row r="195" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B195" s="7"/>
+    </row>
+    <row r="196" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B196" s="7"/>
+    </row>
+    <row r="197" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B197" s="7"/>
+    </row>
+    <row r="198" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B198" s="7"/>
+    </row>
+    <row r="199" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B199" s="7"/>
+    </row>
+    <row r="200" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B200" s="7"/>
+    </row>
+    <row r="201" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B201" s="7"/>
+    </row>
+    <row r="202" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B202" s="7"/>
+    </row>
+    <row r="203" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B203" s="7"/>
+    </row>
+    <row r="204" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B204" s="7"/>
+    </row>
+    <row r="205" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B205" s="7"/>
+    </row>
+    <row r="206" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B206" s="7"/>
+    </row>
+    <row r="207" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B207" s="7"/>
+    </row>
+    <row r="208" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B208" s="7"/>
+    </row>
+    <row r="209" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B209" s="7"/>
+    </row>
+    <row r="210" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B210" s="7"/>
+    </row>
+    <row r="211" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B211" s="7"/>
+    </row>
+    <row r="212" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B212" s="7"/>
+    </row>
+    <row r="213" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B213" s="7"/>
+    </row>
+    <row r="214" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B214" s="7"/>
+    </row>
+    <row r="215" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B215" s="7"/>
+    </row>
+    <row r="216" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B216" s="7"/>
+    </row>
+    <row r="217" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B217" s="7"/>
+    </row>
+    <row r="218" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B218" s="7"/>
+    </row>
+    <row r="219" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B219" s="7"/>
+    </row>
+    <row r="220" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B220" s="7"/>
+    </row>
+    <row r="221" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B221" s="7"/>
+    </row>
+    <row r="222" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B222" s="7"/>
+    </row>
+    <row r="223" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B223" s="7"/>
+    </row>
+    <row r="224" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B224" s="7"/>
+    </row>
+    <row r="225" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B225" s="7"/>
+    </row>
+    <row r="226" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B226" s="7"/>
+    </row>
+    <row r="227" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B227" s="7"/>
+    </row>
+    <row r="228" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B228" s="7"/>
+    </row>
+    <row r="229" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B229" s="7"/>
+    </row>
+    <row r="230" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B230" s="7"/>
+    </row>
+    <row r="231" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B231" s="7"/>
+    </row>
+    <row r="232" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B232" s="7"/>
+    </row>
+    <row r="233" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B233" s="7"/>
+    </row>
+    <row r="234" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B234" s="7"/>
+    </row>
+    <row r="235" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B235" s="7"/>
+    </row>
+    <row r="236" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B236" s="7"/>
+    </row>
+    <row r="237" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B237" s="7"/>
+    </row>
+    <row r="238" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B238" s="7"/>
+    </row>
+    <row r="239" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B239" s="7"/>
+    </row>
+    <row r="240" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B240" s="7"/>
+    </row>
+    <row r="241" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B241" s="7"/>
+    </row>
+    <row r="242" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B242" s="7"/>
+    </row>
+    <row r="243" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B243" s="7"/>
+    </row>
+    <row r="244" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B244" s="7"/>
+    </row>
+    <row r="245" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B245" s="7"/>
+    </row>
+    <row r="246" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B246" s="7"/>
+    </row>
+    <row r="247" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B247" s="7"/>
+    </row>
+    <row r="248" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B248" s="7"/>
+    </row>
+    <row r="249" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B249" s="7"/>
+    </row>
+    <row r="250" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B250" s="7"/>
+    </row>
+    <row r="251" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B251" s="7"/>
+    </row>
+    <row r="252" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B252" s="7"/>
+    </row>
+    <row r="253" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B253" s="7"/>
+    </row>
+    <row r="254" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B254" s="7"/>
+    </row>
+    <row r="255" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B255" s="7"/>
+    </row>
+    <row r="256" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B256" s="7"/>
+    </row>
+    <row r="257" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B257" s="7"/>
+    </row>
+    <row r="258" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B258" s="7"/>
+    </row>
+    <row r="259" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B259" s="7"/>
+    </row>
+    <row r="260" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B260" s="7"/>
+    </row>
+    <row r="261" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B261" s="7"/>
+    </row>
+    <row r="262" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B262" s="7"/>
+    </row>
+    <row r="263" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B263" s="7"/>
+    </row>
+    <row r="264" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B264" s="7"/>
+    </row>
+    <row r="265" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B265" s="7"/>
+    </row>
+    <row r="266" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B266" s="7"/>
+    </row>
+    <row r="267" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B267" s="7"/>
+    </row>
+    <row r="268" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B268" s="7"/>
+    </row>
+    <row r="269" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B269" s="7"/>
+    </row>
+    <row r="270" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B270" s="7"/>
+    </row>
+    <row r="271" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B271" s="7"/>
+    </row>
+    <row r="272" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B272" s="7"/>
+    </row>
+    <row r="273" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B273" s="7"/>
+    </row>
+    <row r="274" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B274" s="7"/>
+    </row>
+    <row r="275" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B275" s="7"/>
+    </row>
+    <row r="276" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B276" s="7"/>
+    </row>
+    <row r="277" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B277" s="7"/>
+    </row>
+    <row r="278" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B278" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2A8891-531F-43A4-B044-6C02F070C564}">
   <dimension ref="A1:I278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3183,7 +5124,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I75"/>
   <sheetViews>
@@ -4353,7 +6294,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="10" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
lode runner v3 - up to lv 6
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1DB18BE-902E-40F5-BD05-8CDC904F7E68}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65F0358-C039-4AA4-A61B-6206815D6C4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43650" yWindow="3900" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="137">
   <si>
     <t>Place</t>
   </si>
@@ -412,10 +412,37 @@
     <t>v4</t>
   </si>
   <si>
-    <t>end = frame S is pressed</t>
-  </si>
-  <si>
     <t>Lv11 End</t>
+  </si>
+  <si>
+    <t>1st dig</t>
+  </si>
+  <si>
+    <t>1st ladder grab</t>
+  </si>
+  <si>
+    <t>X = 0 start</t>
+  </si>
+  <si>
+    <t>Ladder grab</t>
+  </si>
+  <si>
+    <t>6 delay frames for luck manip</t>
+  </si>
+  <si>
+    <t>mysterious lag</t>
+  </si>
+  <si>
+    <t>top dig</t>
+  </si>
+  <si>
+    <t>end = frame S could be pressed</t>
+  </si>
+  <si>
+    <t>Lv5 X=0 Start</t>
+  </si>
+  <si>
+    <t>Lv6 X=0 Start</t>
   </si>
 </sst>
 </file>
@@ -876,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06DA051-0308-42D5-B7F7-51E79FAF1C31}">
-  <dimension ref="A1:F278"/>
+  <dimension ref="A1:F284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -932,7 +959,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -946,7 +973,7 @@
         <v>1408</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:D68" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
+        <f t="shared" ref="D4:D74" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
         <v>19</v>
       </c>
     </row>
@@ -969,33 +996,42 @@
       <c r="A6" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="7"/>
+      <c r="B6" s="7">
+        <v>2634</v>
+      </c>
       <c r="C6" s="7">
         <v>2679</v>
       </c>
-      <c r="D6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A7" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" s="7">
+        <v>2957</v>
+      </c>
+      <c r="C7" s="7">
+        <v>2987</v>
+      </c>
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>66</v>
+      <c r="A8" s="8" t="s">
+        <v>128</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7">
-        <v>3814</v>
+        <v>3004</v>
       </c>
       <c r="D8" s="3" t="str">
         <f t="shared" si="0"/>
@@ -1003,11 +1039,13 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>67</v>
+      <c r="A9" s="8" t="s">
+        <v>127</v>
       </c>
       <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="C9" s="7">
+        <v>3124</v>
+      </c>
       <c r="D9" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1015,116 +1053,145 @@
     </row>
     <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="B10" s="7">
+        <v>3380</v>
+      </c>
       <c r="C10" s="7">
-        <v>4991</v>
-      </c>
-      <c r="D10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>3476</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>66</v>
+      </c>
+      <c r="B11" s="7">
+        <v>3717</v>
+      </c>
+      <c r="C11" s="7">
+        <v>3814</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B12" s="7"/>
+      <c r="A12" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B12" s="7">
+        <v>4031</v>
+      </c>
       <c r="C12" s="7">
-        <v>6010</v>
-      </c>
-      <c r="D12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>4122</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>91</v>
+      </c>
+      <c r="E12" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A13" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="7">
+        <v>4215</v>
+      </c>
+      <c r="C13" s="7">
+        <v>4306</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B14" s="7"/>
+      <c r="A14" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" s="7">
+        <v>4375</v>
+      </c>
       <c r="C14" s="7">
-        <v>7761</v>
-      </c>
-      <c r="D14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>4476</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>101</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>67</v>
+      </c>
+      <c r="B15" s="7">
+        <v>4553</v>
+      </c>
+      <c r="C15" s="7">
+        <v>4654</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B16" s="7"/>
+      <c r="A16" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="7">
+        <v>5209</v>
+      </c>
       <c r="C16" s="7">
-        <v>8902</v>
-      </c>
-      <c r="D16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>5314</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>69</v>
+      </c>
+      <c r="B17" s="7">
+        <v>5536</v>
+      </c>
+      <c r="C17" s="7">
+        <v>5673</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="7"/>
+      <c r="A18" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B18" s="7">
+        <v>6216</v>
+      </c>
       <c r="C18" s="7">
-        <v>10028</v>
-      </c>
-      <c r="D18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>6332</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -1135,12 +1202,10 @@
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B20" s="7"/>
-      <c r="C20" s="7">
-        <v>11780</v>
-      </c>
+      <c r="C20" s="7"/>
       <c r="D20" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1148,7 +1213,7 @@
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -1159,7 +1224,7 @@
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -1169,16 +1234,19 @@
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>127</v>
+      <c r="A23" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1189,7 +1257,7 @@
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1200,7 +1268,7 @@
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
@@ -1211,7 +1279,7 @@
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
@@ -1222,7 +1290,7 @@
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
@@ -1232,19 +1300,16 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>86</v>
+      <c r="A29" s="8" t="s">
+        <v>126</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
-      <c r="D29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1255,7 +1320,7 @@
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1266,7 +1331,7 @@
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1277,7 +1342,7 @@
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1288,7 +1353,7 @@
     </row>
     <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1299,7 +1364,7 @@
     </row>
     <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1310,7 +1375,7 @@
     </row>
     <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1321,7 +1386,7 @@
     </row>
     <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1332,7 +1397,7 @@
     </row>
     <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1343,7 +1408,7 @@
     </row>
     <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1354,7 +1419,7 @@
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1365,7 +1430,7 @@
     </row>
     <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1376,7 +1441,7 @@
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1387,7 +1452,7 @@
     </row>
     <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1398,7 +1463,7 @@
     </row>
     <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1409,7 +1474,7 @@
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1420,7 +1485,7 @@
     </row>
     <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1431,7 +1496,7 @@
     </row>
     <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1442,7 +1507,7 @@
     </row>
     <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1453,7 +1518,7 @@
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1464,7 +1529,7 @@
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1475,7 +1540,7 @@
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1486,7 +1551,7 @@
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1497,7 +1562,7 @@
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1508,7 +1573,7 @@
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1519,7 +1584,7 @@
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1530,7 +1595,7 @@
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1541,7 +1606,7 @@
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1552,7 +1617,7 @@
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1563,7 +1628,7 @@
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1574,7 +1639,7 @@
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1585,7 +1650,7 @@
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1596,7 +1661,7 @@
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1607,7 +1672,7 @@
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1618,7 +1683,7 @@
     </row>
     <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1629,7 +1694,7 @@
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1640,7 +1705,7 @@
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1651,7 +1716,7 @@
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1661,8 +1726,8 @@
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>10</v>
+      <c r="A68" s="7" t="s">
+        <v>119</v>
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1672,85 +1737,85 @@
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
-        <v>31</v>
+      <c r="A69" s="7" t="s">
+        <v>120</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
       <c r="D69" s="3" t="str">
-        <f t="shared" ref="D69:D132" si="1">IF(C69&lt;&gt;"",IF(B69&lt;&gt;"",C69-B69,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
-        <v>11</v>
+      <c r="A70" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
       <c r="D70" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
-        <v>30</v>
+      <c r="A71" s="7" t="s">
+        <v>122</v>
       </c>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
       <c r="D71" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
-        <v>12</v>
+      <c r="A72" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
       <c r="D72" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
-        <v>32</v>
+      <c r="A73" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
       <c r="D73" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
       <c r="D74" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
-        <v>47</v>
+      <c r="A75" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D75:D138" si="1">IF(C75&lt;&gt;"",IF(B75&lt;&gt;"",C75-B75,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
-        <v>48</v>
+      <c r="A76" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
@@ -1760,8 +1825,8 @@
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
-        <v>33</v>
+      <c r="A77" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1772,7 +1837,7 @@
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1783,7 +1848,7 @@
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1794,7 +1859,7 @@
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1804,8 +1869,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
-        <v>35</v>
+      <c r="A81" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1815,8 +1880,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
-        <v>16</v>
+      <c r="A82" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1826,8 +1891,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
-        <v>36</v>
+      <c r="A83" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1838,7 +1903,7 @@
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1849,7 +1914,7 @@
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1860,7 +1925,7 @@
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1871,7 +1936,7 @@
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1882,7 +1947,7 @@
     </row>
     <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1893,7 +1958,7 @@
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1904,7 +1969,7 @@
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1915,7 +1980,7 @@
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1926,7 +1991,7 @@
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -1937,7 +2002,7 @@
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -1948,7 +2013,7 @@
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -1959,7 +2024,7 @@
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -1970,7 +2035,7 @@
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -1981,7 +2046,7 @@
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -1992,7 +2057,7 @@
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -2003,7 +2068,7 @@
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -2014,7 +2079,7 @@
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -2025,7 +2090,7 @@
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -2035,7 +2100,9 @@
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="7"/>
+      <c r="A102" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
       <c r="D102" s="3" t="str">
@@ -2044,7 +2111,9 @@
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A103" s="7"/>
+      <c r="A103" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
       <c r="D103" s="3" t="str">
@@ -2053,7 +2122,9 @@
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="7"/>
+      <c r="A104" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
       <c r="D104" s="3" t="str">
@@ -2062,7 +2133,9 @@
       </c>
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="7"/>
+      <c r="A105" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
       <c r="D105" s="3" t="str">
@@ -2071,7 +2144,9 @@
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="7"/>
+      <c r="A106" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
       <c r="D106" s="3" t="str">
@@ -2080,7 +2155,9 @@
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="7"/>
+      <c r="A107" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
       <c r="D107" s="3" t="str">
@@ -2318,7 +2395,7 @@
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
       <c r="D133" s="3" t="str">
-        <f t="shared" ref="D133:D137" si="2">IF(C133&lt;&gt;"",IF(B133&lt;&gt;"",C133-B133,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2327,7 +2404,7 @@
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
       <c r="D134" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2336,105 +2413,141 @@
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
       <c r="D135" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
+      <c r="C136" s="7"/>
       <c r="D136" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
+      <c r="C137" s="7"/>
       <c r="D137" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
+      <c r="C138" s="7"/>
       <c r="D138" s="3" t="str">
-        <f t="shared" ref="D138:D139" si="3">IF(C138&lt;&gt;"",IF(B138&lt;&gt;"",B138-C138,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
+      <c r="C139" s="7"/>
       <c r="D139" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D139:D143" si="2">IF(C139&lt;&gt;"",IF(B139&lt;&gt;"",C139-B139,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="140" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
+      <c r="C140" s="7"/>
+      <c r="D140" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="141" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
+      <c r="C141" s="7"/>
+      <c r="D141" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="142" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A142" s="7"/>
       <c r="B142" s="7"/>
+      <c r="D142" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="143" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A143" s="7"/>
       <c r="B143" s="7"/>
+      <c r="D143" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="144" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A144" s="7"/>
       <c r="B144" s="7"/>
-    </row>
-    <row r="145" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="D144" s="3" t="str">
+        <f t="shared" ref="D144:D145" si="3">IF(C144&lt;&gt;"",IF(B144&lt;&gt;"",B144-C144,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A145" s="7"/>
       <c r="B145" s="7"/>
-    </row>
-    <row r="146" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="D145" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A146" s="7"/>
       <c r="B146" s="7"/>
     </row>
-    <row r="147" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A147" s="7"/>
       <c r="B147" s="7"/>
     </row>
-    <row r="148" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B148" s="7"/>
     </row>
-    <row r="149" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B149" s="7"/>
     </row>
-    <row r="150" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B150" s="7"/>
     </row>
-    <row r="151" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B151" s="7"/>
     </row>
-    <row r="152" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B152" s="7"/>
     </row>
-    <row r="153" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B153" s="7"/>
     </row>
-    <row r="154" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B154" s="7"/>
     </row>
-    <row r="155" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B155" s="7"/>
     </row>
-    <row r="156" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B156" s="7"/>
     </row>
-    <row r="157" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B157" s="7"/>
     </row>
-    <row r="158" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B158" s="7"/>
     </row>
-    <row r="159" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B159" s="7"/>
     </row>
-    <row r="160" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B160" s="7"/>
     </row>
     <row r="161" spans="2:2" ht="15" x14ac:dyDescent="0.25">
@@ -2790,6 +2903,24 @@
     </row>
     <row r="278" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B278" s="7"/>
+    </row>
+    <row r="279" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B279" s="7"/>
+    </row>
+    <row r="280" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B280" s="7"/>
+    </row>
+    <row r="281" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B281" s="7"/>
+    </row>
+    <row r="282" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B282" s="7"/>
+    </row>
+    <row r="283" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B283" s="7"/>
+    </row>
+    <row r="284" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B284" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Lode Runner v3 - up to level 13, 257 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65F0358-C039-4AA4-A61B-6206815D6C4C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B17E18C-F331-422B-8B62-9F8B8DFFDF53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43650" yWindow="3900" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="144">
   <si>
     <t>Place</t>
   </si>
@@ -424,6 +424,9 @@
     <t>X = 0 start</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>Ladder grab</t>
   </si>
   <si>
@@ -443,6 +446,24 @@
   </si>
   <si>
     <t>Lv6 X=0 Start</t>
+  </si>
+  <si>
+    <t>Lv7 X=0 Start</t>
+  </si>
+  <si>
+    <t>Lv8 X=0 Start</t>
+  </si>
+  <si>
+    <t>Lv9 X=0 Start</t>
+  </si>
+  <si>
+    <t>Lv10 X=0 Start</t>
+  </si>
+  <si>
+    <t>Lv11 X=0 Start</t>
+  </si>
+  <si>
+    <t>Lv13 X=0 Start</t>
   </si>
 </sst>
 </file>
@@ -903,10 +924,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06DA051-0308-42D5-B7F7-51E79FAF1C31}">
-  <dimension ref="A1:F284"/>
+  <dimension ref="A1:F285"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -959,7 +980,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -973,7 +994,7 @@
         <v>1408</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:D74" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
+        <f t="shared" ref="D4:D75" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
         <v>19</v>
       </c>
     </row>
@@ -1022,7 +1043,7 @@
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -1096,12 +1117,12 @@
         <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B13" s="7">
         <v>4215</v>
@@ -1116,7 +1137,7 @@
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B14" s="7">
         <v>4375</v>
@@ -1146,7 +1167,7 @@
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B16" s="7">
         <v>5209</v>
@@ -1176,7 +1197,7 @@
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B18" s="7">
         <v>6216</v>
@@ -1193,167 +1214,230 @@
       <c r="A19" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B19" s="7">
+        <v>7274</v>
+      </c>
+      <c r="C19" s="7">
+        <v>7424</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A20" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="7">
+        <v>7919</v>
+      </c>
+      <c r="C20" s="7">
+        <v>8069</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="7"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B21" s="7">
+        <v>8407</v>
+      </c>
+      <c r="C21" s="7">
+        <v>8564</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A22" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="7">
+        <v>9053</v>
+      </c>
+      <c r="C22" s="7">
+        <v>9210</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="7"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B23" s="7">
+        <v>9481</v>
+      </c>
+      <c r="C23" s="7">
+        <v>9690</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>209</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A24" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" s="7">
+        <v>10126</v>
+      </c>
+      <c r="C24" s="7">
+        <v>10351</v>
+      </c>
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B25" s="7">
+        <v>11221</v>
+      </c>
+      <c r="C25" s="7">
+        <v>11443</v>
+      </c>
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>222</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A26" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B26" s="7">
+        <v>11859</v>
+      </c>
+      <c r="C26" s="7">
+        <v>12081</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A27" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27" s="7">
+        <v>12287</v>
+      </c>
+      <c r="C27" s="7">
+        <v>12567</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="0"/>
+        <v>280</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>79</v>
+      </c>
+      <c r="B28" s="7">
+        <v>12430</v>
+      </c>
+      <c r="C28" s="7">
+        <v>12706</v>
+      </c>
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>276</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" s="7">
+        <v>13089</v>
+      </c>
+      <c r="C29" s="7">
+        <v>13365</v>
+      </c>
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>276</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B30" s="7">
+        <v>13411</v>
+      </c>
+      <c r="C30" s="7">
+        <v>13704</v>
+      </c>
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>293</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>81</v>
+      </c>
+      <c r="B31" s="7">
+        <v>14071</v>
+      </c>
+      <c r="C31" s="7">
+        <v>14363</v>
+      </c>
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
+        <v>292</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>83</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>82</v>
+      </c>
+      <c r="B32" s="7">
+        <v>14758</v>
+      </c>
+      <c r="C32" s="7">
+        <v>15037</v>
+      </c>
+      <c r="D32" s="3">
+        <f t="shared" si="0"/>
+        <v>279</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A33" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B33" s="7">
+        <v>15426</v>
+      </c>
+      <c r="C33" s="7">
+        <v>15683</v>
+      </c>
+      <c r="D33" s="3">
+        <f t="shared" si="0"/>
+        <v>257</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>85</v>
+      <c r="A34" s="8" t="s">
+        <v>130</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1364,7 +1448,7 @@
     </row>
     <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
@@ -1375,7 +1459,7 @@
     </row>
     <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
@@ -1386,7 +1470,7 @@
     </row>
     <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
@@ -1397,7 +1481,7 @@
     </row>
     <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
@@ -1408,7 +1492,7 @@
     </row>
     <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
@@ -1419,7 +1503,7 @@
     </row>
     <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
@@ -1430,7 +1514,7 @@
     </row>
     <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
@@ -1441,7 +1525,7 @@
     </row>
     <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
@@ -1452,7 +1536,7 @@
     </row>
     <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
@@ -1463,7 +1547,7 @@
     </row>
     <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
@@ -1474,7 +1558,7 @@
     </row>
     <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
@@ -1485,7 +1569,7 @@
     </row>
     <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
@@ -1496,7 +1580,7 @@
     </row>
     <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
@@ -1507,7 +1591,7 @@
     </row>
     <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
@@ -1518,7 +1602,7 @@
     </row>
     <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
@@ -1529,7 +1613,7 @@
     </row>
     <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
@@ -1540,7 +1624,7 @@
     </row>
     <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
@@ -1551,7 +1635,7 @@
     </row>
     <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -1562,7 +1646,7 @@
     </row>
     <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
@@ -1573,7 +1657,7 @@
     </row>
     <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="7"/>
@@ -1584,7 +1668,7 @@
     </row>
     <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="7"/>
@@ -1595,7 +1679,7 @@
     </row>
     <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
@@ -1606,7 +1690,7 @@
     </row>
     <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="7"/>
@@ -1617,7 +1701,7 @@
     </row>
     <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B58" s="7"/>
       <c r="C58" s="7"/>
@@ -1628,7 +1712,7 @@
     </row>
     <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="7"/>
@@ -1639,7 +1723,7 @@
     </row>
     <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -1650,7 +1734,7 @@
     </row>
     <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="7"/>
@@ -1661,7 +1745,7 @@
     </row>
     <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B62" s="7"/>
       <c r="C62" s="7"/>
@@ -1672,7 +1756,7 @@
     </row>
     <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B63" s="7"/>
       <c r="C63" s="7"/>
@@ -1683,7 +1767,7 @@
     </row>
     <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -1694,7 +1778,7 @@
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B65" s="7"/>
       <c r="C65" s="7"/>
@@ -1705,7 +1789,7 @@
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1716,7 +1800,7 @@
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1727,7 +1811,7 @@
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1738,7 +1822,7 @@
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1749,7 +1833,7 @@
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1760,7 +1844,7 @@
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1771,7 +1855,7 @@
     </row>
     <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1782,7 +1866,7 @@
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1792,8 +1876,8 @@
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
-        <v>10</v>
+      <c r="A74" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1804,29 +1888,29 @@
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
       <c r="D75" s="3" t="str">
-        <f t="shared" ref="D75:D138" si="1">IF(C75&lt;&gt;"",IF(B75&lt;&gt;"",C75-B75,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D76:D139" si="1">IF(C76&lt;&gt;"",IF(B76&lt;&gt;"",C76-B76,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
-        <v>30</v>
+        <v>11</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
@@ -1837,7 +1921,7 @@
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
@@ -1848,7 +1932,7 @@
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
@@ -1859,7 +1943,7 @@
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
@@ -1869,8 +1953,8 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
-        <v>47</v>
+      <c r="A81" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -1881,7 +1965,7 @@
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -1892,7 +1976,7 @@
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -1902,8 +1986,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
-        <v>14</v>
+      <c r="A84" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -1914,7 +1998,7 @@
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -1925,7 +2009,7 @@
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="5" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -1936,7 +2020,7 @@
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="5" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -1947,7 +2031,7 @@
     </row>
     <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="5" t="s">
-        <v>16</v>
+        <v>35</v>
       </c>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -1958,7 +2042,7 @@
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -1969,7 +2053,7 @@
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -1980,7 +2064,7 @@
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -1991,7 +2075,7 @@
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -2002,7 +2086,7 @@
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -2013,7 +2097,7 @@
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -2024,7 +2108,7 @@
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -2035,7 +2119,7 @@
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -2046,7 +2130,7 @@
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -2057,7 +2141,7 @@
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -2068,7 +2152,7 @@
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -2079,7 +2163,7 @@
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>22</v>
+        <v>41</v>
       </c>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -2090,7 +2174,7 @@
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -2101,7 +2185,7 @@
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -2112,7 +2196,7 @@
     </row>
     <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -2123,7 +2207,7 @@
     </row>
     <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -2134,7 +2218,7 @@
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -2145,7 +2229,7 @@
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -2156,7 +2240,7 @@
     </row>
     <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -2166,7 +2250,9 @@
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="7"/>
+      <c r="A108" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
       <c r="D108" s="3" t="str">
@@ -2449,7 +2535,7 @@
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
       <c r="D139" s="3" t="str">
-        <f t="shared" ref="D139:D143" si="2">IF(C139&lt;&gt;"",IF(B139&lt;&gt;"",C139-B139,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2458,7 +2544,7 @@
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
       <c r="D140" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D140:D144" si="2">IF(C140&lt;&gt;"",IF(B140&lt;&gt;"",C140-B140,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -2474,6 +2560,7 @@
     <row r="142" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
+      <c r="C142" s="7"/>
       <c r="D142" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2491,7 +2578,7 @@
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="D144" s="3" t="str">
-        <f t="shared" ref="D144:D145" si="3">IF(C144&lt;&gt;"",IF(B144&lt;&gt;"",B144-C144,"-"), "-")</f>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
@@ -2499,19 +2586,24 @@
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="D145" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D145:D146" si="3">IF(C145&lt;&gt;"",IF(B145&lt;&gt;"",B145-C145,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
+      <c r="D146" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="147" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="7"/>
       <c r="B147" s="7"/>
     </row>
     <row r="148" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A148" s="7"/>
       <c r="B148" s="7"/>
     </row>
     <row r="149" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -2921,6 +3013,9 @@
     </row>
     <row r="284" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B284" s="7"/>
+    </row>
+    <row r="285" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B285" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Lode Runner v3 - up to lv16 320 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B17E18C-F331-422B-8B62-9F8B8DFFDF53}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4BB2E6-7BF2-4000-AB4E-8A2B9834BCC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43650" yWindow="3900" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="147">
   <si>
     <t>Place</t>
   </si>
@@ -424,9 +424,6 @@
     <t>X = 0 start</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Ladder grab</t>
   </si>
   <si>
@@ -464,6 +461,18 @@
   </si>
   <si>
     <t>Lv13 X=0 Start</t>
+  </si>
+  <si>
+    <t>1 delay frame</t>
+  </si>
+  <si>
+    <t>9 delay frames</t>
+  </si>
+  <si>
+    <t>Lag</t>
+  </si>
+  <si>
+    <t>v3 - 7 digs</t>
   </si>
 </sst>
 </file>
@@ -926,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06DA051-0308-42D5-B7F7-51E79FAF1C31}">
   <dimension ref="A1:F285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -980,7 +989,7 @@
         <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -1043,7 +1052,7 @@
         <v>30</v>
       </c>
       <c r="E7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -1117,12 +1126,12 @@
         <v>91</v>
       </c>
       <c r="E12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B13" s="7">
         <v>4215</v>
@@ -1137,7 +1146,7 @@
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B14" s="7">
         <v>4375</v>
@@ -1167,7 +1176,7 @@
     </row>
     <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B16" s="7">
         <v>5209</v>
@@ -1180,7 +1189,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>69</v>
       </c>
@@ -1195,9 +1204,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B18" s="7">
         <v>6216</v>
@@ -1210,7 +1219,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>71</v>
       </c>
@@ -1225,9 +1234,9 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B20" s="7">
         <v>7919</v>
@@ -1240,7 +1249,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>73</v>
       </c>
@@ -1255,9 +1264,9 @@
         <v>157</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B22" s="7">
         <v>9053</v>
@@ -1270,7 +1279,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>75</v>
       </c>
@@ -1285,9 +1294,9 @@
         <v>209</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B24" s="7">
         <v>10126</v>
@@ -1300,7 +1309,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>77</v>
       </c>
@@ -1315,9 +1324,9 @@
         <v>222</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B26" s="7">
         <v>11859</v>
@@ -1330,9 +1339,9 @@
         <v>222</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B27" s="7">
         <v>12287</v>
@@ -1345,7 +1354,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>79</v>
       </c>
@@ -1360,9 +1369,9 @@
         <v>276</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B29" s="7">
         <v>13089</v>
@@ -1375,22 +1384,25 @@
         <v>276</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>126</v>
       </c>
       <c r="B30" s="7">
-        <v>13411</v>
+        <v>13412</v>
       </c>
       <c r="C30" s="7">
         <v>13704</v>
       </c>
       <c r="D30" s="3">
         <f t="shared" si="0"/>
-        <v>293</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+      <c r="E30" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>81</v>
       </c>
@@ -1405,103 +1417,139 @@
         <v>292</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>82</v>
       </c>
       <c r="B32" s="7">
-        <v>14758</v>
+        <v>14755</v>
       </c>
       <c r="C32" s="7">
         <v>15037</v>
       </c>
       <c r="D32" s="3">
         <f t="shared" si="0"/>
-        <v>279</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B33" s="7">
-        <v>15426</v>
+        <v>15409</v>
       </c>
       <c r="C33" s="7">
         <v>15683</v>
       </c>
       <c r="D33" s="3">
         <f t="shared" si="0"/>
-        <v>257</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>274</v>
+      </c>
+      <c r="E33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="B34" s="7">
+        <v>15994</v>
+      </c>
+      <c r="C34" s="7">
+        <v>16263</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="0"/>
+        <v>269</v>
+      </c>
+      <c r="E34" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B35" s="7">
+        <v>16640</v>
+      </c>
+      <c r="C35" s="7">
+        <v>16910</v>
+      </c>
+      <c r="D35" s="3">
+        <f t="shared" si="0"/>
+        <v>270</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B36" s="7">
+        <v>17228</v>
+      </c>
+      <c r="C36" s="7">
+        <v>17488</v>
+      </c>
+      <c r="D36" s="3">
+        <f t="shared" si="0"/>
+        <v>260</v>
+      </c>
+      <c r="E36" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B37" s="7">
+        <v>17866</v>
+      </c>
+      <c r="C37" s="7">
+        <v>18134</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="0"/>
+        <v>268</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B38" s="7">
+        <v>18604</v>
+      </c>
+      <c r="C38" s="7">
+        <v>18924</v>
+      </c>
+      <c r="D38" s="3">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+      <c r="F38" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B39" s="7">
+        <v>19242</v>
+      </c>
+      <c r="C39" s="7">
+        <v>19562</v>
+      </c>
+      <c r="D39" s="3">
+        <f t="shared" si="0"/>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>90</v>
       </c>
@@ -1512,7 +1560,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>91</v>
       </c>
@@ -1523,7 +1571,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>92</v>
       </c>
@@ -1534,7 +1582,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>93</v>
       </c>
@@ -1545,7 +1593,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>94</v>
       </c>
@@ -1556,7 +1604,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>95</v>
       </c>
@@ -1567,7 +1615,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>96</v>
       </c>
@@ -1578,7 +1626,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>97</v>
       </c>
@@ -1589,7 +1637,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
up to level 19, 421 ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4BB2E6-7BF2-4000-AB4E-8A2B9834BCC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2E1B85-88DF-4EF7-B5A6-4EA1D9067693}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43650" yWindow="3900" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="147">
   <si>
     <t>Place</t>
   </si>
@@ -935,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06DA051-0308-42D5-B7F7-51E79FAF1C31}">
   <dimension ref="A1:F285"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1553,66 +1553,93 @@
       <c r="A40" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7"/>
-      <c r="D40" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B40" s="7">
+        <v>19683</v>
+      </c>
+      <c r="C40" s="7">
+        <v>20001</v>
+      </c>
+      <c r="D40" s="3">
+        <f t="shared" si="0"/>
+        <v>318</v>
+      </c>
+      <c r="E40" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7"/>
-      <c r="D41" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B41" s="7">
+        <v>20330</v>
+      </c>
+      <c r="C41" s="7">
+        <v>20646</v>
+      </c>
+      <c r="D41" s="3">
+        <f t="shared" si="0"/>
+        <v>316</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B42" s="7">
+        <v>21340</v>
+      </c>
+      <c r="C42" s="7">
+        <v>21659</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" si="0"/>
+        <v>319</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B43" s="7">
+        <v>21985</v>
+      </c>
+      <c r="C43" s="7">
+        <v>22304</v>
+      </c>
+      <c r="D43" s="3">
+        <f t="shared" si="0"/>
+        <v>319</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B44" s="8">
+        <v>22936</v>
+      </c>
+      <c r="C44" s="7">
+        <v>23344</v>
+      </c>
+      <c r="D44" s="3">
+        <f t="shared" si="0"/>
+        <v>408</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B45" s="7">
+        <v>23582</v>
+      </c>
+      <c r="C45" s="7">
+        <v>24003</v>
+      </c>
+      <c r="D45" s="3">
+        <f t="shared" si="0"/>
+        <v>421</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Lode Runner v4 - up to lv 22
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2E1B85-88DF-4EF7-B5A6-4EA1D9067693}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235BB682-476B-4A18-88F0-534396D4678A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43650" yWindow="3900" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44580" yWindow="3765" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V4" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="148">
   <si>
     <t>Place</t>
   </si>
@@ -473,6 +473,9 @@
   </si>
   <si>
     <t>v3 - 7 digs</t>
+  </si>
+  <si>
+    <t>1 Delay</t>
   </si>
 </sst>
 </file>
@@ -936,7 +939,7 @@
   <dimension ref="A1:F285"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1646,69 +1649,102 @@
       <c r="A46" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B46" s="7">
+        <v>23922</v>
+      </c>
+      <c r="C46" s="7">
+        <v>24339</v>
+      </c>
+      <c r="D46" s="3">
+        <f t="shared" si="0"/>
+        <v>417</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B47" s="7">
+        <v>24583</v>
+      </c>
+      <c r="C47" s="7">
+        <v>24998</v>
+      </c>
+      <c r="D47" s="3">
+        <f t="shared" si="0"/>
+        <v>415</v>
+      </c>
+      <c r="E47" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B48" s="7">
+        <v>25181</v>
+      </c>
+      <c r="C48" s="7">
+        <v>25628</v>
+      </c>
+      <c r="D48" s="3">
+        <f t="shared" si="0"/>
+        <v>447</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B49" s="7">
+        <v>25839</v>
+      </c>
+      <c r="C49" s="7">
+        <v>26288</v>
+      </c>
+      <c r="D49" s="3">
+        <f t="shared" si="0"/>
+        <v>449</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7"/>
-      <c r="D50" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B50" s="7">
+        <v>26718</v>
+      </c>
+      <c r="C50" s="7">
+        <v>27221</v>
+      </c>
+      <c r="D50" s="3">
+        <f t="shared" si="0"/>
+        <v>503</v>
+      </c>
+      <c r="E50">
+        <v>26718</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7"/>
-      <c r="D51" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B51" s="7">
+        <v>27377</v>
+      </c>
+      <c r="C51" s="7">
+        <v>27866</v>
+      </c>
+      <c r="D51" s="3">
+        <f t="shared" si="0"/>
+        <v>489</v>
+      </c>
+      <c r="E51" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>102</v>
       </c>
@@ -1719,7 +1755,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>103</v>
       </c>
@@ -1730,7 +1766,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>104</v>
       </c>
@@ -1741,7 +1777,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>105</v>
       </c>
@@ -1752,7 +1788,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>106</v>
       </c>
@@ -1763,7 +1799,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>107</v>
       </c>
@@ -1774,7 +1810,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>108</v>
       </c>
@@ -1785,7 +1821,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>109</v>
       </c>
@@ -1796,7 +1832,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>110</v>
       </c>
@@ -1807,7 +1843,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>111</v>
       </c>
@@ -1818,7 +1854,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>112</v>
       </c>
@@ -1829,7 +1865,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>113</v>
       </c>
@@ -1840,7 +1876,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>115</v>
       </c>

</xml_diff>

<commit_message>
Lode Runner v3 - up to Lv27 641 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235BB682-476B-4A18-88F0-534396D4678A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E207FF0-C786-478F-8EBC-442A547C7EEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44580" yWindow="3765" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="152">
   <si>
     <t>Place</t>
   </si>
@@ -476,6 +476,18 @@
   </si>
   <si>
     <t>1 Delay</t>
+  </si>
+  <si>
+    <t>gold</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>dig</t>
+  </si>
+  <si>
+    <t>enemy spawn</t>
   </si>
 </sst>
 </file>
@@ -485,12 +497,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -595,25 +614,26 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -936,10 +956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06DA051-0308-42D5-B7F7-51E79FAF1C31}">
-  <dimension ref="A1:F285"/>
+  <dimension ref="A1:F289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1006,7 +1026,7 @@
         <v>1408</v>
       </c>
       <c r="D4" s="3">
-        <f t="shared" ref="D4:D75" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
+        <f t="shared" ref="D4:D79" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
         <v>19</v>
       </c>
     </row>
@@ -1748,159 +1768,218 @@
       <c r="A52" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B52" s="7">
+        <v>28030</v>
+      </c>
+      <c r="C52" s="7">
+        <v>28531</v>
+      </c>
+      <c r="D52" s="3">
+        <f t="shared" si="0"/>
+        <v>501</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B53" s="7">
+        <v>28675</v>
+      </c>
+      <c r="C53" s="7">
+        <v>29176</v>
+      </c>
+      <c r="D53" s="3">
+        <f t="shared" si="0"/>
+        <v>501</v>
       </c>
     </row>
     <row r="54" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7"/>
-      <c r="D54" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A54" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B54" s="7">
+        <v>29030</v>
+      </c>
+      <c r="C54" s="7">
+        <v>29531</v>
+      </c>
+      <c r="D54" s="3">
+        <f t="shared" si="0"/>
+        <v>501</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A55" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B55" s="7">
+        <v>29392</v>
+      </c>
+      <c r="C55" s="7">
+        <v>29894</v>
+      </c>
+      <c r="D55" s="3">
+        <f t="shared" si="0"/>
+        <v>502</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7"/>
-      <c r="D56" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A56" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B56" s="7">
+        <v>29423</v>
+      </c>
+      <c r="C56" s="7">
+        <v>29924</v>
+      </c>
+      <c r="D56" s="3">
+        <f t="shared" si="0"/>
+        <v>501</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="A57" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B57" s="7">
+        <v>29537</v>
+      </c>
+      <c r="C57" s="7">
+        <v>30032</v>
+      </c>
+      <c r="D57" s="3">
+        <f t="shared" si="0"/>
+        <v>495</v>
+      </c>
+      <c r="E57" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7"/>
-      <c r="D58" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>104</v>
+      </c>
+      <c r="B58" s="7">
+        <v>29883</v>
+      </c>
+      <c r="C58" s="7">
+        <v>30377</v>
+      </c>
+      <c r="D58" s="3">
+        <f t="shared" si="0"/>
+        <v>494</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>105</v>
+      </c>
+      <c r="B59" s="7">
+        <v>30378</v>
+      </c>
+      <c r="C59" s="7">
+        <v>30869</v>
+      </c>
+      <c r="D59" s="3">
+        <f t="shared" si="0"/>
+        <v>491</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>106</v>
+      </c>
+      <c r="B60" s="7">
+        <v>30809</v>
+      </c>
+      <c r="C60" s="7">
+        <v>31301</v>
+      </c>
+      <c r="D60" s="3">
+        <f t="shared" si="0"/>
+        <v>492</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>107</v>
+      </c>
+      <c r="B61" s="7">
+        <v>31448</v>
+      </c>
+      <c r="C61" s="7">
+        <v>31939</v>
+      </c>
+      <c r="D61" s="3">
+        <f t="shared" si="0"/>
+        <v>491</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>108</v>
+      </c>
+      <c r="B62" s="7">
+        <v>32009</v>
+      </c>
+      <c r="C62" s="7">
+        <v>32606</v>
+      </c>
+      <c r="D62" s="3">
+        <f t="shared" si="0"/>
+        <v>597</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7"/>
-      <c r="D63" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>109</v>
+      </c>
+      <c r="B63" s="7">
+        <v>32654</v>
+      </c>
+      <c r="C63" s="7">
+        <v>33251</v>
+      </c>
+      <c r="D63" s="3">
+        <f t="shared" si="0"/>
+        <v>597</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7"/>
-      <c r="D64" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>110</v>
+      </c>
+      <c r="B64" s="7">
+        <v>33576</v>
+      </c>
+      <c r="C64" s="9">
+        <v>34217</v>
+      </c>
+      <c r="D64" s="3">
+        <f t="shared" si="0"/>
+        <v>641</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7"/>
-      <c r="D65" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+        <v>111</v>
+      </c>
+      <c r="B65" s="7">
+        <v>34235</v>
+      </c>
+      <c r="C65" s="7">
+        <v>34876</v>
+      </c>
+      <c r="D65" s="3">
+        <f t="shared" si="0"/>
+        <v>641</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="7"/>
@@ -1911,7 +1990,7 @@
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="7"/>
@@ -1922,7 +2001,7 @@
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="7"/>
@@ -1933,7 +2012,7 @@
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="7"/>
@@ -1944,7 +2023,7 @@
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="B70" s="7"/>
       <c r="C70" s="7"/>
@@ -1955,7 +2034,7 @@
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="B71" s="7"/>
       <c r="C71" s="7"/>
@@ -1966,7 +2045,7 @@
     </row>
     <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="7"/>
@@ -1977,7 +2056,7 @@
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B73" s="7"/>
       <c r="C73" s="7"/>
@@ -1988,7 +2067,7 @@
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B74" s="7"/>
       <c r="C74" s="7"/>
@@ -1998,8 +2077,8 @@
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
-        <v>10</v>
+      <c r="A75" s="7" t="s">
+        <v>121</v>
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
@@ -2009,63 +2088,63 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
-        <v>31</v>
+      <c r="A76" s="7" t="s">
+        <v>122</v>
       </c>
       <c r="B76" s="7"/>
       <c r="C76" s="7"/>
       <c r="D76" s="3" t="str">
-        <f t="shared" ref="D76:D139" si="1">IF(C76&lt;&gt;"",IF(B76&lt;&gt;"",C76-B76,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>11</v>
+      <c r="A77" s="7" t="s">
+        <v>123</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="7"/>
       <c r="D77" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>30</v>
+      <c r="A78" s="7" t="s">
+        <v>124</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="7"/>
       <c r="D78" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="7"/>
       <c r="D79" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="7"/>
       <c r="D80" s="3" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="D80:D143" si="1">IF(C80&lt;&gt;"",IF(B80&lt;&gt;"",C80-B80,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="7"/>
@@ -2075,8 +2154,8 @@
       </c>
     </row>
     <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="7" t="s">
-        <v>47</v>
+      <c r="A82" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="7"/>
@@ -2086,8 +2165,8 @@
       </c>
     </row>
     <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="7" t="s">
-        <v>48</v>
+      <c r="A83" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="7"/>
@@ -2097,8 +2176,8 @@
       </c>
     </row>
     <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="7" t="s">
-        <v>33</v>
+      <c r="A84" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="B84" s="7"/>
       <c r="C84" s="7"/>
@@ -2109,7 +2188,7 @@
     </row>
     <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B85" s="7"/>
       <c r="C85" s="7"/>
@@ -2119,8 +2198,8 @@
       </c>
     </row>
     <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
-        <v>34</v>
+      <c r="A86" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="B86" s="7"/>
       <c r="C86" s="7"/>
@@ -2130,8 +2209,8 @@
       </c>
     </row>
     <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
-        <v>15</v>
+      <c r="A87" s="7" t="s">
+        <v>48</v>
       </c>
       <c r="B87" s="7"/>
       <c r="C87" s="7"/>
@@ -2141,8 +2220,8 @@
       </c>
     </row>
     <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
-        <v>35</v>
+      <c r="A88" s="7" t="s">
+        <v>33</v>
       </c>
       <c r="B88" s="7"/>
       <c r="C88" s="7"/>
@@ -2153,7 +2232,7 @@
     </row>
     <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B89" s="7"/>
       <c r="C89" s="7"/>
@@ -2164,7 +2243,7 @@
     </row>
     <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
@@ -2175,7 +2254,7 @@
     </row>
     <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B91" s="7"/>
       <c r="C91" s="7"/>
@@ -2186,7 +2265,7 @@
     </row>
     <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B92" s="7"/>
       <c r="C92" s="7"/>
@@ -2197,7 +2276,7 @@
     </row>
     <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B93" s="7"/>
       <c r="C93" s="7"/>
@@ -2208,7 +2287,7 @@
     </row>
     <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B94" s="7"/>
       <c r="C94" s="7"/>
@@ -2219,7 +2298,7 @@
     </row>
     <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B95" s="7"/>
       <c r="C95" s="7"/>
@@ -2230,7 +2309,7 @@
     </row>
     <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B96" s="7"/>
       <c r="C96" s="7"/>
@@ -2241,7 +2320,7 @@
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="7"/>
@@ -2252,7 +2331,7 @@
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B98" s="7"/>
       <c r="C98" s="7"/>
@@ -2263,7 +2342,7 @@
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="7"/>
@@ -2274,7 +2353,7 @@
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B100" s="7"/>
       <c r="C100" s="7"/>
@@ -2285,7 +2364,7 @@
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B101" s="7"/>
       <c r="C101" s="7"/>
@@ -2296,7 +2375,7 @@
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B102" s="7"/>
       <c r="C102" s="7"/>
@@ -2307,7 +2386,7 @@
     </row>
     <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B103" s="7"/>
       <c r="C103" s="7"/>
@@ -2318,7 +2397,7 @@
     </row>
     <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B104" s="7"/>
       <c r="C104" s="7"/>
@@ -2329,7 +2408,7 @@
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
@@ -2340,7 +2419,7 @@
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B106" s="7"/>
       <c r="C106" s="7"/>
@@ -2351,7 +2430,7 @@
     </row>
     <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -2362,7 +2441,7 @@
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -2372,7 +2451,9 @@
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="7"/>
+      <c r="A109" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
       <c r="D109" s="3" t="str">
@@ -2381,7 +2462,9 @@
       </c>
     </row>
     <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="7"/>
+      <c r="A110" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
       <c r="D110" s="3" t="str">
@@ -2390,7 +2473,9 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="7"/>
+      <c r="A111" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
       <c r="D111" s="3" t="str">
@@ -2399,7 +2484,9 @@
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A112" s="7"/>
+      <c r="A112" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
       <c r="D112" s="3" t="str">
@@ -2655,7 +2742,7 @@
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
       <c r="D140" s="3" t="str">
-        <f t="shared" ref="D140:D144" si="2">IF(C140&lt;&gt;"",IF(B140&lt;&gt;"",C140-B140,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2664,7 +2751,7 @@
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
       <c r="D141" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2673,60 +2760,84 @@
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
       <c r="D142" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="143" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
+      <c r="C143" s="7"/>
       <c r="D143" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="144" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
+      <c r="C144" s="7"/>
       <c r="D144" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D144:D148" si="2">IF(C144&lt;&gt;"",IF(B144&lt;&gt;"",C144-B144,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
+      <c r="C145" s="7"/>
       <c r="D145" s="3" t="str">
-        <f t="shared" ref="D145:D146" si="3">IF(C145&lt;&gt;"",IF(B145&lt;&gt;"",B145-C145,"-"), "-")</f>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
+      <c r="C146" s="7"/>
       <c r="D146" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="7"/>
       <c r="B147" s="7"/>
+      <c r="D147" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="148" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="7"/>
       <c r="B148" s="7"/>
+      <c r="D148" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="149" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A149" s="7"/>
       <c r="B149" s="7"/>
+      <c r="D149" s="3" t="str">
+        <f t="shared" ref="D149:D150" si="3">IF(C149&lt;&gt;"",IF(B149&lt;&gt;"",B149-C149,"-"), "-")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="150" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A150" s="7"/>
       <c r="B150" s="7"/>
+      <c r="D150" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="151" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A151" s="7"/>
       <c r="B151" s="7"/>
     </row>
     <row r="152" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A152" s="7"/>
       <c r="B152" s="7"/>
     </row>
     <row r="153" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3127,6 +3238,18 @@
     </row>
     <row r="285" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B285" s="7"/>
+    </row>
+    <row r="286" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B286" s="7"/>
+    </row>
+    <row r="287" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B287" s="7"/>
+    </row>
+    <row r="288" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B288" s="7"/>
+    </row>
+    <row r="289" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B289" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6631,7 +6754,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="11" type="noConversion"/>
+  <phoneticPr fontId="12" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
Lode Runner V4 - up to level 36, 902 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E207FF0-C786-478F-8EBC-442A547C7EEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E037B727-0ED5-4E58-9C6F-9925F6F7AB5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="44580" yWindow="3765" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="152">
   <si>
     <t>Place</t>
   </si>
@@ -958,8 +958,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06DA051-0308-42D5-B7F7-51E79FAF1C31}">
   <dimension ref="A1:F289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1981,201 +1981,276 @@
       <c r="A66" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B66" s="7">
+        <v>35341</v>
+      </c>
+      <c r="C66" s="7">
+        <v>36013</v>
+      </c>
+      <c r="D66" s="3">
+        <f t="shared" si="0"/>
+        <v>672</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7"/>
-      <c r="D67" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B67" s="7">
+        <v>35986</v>
+      </c>
+      <c r="C67" s="7">
+        <v>36658</v>
+      </c>
+      <c r="D67" s="3">
+        <f t="shared" si="0"/>
+        <v>672</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B68" s="7">
+        <v>36861</v>
+      </c>
+      <c r="C68" s="7">
+        <v>37560</v>
+      </c>
+      <c r="D68" s="3">
+        <f t="shared" si="0"/>
+        <v>699</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B69" s="7">
+        <v>37461</v>
+      </c>
+      <c r="C69" s="7">
+        <v>38160</v>
+      </c>
+      <c r="D69" s="3">
+        <f t="shared" si="0"/>
+        <v>699</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7"/>
-      <c r="D70" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B70" s="7">
+        <v>38564</v>
+      </c>
+      <c r="C70" s="7">
+        <v>39292</v>
+      </c>
+      <c r="D70" s="3">
+        <f t="shared" si="0"/>
+        <v>728</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>117</v>
       </c>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7"/>
-      <c r="D71" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B71" s="7">
+        <v>39057</v>
+      </c>
+      <c r="C71" s="7">
+        <v>39784</v>
+      </c>
+      <c r="D71" s="3">
+        <f t="shared" si="0"/>
+        <v>727</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7"/>
-      <c r="D72" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B72" s="7">
+        <v>39781</v>
+      </c>
+      <c r="C72" s="7">
+        <v>40599</v>
+      </c>
+      <c r="D72" s="3">
+        <f t="shared" si="0"/>
+        <v>818</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7"/>
-      <c r="D73" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B73" s="7">
+        <v>40405</v>
+      </c>
+      <c r="C73" s="7">
+        <v>41223</v>
+      </c>
+      <c r="D73" s="3">
+        <f t="shared" si="0"/>
+        <v>818</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7"/>
-      <c r="D74" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B74" s="9">
+        <v>40588</v>
+      </c>
+      <c r="C74" s="7">
+        <v>41408</v>
+      </c>
+      <c r="D74" s="3">
+        <f t="shared" si="0"/>
+        <v>820</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7"/>
-      <c r="D75" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B75" s="7">
+        <v>41228</v>
+      </c>
+      <c r="C75" s="7">
+        <v>42047</v>
+      </c>
+      <c r="D75" s="3">
+        <f t="shared" si="0"/>
+        <v>819</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7"/>
-      <c r="D76" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B76" s="9">
+        <v>41865</v>
+      </c>
+      <c r="C76" s="7">
+        <v>42750</v>
+      </c>
+      <c r="D76" s="3">
+        <f t="shared" si="0"/>
+        <v>885</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B77" s="7">
+        <v>42511</v>
+      </c>
+      <c r="C77" s="7">
+        <v>43396</v>
+      </c>
+      <c r="D77" s="3">
+        <f t="shared" si="0"/>
+        <v>885</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7"/>
-      <c r="D78" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B78" s="7">
+        <v>43110</v>
+      </c>
+      <c r="C78" s="7">
+        <v>44013</v>
+      </c>
+      <c r="D78" s="3">
+        <f t="shared" si="0"/>
+        <v>903</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7"/>
-      <c r="D79" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
+      <c r="B79" s="7">
+        <v>43756</v>
+      </c>
+      <c r="C79" s="7">
+        <v>44660</v>
+      </c>
+      <c r="D79" s="3">
+        <f t="shared" si="0"/>
+        <v>904</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B80" s="7"/>
-      <c r="C80" s="7"/>
-      <c r="D80" s="3" t="str">
+      <c r="B80" s="7">
+        <v>44418</v>
+      </c>
+      <c r="C80" s="7">
+        <v>45323</v>
+      </c>
+      <c r="D80" s="3">
         <f t="shared" ref="D80:D143" si="1">IF(C80&lt;&gt;"",IF(B80&lt;&gt;"",C80-B80,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <v>905</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7"/>
-      <c r="D81" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B81" s="7">
+        <v>45077</v>
+      </c>
+      <c r="C81" s="7">
+        <v>45982</v>
+      </c>
+      <c r="D81" s="3">
+        <f t="shared" si="1"/>
+        <v>905</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
-      <c r="D82" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B82" s="7">
+        <v>45719</v>
+      </c>
+      <c r="C82" s="7">
+        <v>46621</v>
+      </c>
+      <c r="D82" s="3">
+        <f t="shared" si="1"/>
+        <v>902</v>
+      </c>
+      <c r="E82" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B83" s="7"/>
-      <c r="C83" s="7"/>
-      <c r="D83" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B83" s="7">
+        <v>46378</v>
+      </c>
+      <c r="C83" s="7">
+        <v>47280</v>
+      </c>
+      <c r="D83" s="3">
+        <f t="shared" si="1"/>
+        <v>902</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
         <v>32</v>
       </c>
@@ -2186,7 +2261,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>13</v>
       </c>
@@ -2197,7 +2272,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>47</v>
       </c>
@@ -2208,7 +2283,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>48</v>
       </c>
@@ -2219,7 +2294,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>33</v>
       </c>
@@ -2230,7 +2305,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>14</v>
       </c>
@@ -2241,7 +2316,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>34</v>
       </c>
@@ -2252,7 +2327,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>15</v>
       </c>
@@ -2263,7 +2338,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>35</v>
       </c>
@@ -2274,7 +2349,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>16</v>
       </c>
@@ -2285,7 +2360,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
         <v>36</v>
       </c>
@@ -2296,7 +2371,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>17</v>
       </c>
@@ -2307,7 +2382,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>37</v>
       </c>

</xml_diff>

<commit_message>
Lode Runner v4 - up to level 39, 953 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E037B727-0ED5-4E58-9C6F-9925F6F7AB5D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E176463-DF8E-4100-BA38-5F402559B9F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44580" yWindow="3765" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45570" yWindow="3270" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V4" sheetId="4" r:id="rId1"/>
@@ -497,12 +497,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -614,25 +621,26 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -958,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06DA051-0308-42D5-B7F7-51E79FAF1C31}">
   <dimension ref="A1:F289"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="C84" sqref="C84"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="B89" sqref="B89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2254,55 +2262,75 @@
       <c r="A84" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B84" s="7"/>
-      <c r="C84" s="7"/>
-      <c r="D84" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B84" s="7">
+        <v>46984</v>
+      </c>
+      <c r="C84" s="7">
+        <v>47936</v>
+      </c>
+      <c r="D84" s="3">
+        <f t="shared" si="1"/>
+        <v>952</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B85" s="7"/>
-      <c r="C85" s="7"/>
-      <c r="D85" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B85" s="7">
+        <v>47629</v>
+      </c>
+      <c r="C85" s="7">
+        <v>48581</v>
+      </c>
+      <c r="D85" s="3">
+        <f t="shared" si="1"/>
+        <v>952</v>
       </c>
     </row>
     <row r="86" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B86" s="7"/>
-      <c r="C86" s="7"/>
-      <c r="D86" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B86" s="7">
+        <v>48410</v>
+      </c>
+      <c r="C86" s="10">
+        <v>49362</v>
+      </c>
+      <c r="D86" s="3">
+        <f t="shared" si="1"/>
+        <v>952</v>
       </c>
     </row>
     <row r="87" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B87" s="7"/>
-      <c r="C87" s="7"/>
-      <c r="D87" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B87" s="7">
+        <v>48908</v>
+      </c>
+      <c r="C87" s="7">
+        <v>49860</v>
+      </c>
+      <c r="D87" s="3">
+        <f t="shared" si="1"/>
+        <v>952</v>
       </c>
     </row>
     <row r="88" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B88" s="7"/>
-      <c r="C88" s="7"/>
-      <c r="D88" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B88" s="7">
+        <v>49892</v>
+      </c>
+      <c r="C88" s="7">
+        <v>50845</v>
+      </c>
+      <c r="D88" s="3">
+        <f t="shared" si="1"/>
+        <v>953</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="15" x14ac:dyDescent="0.25">
@@ -6829,7 +6857,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="13" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
Lode Runner v4 - up to Level 41, 1014 Frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E176463-DF8E-4100-BA38-5F402559B9F5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3808ECFB-20E9-4EE3-ABD1-1FA5691253A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45570" yWindow="3270" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -967,7 +967,7 @@
   <dimension ref="A1:F289"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="B89" sqref="B89"/>
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2323,69 +2323,89 @@
         <v>33</v>
       </c>
       <c r="B88" s="7">
-        <v>49892</v>
+        <v>49856</v>
       </c>
       <c r="C88" s="7">
         <v>50845</v>
       </c>
       <c r="D88" s="3">
         <f t="shared" si="1"/>
-        <v>953</v>
+        <v>989</v>
       </c>
     </row>
     <row r="89" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B89" s="7"/>
-      <c r="C89" s="7"/>
-      <c r="D89" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B89" s="7">
+        <v>50516</v>
+      </c>
+      <c r="C89" s="7">
+        <v>51505</v>
+      </c>
+      <c r="D89" s="3">
+        <f t="shared" si="1"/>
+        <v>989</v>
       </c>
     </row>
     <row r="90" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B90" s="7"/>
-      <c r="C90" s="7"/>
-      <c r="D90" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B90" s="7">
+        <v>50874</v>
+      </c>
+      <c r="C90" s="7">
+        <v>51888</v>
+      </c>
+      <c r="D90" s="3">
+        <f t="shared" si="1"/>
+        <v>1014</v>
       </c>
     </row>
     <row r="91" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7"/>
-      <c r="D91" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B91" s="7">
+        <v>51486</v>
+      </c>
+      <c r="C91" s="7">
+        <v>52500</v>
+      </c>
+      <c r="D91" s="3">
+        <f t="shared" si="1"/>
+        <v>1014</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B92" s="7"/>
-      <c r="C92" s="7"/>
-      <c r="D92" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B92" s="7">
+        <v>52507</v>
+      </c>
+      <c r="C92" s="7">
+        <v>53522</v>
+      </c>
+      <c r="D92" s="3">
+        <f t="shared" si="1"/>
+        <v>1015</v>
       </c>
     </row>
     <row r="93" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B93" s="7"/>
-      <c r="C93" s="7"/>
-      <c r="D93" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B93" s="7">
+        <v>53153</v>
+      </c>
+      <c r="C93" s="7">
+        <v>54167</v>
+      </c>
+      <c r="D93" s="3">
+        <f t="shared" si="1"/>
+        <v>1014</v>
       </c>
     </row>
     <row r="94" spans="1:5" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Lode Runner v4 - up to level 46, 1267 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3808ECFB-20E9-4EE3-ABD1-1FA5691253A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC595E55-A468-4CBC-8A6E-DA41D97B8F84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45570" yWindow="3270" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="154">
   <si>
     <t>Place</t>
   </si>
@@ -488,6 +488,12 @@
   </si>
   <si>
     <t>enemy spawn</t>
+  </si>
+  <si>
+    <t>3rd gold</t>
+  </si>
+  <si>
+    <t>Gold = 4</t>
   </si>
 </sst>
 </file>
@@ -964,10 +970,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06DA051-0308-42D5-B7F7-51E79FAF1C31}">
-  <dimension ref="A1:F289"/>
+  <dimension ref="A1:F292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2206,7 +2212,7 @@
         <v>45323</v>
       </c>
       <c r="D80" s="3">
-        <f t="shared" ref="D80:D143" si="1">IF(C80&lt;&gt;"",IF(B80&lt;&gt;"",C80-B80,"-"), "-")</f>
+        <f t="shared" ref="D80:D146" si="1">IF(C80&lt;&gt;"",IF(B80&lt;&gt;"",C80-B80,"-"), "-")</f>
         <v>905</v>
       </c>
     </row>
@@ -2412,148 +2418,198 @@
       <c r="A94" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B94" s="7"/>
-      <c r="C94" s="7"/>
-      <c r="D94" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B94" s="7">
+        <v>53942</v>
+      </c>
+      <c r="C94" s="7">
+        <v>55036</v>
+      </c>
+      <c r="D94" s="3">
+        <f t="shared" si="1"/>
+        <v>1094</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B95" s="7"/>
-      <c r="C95" s="7"/>
-      <c r="D95" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B95" s="7">
+        <v>54564</v>
+      </c>
+      <c r="C95" s="7">
+        <v>55658</v>
+      </c>
+      <c r="D95" s="3">
+        <f t="shared" si="1"/>
+        <v>1094</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7"/>
-      <c r="D96" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B96" s="7">
+        <v>55596</v>
+      </c>
+      <c r="C96" s="7">
+        <v>56780</v>
+      </c>
+      <c r="D96" s="3">
+        <f t="shared" si="1"/>
+        <v>1184</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B97" s="7"/>
-      <c r="C97" s="7"/>
-      <c r="D97" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B97" s="7">
+        <v>56185</v>
+      </c>
+      <c r="C97" s="7">
+        <v>57370</v>
+      </c>
+      <c r="D97" s="3">
+        <f t="shared" si="1"/>
+        <v>1185</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B98" s="7"/>
-      <c r="C98" s="7"/>
-      <c r="D98" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="A98" s="5"/>
+      <c r="B98" s="7">
+        <v>56464</v>
+      </c>
+      <c r="C98" s="7">
+        <v>57647</v>
+      </c>
+      <c r="D98" s="3">
+        <f t="shared" si="1"/>
+        <v>1183</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B99" s="7"/>
-      <c r="C99" s="7"/>
-      <c r="D99" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>38</v>
+      </c>
+      <c r="B99" s="7">
+        <v>56572</v>
+      </c>
+      <c r="C99" s="7">
+        <v>57753</v>
+      </c>
+      <c r="D99" s="3">
+        <f t="shared" si="1"/>
+        <v>1181</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B100" s="7"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>19</v>
+      </c>
+      <c r="B100" s="7">
+        <v>57217</v>
+      </c>
+      <c r="C100" s="7">
+        <v>58399</v>
+      </c>
+      <c r="D100" s="3">
+        <f t="shared" si="1"/>
+        <v>1182</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B101" s="7"/>
-      <c r="C101" s="7"/>
-      <c r="D101" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="A101" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B101" s="7">
+        <v>57373</v>
+      </c>
+      <c r="C101" s="7">
+        <v>58573</v>
+      </c>
+      <c r="D101" s="3">
+        <f t="shared" si="1"/>
+        <v>1200</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B102" s="7"/>
-      <c r="C102" s="7"/>
-      <c r="D102" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="A102" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="B102" s="7">
+        <v>57657</v>
+      </c>
+      <c r="C102" s="7">
+        <v>58806</v>
+      </c>
+      <c r="D102" s="3">
+        <f t="shared" si="1"/>
+        <v>1149</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B103" s="7"/>
-      <c r="C103" s="7"/>
-      <c r="D103" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>39</v>
+      </c>
+      <c r="B103" s="7">
+        <v>58008</v>
+      </c>
+      <c r="C103" s="7">
+        <v>59225</v>
+      </c>
+      <c r="D103" s="3">
+        <f t="shared" si="1"/>
+        <v>1217</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B104" s="7"/>
-      <c r="C104" s="7"/>
-      <c r="D104" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>20</v>
+      </c>
+      <c r="B104" s="7">
+        <v>58608</v>
+      </c>
+      <c r="C104" s="7">
+        <v>59837</v>
+      </c>
+      <c r="D104" s="3">
+        <f t="shared" si="1"/>
+        <v>1229</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B105" s="7"/>
-      <c r="C105" s="7"/>
-      <c r="D105" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>40</v>
+      </c>
+      <c r="B105" s="7">
+        <v>59190</v>
+      </c>
+      <c r="C105" s="7">
+        <v>60457</v>
+      </c>
+      <c r="D105" s="3">
+        <f t="shared" si="1"/>
+        <v>1267</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>21</v>
+      </c>
+      <c r="B106" s="7">
+        <v>59825</v>
+      </c>
+      <c r="C106" s="7">
+        <v>61092</v>
+      </c>
+      <c r="D106" s="3">
+        <f t="shared" si="1"/>
+        <v>1267</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A107" s="5" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B107" s="7"/>
       <c r="C107" s="7"/>
@@ -2564,7 +2620,7 @@
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="B108" s="7"/>
       <c r="C108" s="7"/>
@@ -2575,7 +2631,7 @@
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B109" s="7"/>
       <c r="C109" s="7"/>
@@ -2586,7 +2642,7 @@
     </row>
     <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B110" s="7"/>
       <c r="C110" s="7"/>
@@ -2597,7 +2653,7 @@
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="B111" s="7"/>
       <c r="C111" s="7"/>
@@ -2608,7 +2664,7 @@
     </row>
     <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B112" s="7"/>
       <c r="C112" s="7"/>
@@ -2618,7 +2674,9 @@
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113" s="7"/>
+      <c r="A113" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="B113" s="7"/>
       <c r="C113" s="7"/>
       <c r="D113" s="3" t="str">
@@ -2627,7 +2685,9 @@
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="7"/>
+      <c r="A114" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="B114" s="7"/>
       <c r="C114" s="7"/>
       <c r="D114" s="3" t="str">
@@ -2636,7 +2696,9 @@
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115" s="7"/>
+      <c r="A115" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="3" t="str">
@@ -2901,7 +2963,7 @@
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
       <c r="D144" s="3" t="str">
-        <f t="shared" ref="D144:D148" si="2">IF(C144&lt;&gt;"",IF(B144&lt;&gt;"",C144-B144,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2910,7 +2972,7 @@
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
       <c r="D145" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2919,21 +2981,23 @@
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="7"/>
       <c r="B147" s="7"/>
+      <c r="C147" s="7"/>
       <c r="D147" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D147:D151" si="2">IF(C147&lt;&gt;"",IF(B147&lt;&gt;"",C147-B147,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="7"/>
       <c r="B148" s="7"/>
+      <c r="C148" s="7"/>
       <c r="D148" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2942,8 +3006,9 @@
     <row r="149" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="7"/>
       <c r="B149" s="7"/>
+      <c r="C149" s="7"/>
       <c r="D149" s="3" t="str">
-        <f t="shared" ref="D149:D150" si="3">IF(C149&lt;&gt;"",IF(B149&lt;&gt;"",B149-C149,"-"), "-")</f>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
@@ -2951,25 +3016,40 @@
       <c r="A150" s="7"/>
       <c r="B150" s="7"/>
       <c r="D150" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="7"/>
       <c r="B151" s="7"/>
+      <c r="D151" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="152" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="7"/>
       <c r="B152" s="7"/>
+      <c r="D152" s="3" t="str">
+        <f t="shared" ref="D152:D153" si="3">IF(C152&lt;&gt;"",IF(B152&lt;&gt;"",B152-C152,"-"), "-")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="153" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A153" s="7"/>
       <c r="B153" s="7"/>
+      <c r="D153" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="154" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A154" s="7"/>
       <c r="B154" s="7"/>
     </row>
     <row r="155" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A155" s="7"/>
       <c r="B155" s="7"/>
     </row>
     <row r="156" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -3373,6 +3453,15 @@
     </row>
     <row r="289" spans="2:2" ht="15" x14ac:dyDescent="0.25">
       <c r="B289" s="7"/>
+    </row>
+    <row r="290" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B290" s="7"/>
+    </row>
+    <row r="291" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B291" s="7"/>
+    </row>
+    <row r="292" spans="2:2" ht="15" x14ac:dyDescent="0.25">
+      <c r="B292" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Lode Runner v4 - tentatively done, 1296 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC595E55-A468-4CBC-8A6E-DA41D97B8F84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689AAB8E-182F-4FF7-B1C4-1EC8081C064D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45570" yWindow="3270" windowWidth="15555" windowHeight="11775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="155">
   <si>
     <t>Place</t>
   </si>
@@ -488,6 +488,9 @@
   </si>
   <si>
     <t>enemy spawn</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>3rd gold</t>
@@ -972,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D06DA051-0308-42D5-B7F7-51E79FAF1C31}">
   <dimension ref="A1:F292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="B107" sqref="B107"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2519,7 +2522,7 @@
     </row>
     <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B101" s="7">
         <v>57373</v>
@@ -2534,7 +2537,7 @@
     </row>
     <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="10" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B102" s="7">
         <v>57657</v>
@@ -2611,105 +2614,143 @@
       <c r="A107" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B107" s="7"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B107" s="7">
+        <v>60441</v>
+      </c>
+      <c r="C107" s="7">
+        <v>61730</v>
+      </c>
+      <c r="D107" s="3">
+        <f t="shared" si="1"/>
+        <v>1289</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A108" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B108" s="7"/>
-      <c r="C108" s="7"/>
-      <c r="D108" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B108" s="7">
+        <v>61093</v>
+      </c>
+      <c r="C108" s="7">
+        <v>62383</v>
+      </c>
+      <c r="D108" s="3">
+        <f t="shared" si="1"/>
+        <v>1290</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A109" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B109" s="7"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B109" s="10">
+        <v>61914</v>
+      </c>
+      <c r="C109" s="7">
+        <v>63213</v>
+      </c>
+      <c r="D109" s="3">
+        <f t="shared" si="1"/>
+        <v>1299</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A110" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B110" s="7"/>
-      <c r="C110" s="7"/>
-      <c r="D110" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B110" s="7">
+        <v>62575</v>
+      </c>
+      <c r="C110" s="7">
+        <v>63858</v>
+      </c>
+      <c r="D110" s="3">
+        <f t="shared" si="1"/>
+        <v>1283</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A111" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B111" s="7"/>
-      <c r="C111" s="7"/>
-      <c r="D111" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B111" s="7">
+        <v>63180</v>
+      </c>
+      <c r="C111" s="7">
+        <v>64481</v>
+      </c>
+      <c r="D111" s="3">
+        <f t="shared" si="1"/>
+        <v>1301</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A112" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B112" s="7"/>
-      <c r="C112" s="7"/>
-      <c r="D112" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B112" s="7">
+        <v>63825</v>
+      </c>
+      <c r="C112" s="7">
+        <v>65126</v>
+      </c>
+      <c r="D112" s="3">
+        <f t="shared" si="1"/>
+        <v>1301</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A113" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B113" s="7"/>
-      <c r="C113" s="7"/>
-      <c r="D113" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B113" s="7">
+        <v>64585</v>
+      </c>
+      <c r="C113" s="7">
+        <v>65887</v>
+      </c>
+      <c r="D113" s="3">
+        <f t="shared" si="1"/>
+        <v>1302</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A114" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B114" s="7"/>
-      <c r="C114" s="7"/>
-      <c r="D114" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B114" s="7">
+        <v>65231</v>
+      </c>
+      <c r="C114" s="7">
+        <v>66532</v>
+      </c>
+      <c r="D114" s="3">
+        <f t="shared" si="1"/>
+        <v>1301</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A115" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B115" s="7"/>
-      <c r="C115" s="7"/>
-      <c r="D115" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="B115" s="7">
+        <v>65819</v>
+      </c>
+      <c r="C115" s="7">
+        <v>67115</v>
+      </c>
+      <c r="D115" s="3">
+        <f t="shared" si="1"/>
+        <v>1296</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
-      <c r="C116" s="7"/>
+      <c r="C116" s="10" t="s">
+        <v>152</v>
+      </c>
       <c r="D116" s="3" t="str">
         <f t="shared" si="1"/>
         <v>-</v>

</xml_diff>

<commit_message>
lode runner v5 - level 2 done
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAE06809-C87A-4E72-B8AC-15F86110C80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52A285B-B2FA-49A9-B3DD-BAF412DC7B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32775" yWindow="2100" windowWidth="19020" windowHeight="11775" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48105" yWindow="690" windowWidth="9060" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V5" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="170">
   <si>
     <t>Place</t>
   </si>
@@ -535,6 +535,15 @@
   </si>
   <si>
     <t>Total Frames:</t>
+  </si>
+  <si>
+    <t>Tk</t>
+  </si>
+  <si>
+    <t>Tk diff</t>
+  </si>
+  <si>
+    <t>1697 best</t>
   </si>
 </sst>
 </file>
@@ -1302,10 +1311,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B3565E-C480-4A10-8524-B7BC06C9B703}">
-  <dimension ref="A1:F292"/>
+  <dimension ref="A1:G292"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H115" sqref="H115"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1313,7 +1322,7 @@
     <col min="1" max="1" width="11.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1324,29 +1333,38 @@
         <v>125</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="F1" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3" t="str">
+      <c r="B2" s="2">
+        <v>735</v>
+      </c>
+      <c r="C2" s="2">
+        <v>735</v>
+      </c>
+      <c r="D2" s="2">
+        <v>736</v>
+      </c>
+      <c r="E2" s="3">
         <f>IF(C2&lt;&gt;"",IF(B2&lt;&gt;"",C2-B2,"-"), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="3" t="str">
-        <f>IF(E2&lt;&gt;"",IF(B2&lt;&gt;"",E2-B2,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F2" s="3">
+        <f>IF(D2&lt;&gt;"",IF(B2&lt;&gt;"",D2-B2,"-"), "-")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>52</v>
       </c>
@@ -1356,265 +1374,256 @@
       <c r="C3" s="7">
         <v>1052</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="7">
+        <v>1104</v>
+      </c>
+      <c r="E3" s="3">
         <f>IF(C3&lt;&gt;"",IF(B3&lt;&gt;"",C3-B3,"-"), "-")</f>
         <v>0</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="3" t="str">
-        <f t="shared" ref="F3:F66" si="0">IF(E3&lt;&gt;"",IF(B3&lt;&gt;"",E3-B3,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="F3" s="3">
+        <f>IF(D3&lt;&gt;"",IF(B3&lt;&gt;"",D3-B3,"-"), "-")</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>54</v>
       </c>
       <c r="B4" s="7">
-        <v>1389</v>
+        <v>1697</v>
       </c>
       <c r="C4" s="7">
-        <v>1389</v>
-      </c>
-      <c r="D4" s="3">
-        <f t="shared" ref="D4:D79" si="1">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
+        <v>1697</v>
+      </c>
+      <c r="D4" s="7">
+        <v>1764</v>
+      </c>
+      <c r="E4" s="3">
+        <f t="shared" ref="E4:E79" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
         <v>0</v>
       </c>
-      <c r="E4" s="7"/>
-      <c r="F4" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="F4" s="3">
+        <f t="shared" ref="F4:F67" si="1">IF(D4&lt;&gt;"",IF(B4&lt;&gt;"",D4-B4,"-"), "-")</f>
+        <v>67</v>
+      </c>
+      <c r="G4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="7">
-        <v>2296</v>
+        <v>2189</v>
       </c>
       <c r="C5" s="7">
         <v>2296</v>
       </c>
-      <c r="D5" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="D5" s="7">
+        <v>2222</v>
+      </c>
+      <c r="E5" s="3">
+        <f t="shared" si="0"/>
+        <v>107</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="7">
-        <v>2634</v>
-      </c>
+      <c r="B6" s="7"/>
       <c r="C6" s="7">
         <v>2634</v>
       </c>
-      <c r="D6" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B7" s="7">
-        <v>2957</v>
-      </c>
+      <c r="B7" s="7"/>
       <c r="C7" s="7">
         <v>2957</v>
       </c>
-      <c r="D7" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>128</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>127</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="7">
-        <v>3380</v>
-      </c>
+      <c r="B10" s="7"/>
       <c r="C10" s="7">
         <v>3380</v>
       </c>
-      <c r="D10" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="7">
-        <v>3717</v>
-      </c>
+      <c r="B11" s="7"/>
       <c r="C11" s="7">
         <v>3717</v>
       </c>
-      <c r="D11" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B12" s="7">
-        <v>4031</v>
-      </c>
+      <c r="B12" s="7"/>
       <c r="C12" s="7">
         <v>4031</v>
       </c>
-      <c r="D12" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B13" s="7">
-        <v>4215</v>
-      </c>
+      <c r="B13" s="7"/>
       <c r="C13" s="7">
         <v>4215</v>
       </c>
-      <c r="D13" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B14" s="7">
-        <v>4375</v>
-      </c>
+      <c r="B14" s="7"/>
       <c r="C14" s="7">
         <v>4375</v>
       </c>
-      <c r="D14" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="7">
-        <v>4553</v>
-      </c>
+      <c r="B15" s="7"/>
       <c r="C15" s="7">
         <v>4553</v>
       </c>
-      <c r="D15" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B16" s="7">
-        <v>5209</v>
-      </c>
+      <c r="B16" s="7"/>
       <c r="C16" s="7">
         <v>5209</v>
       </c>
-      <c r="D16" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F16" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1622,19 +1631,17 @@
       <c r="A17" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B17" s="7">
-        <v>5536</v>
-      </c>
+      <c r="B17" s="7"/>
       <c r="C17" s="7">
         <v>5536</v>
       </c>
-      <c r="D17" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F17" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1642,19 +1649,17 @@
       <c r="A18" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B18" s="7">
-        <v>6216</v>
-      </c>
+      <c r="B18" s="7"/>
       <c r="C18" s="7">
         <v>6216</v>
       </c>
-      <c r="D18" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E18" s="7"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F18" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1662,19 +1667,17 @@
       <c r="A19" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="B19" s="7">
-        <v>7274</v>
-      </c>
+      <c r="B19" s="7"/>
       <c r="C19" s="7">
         <v>7274</v>
       </c>
-      <c r="D19" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F19" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1682,19 +1685,17 @@
       <c r="A20" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="B20" s="7">
-        <v>7919</v>
-      </c>
+      <c r="B20" s="7"/>
       <c r="C20" s="7">
         <v>7919</v>
       </c>
-      <c r="D20" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F20" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1702,19 +1703,17 @@
       <c r="A21" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="7">
-        <v>8407</v>
-      </c>
+      <c r="B21" s="7"/>
       <c r="C21" s="7">
         <v>8407</v>
       </c>
-      <c r="D21" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E21" s="7"/>
+      <c r="D21" s="7"/>
+      <c r="E21" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F21" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1722,19 +1721,17 @@
       <c r="A22" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="B22" s="7">
-        <v>9053</v>
-      </c>
+      <c r="B22" s="7"/>
       <c r="C22" s="7">
         <v>9053</v>
       </c>
-      <c r="D22" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F22" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1742,19 +1739,17 @@
       <c r="A23" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B23" s="7">
-        <v>9481</v>
-      </c>
+      <c r="B23" s="7"/>
       <c r="C23" s="7">
         <v>9481</v>
       </c>
-      <c r="D23" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F23" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1762,19 +1757,17 @@
       <c r="A24" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="B24" s="7">
-        <v>10126</v>
-      </c>
+      <c r="B24" s="7"/>
       <c r="C24" s="7">
         <v>10126</v>
       </c>
-      <c r="D24" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E24" s="7"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F24" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1782,19 +1775,17 @@
       <c r="A25" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="7">
-        <v>11221</v>
-      </c>
+      <c r="B25" s="7"/>
       <c r="C25" s="7">
         <v>11221</v>
       </c>
-      <c r="D25" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F25" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1802,19 +1793,17 @@
       <c r="A26" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B26" s="7">
-        <v>11859</v>
-      </c>
+      <c r="B26" s="7"/>
       <c r="C26" s="7">
         <v>11859</v>
       </c>
-      <c r="D26" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F26" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1822,19 +1811,17 @@
       <c r="A27" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B27" s="7">
-        <v>12287</v>
-      </c>
+      <c r="B27" s="7"/>
       <c r="C27" s="7">
         <v>12287</v>
       </c>
-      <c r="D27" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F27" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1842,19 +1829,17 @@
       <c r="A28" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="7">
-        <v>12430</v>
-      </c>
+      <c r="B28" s="7"/>
       <c r="C28" s="7">
         <v>12430</v>
       </c>
-      <c r="D28" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E28" s="7"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F28" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1862,19 +1847,17 @@
       <c r="A29" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="B29" s="7">
-        <v>13089</v>
-      </c>
+      <c r="B29" s="7"/>
       <c r="C29" s="7">
         <v>13089</v>
       </c>
-      <c r="D29" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F29" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1882,19 +1865,17 @@
       <c r="A30" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B30" s="7">
-        <v>13412</v>
-      </c>
+      <c r="B30" s="7"/>
       <c r="C30" s="7">
         <v>13412</v>
       </c>
-      <c r="D30" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E30" s="7"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F30" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1902,19 +1883,17 @@
       <c r="A31" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="7">
-        <v>14071</v>
-      </c>
+      <c r="B31" s="7"/>
       <c r="C31" s="7">
         <v>14071</v>
       </c>
-      <c r="D31" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F31" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1922,19 +1901,17 @@
       <c r="A32" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="7">
-        <v>14755</v>
-      </c>
+      <c r="B32" s="7"/>
       <c r="C32" s="7">
         <v>14755</v>
       </c>
-      <c r="D32" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F32" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1942,19 +1919,17 @@
       <c r="A33" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="B33" s="7">
-        <v>15409</v>
-      </c>
+      <c r="B33" s="7"/>
       <c r="C33" s="7">
         <v>15409</v>
       </c>
-      <c r="D33" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="7"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F33" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1962,19 +1937,17 @@
       <c r="A34" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B34" s="7">
-        <v>15994</v>
-      </c>
+      <c r="B34" s="7"/>
       <c r="C34" s="7">
         <v>15994</v>
       </c>
-      <c r="D34" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E34" s="7"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F34" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -1982,19 +1955,17 @@
       <c r="A35" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="B35" s="7">
-        <v>16640</v>
-      </c>
+      <c r="B35" s="7"/>
       <c r="C35" s="7">
         <v>16640</v>
       </c>
-      <c r="D35" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E35" s="7"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F35" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2002,19 +1973,17 @@
       <c r="A36" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="B36" s="7">
-        <v>17228</v>
-      </c>
+      <c r="B36" s="7"/>
       <c r="C36" s="7">
         <v>17228</v>
       </c>
-      <c r="D36" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E36" s="7"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F36" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2022,19 +1991,17 @@
       <c r="A37" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="B37" s="7">
-        <v>17866</v>
-      </c>
+      <c r="B37" s="7"/>
       <c r="C37" s="7">
         <v>17866</v>
       </c>
-      <c r="D37" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E37" s="7"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F37" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2042,19 +2009,17 @@
       <c r="A38" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="7">
-        <v>18604</v>
-      </c>
+      <c r="B38" s="7"/>
       <c r="C38" s="7">
         <v>18604</v>
       </c>
-      <c r="D38" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E38" s="7"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F38" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2062,19 +2027,17 @@
       <c r="A39" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="B39" s="7">
-        <v>19242</v>
-      </c>
+      <c r="B39" s="7"/>
       <c r="C39" s="7">
         <v>19242</v>
       </c>
-      <c r="D39" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E39" s="7"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F39" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2082,19 +2045,17 @@
       <c r="A40" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B40" s="7">
-        <v>19683</v>
-      </c>
+      <c r="B40" s="7"/>
       <c r="C40" s="7">
         <v>19683</v>
       </c>
-      <c r="D40" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F40" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2102,63 +2063,53 @@
       <c r="A41" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B41" s="7">
-        <v>20330</v>
-      </c>
+      <c r="B41" s="7"/>
       <c r="C41" s="7">
         <v>20330</v>
       </c>
-      <c r="D41" s="3">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="7">
-        <v>20217</v>
-      </c>
-      <c r="F41" s="3">
-        <f t="shared" si="0"/>
-        <v>-113</v>
+      <c r="D41" s="7"/>
+      <c r="E41" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F41" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B42" s="7">
-        <v>21222</v>
-      </c>
+      <c r="B42" s="7"/>
       <c r="C42" s="7">
         <v>21340</v>
       </c>
-      <c r="D42" s="3">
-        <f t="shared" si="1"/>
-        <v>118</v>
-      </c>
-      <c r="E42" s="7">
-        <v>21087</v>
-      </c>
-      <c r="F42" s="3">
-        <f t="shared" si="0"/>
-        <v>-135</v>
+      <c r="D42" s="7"/>
+      <c r="E42" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F42" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B43" s="7">
-        <v>21868</v>
-      </c>
+      <c r="B43" s="7"/>
       <c r="C43" s="7">
         <v>21985</v>
       </c>
-      <c r="D43" s="3">
-        <f t="shared" si="1"/>
-        <v>117</v>
-      </c>
-      <c r="E43" s="7"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F43" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2170,13 +2121,13 @@
       <c r="C44" s="8">
         <v>22936</v>
       </c>
-      <c r="D44" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E44" s="7"/>
+      <c r="D44" s="8"/>
+      <c r="E44" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F44" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2188,13 +2139,13 @@
       <c r="C45" s="7">
         <v>23582</v>
       </c>
-      <c r="D45" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E45" s="7"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F45" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2206,13 +2157,13 @@
       <c r="C46" s="7">
         <v>23922</v>
       </c>
-      <c r="D46" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E46" s="7"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F46" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2224,13 +2175,13 @@
       <c r="C47" s="7">
         <v>24583</v>
       </c>
-      <c r="D47" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E47" s="7"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F47" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2242,13 +2193,13 @@
       <c r="C48" s="7">
         <v>25181</v>
       </c>
-      <c r="D48" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E48" s="7"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F48" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2260,13 +2211,13 @@
       <c r="C49" s="7">
         <v>25839</v>
       </c>
-      <c r="D49" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F49" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2278,13 +2229,13 @@
       <c r="C50" s="7">
         <v>26718</v>
       </c>
-      <c r="D50" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E50" s="7"/>
+      <c r="D50" s="7"/>
+      <c r="E50" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F50" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2296,13 +2247,13 @@
       <c r="C51" s="7">
         <v>27377</v>
       </c>
-      <c r="D51" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E51" s="7"/>
+      <c r="D51" s="7"/>
+      <c r="E51" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F51" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2314,13 +2265,13 @@
       <c r="C52" s="7">
         <v>28030</v>
       </c>
-      <c r="D52" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E52" s="7"/>
+      <c r="D52" s="7"/>
+      <c r="E52" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F52" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2332,13 +2283,13 @@
       <c r="C53" s="7">
         <v>28675</v>
       </c>
-      <c r="D53" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E53" s="7"/>
+      <c r="D53" s="7"/>
+      <c r="E53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F53" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2350,13 +2301,13 @@
       <c r="C54" s="7">
         <v>29030</v>
       </c>
-      <c r="D54" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E54" s="7"/>
+      <c r="D54" s="7"/>
+      <c r="E54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F54" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2368,13 +2319,13 @@
       <c r="C55" s="7">
         <v>29392</v>
       </c>
-      <c r="D55" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E55" s="7"/>
+      <c r="D55" s="7"/>
+      <c r="E55" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F55" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2386,13 +2337,13 @@
       <c r="C56" s="7">
         <v>29423</v>
       </c>
-      <c r="D56" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E56" s="7"/>
+      <c r="D56" s="7"/>
+      <c r="E56" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F56" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2404,13 +2355,13 @@
       <c r="C57" s="7">
         <v>29537</v>
       </c>
-      <c r="D57" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E57" s="7"/>
+      <c r="D57" s="7"/>
+      <c r="E57" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F57" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2422,13 +2373,13 @@
       <c r="C58" s="7">
         <v>29883</v>
       </c>
-      <c r="D58" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E58" s="7"/>
+      <c r="D58" s="7"/>
+      <c r="E58" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F58" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2440,13 +2391,13 @@
       <c r="C59" s="7">
         <v>30378</v>
       </c>
-      <c r="D59" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E59" s="7"/>
+      <c r="D59" s="7"/>
+      <c r="E59" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F59" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2458,13 +2409,13 @@
       <c r="C60" s="7">
         <v>30809</v>
       </c>
-      <c r="D60" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E60" s="7"/>
+      <c r="D60" s="7"/>
+      <c r="E60" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F60" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2476,13 +2427,13 @@
       <c r="C61" s="7">
         <v>31448</v>
       </c>
-      <c r="D61" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E61" s="7"/>
+      <c r="D61" s="7"/>
+      <c r="E61" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F61" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2494,13 +2445,13 @@
       <c r="C62" s="7">
         <v>32009</v>
       </c>
-      <c r="D62" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E62" s="7"/>
+      <c r="D62" s="7"/>
+      <c r="E62" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F62" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2512,13 +2463,13 @@
       <c r="C63" s="7">
         <v>32654</v>
       </c>
-      <c r="D63" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E63" s="7"/>
+      <c r="D63" s="7"/>
+      <c r="E63" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F63" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2530,13 +2481,13 @@
       <c r="C64" s="7">
         <v>33576</v>
       </c>
-      <c r="D64" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E64" s="7"/>
+      <c r="D64" s="7"/>
+      <c r="E64" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F64" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2548,13 +2499,13 @@
       <c r="C65" s="7">
         <v>34235</v>
       </c>
-      <c r="D65" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E65" s="7"/>
+      <c r="D65" s="7"/>
+      <c r="E65" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F65" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2566,13 +2517,13 @@
       <c r="C66" s="7">
         <v>35341</v>
       </c>
-      <c r="D66" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E66" s="7"/>
+      <c r="D66" s="7"/>
+      <c r="E66" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F66" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2584,13 +2535,13 @@
       <c r="C67" s="7">
         <v>35986</v>
       </c>
-      <c r="D67" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F67" s="3" t="str">
-        <f t="shared" ref="F67:F130" si="2">IF(E67&lt;&gt;"",IF(B67&lt;&gt;"",E67-B67,"-"), "-")</f>
+        <f t="shared" si="1"/>
         <v>-</v>
       </c>
     </row>
@@ -2602,13 +2553,13 @@
       <c r="C68" s="7">
         <v>36861</v>
       </c>
-      <c r="D68" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F68" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F68:F131" si="2">IF(D68&lt;&gt;"",IF(B68&lt;&gt;"",D68-B68,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -2620,11 +2571,11 @@
       <c r="C69" s="7">
         <v>37461</v>
       </c>
-      <c r="D69" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F69" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2638,11 +2589,11 @@
       <c r="C70" s="7">
         <v>38564</v>
       </c>
-      <c r="D70" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F70" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2656,11 +2607,11 @@
       <c r="C71" s="7">
         <v>39057</v>
       </c>
-      <c r="D71" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F71" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2674,11 +2625,11 @@
       <c r="C72" s="7">
         <v>39781</v>
       </c>
-      <c r="D72" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F72" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2692,11 +2643,11 @@
       <c r="C73" s="7">
         <v>40405</v>
       </c>
-      <c r="D73" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E73" s="7"/>
+      <c r="D73" s="7"/>
+      <c r="E73" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F73" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2710,11 +2661,11 @@
       <c r="C74" s="9">
         <v>40588</v>
       </c>
-      <c r="D74" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E74" s="7"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F74" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2728,11 +2679,11 @@
       <c r="C75" s="7">
         <v>41228</v>
       </c>
-      <c r="D75" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E75" s="7"/>
+      <c r="D75" s="7"/>
+      <c r="E75" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F75" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2746,11 +2697,11 @@
       <c r="C76" s="9">
         <v>41865</v>
       </c>
-      <c r="D76" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E76" s="7"/>
+      <c r="D76" s="9"/>
+      <c r="E76" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F76" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2764,11 +2715,11 @@
       <c r="C77" s="7">
         <v>42511</v>
       </c>
-      <c r="D77" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E77" s="7"/>
+      <c r="D77" s="7"/>
+      <c r="E77" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F77" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2782,11 +2733,11 @@
       <c r="C78" s="7">
         <v>43110</v>
       </c>
-      <c r="D78" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E78" s="7"/>
+      <c r="D78" s="7"/>
+      <c r="E78" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F78" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2800,11 +2751,11 @@
       <c r="C79" s="7">
         <v>43756</v>
       </c>
-      <c r="D79" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="E79" s="7"/>
+      <c r="D79" s="7"/>
+      <c r="E79" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
       <c r="F79" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2818,11 +2769,11 @@
       <c r="C80" s="7">
         <v>44418</v>
       </c>
-      <c r="D80" s="3" t="str">
-        <f t="shared" ref="D80:D146" si="3">IF(C80&lt;&gt;"",IF(B80&lt;&gt;"",C80-B80,"-"), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="E80" s="7"/>
+      <c r="D80" s="7"/>
+      <c r="E80" s="3" t="str">
+        <f t="shared" ref="E80:E146" si="3">IF(C80&lt;&gt;"",IF(B80&lt;&gt;"",C80-B80,"-"), "-")</f>
+        <v>-</v>
+      </c>
       <c r="F80" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2836,11 +2787,11 @@
       <c r="C81" s="7">
         <v>45077</v>
       </c>
-      <c r="D81" s="3" t="str">
+      <c r="D81" s="7"/>
+      <c r="E81" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E81" s="7"/>
       <c r="F81" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2854,11 +2805,11 @@
       <c r="C82" s="7">
         <v>45719</v>
       </c>
-      <c r="D82" s="3" t="str">
+      <c r="D82" s="7"/>
+      <c r="E82" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E82" s="7"/>
       <c r="F82" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2872,11 +2823,11 @@
       <c r="C83" s="7">
         <v>46378</v>
       </c>
-      <c r="D83" s="3" t="str">
+      <c r="D83" s="7"/>
+      <c r="E83" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E83" s="7"/>
       <c r="F83" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2890,11 +2841,11 @@
       <c r="C84" s="7">
         <v>46984</v>
       </c>
-      <c r="D84" s="3" t="str">
+      <c r="D84" s="7"/>
+      <c r="E84" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E84" s="7"/>
       <c r="F84" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2908,11 +2859,11 @@
       <c r="C85" s="7">
         <v>47629</v>
       </c>
-      <c r="D85" s="3" t="str">
+      <c r="D85" s="7"/>
+      <c r="E85" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E85" s="7"/>
       <c r="F85" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2926,11 +2877,11 @@
       <c r="C86" s="7">
         <v>48410</v>
       </c>
-      <c r="D86" s="3" t="str">
+      <c r="D86" s="7"/>
+      <c r="E86" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E86" s="7"/>
       <c r="F86" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2944,11 +2895,11 @@
       <c r="C87" s="7">
         <v>48908</v>
       </c>
-      <c r="D87" s="3" t="str">
+      <c r="D87" s="7"/>
+      <c r="E87" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E87" s="7"/>
       <c r="F87" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2962,11 +2913,11 @@
       <c r="C88" s="7">
         <v>49856</v>
       </c>
-      <c r="D88" s="3" t="str">
+      <c r="D88" s="7"/>
+      <c r="E88" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E88" s="7"/>
       <c r="F88" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2980,11 +2931,11 @@
       <c r="C89" s="7">
         <v>50516</v>
       </c>
-      <c r="D89" s="3" t="str">
+      <c r="D89" s="7"/>
+      <c r="E89" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E89" s="7"/>
       <c r="F89" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2998,11 +2949,11 @@
       <c r="C90" s="7">
         <v>50874</v>
       </c>
-      <c r="D90" s="3" t="str">
+      <c r="D90" s="7"/>
+      <c r="E90" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E90" s="7"/>
       <c r="F90" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3016,11 +2967,11 @@
       <c r="C91" s="7">
         <v>51486</v>
       </c>
-      <c r="D91" s="3" t="str">
+      <c r="D91" s="7"/>
+      <c r="E91" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E91" s="7"/>
       <c r="F91" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3034,11 +2985,11 @@
       <c r="C92" s="7">
         <v>52507</v>
       </c>
-      <c r="D92" s="3" t="str">
+      <c r="D92" s="7"/>
+      <c r="E92" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E92" s="7"/>
       <c r="F92" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3052,11 +3003,11 @@
       <c r="C93" s="7">
         <v>53153</v>
       </c>
-      <c r="D93" s="3" t="str">
+      <c r="D93" s="7"/>
+      <c r="E93" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E93" s="7"/>
       <c r="F93" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3070,11 +3021,11 @@
       <c r="C94" s="7">
         <v>53942</v>
       </c>
-      <c r="D94" s="3" t="str">
+      <c r="D94" s="7"/>
+      <c r="E94" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E94" s="7"/>
       <c r="F94" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3088,11 +3039,11 @@
       <c r="C95" s="7">
         <v>54564</v>
       </c>
-      <c r="D95" s="3" t="str">
+      <c r="D95" s="7"/>
+      <c r="E95" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E95" s="7"/>
       <c r="F95" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3106,11 +3057,11 @@
       <c r="C96" s="7">
         <v>55596</v>
       </c>
-      <c r="D96" s="3" t="str">
+      <c r="D96" s="7"/>
+      <c r="E96" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E96" s="7"/>
       <c r="F96" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3124,11 +3075,11 @@
       <c r="C97" s="7">
         <v>56185</v>
       </c>
-      <c r="D97" s="3" t="str">
+      <c r="D97" s="7"/>
+      <c r="E97" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E97" s="7"/>
       <c r="F97" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3140,11 +3091,11 @@
       <c r="C98" s="7">
         <v>56464</v>
       </c>
-      <c r="D98" s="3" t="str">
+      <c r="D98" s="7"/>
+      <c r="E98" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E98" s="7"/>
       <c r="F98" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3158,11 +3109,11 @@
       <c r="C99" s="7">
         <v>56572</v>
       </c>
-      <c r="D99" s="3" t="str">
+      <c r="D99" s="7"/>
+      <c r="E99" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E99" s="7"/>
       <c r="F99" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3176,11 +3127,11 @@
       <c r="C100" s="7">
         <v>57217</v>
       </c>
-      <c r="D100" s="3" t="str">
+      <c r="D100" s="7"/>
+      <c r="E100" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E100" s="7"/>
       <c r="F100" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3194,11 +3145,11 @@
       <c r="C101" s="7">
         <v>57373</v>
       </c>
-      <c r="D101" s="3" t="str">
+      <c r="D101" s="7"/>
+      <c r="E101" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E101" s="7"/>
       <c r="F101" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3212,11 +3163,11 @@
       <c r="C102" s="7">
         <v>57657</v>
       </c>
-      <c r="D102" s="3" t="str">
+      <c r="D102" s="7"/>
+      <c r="E102" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E102" s="7"/>
       <c r="F102" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3230,11 +3181,11 @@
       <c r="C103" s="7">
         <v>58008</v>
       </c>
-      <c r="D103" s="3" t="str">
+      <c r="D103" s="7"/>
+      <c r="E103" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E103" s="7"/>
       <c r="F103" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3248,11 +3199,11 @@
       <c r="C104" s="7">
         <v>58608</v>
       </c>
-      <c r="D104" s="3" t="str">
+      <c r="D104" s="7"/>
+      <c r="E104" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E104" s="7"/>
       <c r="F104" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3266,11 +3217,11 @@
       <c r="C105" s="7">
         <v>59190</v>
       </c>
-      <c r="D105" s="3" t="str">
+      <c r="D105" s="7"/>
+      <c r="E105" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E105" s="7"/>
       <c r="F105" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3284,11 +3235,11 @@
       <c r="C106" s="7">
         <v>59825</v>
       </c>
-      <c r="D106" s="3" t="str">
+      <c r="D106" s="7"/>
+      <c r="E106" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E106" s="7"/>
       <c r="F106" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3302,11 +3253,11 @@
       <c r="C107" s="7">
         <v>60441</v>
       </c>
-      <c r="D107" s="3" t="str">
+      <c r="D107" s="7"/>
+      <c r="E107" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E107" s="7"/>
       <c r="F107" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3320,11 +3271,11 @@
       <c r="C108" s="7">
         <v>61093</v>
       </c>
-      <c r="D108" s="3" t="str">
+      <c r="D108" s="7"/>
+      <c r="E108" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E108" s="7"/>
       <c r="F108" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3338,11 +3289,11 @@
       <c r="C109" s="10">
         <v>61914</v>
       </c>
-      <c r="D109" s="3" t="str">
+      <c r="D109" s="10"/>
+      <c r="E109" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E109" s="7"/>
       <c r="F109" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3356,11 +3307,11 @@
       <c r="C110" s="7">
         <v>62575</v>
       </c>
-      <c r="D110" s="3" t="str">
+      <c r="D110" s="7"/>
+      <c r="E110" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E110" s="7"/>
       <c r="F110" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3374,11 +3325,11 @@
       <c r="C111" s="7">
         <v>63180</v>
       </c>
-      <c r="D111" s="3" t="str">
+      <c r="D111" s="7"/>
+      <c r="E111" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E111" s="7"/>
       <c r="F111" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3392,11 +3343,11 @@
       <c r="C112" s="7">
         <v>63825</v>
       </c>
-      <c r="D112" s="3" t="str">
+      <c r="D112" s="7"/>
+      <c r="E112" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E112" s="7"/>
       <c r="F112" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3410,11 +3361,11 @@
       <c r="C113" s="7">
         <v>64581</v>
       </c>
-      <c r="D113" s="3" t="str">
+      <c r="D113" s="7"/>
+      <c r="E113" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E113" s="7"/>
       <c r="F113" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3428,11 +3379,11 @@
       <c r="C114" s="7">
         <v>65231</v>
       </c>
-      <c r="D114" s="3" t="str">
+      <c r="D114" s="7"/>
+      <c r="E114" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E114" s="7"/>
       <c r="F114" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3448,27 +3399,25 @@
       <c r="C115" s="7">
         <v>65818</v>
       </c>
-      <c r="D115" s="3">
+      <c r="D115" s="7"/>
+      <c r="E115" s="3">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E115" s="7">
-        <v>65085</v>
-      </c>
-      <c r="F115" s="3">
+      <c r="F115" s="3" t="str">
         <f t="shared" si="2"/>
-        <v>-733</v>
+        <v>-</v>
       </c>
     </row>
     <row r="116" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
-      <c r="D116" s="3" t="str">
+      <c r="D116" s="7"/>
+      <c r="E116" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E116" s="7"/>
       <c r="F116" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3478,11 +3427,11 @@
       <c r="A117" s="7"/>
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
-      <c r="D117" s="3" t="str">
+      <c r="D117" s="7"/>
+      <c r="E117" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E117" s="7"/>
       <c r="F117" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3492,11 +3441,11 @@
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
       <c r="C118" s="7"/>
-      <c r="D118" s="3" t="str">
+      <c r="D118" s="7"/>
+      <c r="E118" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E118" s="7"/>
       <c r="F118" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3506,11 +3455,11 @@
       <c r="A119" s="7"/>
       <c r="B119" s="7"/>
       <c r="C119" s="7"/>
-      <c r="D119" s="3" t="str">
+      <c r="D119" s="7"/>
+      <c r="E119" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E119" s="7"/>
       <c r="F119" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3520,11 +3469,11 @@
       <c r="A120" s="7"/>
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
-      <c r="D120" s="3" t="str">
+      <c r="D120" s="7"/>
+      <c r="E120" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E120" s="7"/>
       <c r="F120" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3534,11 +3483,11 @@
       <c r="A121" s="7"/>
       <c r="B121" s="7"/>
       <c r="C121" s="7"/>
-      <c r="D121" s="3" t="str">
+      <c r="D121" s="7"/>
+      <c r="E121" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E121" s="7"/>
       <c r="F121" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3548,11 +3497,11 @@
       <c r="A122" s="7"/>
       <c r="B122" s="7"/>
       <c r="C122" s="7"/>
-      <c r="D122" s="3" t="str">
+      <c r="D122" s="7"/>
+      <c r="E122" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E122" s="7"/>
       <c r="F122" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3562,11 +3511,11 @@
       <c r="A123" s="7"/>
       <c r="B123" s="7"/>
       <c r="C123" s="7"/>
-      <c r="D123" s="3" t="str">
+      <c r="D123" s="7"/>
+      <c r="E123" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E123" s="7"/>
       <c r="F123" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3576,11 +3525,11 @@
       <c r="A124" s="7"/>
       <c r="B124" s="7"/>
       <c r="C124" s="7"/>
-      <c r="D124" s="3" t="str">
+      <c r="D124" s="7"/>
+      <c r="E124" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E124" s="7"/>
       <c r="F124" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3590,11 +3539,11 @@
       <c r="A125" s="7"/>
       <c r="B125" s="7"/>
       <c r="C125" s="7"/>
-      <c r="D125" s="3" t="str">
+      <c r="D125" s="7"/>
+      <c r="E125" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E125" s="7"/>
       <c r="F125" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3604,11 +3553,11 @@
       <c r="A126" s="7"/>
       <c r="B126" s="7"/>
       <c r="C126" s="7"/>
-      <c r="D126" s="3" t="str">
+      <c r="D126" s="7"/>
+      <c r="E126" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E126" s="7"/>
       <c r="F126" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3618,11 +3567,11 @@
       <c r="A127" s="7"/>
       <c r="B127" s="7"/>
       <c r="C127" s="7"/>
-      <c r="D127" s="3" t="str">
+      <c r="D127" s="7"/>
+      <c r="E127" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E127" s="7"/>
       <c r="F127" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3632,11 +3581,11 @@
       <c r="A128" s="7"/>
       <c r="B128" s="7"/>
       <c r="C128" s="7"/>
-      <c r="D128" s="3" t="str">
+      <c r="D128" s="7"/>
+      <c r="E128" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E128" s="7"/>
       <c r="F128" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3646,11 +3595,11 @@
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
-      <c r="D129" s="3" t="str">
+      <c r="D129" s="7"/>
+      <c r="E129" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E129" s="7"/>
       <c r="F129" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3660,11 +3609,11 @@
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
-      <c r="D130" s="3" t="str">
+      <c r="D130" s="7"/>
+      <c r="E130" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E130" s="7"/>
       <c r="F130" s="3" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3674,13 +3623,13 @@
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
-      <c r="D131" s="3" t="str">
+      <c r="D131" s="7"/>
+      <c r="E131" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E131" s="7"/>
       <c r="F131" s="3" t="str">
-        <f t="shared" ref="F131:F145" si="4">IF(E131&lt;&gt;"",IF(B131&lt;&gt;"",E131-B131,"-"), "-")</f>
+        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
@@ -3688,13 +3637,13 @@
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
-      <c r="D132" s="3" t="str">
+      <c r="D132" s="7"/>
+      <c r="E132" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E132" s="7"/>
       <c r="F132" s="3" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F132:F135" si="4">IF(D132&lt;&gt;"",IF(B132&lt;&gt;"",D132-B132,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -3702,11 +3651,11 @@
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
-      <c r="D133" s="3" t="str">
+      <c r="D133" s="7"/>
+      <c r="E133" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E133" s="7"/>
       <c r="F133" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -3716,11 +3665,11 @@
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
-      <c r="D134" s="3" t="str">
+      <c r="D134" s="7"/>
+      <c r="E134" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E134" s="7"/>
       <c r="F134" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -3730,11 +3679,11 @@
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
-      <c r="D135" s="3" t="str">
+      <c r="D135" s="7"/>
+      <c r="E135" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="E135" s="7"/>
       <c r="F135" s="3" t="str">
         <f t="shared" si="4"/>
         <v>-</v>
@@ -3744,12 +3693,9 @@
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
-      <c r="D136" s="3" t="str">
+      <c r="D136" s="7"/>
+      <c r="E136" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F136" s="3" t="str">
-        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3757,12 +3703,9 @@
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
-      <c r="D137" s="3" t="str">
+      <c r="D137" s="7"/>
+      <c r="E137" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F137" s="3" t="str">
-        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3770,12 +3713,9 @@
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
-      <c r="D138" s="3" t="str">
+      <c r="D138" s="7"/>
+      <c r="E138" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F138" s="3" t="str">
-        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3783,12 +3723,9 @@
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
-      <c r="D139" s="3" t="str">
+      <c r="D139" s="7"/>
+      <c r="E139" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F139" s="3" t="str">
-        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3796,12 +3733,9 @@
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
-      <c r="D140" s="3" t="str">
+      <c r="D140" s="7"/>
+      <c r="E140" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F140" s="3" t="str">
-        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3809,12 +3743,9 @@
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
-      <c r="D141" s="3" t="str">
+      <c r="D141" s="7"/>
+      <c r="E141" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F141" s="3" t="str">
-        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3822,12 +3753,9 @@
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
-      <c r="D142" s="3" t="str">
+      <c r="D142" s="7"/>
+      <c r="E142" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F142" s="3" t="str">
-        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3835,12 +3763,9 @@
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
-      <c r="D143" s="3" t="str">
+      <c r="D143" s="7"/>
+      <c r="E143" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F143" s="3" t="str">
-        <f t="shared" si="4"/>
         <v>-</v>
       </c>
     </row>
@@ -3848,657 +3773,798 @@
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
-      <c r="D144" s="3" t="str">
+      <c r="D144" s="7"/>
+      <c r="E144" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F144" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="145" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
-      <c r="D145" s="3" t="str">
+      <c r="D145" s="7"/>
+      <c r="E145" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F145" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
-      <c r="D146" s="3" t="str">
+      <c r="D146" s="7"/>
+      <c r="E146" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
-    <row r="147" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="7"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
-      <c r="D147" s="3" t="str">
-        <f t="shared" ref="D147:D151" si="5">IF(C147&lt;&gt;"",IF(B147&lt;&gt;"",C147-B147,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="D147" s="7"/>
+      <c r="E147" s="3" t="str">
+        <f t="shared" ref="E147:E151" si="5">IF(C147&lt;&gt;"",IF(B147&lt;&gt;"",C147-B147,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A148" s="7"/>
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
-      <c r="D148" s="3" t="str">
+      <c r="D148" s="7"/>
+      <c r="E148" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
-    <row r="149" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A149" s="7"/>
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
-      <c r="D149" s="3" t="str">
+      <c r="D149" s="7"/>
+      <c r="E149" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A150" s="7"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
-      <c r="D150" s="3" t="str">
+      <c r="D150" s="7"/>
+      <c r="E150" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
-    <row r="151" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A151" s="7"/>
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
-      <c r="D151" s="3" t="str">
+      <c r="D151" s="7"/>
+      <c r="E151" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
-    <row r="152" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A152" s="7"/>
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
-      <c r="D152" s="3" t="str">
-        <f t="shared" ref="D152:D153" si="6">IF(C152&lt;&gt;"",IF(B152&lt;&gt;"",B152-C152,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="D152" s="7"/>
+      <c r="E152" s="3" t="str">
+        <f t="shared" ref="E152:E153" si="6">IF(C152&lt;&gt;"",IF(B152&lt;&gt;"",B152-C152,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A153" s="7"/>
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
-      <c r="D153" s="3" t="str">
+      <c r="D153" s="7"/>
+      <c r="E153" s="3" t="str">
         <f t="shared" si="6"/>
         <v>-</v>
       </c>
     </row>
-    <row r="154" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A154" s="7"/>
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
-    </row>
-    <row r="155" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="D154" s="7"/>
+    </row>
+    <row r="155" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A155" s="7"/>
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
-    </row>
-    <row r="156" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="D155" s="7"/>
+    </row>
+    <row r="156" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
-    </row>
-    <row r="157" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="D156" s="7"/>
+    </row>
+    <row r="157" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
-    </row>
-    <row r="158" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="D157" s="7"/>
+    </row>
+    <row r="158" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
-    </row>
-    <row r="159" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="D158" s="7"/>
+    </row>
+    <row r="159" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
-    </row>
-    <row r="160" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="D159" s="7"/>
+    </row>
+    <row r="160" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
-    </row>
-    <row r="161" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D160" s="7"/>
+    </row>
+    <row r="161" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B161" s="7"/>
       <c r="C161" s="7"/>
-    </row>
-    <row r="162" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D161" s="7"/>
+    </row>
+    <row r="162" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B162" s="7"/>
       <c r="C162" s="7"/>
-    </row>
-    <row r="163" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D162" s="7"/>
+    </row>
+    <row r="163" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B163" s="7"/>
       <c r="C163" s="7"/>
-    </row>
-    <row r="164" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D163" s="7"/>
+    </row>
+    <row r="164" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B164" s="7"/>
       <c r="C164" s="7"/>
-    </row>
-    <row r="165" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D164" s="7"/>
+    </row>
+    <row r="165" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B165" s="7"/>
       <c r="C165" s="7"/>
-    </row>
-    <row r="166" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D165" s="7"/>
+    </row>
+    <row r="166" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B166" s="7"/>
       <c r="C166" s="7"/>
-    </row>
-    <row r="167" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D166" s="7"/>
+    </row>
+    <row r="167" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
-    </row>
-    <row r="168" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D167" s="7"/>
+    </row>
+    <row r="168" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B168" s="7"/>
       <c r="C168" s="7"/>
-    </row>
-    <row r="169" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D168" s="7"/>
+    </row>
+    <row r="169" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B169" s="7"/>
       <c r="C169" s="7"/>
-    </row>
-    <row r="170" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D169" s="7"/>
+    </row>
+    <row r="170" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B170" s="7"/>
       <c r="C170" s="7"/>
-    </row>
-    <row r="171" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D170" s="7"/>
+    </row>
+    <row r="171" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B171" s="7"/>
       <c r="C171" s="7"/>
-    </row>
-    <row r="172" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D171" s="7"/>
+    </row>
+    <row r="172" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B172" s="7"/>
       <c r="C172" s="7"/>
-    </row>
-    <row r="173" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D172" s="7"/>
+    </row>
+    <row r="173" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B173" s="7"/>
       <c r="C173" s="7"/>
-    </row>
-    <row r="174" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D173" s="7"/>
+    </row>
+    <row r="174" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B174" s="7"/>
       <c r="C174" s="7"/>
-    </row>
-    <row r="175" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D174" s="7"/>
+    </row>
+    <row r="175" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B175" s="7"/>
       <c r="C175" s="7"/>
-    </row>
-    <row r="176" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D175" s="7"/>
+    </row>
+    <row r="176" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B176" s="7"/>
       <c r="C176" s="7"/>
-    </row>
-    <row r="177" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D176" s="7"/>
+    </row>
+    <row r="177" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B177" s="7"/>
       <c r="C177" s="7"/>
-    </row>
-    <row r="178" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D177" s="7"/>
+    </row>
+    <row r="178" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B178" s="7"/>
       <c r="C178" s="7"/>
-    </row>
-    <row r="179" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D178" s="7"/>
+    </row>
+    <row r="179" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B179" s="7"/>
       <c r="C179" s="7"/>
-    </row>
-    <row r="180" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D179" s="7"/>
+    </row>
+    <row r="180" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B180" s="7"/>
       <c r="C180" s="7"/>
-    </row>
-    <row r="181" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D180" s="7"/>
+    </row>
+    <row r="181" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B181" s="7"/>
       <c r="C181" s="7"/>
-    </row>
-    <row r="182" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D181" s="7"/>
+    </row>
+    <row r="182" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B182" s="7"/>
       <c r="C182" s="7"/>
-    </row>
-    <row r="183" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D182" s="7"/>
+    </row>
+    <row r="183" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B183" s="7"/>
       <c r="C183" s="7"/>
-    </row>
-    <row r="184" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D183" s="7"/>
+    </row>
+    <row r="184" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B184" s="7"/>
       <c r="C184" s="7"/>
-    </row>
-    <row r="185" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D184" s="7"/>
+    </row>
+    <row r="185" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B185" s="7"/>
       <c r="C185" s="7"/>
-    </row>
-    <row r="186" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D185" s="7"/>
+    </row>
+    <row r="186" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B186" s="7"/>
       <c r="C186" s="7"/>
-    </row>
-    <row r="187" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D186" s="7"/>
+    </row>
+    <row r="187" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B187" s="7"/>
       <c r="C187" s="7"/>
-    </row>
-    <row r="188" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D187" s="7"/>
+    </row>
+    <row r="188" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B188" s="7"/>
       <c r="C188" s="7"/>
-    </row>
-    <row r="189" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D188" s="7"/>
+    </row>
+    <row r="189" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B189" s="7"/>
       <c r="C189" s="7"/>
-    </row>
-    <row r="190" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D189" s="7"/>
+    </row>
+    <row r="190" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B190" s="7"/>
       <c r="C190" s="7"/>
-    </row>
-    <row r="191" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D190" s="7"/>
+    </row>
+    <row r="191" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B191" s="7"/>
       <c r="C191" s="7"/>
-    </row>
-    <row r="192" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D191" s="7"/>
+    </row>
+    <row r="192" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B192" s="7"/>
       <c r="C192" s="7"/>
-    </row>
-    <row r="193" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D192" s="7"/>
+    </row>
+    <row r="193" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B193" s="7"/>
       <c r="C193" s="7"/>
-    </row>
-    <row r="194" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D193" s="7"/>
+    </row>
+    <row r="194" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B194" s="7"/>
       <c r="C194" s="7"/>
-    </row>
-    <row r="195" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D194" s="7"/>
+    </row>
+    <row r="195" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B195" s="7"/>
       <c r="C195" s="7"/>
-    </row>
-    <row r="196" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D195" s="7"/>
+    </row>
+    <row r="196" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B196" s="7"/>
       <c r="C196" s="7"/>
-    </row>
-    <row r="197" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D196" s="7"/>
+    </row>
+    <row r="197" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B197" s="7"/>
       <c r="C197" s="7"/>
-    </row>
-    <row r="198" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D197" s="7"/>
+    </row>
+    <row r="198" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B198" s="7"/>
       <c r="C198" s="7"/>
-    </row>
-    <row r="199" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D198" s="7"/>
+    </row>
+    <row r="199" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B199" s="7"/>
       <c r="C199" s="7"/>
-    </row>
-    <row r="200" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D199" s="7"/>
+    </row>
+    <row r="200" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B200" s="7"/>
       <c r="C200" s="7"/>
-    </row>
-    <row r="201" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D200" s="7"/>
+    </row>
+    <row r="201" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B201" s="7"/>
       <c r="C201" s="7"/>
-    </row>
-    <row r="202" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D201" s="7"/>
+    </row>
+    <row r="202" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B202" s="7"/>
       <c r="C202" s="7"/>
-    </row>
-    <row r="203" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D202" s="7"/>
+    </row>
+    <row r="203" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B203" s="7"/>
       <c r="C203" s="7"/>
-    </row>
-    <row r="204" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D203" s="7"/>
+    </row>
+    <row r="204" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B204" s="7"/>
       <c r="C204" s="7"/>
-    </row>
-    <row r="205" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D204" s="7"/>
+    </row>
+    <row r="205" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B205" s="7"/>
       <c r="C205" s="7"/>
-    </row>
-    <row r="206" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D205" s="7"/>
+    </row>
+    <row r="206" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B206" s="7"/>
       <c r="C206" s="7"/>
-    </row>
-    <row r="207" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D206" s="7"/>
+    </row>
+    <row r="207" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B207" s="7"/>
       <c r="C207" s="7"/>
-    </row>
-    <row r="208" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D207" s="7"/>
+    </row>
+    <row r="208" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B208" s="7"/>
       <c r="C208" s="7"/>
-    </row>
-    <row r="209" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D208" s="7"/>
+    </row>
+    <row r="209" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B209" s="7"/>
       <c r="C209" s="7"/>
-    </row>
-    <row r="210" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D209" s="7"/>
+    </row>
+    <row r="210" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B210" s="7"/>
       <c r="C210" s="7"/>
-    </row>
-    <row r="211" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D210" s="7"/>
+    </row>
+    <row r="211" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B211" s="7"/>
       <c r="C211" s="7"/>
-    </row>
-    <row r="212" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D211" s="7"/>
+    </row>
+    <row r="212" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B212" s="7"/>
       <c r="C212" s="7"/>
-    </row>
-    <row r="213" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D212" s="7"/>
+    </row>
+    <row r="213" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B213" s="7"/>
       <c r="C213" s="7"/>
-    </row>
-    <row r="214" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D213" s="7"/>
+    </row>
+    <row r="214" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B214" s="7"/>
       <c r="C214" s="7"/>
-    </row>
-    <row r="215" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D214" s="7"/>
+    </row>
+    <row r="215" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B215" s="7"/>
       <c r="C215" s="7"/>
-    </row>
-    <row r="216" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D215" s="7"/>
+    </row>
+    <row r="216" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B216" s="7"/>
       <c r="C216" s="7"/>
-    </row>
-    <row r="217" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D216" s="7"/>
+    </row>
+    <row r="217" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B217" s="7"/>
       <c r="C217" s="7"/>
-    </row>
-    <row r="218" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D217" s="7"/>
+    </row>
+    <row r="218" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B218" s="7"/>
       <c r="C218" s="7"/>
-    </row>
-    <row r="219" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D218" s="7"/>
+    </row>
+    <row r="219" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B219" s="7"/>
       <c r="C219" s="7"/>
-    </row>
-    <row r="220" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D219" s="7"/>
+    </row>
+    <row r="220" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B220" s="7"/>
       <c r="C220" s="7"/>
-    </row>
-    <row r="221" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D220" s="7"/>
+    </row>
+    <row r="221" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B221" s="7"/>
       <c r="C221" s="7"/>
-    </row>
-    <row r="222" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D221" s="7"/>
+    </row>
+    <row r="222" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B222" s="7"/>
       <c r="C222" s="7"/>
-    </row>
-    <row r="223" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D222" s="7"/>
+    </row>
+    <row r="223" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B223" s="7"/>
       <c r="C223" s="7"/>
-    </row>
-    <row r="224" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D223" s="7"/>
+    </row>
+    <row r="224" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B224" s="7"/>
       <c r="C224" s="7"/>
-    </row>
-    <row r="225" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D224" s="7"/>
+    </row>
+    <row r="225" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B225" s="7"/>
       <c r="C225" s="7"/>
-    </row>
-    <row r="226" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D225" s="7"/>
+    </row>
+    <row r="226" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B226" s="7"/>
       <c r="C226" s="7"/>
-    </row>
-    <row r="227" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D226" s="7"/>
+    </row>
+    <row r="227" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B227" s="7"/>
       <c r="C227" s="7"/>
-    </row>
-    <row r="228" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D227" s="7"/>
+    </row>
+    <row r="228" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B228" s="7"/>
       <c r="C228" s="7"/>
-    </row>
-    <row r="229" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D228" s="7"/>
+    </row>
+    <row r="229" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B229" s="7"/>
       <c r="C229" s="7"/>
-    </row>
-    <row r="230" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D229" s="7"/>
+    </row>
+    <row r="230" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B230" s="7"/>
       <c r="C230" s="7"/>
-    </row>
-    <row r="231" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D230" s="7"/>
+    </row>
+    <row r="231" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B231" s="7"/>
       <c r="C231" s="7"/>
-    </row>
-    <row r="232" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D231" s="7"/>
+    </row>
+    <row r="232" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B232" s="7"/>
       <c r="C232" s="7"/>
-    </row>
-    <row r="233" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D232" s="7"/>
+    </row>
+    <row r="233" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B233" s="7"/>
       <c r="C233" s="7"/>
-    </row>
-    <row r="234" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D233" s="7"/>
+    </row>
+    <row r="234" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B234" s="7"/>
       <c r="C234" s="7"/>
-    </row>
-    <row r="235" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D234" s="7"/>
+    </row>
+    <row r="235" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B235" s="7"/>
       <c r="C235" s="7"/>
-    </row>
-    <row r="236" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D235" s="7"/>
+    </row>
+    <row r="236" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B236" s="7"/>
       <c r="C236" s="7"/>
-    </row>
-    <row r="237" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D236" s="7"/>
+    </row>
+    <row r="237" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B237" s="7"/>
       <c r="C237" s="7"/>
-    </row>
-    <row r="238" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D237" s="7"/>
+    </row>
+    <row r="238" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B238" s="7"/>
       <c r="C238" s="7"/>
-    </row>
-    <row r="239" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D238" s="7"/>
+    </row>
+    <row r="239" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B239" s="7"/>
       <c r="C239" s="7"/>
-    </row>
-    <row r="240" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D239" s="7"/>
+    </row>
+    <row r="240" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B240" s="7"/>
       <c r="C240" s="7"/>
-    </row>
-    <row r="241" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D240" s="7"/>
+    </row>
+    <row r="241" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B241" s="7"/>
       <c r="C241" s="7"/>
-    </row>
-    <row r="242" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D241" s="7"/>
+    </row>
+    <row r="242" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B242" s="7"/>
       <c r="C242" s="7"/>
-    </row>
-    <row r="243" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D242" s="7"/>
+    </row>
+    <row r="243" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B243" s="7"/>
       <c r="C243" s="7"/>
-    </row>
-    <row r="244" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D243" s="7"/>
+    </row>
+    <row r="244" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B244" s="7"/>
       <c r="C244" s="7"/>
-    </row>
-    <row r="245" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D244" s="7"/>
+    </row>
+    <row r="245" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B245" s="7"/>
       <c r="C245" s="7"/>
-    </row>
-    <row r="246" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D245" s="7"/>
+    </row>
+    <row r="246" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B246" s="7"/>
       <c r="C246" s="7"/>
-    </row>
-    <row r="247" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D246" s="7"/>
+    </row>
+    <row r="247" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B247" s="7"/>
       <c r="C247" s="7"/>
-    </row>
-    <row r="248" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D247" s="7"/>
+    </row>
+    <row r="248" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B248" s="7"/>
       <c r="C248" s="7"/>
-    </row>
-    <row r="249" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D248" s="7"/>
+    </row>
+    <row r="249" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B249" s="7"/>
       <c r="C249" s="7"/>
-    </row>
-    <row r="250" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D249" s="7"/>
+    </row>
+    <row r="250" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B250" s="7"/>
       <c r="C250" s="7"/>
-    </row>
-    <row r="251" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D250" s="7"/>
+    </row>
+    <row r="251" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B251" s="7"/>
       <c r="C251" s="7"/>
-    </row>
-    <row r="252" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D251" s="7"/>
+    </row>
+    <row r="252" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B252" s="7"/>
       <c r="C252" s="7"/>
-    </row>
-    <row r="253" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D252" s="7"/>
+    </row>
+    <row r="253" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B253" s="7"/>
       <c r="C253" s="7"/>
-    </row>
-    <row r="254" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D253" s="7"/>
+    </row>
+    <row r="254" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B254" s="7"/>
       <c r="C254" s="7"/>
-    </row>
-    <row r="255" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D254" s="7"/>
+    </row>
+    <row r="255" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B255" s="7"/>
       <c r="C255" s="7"/>
-    </row>
-    <row r="256" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D255" s="7"/>
+    </row>
+    <row r="256" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B256" s="7"/>
       <c r="C256" s="7"/>
-    </row>
-    <row r="257" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D256" s="7"/>
+    </row>
+    <row r="257" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B257" s="7"/>
       <c r="C257" s="7"/>
-    </row>
-    <row r="258" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D257" s="7"/>
+    </row>
+    <row r="258" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B258" s="7"/>
       <c r="C258" s="7"/>
-    </row>
-    <row r="259" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D258" s="7"/>
+    </row>
+    <row r="259" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B259" s="7"/>
       <c r="C259" s="7"/>
-    </row>
-    <row r="260" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D259" s="7"/>
+    </row>
+    <row r="260" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B260" s="7"/>
       <c r="C260" s="7"/>
-    </row>
-    <row r="261" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D260" s="7"/>
+    </row>
+    <row r="261" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B261" s="7"/>
       <c r="C261" s="7"/>
-    </row>
-    <row r="262" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D261" s="7"/>
+    </row>
+    <row r="262" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B262" s="7"/>
       <c r="C262" s="7"/>
-    </row>
-    <row r="263" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D262" s="7"/>
+    </row>
+    <row r="263" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B263" s="7"/>
       <c r="C263" s="7"/>
-    </row>
-    <row r="264" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D263" s="7"/>
+    </row>
+    <row r="264" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B264" s="7"/>
       <c r="C264" s="7"/>
-    </row>
-    <row r="265" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D264" s="7"/>
+    </row>
+    <row r="265" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B265" s="7"/>
       <c r="C265" s="7"/>
-    </row>
-    <row r="266" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D265" s="7"/>
+    </row>
+    <row r="266" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B266" s="7"/>
       <c r="C266" s="7"/>
-    </row>
-    <row r="267" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D266" s="7"/>
+    </row>
+    <row r="267" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B267" s="7"/>
       <c r="C267" s="7"/>
-    </row>
-    <row r="268" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D267" s="7"/>
+    </row>
+    <row r="268" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B268" s="7"/>
       <c r="C268" s="7"/>
-    </row>
-    <row r="269" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D268" s="7"/>
+    </row>
+    <row r="269" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B269" s="7"/>
       <c r="C269" s="7"/>
-    </row>
-    <row r="270" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D269" s="7"/>
+    </row>
+    <row r="270" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B270" s="7"/>
       <c r="C270" s="7"/>
-    </row>
-    <row r="271" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D270" s="7"/>
+    </row>
+    <row r="271" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B271" s="7"/>
       <c r="C271" s="7"/>
-    </row>
-    <row r="272" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D271" s="7"/>
+    </row>
+    <row r="272" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B272" s="7"/>
       <c r="C272" s="7"/>
-    </row>
-    <row r="273" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D272" s="7"/>
+    </row>
+    <row r="273" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B273" s="7"/>
       <c r="C273" s="7"/>
-    </row>
-    <row r="274" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D273" s="7"/>
+    </row>
+    <row r="274" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B274" s="7"/>
       <c r="C274" s="7"/>
-    </row>
-    <row r="275" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D274" s="7"/>
+    </row>
+    <row r="275" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B275" s="7"/>
       <c r="C275" s="7"/>
-    </row>
-    <row r="276" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D275" s="7"/>
+    </row>
+    <row r="276" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B276" s="7"/>
       <c r="C276" s="7"/>
-    </row>
-    <row r="277" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D276" s="7"/>
+    </row>
+    <row r="277" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B277" s="7"/>
       <c r="C277" s="7"/>
-    </row>
-    <row r="278" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D277" s="7"/>
+    </row>
+    <row r="278" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B278" s="7"/>
       <c r="C278" s="7"/>
-    </row>
-    <row r="279" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D278" s="7"/>
+    </row>
+    <row r="279" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B279" s="7"/>
       <c r="C279" s="7"/>
-    </row>
-    <row r="280" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D279" s="7"/>
+    </row>
+    <row r="280" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B280" s="7"/>
       <c r="C280" s="7"/>
-    </row>
-    <row r="281" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D280" s="7"/>
+    </row>
+    <row r="281" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B281" s="7"/>
       <c r="C281" s="7"/>
-    </row>
-    <row r="282" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D281" s="7"/>
+    </row>
+    <row r="282" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B282" s="7"/>
       <c r="C282" s="7"/>
-    </row>
-    <row r="283" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D282" s="7"/>
+    </row>
+    <row r="283" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B283" s="7"/>
       <c r="C283" s="7"/>
-    </row>
-    <row r="284" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D283" s="7"/>
+    </row>
+    <row r="284" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B284" s="7"/>
       <c r="C284" s="7"/>
-    </row>
-    <row r="285" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D284" s="7"/>
+    </row>
+    <row r="285" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B285" s="7"/>
       <c r="C285" s="7"/>
-    </row>
-    <row r="286" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D285" s="7"/>
+    </row>
+    <row r="286" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B286" s="7"/>
       <c r="C286" s="7"/>
-    </row>
-    <row r="287" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D286" s="7"/>
+    </row>
+    <row r="287" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B287" s="7"/>
       <c r="C287" s="7"/>
-    </row>
-    <row r="288" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D287" s="7"/>
+    </row>
+    <row r="288" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B288" s="7"/>
       <c r="C288" s="7"/>
-    </row>
-    <row r="289" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D288" s="7"/>
+    </row>
+    <row r="289" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B289" s="7"/>
       <c r="C289" s="7"/>
-    </row>
-    <row r="290" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D289" s="7"/>
+    </row>
+    <row r="290" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B290" s="7"/>
       <c r="C290" s="7"/>
-    </row>
-    <row r="291" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D290" s="7"/>
+    </row>
+    <row r="291" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B291" s="7"/>
       <c r="C291" s="7"/>
-    </row>
-    <row r="292" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+      <c r="D291" s="7"/>
+    </row>
+    <row r="292" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B292" s="7"/>
       <c r="C292" s="7"/>
+      <c r="D292" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10564,8 +10630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F82A59-57DF-46F6-BCD0-E7A53E611046}">
   <dimension ref="A1:L54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:L54"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
lode runner v5 - up to level 13, 312 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52A285B-B2FA-49A9-B3DD-BAF412DC7B39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805558B0-FBFA-4948-8E9C-5F75C911911E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48105" yWindow="690" windowWidth="9060" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48960" yWindow="750" windowWidth="9060" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V5" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="232">
   <si>
     <t>Place</t>
   </si>
@@ -543,7 +543,193 @@
     <t>Tk diff</t>
   </si>
   <si>
-    <t>1697 best</t>
+    <t>Tk Gained</t>
+  </si>
+  <si>
+    <t>01 Start</t>
+  </si>
+  <si>
+    <t>01 End</t>
+  </si>
+  <si>
+    <t>02 Start</t>
+  </si>
+  <si>
+    <t>02 End</t>
+  </si>
+  <si>
+    <t>03 Start</t>
+  </si>
+  <si>
+    <t>03 End</t>
+  </si>
+  <si>
+    <t>04 Start</t>
+  </si>
+  <si>
+    <t>04 End</t>
+  </si>
+  <si>
+    <t>05 Start</t>
+  </si>
+  <si>
+    <t>05 End</t>
+  </si>
+  <si>
+    <t>06 Start</t>
+  </si>
+  <si>
+    <t>06 End</t>
+  </si>
+  <si>
+    <t>07 Start</t>
+  </si>
+  <si>
+    <t>07 End</t>
+  </si>
+  <si>
+    <t>08 Start</t>
+  </si>
+  <si>
+    <t>08 End</t>
+  </si>
+  <si>
+    <t>09 Start</t>
+  </si>
+  <si>
+    <t>09 End</t>
+  </si>
+  <si>
+    <t>10 Start</t>
+  </si>
+  <si>
+    <t>10 End</t>
+  </si>
+  <si>
+    <t>11 Start</t>
+  </si>
+  <si>
+    <t>11 End</t>
+  </si>
+  <si>
+    <t>12 Start</t>
+  </si>
+  <si>
+    <t>12 End</t>
+  </si>
+  <si>
+    <t>13 Start</t>
+  </si>
+  <si>
+    <t>14 End</t>
+  </si>
+  <si>
+    <t>14 Start</t>
+  </si>
+  <si>
+    <t>15 Start</t>
+  </si>
+  <si>
+    <t>15 End</t>
+  </si>
+  <si>
+    <t>16 Start</t>
+  </si>
+  <si>
+    <t>16 End</t>
+  </si>
+  <si>
+    <t>17 Start</t>
+  </si>
+  <si>
+    <t>17 End</t>
+  </si>
+  <si>
+    <t>18 Start</t>
+  </si>
+  <si>
+    <t>18 End</t>
+  </si>
+  <si>
+    <t>19 Start</t>
+  </si>
+  <si>
+    <t>19 End</t>
+  </si>
+  <si>
+    <t>20 Start</t>
+  </si>
+  <si>
+    <t>20 End</t>
+  </si>
+  <si>
+    <t>21 Start</t>
+  </si>
+  <si>
+    <t>21 End</t>
+  </si>
+  <si>
+    <t>22 Start</t>
+  </si>
+  <si>
+    <t>22 End</t>
+  </si>
+  <si>
+    <t>23 Start</t>
+  </si>
+  <si>
+    <t>23 End</t>
+  </si>
+  <si>
+    <t>24 Start</t>
+  </si>
+  <si>
+    <t>24 End</t>
+  </si>
+  <si>
+    <t>25 Start</t>
+  </si>
+  <si>
+    <t>25 End</t>
+  </si>
+  <si>
+    <t>26 Start</t>
+  </si>
+  <si>
+    <t>26 End</t>
+  </si>
+  <si>
+    <t>27 Start</t>
+  </si>
+  <si>
+    <t>27 End</t>
+  </si>
+  <si>
+    <t>28 Start</t>
+  </si>
+  <si>
+    <t>28 End</t>
+  </si>
+  <si>
+    <t>29 Start</t>
+  </si>
+  <si>
+    <t>30 Start</t>
+  </si>
+  <si>
+    <t>30 End</t>
+  </si>
+  <si>
+    <t>31 Start</t>
+  </si>
+  <si>
+    <t>31 End</t>
+  </si>
+  <si>
+    <t>32 Start</t>
+  </si>
+  <si>
+    <t>32 End</t>
   </si>
 </sst>
 </file>
@@ -553,12 +739,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -878,119 +1071,120 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -1311,15 +1505,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B3565E-C480-4A10-8524-B7BC06C9B703}">
-  <dimension ref="A1:G292"/>
+  <dimension ref="A1:G278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.25" customWidth="1"/>
+    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.75" customWidth="1"/>
+    <col min="3" max="4" width="8.625" customWidth="1"/>
+    <col min="5" max="7" width="6.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1341,10 +1539,13 @@
       <c r="F1" s="1" t="s">
         <v>168</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>53</v>
+      <c r="A2" s="41" t="s">
+        <v>170</v>
       </c>
       <c r="B2" s="2">
         <v>735</v>
@@ -1365,8 +1566,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>52</v>
+      <c r="A3" s="41" t="s">
+        <v>171</v>
       </c>
       <c r="B3" s="7">
         <v>1052</v>
@@ -1385,13 +1586,17 @@
         <f>IF(D3&lt;&gt;"",IF(B3&lt;&gt;"",D3-B3,"-"), "-")</f>
         <v>52</v>
       </c>
+      <c r="G3">
+        <f>(C3-C2) - (D3-D2)</f>
+        <v>-51</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>54</v>
+      <c r="A4" s="41" t="s">
+        <v>172</v>
       </c>
       <c r="B4" s="7">
-        <v>1697</v>
+        <v>1734</v>
       </c>
       <c r="C4" s="7">
         <v>1697</v>
@@ -1400,20 +1605,21 @@
         <v>1764</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E79" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
-        <v>0</v>
+        <f t="shared" ref="E4:E68" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
+        <v>-37</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:F67" si="1">IF(D4&lt;&gt;"",IF(B4&lt;&gt;"",D4-B4,"-"), "-")</f>
-        <v>67</v>
-      </c>
-      <c r="G4" t="s">
-        <v>169</v>
+        <f t="shared" ref="F4:F56" si="1">IF(D4&lt;&gt;"",IF(B4&lt;&gt;"",D4-B4,"-"), "-")</f>
+        <v>30</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G67" si="2">(C4-C3) - (D4-D3)</f>
+        <v>-15</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>63</v>
+      <c r="A5" s="41" t="s">
+        <v>173</v>
       </c>
       <c r="B5" s="7">
         <v>2189</v>
@@ -1432,390 +1638,568 @@
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>141</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B6" s="7"/>
+      <c r="A6" s="41" t="s">
+        <v>174</v>
+      </c>
+      <c r="B6" s="7">
+        <v>2835</v>
+      </c>
       <c r="C6" s="7">
-        <v>2634</v>
-      </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F6" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>2957</v>
+      </c>
+      <c r="D6" s="7">
+        <v>2882</v>
+      </c>
+      <c r="E6" s="3">
+        <f t="shared" si="0"/>
+        <v>122</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B7" s="7"/>
+      <c r="A7" s="41" t="s">
+        <v>175</v>
+      </c>
+      <c r="B7" s="7">
+        <v>3256</v>
+      </c>
       <c r="C7" s="7">
-        <v>2957</v>
-      </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F7" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>3380</v>
+      </c>
+      <c r="D7" s="7">
+        <v>3351</v>
+      </c>
+      <c r="E7" s="3">
+        <f t="shared" si="0"/>
+        <v>124</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>-46</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F8" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="A8" s="41" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" s="7">
+        <v>3901</v>
+      </c>
+      <c r="C8" s="7">
+        <v>4031</v>
+      </c>
+      <c r="D8" s="7">
+        <v>4010</v>
+      </c>
+      <c r="E8" s="3">
+        <f t="shared" si="0"/>
+        <v>130</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>-8</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F9" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="A9" s="41" t="s">
+        <v>177</v>
+      </c>
+      <c r="B9" s="7">
+        <v>4382</v>
+      </c>
+      <c r="C9" s="7">
+        <v>4553</v>
+      </c>
+      <c r="D9" s="7">
+        <v>4491</v>
+      </c>
+      <c r="E9" s="3">
+        <f t="shared" si="0"/>
+        <v>171</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="7"/>
+      <c r="A10" s="41" t="s">
+        <v>178</v>
+      </c>
+      <c r="B10" s="7">
+        <v>5042</v>
+      </c>
       <c r="C10" s="7">
-        <v>3380</v>
-      </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F10" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>5209</v>
+      </c>
+      <c r="D10" s="7">
+        <v>5150</v>
+      </c>
+      <c r="E10" s="3">
+        <f t="shared" si="0"/>
+        <v>167</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>-3</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11" s="7"/>
+      <c r="A11" s="41" t="s">
+        <v>179</v>
+      </c>
+      <c r="B11" s="7">
+        <v>5332</v>
+      </c>
       <c r="C11" s="7">
-        <v>3717</v>
-      </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F11" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>5536</v>
+      </c>
+      <c r="D11" s="7">
+        <v>5463</v>
+      </c>
+      <c r="E11" s="3">
+        <f t="shared" si="0"/>
+        <v>204</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" s="7"/>
+      <c r="A12" s="41" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="7">
+        <v>5978</v>
+      </c>
       <c r="C12" s="7">
-        <v>4031</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F12" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>6216</v>
+      </c>
+      <c r="D12" s="7">
+        <v>6108</v>
+      </c>
+      <c r="E12" s="3">
+        <f t="shared" si="0"/>
+        <v>238</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="B13" s="7"/>
+      <c r="A13" s="41" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="7">
+        <v>6999</v>
+      </c>
       <c r="C13" s="7">
-        <v>4215</v>
-      </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F13" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>7274</v>
+      </c>
+      <c r="D13" s="7">
+        <v>7132</v>
+      </c>
+      <c r="E13" s="3">
+        <f t="shared" si="0"/>
+        <v>275</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="1"/>
+        <v>133</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B14" s="7"/>
+      <c r="A14" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="B14" s="7">
+        <v>7646</v>
+      </c>
       <c r="C14" s="7">
-        <v>4375</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F14" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>7919</v>
+      </c>
+      <c r="D14" s="7">
+        <v>7777</v>
+      </c>
+      <c r="E14" s="3">
+        <f t="shared" si="0"/>
+        <v>273</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="1"/>
+        <v>131</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="7"/>
+      <c r="A15" s="41" t="s">
+        <v>183</v>
+      </c>
+      <c r="B15" s="7">
+        <v>8112</v>
+      </c>
       <c r="C15" s="7">
-        <v>4553</v>
-      </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F15" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>8407</v>
+      </c>
+      <c r="D15" s="7">
+        <v>8259</v>
+      </c>
+      <c r="E15" s="3">
+        <f t="shared" si="0"/>
+        <v>295</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="1"/>
+        <v>147</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="B16" s="7"/>
+      <c r="A16" s="41" t="s">
+        <v>184</v>
+      </c>
+      <c r="B16" s="7">
+        <v>8758</v>
+      </c>
       <c r="C16" s="7">
-        <v>5209</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F16" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B17" s="7"/>
+        <v>9053</v>
+      </c>
+      <c r="D16" s="7">
+        <v>8904</v>
+      </c>
+      <c r="E16" s="3">
+        <f t="shared" si="0"/>
+        <v>295</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="1"/>
+        <v>146</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="B17" s="7">
+        <v>9166</v>
+      </c>
       <c r="C17" s="7">
-        <v>5536</v>
-      </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F17" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="B18" s="7"/>
+        <v>9481</v>
+      </c>
+      <c r="D17" s="7">
+        <v>9313</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" si="0"/>
+        <v>315</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="1"/>
+        <v>147</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="41" t="s">
+        <v>186</v>
+      </c>
+      <c r="B18" s="7">
+        <v>9811</v>
+      </c>
       <c r="C18" s="7">
-        <v>6216</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F18" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="7"/>
+        <v>10126</v>
+      </c>
+      <c r="D18" s="7">
+        <v>9958</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" si="0"/>
+        <v>315</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="1"/>
+        <v>147</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="B19" s="7">
+        <v>10903</v>
+      </c>
       <c r="C19" s="7">
-        <v>7274</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F19" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B20" s="7"/>
+        <v>11221</v>
+      </c>
+      <c r="D19" s="7">
+        <v>11049</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" si="0"/>
+        <v>318</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="1"/>
+        <v>146</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="B20" s="7">
+        <v>11541</v>
+      </c>
       <c r="C20" s="7">
-        <v>7919</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F20" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="7"/>
+        <v>11859</v>
+      </c>
+      <c r="D20" s="41">
+        <v>11687</v>
+      </c>
+      <c r="E20" s="3">
+        <f t="shared" si="0"/>
+        <v>318</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="1"/>
+        <v>146</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="41" t="s">
+        <v>189</v>
+      </c>
+      <c r="B21" s="7">
+        <v>12111</v>
+      </c>
       <c r="C21" s="7">
-        <v>8407</v>
-      </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F21" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="B22" s="7"/>
+        <v>12432</v>
+      </c>
+      <c r="D21" s="7">
+        <v>12339</v>
+      </c>
+      <c r="E21" s="3">
+        <f t="shared" si="0"/>
+        <v>321</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="1"/>
+        <v>228</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="2"/>
+        <v>-79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="B22" s="7">
+        <v>12770</v>
+      </c>
       <c r="C22" s="7">
-        <v>9053</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F22" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="7"/>
+        <v>13091</v>
+      </c>
+      <c r="D22" s="7">
+        <v>12998</v>
+      </c>
+      <c r="E22" s="3">
+        <f t="shared" si="0"/>
+        <v>321</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="1"/>
+        <v>228</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="B23" s="7">
+        <v>13076</v>
+      </c>
       <c r="C23" s="7">
-        <v>9481</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F23" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="B24" s="7"/>
+        <v>13412</v>
+      </c>
+      <c r="D23" s="7">
+        <v>13389</v>
+      </c>
+      <c r="E23" s="3">
+        <f t="shared" si="0"/>
+        <v>336</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="1"/>
+        <v>313</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="2"/>
+        <v>-70</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="41" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="41">
+        <v>13735</v>
+      </c>
       <c r="C24" s="7">
-        <v>10126</v>
-      </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F24" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B25" s="7"/>
+        <v>14071</v>
+      </c>
+      <c r="D24" s="7">
+        <v>14048</v>
+      </c>
+      <c r="E24" s="3">
+        <f t="shared" si="0"/>
+        <v>336</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="1"/>
+        <v>313</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="41" t="s">
+        <v>193</v>
+      </c>
+      <c r="B25" s="7">
+        <v>14417</v>
+      </c>
       <c r="C25" s="7">
-        <v>11221</v>
-      </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F25" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B26" s="7"/>
+        <v>14755</v>
+      </c>
+      <c r="D25" s="7">
+        <v>14730</v>
+      </c>
+      <c r="E25" s="3">
+        <f t="shared" si="0"/>
+        <v>338</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="1"/>
+        <v>313</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="B26" s="7">
+        <v>15063</v>
+      </c>
       <c r="C26" s="7">
-        <v>11859</v>
-      </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F26" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <v>15409</v>
+      </c>
+      <c r="D26" s="7">
+        <v>15375</v>
+      </c>
+      <c r="E26" s="3">
+        <f t="shared" si="0"/>
+        <v>346</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="1"/>
+        <v>312</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>130</v>
+        <v>195</v>
       </c>
       <c r="B27" s="7"/>
       <c r="C27" s="7">
-        <v>12287</v>
-      </c>
-      <c r="D27" s="7"/>
+        <v>15994</v>
+      </c>
+      <c r="D27" s="7">
+        <v>15987</v>
+      </c>
       <c r="E27" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1824,16 +2208,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <f t="shared" si="2"/>
+        <v>-27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>79</v>
+        <v>196</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="7">
-        <v>12430</v>
-      </c>
-      <c r="D28" s="7"/>
+        <v>16640</v>
+      </c>
+      <c r="D28" s="7">
+        <v>16632</v>
+      </c>
       <c r="E28" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1842,16 +2232,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="8" t="s">
-        <v>141</v>
+      <c r="G28">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>195</v>
       </c>
       <c r="B29" s="7"/>
       <c r="C29" s="7">
-        <v>13089</v>
-      </c>
-      <c r="D29" s="7"/>
+        <v>17228</v>
+      </c>
+      <c r="D29" s="7">
+        <v>17152</v>
+      </c>
       <c r="E29" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1860,16 +2256,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A30" s="8" t="s">
-        <v>126</v>
+      <c r="G29">
+        <f t="shared" si="2"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>197</v>
       </c>
       <c r="B30" s="7"/>
       <c r="C30" s="7">
-        <v>13412</v>
-      </c>
-      <c r="D30" s="7"/>
+        <v>17866</v>
+      </c>
+      <c r="D30" s="7">
+        <v>17797</v>
+      </c>
       <c r="E30" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1878,16 +2280,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G30">
+        <f t="shared" si="2"/>
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>81</v>
+        <v>198</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7">
-        <v>14071</v>
-      </c>
-      <c r="D31" s="7"/>
+        <v>18604</v>
+      </c>
+      <c r="D31" s="7">
+        <v>18546</v>
+      </c>
       <c r="E31" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1896,16 +2304,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G31">
+        <f t="shared" si="2"/>
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>82</v>
+        <v>199</v>
       </c>
       <c r="B32" s="7"/>
       <c r="C32" s="7">
-        <v>14755</v>
-      </c>
-      <c r="D32" s="7"/>
+        <v>19242</v>
+      </c>
+      <c r="D32" s="7">
+        <v>19184</v>
+      </c>
       <c r="E32" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1914,16 +2328,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>142</v>
+      <c r="G32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A33" s="7" t="s">
+        <v>200</v>
       </c>
       <c r="B33" s="7"/>
       <c r="C33" s="7">
-        <v>15409</v>
-      </c>
-      <c r="D33" s="7"/>
+        <v>19683</v>
+      </c>
+      <c r="D33" s="7">
+        <v>19572</v>
+      </c>
       <c r="E33" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1932,16 +2352,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>86</v>
+      <c r="G33">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A34" s="7" t="s">
+        <v>201</v>
       </c>
       <c r="B34" s="7"/>
       <c r="C34" s="7">
-        <v>15994</v>
-      </c>
-      <c r="D34" s="7"/>
+        <v>20330</v>
+      </c>
+      <c r="D34" s="7">
+        <v>20217</v>
+      </c>
       <c r="E34" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1950,16 +2376,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>85</v>
+        <v>202</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="7">
-        <v>16640</v>
-      </c>
-      <c r="D35" s="7"/>
+        <v>21340</v>
+      </c>
+      <c r="D35" s="7">
+        <v>21086</v>
+      </c>
       <c r="E35" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1968,16 +2400,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G35">
+        <f t="shared" si="2"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
-        <v>86</v>
+        <v>203</v>
       </c>
       <c r="B36" s="7"/>
       <c r="C36" s="7">
-        <v>17228</v>
-      </c>
-      <c r="D36" s="7"/>
+        <v>21985</v>
+      </c>
+      <c r="D36" s="7">
+        <v>21731</v>
+      </c>
       <c r="E36" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -1986,16 +2424,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7">
-        <v>17866</v>
-      </c>
-      <c r="D37" s="7"/>
+        <v>204</v>
+      </c>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8">
+        <v>22936</v>
+      </c>
+      <c r="D37" s="8">
+        <v>22797</v>
+      </c>
       <c r="E37" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2004,16 +2448,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <f t="shared" si="2"/>
+        <v>-115</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>88</v>
+        <v>205</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="7">
-        <v>18604</v>
-      </c>
-      <c r="D38" s="7"/>
+        <v>23582</v>
+      </c>
+      <c r="D38" s="7">
+        <v>23442</v>
+      </c>
       <c r="E38" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2022,16 +2472,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G38">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>89</v>
+        <v>206</v>
       </c>
       <c r="B39" s="7"/>
       <c r="C39" s="7">
-        <v>19242</v>
-      </c>
-      <c r="D39" s="7"/>
+        <v>23922</v>
+      </c>
+      <c r="D39" s="7">
+        <v>23797</v>
+      </c>
       <c r="E39" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2040,16 +2496,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <f t="shared" si="2"/>
+        <v>-15</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>90</v>
+        <v>207</v>
       </c>
       <c r="B40" s="7"/>
       <c r="C40" s="7">
-        <v>19683</v>
-      </c>
-      <c r="D40" s="7"/>
+        <v>24583</v>
+      </c>
+      <c r="D40" s="7">
+        <v>24442</v>
+      </c>
       <c r="E40" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2058,16 +2520,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G40">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
-        <v>91</v>
+        <v>208</v>
       </c>
       <c r="B41" s="7"/>
       <c r="C41" s="7">
-        <v>20330</v>
-      </c>
-      <c r="D41" s="7"/>
+        <v>25181</v>
+      </c>
+      <c r="D41" s="7">
+        <v>25025</v>
+      </c>
       <c r="E41" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2076,16 +2544,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G41">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>92</v>
+        <v>209</v>
       </c>
       <c r="B42" s="7"/>
       <c r="C42" s="7">
-        <v>21340</v>
-      </c>
-      <c r="D42" s="7"/>
+        <v>25839</v>
+      </c>
+      <c r="D42" s="7">
+        <v>25684</v>
+      </c>
       <c r="E42" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2094,16 +2568,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G42">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>93</v>
+        <v>210</v>
       </c>
       <c r="B43" s="7"/>
       <c r="C43" s="7">
-        <v>21985</v>
-      </c>
-      <c r="D43" s="7"/>
+        <v>26718</v>
+      </c>
+      <c r="D43" s="7">
+        <v>26528</v>
+      </c>
       <c r="E43" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2112,16 +2592,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G43">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8">
-        <v>22936</v>
-      </c>
-      <c r="D44" s="8"/>
+        <v>211</v>
+      </c>
+      <c r="B44" s="7"/>
+      <c r="C44" s="7">
+        <v>27377</v>
+      </c>
+      <c r="D44" s="7">
+        <v>27187</v>
+      </c>
       <c r="E44" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2130,16 +2616,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G44">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>95</v>
+        <v>212</v>
       </c>
       <c r="B45" s="7"/>
       <c r="C45" s="7">
-        <v>23582</v>
-      </c>
-      <c r="D45" s="7"/>
+        <v>28030</v>
+      </c>
+      <c r="D45" s="7">
+        <v>27750</v>
+      </c>
       <c r="E45" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2148,16 +2640,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G45">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>96</v>
+        <v>213</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="7">
-        <v>23922</v>
-      </c>
-      <c r="D46" s="7"/>
+        <v>28675</v>
+      </c>
+      <c r="D46" s="7">
+        <v>28395</v>
+      </c>
       <c r="E46" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2166,16 +2664,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G46">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
-        <v>97</v>
+        <v>214</v>
       </c>
       <c r="B47" s="7"/>
       <c r="C47" s="7">
-        <v>24583</v>
-      </c>
-      <c r="D47" s="7"/>
+        <v>29883</v>
+      </c>
+      <c r="D47" s="7">
+        <v>29432</v>
+      </c>
       <c r="E47" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2184,16 +2688,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G47">
+        <f t="shared" si="2"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>98</v>
+        <v>215</v>
       </c>
       <c r="B48" s="7"/>
       <c r="C48" s="7">
-        <v>25181</v>
-      </c>
-      <c r="D48" s="7"/>
+        <v>30378</v>
+      </c>
+      <c r="D48" s="7">
+        <v>29930</v>
+      </c>
       <c r="E48" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2202,16 +2712,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>99</v>
+        <v>216</v>
       </c>
       <c r="B49" s="7"/>
       <c r="C49" s="7">
-        <v>25839</v>
-      </c>
-      <c r="D49" s="7"/>
+        <v>30809</v>
+      </c>
+      <c r="D49" s="7">
+        <v>30422</v>
+      </c>
       <c r="E49" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2220,16 +2736,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G49">
+        <f t="shared" si="2"/>
+        <v>-61</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>100</v>
+        <v>217</v>
       </c>
       <c r="B50" s="7"/>
       <c r="C50" s="7">
-        <v>26718</v>
-      </c>
-      <c r="D50" s="7"/>
+        <v>31448</v>
+      </c>
+      <c r="D50" s="7">
+        <v>31060</v>
+      </c>
       <c r="E50" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2238,16 +2760,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G50">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>101</v>
+        <v>218</v>
       </c>
       <c r="B51" s="7"/>
       <c r="C51" s="7">
-        <v>27377</v>
-      </c>
-      <c r="D51" s="7"/>
+        <v>32009</v>
+      </c>
+      <c r="D51" s="7">
+        <v>31627</v>
+      </c>
       <c r="E51" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2256,16 +2784,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G51">
+        <f t="shared" si="2"/>
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
-        <v>102</v>
+        <v>219</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="7">
-        <v>28030</v>
-      </c>
-      <c r="D52" s="7"/>
+        <v>32654</v>
+      </c>
+      <c r="D52" s="7">
+        <v>32272</v>
+      </c>
       <c r="E52" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2274,16 +2808,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G52">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>103</v>
+        <v>220</v>
       </c>
       <c r="B53" s="7"/>
       <c r="C53" s="7">
-        <v>28675</v>
-      </c>
-      <c r="D53" s="7"/>
+        <v>33576</v>
+      </c>
+      <c r="D53" s="7">
+        <v>33186</v>
+      </c>
       <c r="E53" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2292,16 +2832,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>148</v>
+      <c r="G53">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
+        <v>221</v>
       </c>
       <c r="B54" s="7"/>
       <c r="C54" s="7">
-        <v>29030</v>
-      </c>
-      <c r="D54" s="7"/>
+        <v>34235</v>
+      </c>
+      <c r="D54" s="7">
+        <v>33845</v>
+      </c>
       <c r="E54" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2310,16 +2856,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="9" t="s">
-        <v>149</v>
+      <c r="G54">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
+        <v>222</v>
       </c>
       <c r="B55" s="7"/>
       <c r="C55" s="7">
-        <v>29392</v>
-      </c>
-      <c r="D55" s="7"/>
+        <v>35341</v>
+      </c>
+      <c r="D55" s="7">
+        <v>34891</v>
+      </c>
       <c r="E55" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2328,16 +2880,22 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="9" t="s">
-        <v>150</v>
+      <c r="G55">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
+        <v>223</v>
       </c>
       <c r="B56" s="7"/>
       <c r="C56" s="7">
-        <v>29423</v>
-      </c>
-      <c r="D56" s="7"/>
+        <v>35986</v>
+      </c>
+      <c r="D56" s="7">
+        <v>35550</v>
+      </c>
       <c r="E56" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
@@ -2346,1066 +2904,1284 @@
         <f t="shared" si="1"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
-        <v>148</v>
+      <c r="G56">
+        <f t="shared" si="2"/>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
+        <v>224</v>
       </c>
       <c r="B57" s="7"/>
       <c r="C57" s="7">
-        <v>29537</v>
-      </c>
-      <c r="D57" s="7"/>
+        <v>36861</v>
+      </c>
+      <c r="D57" s="7">
+        <v>36365</v>
+      </c>
       <c r="E57" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="F57" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F57:F117" si="3">IF(D57&lt;&gt;"",IF(B57&lt;&gt;"",D57-B57,"-"), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="G57">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>104</v>
+        <v>225</v>
       </c>
       <c r="B58" s="7"/>
       <c r="C58" s="7">
-        <v>29883</v>
-      </c>
-      <c r="D58" s="7"/>
+        <v>37461</v>
+      </c>
+      <c r="D58" s="7">
+        <v>36977</v>
+      </c>
       <c r="E58" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="F58" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G58">
+        <f t="shared" si="2"/>
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
-        <v>105</v>
+        <v>27</v>
       </c>
       <c r="B59" s="7"/>
       <c r="C59" s="7">
-        <v>30378</v>
-      </c>
-      <c r="D59" s="7"/>
+        <v>38564</v>
+      </c>
+      <c r="D59" s="7">
+        <v>38073</v>
+      </c>
       <c r="E59" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="F59" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G59">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
-        <v>106</v>
+        <v>226</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="7">
-        <v>30809</v>
-      </c>
-      <c r="D60" s="7"/>
+        <v>39057</v>
+      </c>
+      <c r="D60" s="7">
+        <v>38571</v>
+      </c>
       <c r="E60" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="F60" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
-        <v>107</v>
+        <v>227</v>
       </c>
       <c r="B61" s="7"/>
       <c r="C61" s="7">
-        <v>31448</v>
-      </c>
-      <c r="D61" s="7"/>
+        <v>39781</v>
+      </c>
+      <c r="D61" s="7">
+        <v>39448</v>
+      </c>
       <c r="E61" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="F61" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="2"/>
+        <v>-153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
-        <v>108</v>
+        <v>228</v>
       </c>
       <c r="B62" s="7"/>
       <c r="C62" s="7">
-        <v>32009</v>
-      </c>
-      <c r="D62" s="7"/>
+        <v>40405</v>
+      </c>
+      <c r="D62" s="7">
+        <v>40072</v>
+      </c>
       <c r="E62" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="F62" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G62">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7">
-        <v>32654</v>
-      </c>
-      <c r="D63" s="7"/>
+        <v>229</v>
+      </c>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9">
+        <v>40588</v>
+      </c>
+      <c r="D63" s="9">
+        <v>40256</v>
+      </c>
       <c r="E63" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="F63" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>110</v>
+        <v>230</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7">
-        <v>33576</v>
-      </c>
-      <c r="D64" s="7"/>
+        <v>41228</v>
+      </c>
+      <c r="D64" s="7">
+        <v>40894</v>
+      </c>
       <c r="E64" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="F64" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G64">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7">
-        <v>34235</v>
-      </c>
-      <c r="D65" s="7"/>
+        <v>231</v>
+      </c>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9">
+        <v>41865</v>
+      </c>
+      <c r="D65" s="9">
+        <v>41440</v>
+      </c>
       <c r="E65" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="F65" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G65">
+        <f t="shared" si="2"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="B66" s="7"/>
       <c r="C66" s="7">
-        <v>35341</v>
-      </c>
-      <c r="D66" s="7"/>
+        <v>42511</v>
+      </c>
+      <c r="D66" s="7">
+        <v>42085</v>
+      </c>
       <c r="E66" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="F66" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G66">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B67" s="7"/>
       <c r="C67" s="7">
-        <v>35986</v>
-      </c>
-      <c r="D67" s="7"/>
+        <v>43110</v>
+      </c>
+      <c r="D67" s="7">
+        <v>42757</v>
+      </c>
       <c r="E67" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="F67" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
-        <v>115</v>
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="2"/>
+        <v>-73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="B68" s="7"/>
       <c r="C68" s="7">
-        <v>36861</v>
-      </c>
-      <c r="D68" s="7"/>
+        <v>43756</v>
+      </c>
+      <c r="D68" s="7">
+        <v>43402</v>
+      </c>
       <c r="E68" s="3" t="str">
         <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="F68" s="3" t="str">
-        <f t="shared" ref="F68:F131" si="2">IF(D68&lt;&gt;"",IF(B68&lt;&gt;"",D68-B68,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="7" t="s">
-        <v>116</v>
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G68">
+        <f t="shared" ref="G68:G101" si="4">(C68-C67) - (D68-D67)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="7">
-        <v>37461</v>
-      </c>
-      <c r="D69" s="7"/>
+        <v>44418</v>
+      </c>
+      <c r="D69" s="7">
+        <v>44061</v>
+      </c>
       <c r="E69" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E69:E132" si="5">IF(C69&lt;&gt;"",IF(B69&lt;&gt;"",C69-B69,"-"), "-")</f>
         <v>-</v>
       </c>
       <c r="F69" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="7" t="s">
-        <v>114</v>
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>11</v>
       </c>
       <c r="B70" s="7"/>
       <c r="C70" s="7">
-        <v>38564</v>
-      </c>
-      <c r="D70" s="7"/>
+        <v>45077</v>
+      </c>
+      <c r="D70" s="7">
+        <v>44720</v>
+      </c>
       <c r="E70" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F70" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="7" t="s">
-        <v>117</v>
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="B71" s="7"/>
       <c r="C71" s="7">
-        <v>39057</v>
-      </c>
-      <c r="D71" s="7"/>
+        <v>45719</v>
+      </c>
+      <c r="D71" s="7">
+        <v>45363</v>
+      </c>
       <c r="E71" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F71" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="7" t="s">
-        <v>118</v>
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G71">
+        <f t="shared" si="4"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B72" s="7"/>
       <c r="C72" s="7">
-        <v>39781</v>
-      </c>
-      <c r="D72" s="7"/>
+        <v>46378</v>
+      </c>
+      <c r="D72" s="7">
+        <v>46022</v>
+      </c>
       <c r="E72" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F72" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="7" t="s">
-        <v>119</v>
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G72">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="B73" s="7"/>
       <c r="C73" s="7">
-        <v>40405</v>
-      </c>
-      <c r="D73" s="7"/>
+        <v>46984</v>
+      </c>
+      <c r="D73" s="41">
+        <v>46679</v>
+      </c>
       <c r="E73" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F73" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9">
-        <v>40588</v>
-      </c>
-      <c r="D74" s="9"/>
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G73">
+        <f t="shared" si="4"/>
+        <v>-51</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7">
+        <v>47629</v>
+      </c>
+      <c r="D74" s="7">
+        <v>47338</v>
+      </c>
       <c r="E74" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F74" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G74">
+        <f t="shared" si="4"/>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>121</v>
+        <v>47</v>
       </c>
       <c r="B75" s="7"/>
       <c r="C75" s="7">
-        <v>41228</v>
-      </c>
-      <c r="D75" s="7"/>
+        <v>48410</v>
+      </c>
+      <c r="D75" s="7">
+        <v>48121</v>
+      </c>
       <c r="E75" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F75" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G75">
+        <f t="shared" si="4"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B76" s="9"/>
-      <c r="C76" s="9">
-        <v>41865</v>
-      </c>
-      <c r="D76" s="9"/>
+        <v>48</v>
+      </c>
+      <c r="B76" s="7"/>
+      <c r="C76" s="7">
+        <v>48908</v>
+      </c>
+      <c r="D76" s="7">
+        <v>48619</v>
+      </c>
       <c r="E76" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F76" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>123</v>
+        <v>33</v>
       </c>
       <c r="B77" s="7"/>
       <c r="C77" s="7">
-        <v>42511</v>
-      </c>
-      <c r="D77" s="7"/>
+        <v>49856</v>
+      </c>
+      <c r="D77" s="7">
+        <v>49502</v>
+      </c>
       <c r="E77" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F77" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
-        <v>124</v>
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
+        <v>14</v>
       </c>
       <c r="B78" s="7"/>
       <c r="C78" s="7">
-        <v>43110</v>
-      </c>
-      <c r="D78" s="7"/>
+        <v>50516</v>
+      </c>
+      <c r="D78" s="7">
+        <v>50148</v>
+      </c>
       <c r="E78" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F78" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B79" s="7"/>
       <c r="C79" s="7">
-        <v>43756</v>
-      </c>
-      <c r="D79" s="7"/>
+        <v>50874</v>
+      </c>
+      <c r="D79" s="7">
+        <v>50417</v>
+      </c>
       <c r="E79" s="3" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F79" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="4"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B80" s="7"/>
       <c r="C80" s="7">
-        <v>44418</v>
-      </c>
-      <c r="D80" s="7"/>
+        <v>51486</v>
+      </c>
+      <c r="D80" s="7">
+        <v>51016</v>
+      </c>
       <c r="E80" s="3" t="str">
-        <f t="shared" ref="E80:E146" si="3">IF(C80&lt;&gt;"",IF(B80&lt;&gt;"",C80-B80,"-"), "-")</f>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F80" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G80">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="B81" s="7"/>
       <c r="C81" s="7">
-        <v>45077</v>
-      </c>
-      <c r="D81" s="7"/>
+        <v>52507</v>
+      </c>
+      <c r="D81" s="7">
+        <v>52007</v>
+      </c>
       <c r="E81" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F81" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F81" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G81">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B82" s="7"/>
       <c r="C82" s="7">
-        <v>45719</v>
-      </c>
-      <c r="D82" s="7"/>
+        <v>53153</v>
+      </c>
+      <c r="D82" s="7">
+        <v>52667</v>
+      </c>
       <c r="E82" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F82" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F82" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G82">
+        <f t="shared" si="4"/>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B83" s="7"/>
       <c r="C83" s="7">
-        <v>46378</v>
-      </c>
-      <c r="D83" s="7"/>
+        <v>53942</v>
+      </c>
+      <c r="D83" s="7">
+        <v>53473</v>
+      </c>
       <c r="E83" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F83" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F83" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G83">
+        <f t="shared" si="4"/>
+        <v>-17</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A84" s="5" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B84" s="7"/>
       <c r="C84" s="7">
-        <v>46984</v>
-      </c>
-      <c r="D84" s="7"/>
+        <v>54564</v>
+      </c>
+      <c r="D84" s="7">
+        <v>54095</v>
+      </c>
       <c r="E84" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F84" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F84" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G84">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
       <c r="B85" s="7"/>
       <c r="C85" s="7">
-        <v>47629</v>
-      </c>
-      <c r="D85" s="7"/>
+        <v>55596</v>
+      </c>
+      <c r="D85" s="7">
+        <v>55108</v>
+      </c>
       <c r="E85" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F85" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F85" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="7" t="s">
-        <v>47</v>
+      <c r="G85">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>18</v>
       </c>
       <c r="B86" s="7"/>
       <c r="C86" s="7">
-        <v>48410</v>
-      </c>
-      <c r="D86" s="7"/>
+        <v>56185</v>
+      </c>
+      <c r="D86" s="7">
+        <v>55708</v>
+      </c>
       <c r="E86" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F86" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F86" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="7" t="s">
-        <v>48</v>
+      <c r="G86">
+        <f t="shared" si="4"/>
+        <v>-11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="B87" s="7"/>
       <c r="C87" s="7">
-        <v>48908</v>
-      </c>
-      <c r="D87" s="7"/>
+        <v>56572</v>
+      </c>
+      <c r="D87" s="7">
+        <v>56104</v>
+      </c>
       <c r="E87" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F87" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F87" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="7" t="s">
-        <v>33</v>
+      <c r="G87">
+        <f t="shared" si="4"/>
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="B88" s="7"/>
       <c r="C88" s="7">
-        <v>49856</v>
-      </c>
-      <c r="D88" s="7"/>
+        <v>57217</v>
+      </c>
+      <c r="D88" s="7">
+        <v>56749</v>
+      </c>
       <c r="E88" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F88" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F88" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G88">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B89" s="7"/>
       <c r="C89" s="7">
-        <v>50516</v>
-      </c>
-      <c r="D89" s="7"/>
+        <v>58008</v>
+      </c>
+      <c r="D89" s="7">
+        <v>57450</v>
+      </c>
       <c r="E89" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F89" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F89" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G89">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B90" s="7"/>
       <c r="C90" s="7">
-        <v>50874</v>
-      </c>
-      <c r="D90" s="7"/>
+        <v>58608</v>
+      </c>
+      <c r="D90" s="7">
+        <v>58050</v>
+      </c>
       <c r="E90" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F90" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F90" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G90">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A91" s="5" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="B91" s="7"/>
       <c r="C91" s="7">
-        <v>51486</v>
-      </c>
-      <c r="D91" s="7"/>
+        <v>59190</v>
+      </c>
+      <c r="D91" s="7">
+        <v>58612</v>
+      </c>
       <c r="E91" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F91" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F91" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G91">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B92" s="7"/>
       <c r="C92" s="7">
-        <v>52507</v>
-      </c>
-      <c r="D92" s="7"/>
+        <v>59825</v>
+      </c>
+      <c r="D92" s="7">
+        <v>59247</v>
+      </c>
       <c r="E92" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F92" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F92" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G92">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A93" s="5" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="B93" s="7"/>
       <c r="C93" s="7">
-        <v>53153</v>
-      </c>
-      <c r="D93" s="7"/>
+        <v>60441</v>
+      </c>
+      <c r="D93" s="7">
+        <v>59838</v>
+      </c>
       <c r="E93" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F93" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F93" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G93">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B94" s="7"/>
       <c r="C94" s="7">
-        <v>53942</v>
-      </c>
-      <c r="D94" s="7"/>
+        <v>61093</v>
+      </c>
+      <c r="D94" s="7">
+        <v>60490</v>
+      </c>
       <c r="E94" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F94" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F94" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G94">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A95" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B95" s="7"/>
-      <c r="C95" s="7">
-        <v>54564</v>
-      </c>
-      <c r="D95" s="7"/>
+        <v>42</v>
+      </c>
+      <c r="B95" s="10"/>
+      <c r="C95" s="10">
+        <v>61914</v>
+      </c>
+      <c r="D95" s="10">
+        <v>61295</v>
+      </c>
       <c r="E95" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F95" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F95" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G95">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B96" s="7"/>
       <c r="C96" s="7">
-        <v>55596</v>
-      </c>
-      <c r="D96" s="7"/>
+        <v>62575</v>
+      </c>
+      <c r="D96" s="7">
+        <v>61940</v>
+      </c>
       <c r="E96" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F96" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F96" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G96">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="7">
-        <v>56185</v>
-      </c>
-      <c r="D97" s="7"/>
+        <v>63180</v>
+      </c>
+      <c r="D97" s="7">
+        <v>62513</v>
+      </c>
       <c r="E97" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F97" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F97" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="5"/>
+      <c r="G97">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="B98" s="7"/>
       <c r="C98" s="7">
-        <v>56464</v>
-      </c>
-      <c r="D98" s="7"/>
+        <v>63825</v>
+      </c>
+      <c r="D98" s="7">
+        <v>63172</v>
+      </c>
       <c r="E98" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F98" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F98" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G98">
+        <f t="shared" si="4"/>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="7">
-        <v>56572</v>
-      </c>
-      <c r="D99" s="7"/>
+        <v>64581</v>
+      </c>
+      <c r="D99" s="7">
+        <v>63896</v>
+      </c>
       <c r="E99" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F99" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F99" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="G99">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B100" s="7"/>
       <c r="C100" s="7">
-        <v>57217</v>
-      </c>
-      <c r="D100" s="7"/>
+        <v>65231</v>
+      </c>
+      <c r="D100" s="7">
+        <v>64541</v>
+      </c>
       <c r="E100" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F100" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F100" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="10" t="s">
-        <v>153</v>
+      <c r="G100">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="B101" s="7"/>
       <c r="C101" s="7">
-        <v>57373</v>
-      </c>
-      <c r="D101" s="7"/>
+        <v>65820</v>
+      </c>
+      <c r="D101" s="7">
+        <v>65084</v>
+      </c>
       <c r="E101" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F101" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F101" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="10" t="s">
-        <v>154</v>
-      </c>
+      <c r="G101">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="7"/>
       <c r="B102" s="7"/>
-      <c r="C102" s="7">
-        <v>57657</v>
-      </c>
+      <c r="C102" s="7"/>
       <c r="D102" s="7"/>
       <c r="E102" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F102" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F102" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
-        <v>39</v>
-      </c>
+    </row>
+    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="7"/>
       <c r="B103" s="7"/>
-      <c r="C103" s="7">
-        <v>58008</v>
-      </c>
+      <c r="C103" s="7"/>
       <c r="D103" s="7"/>
       <c r="E103" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F103" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F103" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
-        <v>20</v>
-      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="7"/>
       <c r="B104" s="7"/>
-      <c r="C104" s="7">
-        <v>58608</v>
-      </c>
+      <c r="C104" s="7"/>
       <c r="D104" s="7"/>
       <c r="E104" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F104" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F104" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
-        <v>40</v>
-      </c>
+    </row>
+    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="7"/>
       <c r="B105" s="7"/>
-      <c r="C105" s="7">
-        <v>59190</v>
-      </c>
+      <c r="C105" s="7"/>
       <c r="D105" s="7"/>
       <c r="E105" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F105" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F105" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
-        <v>21</v>
-      </c>
+    </row>
+    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="7"/>
       <c r="B106" s="7"/>
-      <c r="C106" s="7">
-        <v>59825</v>
-      </c>
+      <c r="C106" s="7"/>
       <c r="D106" s="7"/>
       <c r="E106" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F106" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F106" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
-        <v>41</v>
-      </c>
+    </row>
+    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="7"/>
       <c r="B107" s="7"/>
-      <c r="C107" s="7">
-        <v>60441</v>
-      </c>
+      <c r="C107" s="7"/>
       <c r="D107" s="7"/>
       <c r="E107" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F107" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F107" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>22</v>
-      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="7"/>
       <c r="B108" s="7"/>
-      <c r="C108" s="7">
-        <v>61093</v>
-      </c>
+      <c r="C108" s="7"/>
       <c r="D108" s="7"/>
       <c r="E108" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F108" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F108" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B109" s="10"/>
-      <c r="C109" s="10">
-        <v>61914</v>
-      </c>
-      <c r="D109" s="10"/>
+    </row>
+    <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="7"/>
+      <c r="B109" s="7"/>
+      <c r="C109" s="7"/>
+      <c r="D109" s="7"/>
       <c r="E109" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F109" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F109" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="5" t="s">
-        <v>23</v>
-      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="7"/>
       <c r="B110" s="7"/>
-      <c r="C110" s="7">
-        <v>62575</v>
-      </c>
+      <c r="C110" s="7"/>
       <c r="D110" s="7"/>
       <c r="E110" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F110" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F110" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A111" s="5" t="s">
-        <v>43</v>
-      </c>
+    </row>
+    <row r="111" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A111" s="7"/>
       <c r="B111" s="7"/>
-      <c r="C111" s="7">
-        <v>63180</v>
-      </c>
+      <c r="C111" s="7"/>
       <c r="D111" s="7"/>
       <c r="E111" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F111" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F111" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A112" s="5" t="s">
-        <v>24</v>
-      </c>
+    </row>
+    <row r="112" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A112" s="7"/>
       <c r="B112" s="7"/>
-      <c r="C112" s="7">
-        <v>63825</v>
-      </c>
+      <c r="C112" s="7"/>
       <c r="D112" s="7"/>
       <c r="E112" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F112" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F112" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
     </row>
     <row r="113" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A113" s="5" t="s">
-        <v>44</v>
-      </c>
+      <c r="A113" s="7"/>
       <c r="B113" s="7"/>
-      <c r="C113" s="7">
-        <v>64581</v>
-      </c>
+      <c r="C113" s="7"/>
       <c r="D113" s="7"/>
       <c r="E113" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F113" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F113" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
     </row>
     <row r="114" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A114" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="A114" s="7"/>
       <c r="B114" s="7"/>
-      <c r="C114" s="7">
-        <v>65231</v>
-      </c>
+      <c r="C114" s="7"/>
       <c r="D114" s="7"/>
       <c r="E114" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F114" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="F114" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
     </row>
     <row r="115" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A115" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B115" s="7">
-        <v>65818</v>
-      </c>
-      <c r="C115" s="7">
-        <v>65818</v>
-      </c>
+      <c r="A115" s="7"/>
+      <c r="B115" s="7"/>
+      <c r="C115" s="7"/>
       <c r="D115" s="7"/>
-      <c r="E115" s="3">
+      <c r="E115" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F115" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="F115" s="3" t="str">
-        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
@@ -3415,11 +4191,11 @@
       <c r="C116" s="7"/>
       <c r="D116" s="7"/>
       <c r="E116" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F116" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F116" s="3" t="str">
-        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
@@ -3429,11 +4205,11 @@
       <c r="C117" s="7"/>
       <c r="D117" s="7"/>
       <c r="E117" s="3" t="str">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+      <c r="F117" s="3" t="str">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F117" s="3" t="str">
-        <f t="shared" si="2"/>
         <v>-</v>
       </c>
     </row>
@@ -3443,11 +4219,11 @@
       <c r="C118" s="7"/>
       <c r="D118" s="7"/>
       <c r="E118" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F118" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="F118:F121" si="6">IF(D118&lt;&gt;"",IF(B118&lt;&gt;"",D118-B118,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -3457,11 +4233,11 @@
       <c r="C119" s="7"/>
       <c r="D119" s="7"/>
       <c r="E119" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F119" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
     </row>
@@ -3471,11 +4247,11 @@
       <c r="C120" s="7"/>
       <c r="D120" s="7"/>
       <c r="E120" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F120" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
     </row>
@@ -3485,11 +4261,11 @@
       <c r="C121" s="7"/>
       <c r="D121" s="7"/>
       <c r="E121" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
       <c r="F121" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
     </row>
@@ -3499,11 +4275,7 @@
       <c r="C122" s="7"/>
       <c r="D122" s="7"/>
       <c r="E122" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F122" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3513,11 +4285,7 @@
       <c r="C123" s="7"/>
       <c r="D123" s="7"/>
       <c r="E123" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F123" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3527,11 +4295,7 @@
       <c r="C124" s="7"/>
       <c r="D124" s="7"/>
       <c r="E124" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F124" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3541,11 +4305,7 @@
       <c r="C125" s="7"/>
       <c r="D125" s="7"/>
       <c r="E125" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F125" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3555,11 +4315,7 @@
       <c r="C126" s="7"/>
       <c r="D126" s="7"/>
       <c r="E126" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F126" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3569,11 +4325,7 @@
       <c r="C127" s="7"/>
       <c r="D127" s="7"/>
       <c r="E127" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F127" s="3" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -3583,325 +4335,223 @@
       <c r="C128" s="7"/>
       <c r="D128" s="7"/>
       <c r="E128" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F128" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
       <c r="D129" s="7"/>
       <c r="E129" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F129" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
       <c r="D130" s="7"/>
       <c r="E130" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F130" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
       <c r="D131" s="7"/>
       <c r="E131" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F131" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
       <c r="D132" s="7"/>
       <c r="E132" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F132" s="3" t="str">
-        <f t="shared" ref="F132:F135" si="4">IF(D132&lt;&gt;"",IF(B132&lt;&gt;"",D132-B132,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
       <c r="E133" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F133" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E133:E137" si="7">IF(C133&lt;&gt;"",IF(B133&lt;&gt;"",C133-B133,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
       <c r="E134" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F134" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
       <c r="D135" s="7"/>
       <c r="E135" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="F135" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
       <c r="D136" s="7"/>
       <c r="E136" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
       <c r="D137" s="7"/>
       <c r="E137" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
       <c r="E138" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E138:E139" si="8">IF(C138&lt;&gt;"",IF(B138&lt;&gt;"",B138-C138,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
       <c r="E139" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
-      <c r="E140" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="141" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
       <c r="D141" s="7"/>
-      <c r="E141" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A142" s="7"/>
+    </row>
+    <row r="142" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
-      <c r="E142" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A143" s="7"/>
+    </row>
+    <row r="143" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
-      <c r="E143" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A144" s="7"/>
+    </row>
+    <row r="144" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
-      <c r="E144" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A145" s="7"/>
+    </row>
+    <row r="145" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
-      <c r="E145" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A146" s="7"/>
+    </row>
+    <row r="146" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
-      <c r="E146" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A147" s="7"/>
+    </row>
+    <row r="147" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
-      <c r="E147" s="3" t="str">
-        <f t="shared" ref="E147:E151" si="5">IF(C147&lt;&gt;"",IF(B147&lt;&gt;"",C147-B147,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="148" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A148" s="7"/>
+    </row>
+    <row r="148" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
-      <c r="E148" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="149" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A149" s="7"/>
+    </row>
+    <row r="149" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
-      <c r="E149" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="150" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A150" s="7"/>
+    </row>
+    <row r="150" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
-      <c r="E150" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A151" s="7"/>
+    </row>
+    <row r="151" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
-      <c r="E151" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A152" s="7"/>
+    </row>
+    <row r="152" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
-      <c r="E152" s="3" t="str">
-        <f t="shared" ref="E152:E153" si="6">IF(C152&lt;&gt;"",IF(B152&lt;&gt;"",B152-C152,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A153" s="7"/>
+    </row>
+    <row r="153" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
-      <c r="E153" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A154" s="7"/>
+    </row>
+    <row r="154" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A155" s="7"/>
+    <row r="155" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
     </row>
-    <row r="157" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
     </row>
-    <row r="160" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
@@ -4496,78 +5146,9 @@
       <c r="C278" s="7"/>
       <c r="D278" s="7"/>
     </row>
-    <row r="279" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B279" s="7"/>
-      <c r="C279" s="7"/>
-      <c r="D279" s="7"/>
-    </row>
-    <row r="280" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B280" s="7"/>
-      <c r="C280" s="7"/>
-      <c r="D280" s="7"/>
-    </row>
-    <row r="281" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B281" s="7"/>
-      <c r="C281" s="7"/>
-      <c r="D281" s="7"/>
-    </row>
-    <row r="282" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B282" s="7"/>
-      <c r="C282" s="7"/>
-      <c r="D282" s="7"/>
-    </row>
-    <row r="283" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B283" s="7"/>
-      <c r="C283" s="7"/>
-      <c r="D283" s="7"/>
-    </row>
-    <row r="284" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B284" s="7"/>
-      <c r="C284" s="7"/>
-      <c r="D284" s="7"/>
-    </row>
-    <row r="285" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B285" s="7"/>
-      <c r="C285" s="7"/>
-      <c r="D285" s="7"/>
-    </row>
-    <row r="286" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B286" s="7"/>
-      <c r="C286" s="7"/>
-      <c r="D286" s="7"/>
-    </row>
-    <row r="287" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B287" s="7"/>
-      <c r="C287" s="7"/>
-      <c r="D287" s="7"/>
-    </row>
-    <row r="288" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B288" s="7"/>
-      <c r="C288" s="7"/>
-      <c r="D288" s="7"/>
-    </row>
-    <row r="289" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B289" s="7"/>
-      <c r="C289" s="7"/>
-      <c r="D289" s="7"/>
-    </row>
-    <row r="290" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B290" s="7"/>
-      <c r="C290" s="7"/>
-      <c r="D290" s="7"/>
-    </row>
-    <row r="291" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B291" s="7"/>
-      <c r="C291" s="7"/>
-      <c r="D291" s="7"/>
-    </row>
-    <row r="292" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B292" s="7"/>
-      <c r="C292" s="7"/>
-      <c r="D292" s="7"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10616,7 +11197,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="13" type="noConversion"/>
+  <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
lode runner v5 - up to level 23, 786 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805558B0-FBFA-4948-8E9C-5F75C911911E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF00178-DB2D-4D9D-AAB4-8F821CB0E117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48960" yWindow="750" windowWidth="9060" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="45525" yWindow="1620" windowWidth="9060" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V5" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="421" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="233">
   <si>
     <t>Place</t>
   </si>
@@ -730,6 +730,9 @@
   </si>
   <si>
     <t>32 End</t>
+  </si>
+  <si>
+    <t>ladder</t>
   </si>
 </sst>
 </file>
@@ -1160,6 +1163,7 @@
     <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1184,7 +1188,6 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -1505,11 +1508,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B3565E-C480-4A10-8524-B7BC06C9B703}">
-  <dimension ref="A1:G278"/>
+  <dimension ref="A1:H279"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B27" sqref="B27"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1544,7 +1547,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="33" t="s">
         <v>170</v>
       </c>
       <c r="B2" s="2">
@@ -1566,7 +1569,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="33" t="s">
         <v>171</v>
       </c>
       <c r="B3" s="7">
@@ -1592,7 +1595,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="33" t="s">
         <v>172</v>
       </c>
       <c r="B4" s="7">
@@ -1605,20 +1608,20 @@
         <v>1764</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E68" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
+        <f t="shared" ref="E4:E69" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
         <v>-37</v>
       </c>
       <c r="F4" s="3">
-        <f t="shared" ref="F4:F56" si="1">IF(D4&lt;&gt;"",IF(B4&lt;&gt;"",D4-B4,"-"), "-")</f>
+        <f t="shared" ref="F4:F57" si="1">IF(D4&lt;&gt;"",IF(B4&lt;&gt;"",D4-B4,"-"), "-")</f>
         <v>30</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G67" si="2">(C4-C3) - (D4-D3)</f>
+        <f t="shared" ref="G4:G68" si="2">(C4-C3) - (D4-D3)</f>
         <v>-15</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="33" t="s">
         <v>173</v>
       </c>
       <c r="B5" s="7">
@@ -1644,7 +1647,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="33" t="s">
         <v>174</v>
       </c>
       <c r="B6" s="7">
@@ -1670,7 +1673,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="33" t="s">
         <v>175</v>
       </c>
       <c r="B7" s="7">
@@ -1696,7 +1699,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="33" t="s">
         <v>176</v>
       </c>
       <c r="B8" s="7">
@@ -1722,7 +1725,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="33" t="s">
         <v>177</v>
       </c>
       <c r="B9" s="7">
@@ -1748,7 +1751,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="33" t="s">
         <v>178</v>
       </c>
       <c r="B10" s="7">
@@ -1774,7 +1777,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="33" t="s">
         <v>179</v>
       </c>
       <c r="B11" s="7">
@@ -1800,7 +1803,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="33" t="s">
         <v>180</v>
       </c>
       <c r="B12" s="7">
@@ -1826,7 +1829,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+      <c r="A13" s="33" t="s">
         <v>181</v>
       </c>
       <c r="B13" s="7">
@@ -1852,7 +1855,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="33" t="s">
         <v>182</v>
       </c>
       <c r="B14" s="7">
@@ -1878,7 +1881,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="41" t="s">
+      <c r="A15" s="33" t="s">
         <v>183</v>
       </c>
       <c r="B15" s="7">
@@ -1904,7 +1907,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="41" t="s">
+      <c r="A16" s="33" t="s">
         <v>184</v>
       </c>
       <c r="B16" s="7">
@@ -1929,8 +1932,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="41" t="s">
+    <row r="17" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="33" t="s">
         <v>185</v>
       </c>
       <c r="B17" s="7">
@@ -1955,8 +1958,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+    <row r="18" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="33" t="s">
         <v>186</v>
       </c>
       <c r="B18" s="7">
@@ -1981,8 +1984,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="41" t="s">
+    <row r="19" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="33" t="s">
         <v>187</v>
       </c>
       <c r="B19" s="7">
@@ -2007,8 +2010,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+    <row r="20" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="33" t="s">
         <v>188</v>
       </c>
       <c r="B20" s="7">
@@ -2017,7 +2020,7 @@
       <c r="C20" s="7">
         <v>11859</v>
       </c>
-      <c r="D20" s="41">
+      <c r="D20" s="33">
         <v>11687</v>
       </c>
       <c r="E20" s="3">
@@ -2033,8 +2036,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="41" t="s">
+    <row r="21" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="33" t="s">
         <v>189</v>
       </c>
       <c r="B21" s="7">
@@ -2059,8 +2062,8 @@
         <v>-79</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="41" t="s">
+    <row r="22" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="33" t="s">
         <v>190</v>
       </c>
       <c r="B22" s="7">
@@ -2085,8 +2088,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="41" t="s">
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="33" t="s">
         <v>191</v>
       </c>
       <c r="B23" s="7">
@@ -2111,11 +2114,11 @@
         <v>-70</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="41" t="s">
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="41">
+      <c r="B24" s="33">
         <v>13735</v>
       </c>
       <c r="C24" s="7">
@@ -2137,8 +2140,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="41" t="s">
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="33" t="s">
         <v>193</v>
       </c>
       <c r="B25" s="7">
@@ -2163,8 +2166,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="33" t="s">
         <v>194</v>
       </c>
       <c r="B26" s="7">
@@ -2189,1027 +2192,1071 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B27" s="7"/>
+      <c r="B27" s="7">
+        <v>15660</v>
+      </c>
       <c r="C27" s="7">
         <v>15994</v>
       </c>
       <c r="D27" s="7">
         <v>15987</v>
       </c>
-      <c r="E27" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F27" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E27" s="3">
+        <f t="shared" si="0"/>
+        <v>334</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="1"/>
+        <v>327</v>
       </c>
       <c r="G27">
         <f t="shared" si="2"/>
         <v>-27</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>196</v>
       </c>
-      <c r="B28" s="7"/>
+      <c r="B28" s="7">
+        <v>16305</v>
+      </c>
       <c r="C28" s="7">
         <v>16640</v>
       </c>
       <c r="D28" s="7">
         <v>16632</v>
       </c>
-      <c r="E28" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F28" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E28" s="3">
+        <f t="shared" si="0"/>
+        <v>335</v>
+      </c>
+      <c r="F28" s="3">
+        <f t="shared" si="1"/>
+        <v>327</v>
       </c>
       <c r="G28">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="B29" s="7"/>
+      <c r="B29" s="7">
+        <v>16830</v>
+      </c>
       <c r="C29" s="7">
         <v>17228</v>
       </c>
       <c r="D29" s="7">
         <v>17152</v>
       </c>
-      <c r="E29" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F29" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E29" s="3">
+        <f t="shared" si="0"/>
+        <v>398</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="1"/>
+        <v>322</v>
       </c>
       <c r="G29">
         <f t="shared" si="2"/>
         <v>68</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B30" s="7"/>
+      <c r="B30" s="7">
+        <v>17476</v>
+      </c>
       <c r="C30" s="7">
         <v>17866</v>
       </c>
       <c r="D30" s="7">
         <v>17797</v>
       </c>
-      <c r="E30" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F30" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E30" s="3">
+        <f t="shared" si="0"/>
+        <v>390</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="1"/>
+        <v>321</v>
       </c>
       <c r="G30">
         <f t="shared" si="2"/>
         <v>-7</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>198</v>
       </c>
-      <c r="B31" s="7"/>
+      <c r="B31" s="7">
+        <v>18217</v>
+      </c>
       <c r="C31" s="7">
         <v>18604</v>
       </c>
       <c r="D31" s="7">
         <v>18546</v>
       </c>
-      <c r="E31" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F31" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E31" s="3">
+        <f t="shared" si="0"/>
+        <v>387</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="1"/>
+        <v>329</v>
       </c>
       <c r="G31">
         <f t="shared" si="2"/>
         <v>-11</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>199</v>
       </c>
-      <c r="B32" s="7"/>
+      <c r="B32" s="7">
+        <v>18855</v>
+      </c>
       <c r="C32" s="7">
         <v>19242</v>
       </c>
       <c r="D32" s="7">
         <v>19184</v>
       </c>
-      <c r="E32" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F32" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E32" s="3">
+        <f t="shared" si="0"/>
+        <v>387</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="1"/>
+        <v>329</v>
       </c>
       <c r="G32">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="H32" s="7"/>
+    </row>
+    <row r="33" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>200</v>
       </c>
-      <c r="B33" s="7"/>
+      <c r="B33" s="7">
+        <v>19222</v>
+      </c>
       <c r="C33" s="7">
         <v>19683</v>
       </c>
       <c r="D33" s="7">
         <v>19572</v>
       </c>
-      <c r="E33" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F33" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E33" s="3">
+        <f t="shared" si="0"/>
+        <v>461</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" si="1"/>
+        <v>350</v>
       </c>
       <c r="G33">
-        <f t="shared" si="2"/>
+        <f>(C33-C32) - (D33-D32)</f>
         <v>53</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="H33" s="7"/>
+    </row>
+    <row r="34" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>201</v>
       </c>
-      <c r="B34" s="7"/>
+      <c r="B34" s="7">
+        <v>19867</v>
+      </c>
       <c r="C34" s="7">
         <v>20330</v>
       </c>
       <c r="D34" s="7">
         <v>20217</v>
       </c>
-      <c r="E34" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F34" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E34" s="3">
+        <f t="shared" si="0"/>
+        <v>463</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="1"/>
+        <v>350</v>
       </c>
       <c r="G34">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
-        <v>202</v>
-      </c>
-      <c r="B35" s="7"/>
+    <row r="35" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>232</v>
+      </c>
+      <c r="B35" s="7">
+        <v>20034</v>
+      </c>
       <c r="C35" s="7">
-        <v>21340</v>
+        <v>20501</v>
       </c>
       <c r="D35" s="7">
-        <v>21086</v>
-      </c>
-      <c r="E35" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F35" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+        <v>20383</v>
+      </c>
+      <c r="E35" s="3">
+        <f t="shared" si="0"/>
+        <v>467</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" si="1"/>
+        <v>349</v>
       </c>
       <c r="G35">
         <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A36" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B36" s="7">
+        <v>20738</v>
+      </c>
+      <c r="C36" s="7">
+        <v>21340</v>
+      </c>
+      <c r="D36" s="7">
+        <v>21086</v>
+      </c>
+      <c r="E36" s="3">
+        <f t="shared" si="0"/>
+        <v>602</v>
+      </c>
+      <c r="F36" s="3">
+        <f t="shared" si="1"/>
+        <v>348</v>
+      </c>
+      <c r="G36">
+        <f>(C36-C34) - (D36-D34)</f>
         <v>141</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="7" t="s">
+    <row r="37" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
         <v>203</v>
       </c>
-      <c r="B36" s="7"/>
-      <c r="C36" s="7">
+      <c r="B37" s="7">
+        <v>21383</v>
+      </c>
+      <c r="C37" s="7">
         <v>21985</v>
       </c>
-      <c r="D36" s="7">
+      <c r="D37" s="7">
         <v>21731</v>
       </c>
-      <c r="E36" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F36" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G36">
+      <c r="E37" s="3">
+        <f t="shared" si="0"/>
+        <v>602</v>
+      </c>
+      <c r="F37" s="3">
+        <f t="shared" si="1"/>
+        <v>348</v>
+      </c>
+      <c r="G37">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
+    <row r="38" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8">
+      <c r="B38" s="8">
+        <v>22330</v>
+      </c>
+      <c r="C38" s="8">
         <v>22936</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D38" s="8">
         <v>22797</v>
       </c>
-      <c r="E37" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F37" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G37">
-        <f t="shared" si="2"/>
+      <c r="E38" s="3">
+        <f t="shared" si="0"/>
+        <v>606</v>
+      </c>
+      <c r="F38" s="3">
+        <f t="shared" si="1"/>
+        <v>467</v>
+      </c>
+      <c r="G38">
+        <f>(C38-C37) - (D38-D37)</f>
         <v>-115</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
+    <row r="39" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="B38" s="7"/>
-      <c r="C38" s="7">
+      <c r="B39" s="33">
+        <v>22994</v>
+      </c>
+      <c r="C39" s="7">
         <v>23582</v>
       </c>
-      <c r="D38" s="7">
+      <c r="D39" s="7">
         <v>23442</v>
       </c>
-      <c r="E38" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F38" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G38">
+      <c r="E39" s="3">
+        <f t="shared" si="0"/>
+        <v>588</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" si="1"/>
+        <v>448</v>
+      </c>
+      <c r="G39">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="7" t="s">
+    <row r="40" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="B39" s="7"/>
-      <c r="C39" s="7">
+      <c r="B40" s="7">
+        <v>23293</v>
+      </c>
+      <c r="C40" s="7">
         <v>23922</v>
       </c>
-      <c r="D39" s="7">
+      <c r="D40" s="7">
         <v>23797</v>
       </c>
-      <c r="E39" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F39" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G39">
+      <c r="E40" s="3">
+        <f t="shared" si="0"/>
+        <v>629</v>
+      </c>
+      <c r="F40" s="3">
+        <f t="shared" si="1"/>
+        <v>504</v>
+      </c>
+      <c r="G40">
         <f t="shared" si="2"/>
         <v>-15</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="7" t="s">
+    <row r="41" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="B40" s="7"/>
-      <c r="C40" s="7">
+      <c r="B41" s="7">
+        <v>23953</v>
+      </c>
+      <c r="C41" s="7">
         <v>24583</v>
       </c>
-      <c r="D40" s="7">
+      <c r="D41" s="7">
         <v>24442</v>
       </c>
-      <c r="E40" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F40" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G40">
+      <c r="E41" s="3">
+        <f t="shared" si="0"/>
+        <v>630</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="shared" si="1"/>
+        <v>489</v>
+      </c>
+      <c r="G41">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="7" t="s">
+    <row r="42" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
         <v>208</v>
       </c>
-      <c r="B41" s="7"/>
-      <c r="C41" s="7">
+      <c r="B42" s="7">
+        <v>24530</v>
+      </c>
+      <c r="C42" s="7">
         <v>25181</v>
       </c>
-      <c r="D41" s="7">
+      <c r="D42" s="7">
         <v>25025</v>
       </c>
-      <c r="E41" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F41" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G41">
+      <c r="E42" s="3">
+        <f t="shared" si="0"/>
+        <v>651</v>
+      </c>
+      <c r="F42" s="3">
+        <f t="shared" si="1"/>
+        <v>495</v>
+      </c>
+      <c r="G42">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="7" t="s">
+    <row r="43" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
         <v>209</v>
       </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7">
+      <c r="B43" s="7">
+        <v>25190</v>
+      </c>
+      <c r="C43" s="7">
         <v>25839</v>
       </c>
-      <c r="D42" s="7">
+      <c r="D43" s="7">
         <v>25684</v>
       </c>
-      <c r="E42" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F42" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G42">
+      <c r="E43" s="3">
+        <f t="shared" si="0"/>
+        <v>649</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="shared" si="1"/>
+        <v>494</v>
+      </c>
+      <c r="G43">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="7" t="s">
+    <row r="44" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="7" t="s">
         <v>210</v>
       </c>
-      <c r="B43" s="7"/>
-      <c r="C43" s="7">
+      <c r="B44" s="7">
+        <v>26022</v>
+      </c>
+      <c r="C44" s="7">
         <v>26718</v>
       </c>
-      <c r="D43" s="7">
+      <c r="D44" s="7">
         <v>26528</v>
       </c>
-      <c r="E43" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F43" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G43">
+      <c r="E44" s="3">
+        <f t="shared" si="0"/>
+        <v>696</v>
+      </c>
+      <c r="F44" s="3">
+        <f t="shared" si="1"/>
+        <v>506</v>
+      </c>
+      <c r="G44">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="7" t="s">
+    <row r="45" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="7" t="s">
         <v>211</v>
       </c>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7">
+      <c r="B45" s="7">
+        <v>26681</v>
+      </c>
+      <c r="C45" s="7">
         <v>27377</v>
       </c>
-      <c r="D44" s="7">
+      <c r="D45" s="7">
         <v>27187</v>
       </c>
-      <c r="E44" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F44" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G44">
+      <c r="E45" s="3">
+        <f t="shared" si="0"/>
+        <v>696</v>
+      </c>
+      <c r="F45" s="3">
+        <f t="shared" si="1"/>
+        <v>506</v>
+      </c>
+      <c r="G45">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="7" t="s">
+    <row r="46" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="7" t="s">
         <v>212</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7">
+      <c r="B46" s="7">
+        <v>27244</v>
+      </c>
+      <c r="C46" s="7">
         <v>28030</v>
       </c>
-      <c r="D45" s="7">
+      <c r="D46" s="7">
         <v>27750</v>
       </c>
-      <c r="E45" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F45" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G45">
+      <c r="E46" s="3">
+        <f t="shared" si="0"/>
+        <v>786</v>
+      </c>
+      <c r="F46" s="3">
+        <f t="shared" si="1"/>
+        <v>506</v>
+      </c>
+      <c r="G46">
         <f t="shared" si="2"/>
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="7" t="s">
+    <row r="47" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="7" t="s">
         <v>213</v>
       </c>
-      <c r="B46" s="7"/>
-      <c r="C46" s="7">
+      <c r="B47" s="7">
+        <v>27889</v>
+      </c>
+      <c r="C47" s="7">
         <v>28675</v>
       </c>
-      <c r="D46" s="7">
+      <c r="D47" s="7">
         <v>28395</v>
       </c>
-      <c r="E46" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F46" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G46">
+      <c r="E47" s="3">
+        <f t="shared" si="0"/>
+        <v>786</v>
+      </c>
+      <c r="F47" s="3">
+        <f t="shared" si="1"/>
+        <v>506</v>
+      </c>
+      <c r="G47">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
+    <row r="48" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="B47" s="7"/>
-      <c r="C47" s="7">
+      <c r="B48" s="7"/>
+      <c r="C48" s="7">
         <v>29883</v>
       </c>
-      <c r="D47" s="7">
+      <c r="D48" s="7">
         <v>29432</v>
       </c>
-      <c r="E47" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F47" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G47">
+      <c r="E48" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F48" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="G48">
         <f t="shared" si="2"/>
         <v>171</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="7" t="s">
+    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7">
+      <c r="B49" s="7"/>
+      <c r="C49" s="7">
         <v>30378</v>
       </c>
-      <c r="D48" s="7">
+      <c r="D49" s="7">
         <v>29930</v>
       </c>
-      <c r="E48" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F48" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G48">
+      <c r="E49" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F49" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="G49">
         <f t="shared" si="2"/>
         <v>-3</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="7" t="s">
+    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A50" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7">
+      <c r="B50" s="7"/>
+      <c r="C50" s="7">
         <v>30809</v>
       </c>
-      <c r="D49" s="7">
+      <c r="D50" s="7">
         <v>30422</v>
       </c>
-      <c r="E49" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F49" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G49">
+      <c r="E50" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F50" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="G50">
         <f t="shared" si="2"/>
         <v>-61</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A50" s="7" t="s">
+    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="B50" s="7"/>
-      <c r="C50" s="7">
+      <c r="B51" s="7"/>
+      <c r="C51" s="7">
         <v>31448</v>
       </c>
-      <c r="D50" s="7">
+      <c r="D51" s="7">
         <v>31060</v>
       </c>
-      <c r="E50" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F50" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G50">
+      <c r="E51" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F51" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="G51">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="7" t="s">
+    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="B51" s="7"/>
-      <c r="C51" s="7">
+      <c r="B52" s="7"/>
+      <c r="C52" s="7">
         <v>32009</v>
       </c>
-      <c r="D51" s="7">
+      <c r="D52" s="7">
         <v>31627</v>
       </c>
-      <c r="E51" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F51" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G51">
+      <c r="E52" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F52" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="G52">
         <f t="shared" si="2"/>
         <v>-6</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="7" t="s">
+    <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A53" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7">
+      <c r="B53" s="7"/>
+      <c r="C53" s="7">
         <v>32654</v>
       </c>
-      <c r="D52" s="7">
+      <c r="D53" s="7">
         <v>32272</v>
       </c>
-      <c r="E52" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F52" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G52">
+      <c r="E53" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F53" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="G53">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A53" s="7" t="s">
+    <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7">
+      <c r="B54" s="7"/>
+      <c r="C54" s="7">
         <v>33576</v>
       </c>
-      <c r="D53" s="7">
+      <c r="D54" s="7">
         <v>33186</v>
       </c>
-      <c r="E53" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F53" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G53">
+      <c r="E54" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F54" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="G54">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="7" t="s">
+    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A55" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="7">
+      <c r="B55" s="7"/>
+      <c r="C55" s="7">
         <v>34235</v>
       </c>
-      <c r="D54" s="7">
+      <c r="D55" s="7">
         <v>33845</v>
       </c>
-      <c r="E54" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F54" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G54">
+      <c r="E55" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F55" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="G55">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A55" s="7" t="s">
+    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7">
+      <c r="B56" s="7"/>
+      <c r="C56" s="7">
         <v>35341</v>
       </c>
-      <c r="D55" s="7">
+      <c r="D56" s="7">
         <v>34891</v>
       </c>
-      <c r="E55" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F55" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G55">
+      <c r="E56" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F56" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="G56">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A56" s="7" t="s">
+    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A57" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="B56" s="7"/>
-      <c r="C56" s="7">
+      <c r="B57" s="7"/>
+      <c r="C57" s="7">
         <v>35986</v>
       </c>
-      <c r="D56" s="7">
+      <c r="D57" s="7">
         <v>35550</v>
       </c>
-      <c r="E56" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F56" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
-      </c>
-      <c r="G56">
+      <c r="E57" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F57" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+      <c r="G57">
         <f t="shared" si="2"/>
         <v>-14</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A57" s="7" t="s">
+    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7">
+      <c r="B58" s="7"/>
+      <c r="C58" s="7">
         <v>36861</v>
       </c>
-      <c r="D57" s="7">
+      <c r="D58" s="7">
         <v>36365</v>
       </c>
-      <c r="E57" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F57" s="3" t="str">
-        <f t="shared" ref="F57:F117" si="3">IF(D57&lt;&gt;"",IF(B57&lt;&gt;"",D57-B57,"-"), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="G57">
+      <c r="E58" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F58" s="3" t="str">
+        <f t="shared" ref="F58:F118" si="3">IF(D58&lt;&gt;"",IF(B58&lt;&gt;"",D58-B58,"-"), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="G58">
         <f t="shared" si="2"/>
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A58" s="7" t="s">
+    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A59" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="B58" s="7"/>
-      <c r="C58" s="7">
+      <c r="B59" s="7"/>
+      <c r="C59" s="7">
         <v>37461</v>
       </c>
-      <c r="D58" s="7">
+      <c r="D59" s="7">
         <v>36977</v>
       </c>
-      <c r="E58" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F58" s="3" t="str">
+      <c r="E59" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F59" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G58">
+      <c r="G59">
         <f t="shared" si="2"/>
         <v>-12</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A59" s="7" t="s">
+    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A60" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7">
+      <c r="B60" s="7"/>
+      <c r="C60" s="7">
         <v>38564</v>
       </c>
-      <c r="D59" s="7">
+      <c r="D60" s="7">
         <v>38073</v>
       </c>
-      <c r="E59" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F59" s="3" t="str">
+      <c r="E60" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F60" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G59">
+      <c r="G60">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A60" s="7" t="s">
+    <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A61" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7">
+      <c r="B61" s="7"/>
+      <c r="C61" s="7">
         <v>39057</v>
       </c>
-      <c r="D60" s="7">
+      <c r="D61" s="7">
         <v>38571</v>
       </c>
-      <c r="E60" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F60" s="3" t="str">
+      <c r="E61" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F61" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G60">
+      <c r="G61">
         <f t="shared" si="2"/>
         <v>-5</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="7" t="s">
+    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A62" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7">
+      <c r="B62" s="7"/>
+      <c r="C62" s="7">
         <v>39781</v>
       </c>
-      <c r="D61" s="7">
+      <c r="D62" s="7">
         <v>39448</v>
       </c>
-      <c r="E61" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F61" s="3" t="str">
+      <c r="E62" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F62" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G61">
+      <c r="G62">
         <f t="shared" si="2"/>
         <v>-153</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
+    <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7">
+      <c r="B63" s="7"/>
+      <c r="C63" s="7">
         <v>40405</v>
       </c>
-      <c r="D62" s="7">
+      <c r="D63" s="7">
         <v>40072</v>
       </c>
-      <c r="E62" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F62" s="3" t="str">
+      <c r="E63" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F63" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G62">
+      <c r="G63">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="B63" s="9"/>
-      <c r="C63" s="9">
+      <c r="B64" s="9"/>
+      <c r="C64" s="9">
         <v>40588</v>
       </c>
-      <c r="D63" s="9">
+      <c r="D64" s="9">
         <v>40256</v>
       </c>
-      <c r="E63" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F63" s="3" t="str">
+      <c r="E64" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F64" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G63">
+      <c r="G64">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="B64" s="7"/>
-      <c r="C64" s="7">
+      <c r="B65" s="7"/>
+      <c r="C65" s="7">
         <v>41228</v>
       </c>
-      <c r="D64" s="7">
+      <c r="D65" s="7">
         <v>40894</v>
       </c>
-      <c r="E64" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F64" s="3" t="str">
+      <c r="E65" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F65" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G64">
+      <c r="G65">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
+    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="B65" s="9"/>
-      <c r="C65" s="9">
+      <c r="B66" s="9"/>
+      <c r="C66" s="9">
         <v>41865</v>
       </c>
-      <c r="D65" s="9">
+      <c r="D66" s="9">
         <v>41440</v>
       </c>
-      <c r="E65" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F65" s="3" t="str">
+      <c r="E66" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F66" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G65">
+      <c r="G66">
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
+    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B66" s="7"/>
-      <c r="C66" s="7">
+      <c r="B67" s="7"/>
+      <c r="C67" s="7">
         <v>42511</v>
       </c>
-      <c r="D66" s="7">
+      <c r="D67" s="7">
         <v>42085</v>
       </c>
-      <c r="E66" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F66" s="3" t="str">
+      <c r="E67" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F67" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G66">
+      <c r="G67">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7">
+      <c r="B68" s="7"/>
+      <c r="C68" s="7">
         <v>43110</v>
       </c>
-      <c r="D67" s="7">
+      <c r="D68" s="7">
         <v>42757</v>
       </c>
-      <c r="E67" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F67" s="3" t="str">
+      <c r="E68" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F68" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G67">
+      <c r="G68">
         <f t="shared" si="2"/>
         <v>-73</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7">
-        <v>43756</v>
-      </c>
-      <c r="D68" s="7">
-        <v>43402</v>
-      </c>
-      <c r="E68" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F68" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G68">
-        <f t="shared" ref="G68:G101" si="4">(C68-C67) - (D68-D67)</f>
-        <v>1</v>
-      </c>
-    </row>
     <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="B69" s="7"/>
       <c r="C69" s="7">
-        <v>44418</v>
+        <v>43756</v>
       </c>
       <c r="D69" s="7">
-        <v>44061</v>
+        <v>43402</v>
       </c>
       <c r="E69" s="3" t="str">
-        <f t="shared" ref="E69:E132" si="5">IF(C69&lt;&gt;"",IF(B69&lt;&gt;"",C69-B69,"-"), "-")</f>
+        <f t="shared" si="0"/>
         <v>-</v>
       </c>
       <c r="F69" s="3" t="str">
@@ -3217,644 +3264,644 @@
         <v>-</v>
       </c>
       <c r="G69">
+        <f t="shared" ref="G69:G102" si="4">(C69-C68) - (D69-D68)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7">
+        <v>44418</v>
+      </c>
+      <c r="D70" s="7">
+        <v>44061</v>
+      </c>
+      <c r="E70" s="3" t="str">
+        <f t="shared" ref="E70:E133" si="5">IF(C70&lt;&gt;"",IF(B70&lt;&gt;"",C70-B70,"-"), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="F70" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+      <c r="G70">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7">
+      <c r="B71" s="7"/>
+      <c r="C71" s="7">
         <v>45077</v>
       </c>
-      <c r="D70" s="7">
+      <c r="D71" s="7">
         <v>44720</v>
       </c>
-      <c r="E70" s="3" t="str">
+      <c r="E71" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F70" s="3" t="str">
+      <c r="F71" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G70">
+      <c r="G71">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
+    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7">
+      <c r="B72" s="7"/>
+      <c r="C72" s="7">
         <v>45719</v>
       </c>
-      <c r="D71" s="7">
+      <c r="D72" s="7">
         <v>45363</v>
       </c>
-      <c r="E71" s="3" t="str">
+      <c r="E72" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F71" s="3" t="str">
+      <c r="F72" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G71">
+      <c r="G72">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
+    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7">
+      <c r="B73" s="7"/>
+      <c r="C73" s="7">
         <v>46378</v>
       </c>
-      <c r="D72" s="7">
+      <c r="D73" s="7">
         <v>46022</v>
       </c>
-      <c r="E72" s="3" t="str">
+      <c r="E73" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F72" s="3" t="str">
+      <c r="F73" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G72">
+      <c r="G73">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7">
+      <c r="B74" s="7"/>
+      <c r="C74" s="7">
         <v>46984</v>
       </c>
-      <c r="D73" s="41">
+      <c r="D74" s="33">
         <v>46679</v>
       </c>
-      <c r="E73" s="3" t="str">
+      <c r="E74" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F73" s="3" t="str">
+      <c r="F74" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G73">
+      <c r="G74">
         <f t="shared" si="4"/>
         <v>-51</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7">
+      <c r="B75" s="7"/>
+      <c r="C75" s="7">
         <v>47629</v>
       </c>
-      <c r="D74" s="7">
+      <c r="D75" s="7">
         <v>47338</v>
       </c>
-      <c r="E74" s="3" t="str">
+      <c r="E75" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F74" s="3" t="str">
+      <c r="F75" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G74">
+      <c r="G75">
         <f t="shared" si="4"/>
         <v>-14</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="7" t="s">
+    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7">
+      <c r="B76" s="7"/>
+      <c r="C76" s="7">
         <v>48410</v>
       </c>
-      <c r="D75" s="7">
+      <c r="D76" s="7">
         <v>48121</v>
       </c>
-      <c r="E75" s="3" t="str">
+      <c r="E76" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F75" s="3" t="str">
+      <c r="F76" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G75">
+      <c r="G76">
         <f t="shared" si="4"/>
         <v>-2</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
+    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7">
+      <c r="B77" s="7"/>
+      <c r="C77" s="7">
         <v>48908</v>
       </c>
-      <c r="D76" s="7">
+      <c r="D77" s="7">
         <v>48619</v>
       </c>
-      <c r="E76" s="3" t="str">
+      <c r="E77" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F76" s="3" t="str">
+      <c r="F77" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G76">
+      <c r="G77">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
+    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7">
+      <c r="B78" s="7"/>
+      <c r="C78" s="7">
         <v>49856</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D78" s="7">
         <v>49502</v>
       </c>
-      <c r="E77" s="3" t="str">
+      <c r="E78" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F77" s="3" t="str">
+      <c r="F78" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G77">
+      <c r="G78">
         <f t="shared" si="4"/>
         <v>65</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
+    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7">
+      <c r="B79" s="7"/>
+      <c r="C79" s="7">
         <v>50516</v>
       </c>
-      <c r="D78" s="7">
+      <c r="D79" s="7">
         <v>50148</v>
       </c>
-      <c r="E78" s="3" t="str">
+      <c r="E79" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F78" s="3" t="str">
+      <c r="F79" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G78">
+      <c r="G79">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
+    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7">
+      <c r="B80" s="7"/>
+      <c r="C80" s="7">
         <v>50874</v>
       </c>
-      <c r="D79" s="7">
+      <c r="D80" s="7">
         <v>50417</v>
       </c>
-      <c r="E79" s="3" t="str">
+      <c r="E80" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F79" s="3" t="str">
+      <c r="F80" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G79">
+      <c r="G80">
         <f t="shared" si="4"/>
         <v>89</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
+    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B80" s="7"/>
-      <c r="C80" s="7">
+      <c r="B81" s="7"/>
+      <c r="C81" s="7">
         <v>51486</v>
       </c>
-      <c r="D80" s="7">
+      <c r="D81" s="7">
         <v>51016</v>
       </c>
-      <c r="E80" s="3" t="str">
+      <c r="E81" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F80" s="3" t="str">
+      <c r="F81" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G80">
+      <c r="G81">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
+    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7">
+      <c r="B82" s="7"/>
+      <c r="C82" s="7">
         <v>52507</v>
       </c>
-      <c r="D81" s="7">
+      <c r="D82" s="7">
         <v>52007</v>
       </c>
-      <c r="E81" s="3" t="str">
+      <c r="E82" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F81" s="3" t="str">
+      <c r="F82" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G81">
+      <c r="G82">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7">
+      <c r="B83" s="7"/>
+      <c r="C83" s="7">
         <v>53153</v>
       </c>
-      <c r="D82" s="7">
+      <c r="D83" s="7">
         <v>52667</v>
       </c>
-      <c r="E82" s="3" t="str">
+      <c r="E83" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F82" s="3" t="str">
+      <c r="F83" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G82">
+      <c r="G83">
         <f t="shared" si="4"/>
         <v>-14</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
+    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B83" s="7"/>
-      <c r="C83" s="7">
+      <c r="B84" s="7"/>
+      <c r="C84" s="7">
         <v>53942</v>
       </c>
-      <c r="D83" s="7">
+      <c r="D84" s="7">
         <v>53473</v>
       </c>
-      <c r="E83" s="3" t="str">
+      <c r="E84" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F83" s="3" t="str">
+      <c r="F84" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G83">
+      <c r="G84">
         <f t="shared" si="4"/>
         <v>-17</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
+    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B84" s="7"/>
-      <c r="C84" s="7">
+      <c r="B85" s="7"/>
+      <c r="C85" s="7">
         <v>54564</v>
       </c>
-      <c r="D84" s="7">
+      <c r="D85" s="7">
         <v>54095</v>
       </c>
-      <c r="E84" s="3" t="str">
+      <c r="E85" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F84" s="3" t="str">
+      <c r="F85" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G84">
+      <c r="G85">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
+    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B85" s="7"/>
-      <c r="C85" s="7">
+      <c r="B86" s="7"/>
+      <c r="C86" s="7">
         <v>55596</v>
       </c>
-      <c r="D85" s="7">
+      <c r="D86" s="7">
         <v>55108</v>
       </c>
-      <c r="E85" s="3" t="str">
+      <c r="E86" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F85" s="3" t="str">
+      <c r="F86" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G85">
+      <c r="G86">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
+    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B86" s="7"/>
-      <c r="C86" s="7">
+      <c r="B87" s="7"/>
+      <c r="C87" s="7">
         <v>56185</v>
       </c>
-      <c r="D86" s="7">
+      <c r="D87" s="7">
         <v>55708</v>
       </c>
-      <c r="E86" s="3" t="str">
+      <c r="E87" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F86" s="3" t="str">
+      <c r="F87" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G86">
+      <c r="G87">
         <f t="shared" si="4"/>
         <v>-11</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
+    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B87" s="7"/>
-      <c r="C87" s="7">
+      <c r="B88" s="7"/>
+      <c r="C88" s="7">
         <v>56572</v>
       </c>
-      <c r="D87" s="7">
+      <c r="D88" s="7">
         <v>56104</v>
       </c>
-      <c r="E87" s="3" t="str">
+      <c r="E88" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F87" s="3" t="str">
+      <c r="F88" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G87">
+      <c r="G88">
         <f t="shared" si="4"/>
         <v>-9</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
+    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B88" s="7"/>
-      <c r="C88" s="7">
+      <c r="B89" s="7"/>
+      <c r="C89" s="7">
         <v>57217</v>
       </c>
-      <c r="D88" s="7">
+      <c r="D89" s="7">
         <v>56749</v>
       </c>
-      <c r="E88" s="3" t="str">
+      <c r="E89" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F88" s="3" t="str">
+      <c r="F89" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G88">
+      <c r="G89">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B89" s="7"/>
-      <c r="C89" s="7">
+      <c r="B90" s="7"/>
+      <c r="C90" s="7">
         <v>58008</v>
       </c>
-      <c r="D89" s="7">
+      <c r="D90" s="7">
         <v>57450</v>
       </c>
-      <c r="E89" s="3" t="str">
+      <c r="E90" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F89" s="3" t="str">
+      <c r="F90" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G89">
+      <c r="G90">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
+    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B90" s="7"/>
-      <c r="C90" s="7">
+      <c r="B91" s="7"/>
+      <c r="C91" s="7">
         <v>58608</v>
       </c>
-      <c r="D90" s="7">
+      <c r="D91" s="7">
         <v>58050</v>
       </c>
-      <c r="E90" s="3" t="str">
+      <c r="E91" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F90" s="3" t="str">
+      <c r="F91" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G90">
+      <c r="G91">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
+    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7">
+      <c r="B92" s="7"/>
+      <c r="C92" s="7">
         <v>59190</v>
       </c>
-      <c r="D91" s="7">
+      <c r="D92" s="7">
         <v>58612</v>
       </c>
-      <c r="E91" s="3" t="str">
+      <c r="E92" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F91" s="3" t="str">
+      <c r="F92" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G91">
+      <c r="G92">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
+    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B92" s="7"/>
-      <c r="C92" s="7">
+      <c r="B93" s="7"/>
+      <c r="C93" s="7">
         <v>59825</v>
       </c>
-      <c r="D92" s="7">
+      <c r="D93" s="7">
         <v>59247</v>
       </c>
-      <c r="E92" s="3" t="str">
+      <c r="E93" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F92" s="3" t="str">
+      <c r="F93" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G92">
+      <c r="G93">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
+    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B93" s="7"/>
-      <c r="C93" s="7">
+      <c r="B94" s="7"/>
+      <c r="C94" s="7">
         <v>60441</v>
       </c>
-      <c r="D93" s="7">
+      <c r="D94" s="7">
         <v>59838</v>
       </c>
-      <c r="E93" s="3" t="str">
+      <c r="E94" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F93" s="3" t="str">
+      <c r="F94" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G93">
+      <c r="G94">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
+    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B94" s="7"/>
-      <c r="C94" s="7">
+      <c r="B95" s="7"/>
+      <c r="C95" s="7">
         <v>61093</v>
       </c>
-      <c r="D94" s="7">
+      <c r="D95" s="7">
         <v>60490</v>
       </c>
-      <c r="E94" s="3" t="str">
+      <c r="E95" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F94" s="3" t="str">
+      <c r="F95" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G94">
+      <c r="G95">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B95" s="10"/>
-      <c r="C95" s="10">
-        <v>61914</v>
-      </c>
-      <c r="D95" s="10">
-        <v>61295</v>
-      </c>
-      <c r="E95" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F95" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G95">
-        <f t="shared" si="4"/>
-        <v>16</v>
-      </c>
-    </row>
     <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7">
-        <v>62575</v>
-      </c>
-      <c r="D96" s="7">
-        <v>61940</v>
+        <v>42</v>
+      </c>
+      <c r="B96" s="10"/>
+      <c r="C96" s="10">
+        <v>61914</v>
+      </c>
+      <c r="D96" s="10">
+        <v>61295</v>
       </c>
       <c r="E96" s="3" t="str">
         <f t="shared" si="5"/>
@@ -3871,14 +3918,14 @@
     </row>
     <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A97" s="5" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B97" s="7"/>
       <c r="C97" s="7">
-        <v>63180</v>
+        <v>62575</v>
       </c>
       <c r="D97" s="7">
-        <v>62513</v>
+        <v>61940</v>
       </c>
       <c r="E97" s="3" t="str">
         <f t="shared" si="5"/>
@@ -3890,19 +3937,19 @@
       </c>
       <c r="G97">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A98" s="5" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B98" s="7"/>
       <c r="C98" s="7">
-        <v>63825</v>
+        <v>63180</v>
       </c>
       <c r="D98" s="7">
-        <v>63172</v>
+        <v>62513</v>
       </c>
       <c r="E98" s="3" t="str">
         <f t="shared" si="5"/>
@@ -3914,19 +3961,19 @@
       </c>
       <c r="G98">
         <f t="shared" si="4"/>
-        <v>-14</v>
+        <v>32</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A99" s="5" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B99" s="7"/>
       <c r="C99" s="7">
-        <v>64581</v>
+        <v>63825</v>
       </c>
       <c r="D99" s="7">
-        <v>63896</v>
+        <v>63172</v>
       </c>
       <c r="E99" s="3" t="str">
         <f t="shared" si="5"/>
@@ -3938,19 +3985,19 @@
       </c>
       <c r="G99">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="B100" s="7"/>
       <c r="C100" s="7">
-        <v>65231</v>
+        <v>64581</v>
       </c>
       <c r="D100" s="7">
-        <v>64541</v>
+        <v>63896</v>
       </c>
       <c r="E100" s="3" t="str">
         <f t="shared" si="5"/>
@@ -3962,19 +4009,19 @@
       </c>
       <c r="G100">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>32</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B101" s="7"/>
       <c r="C101" s="7">
-        <v>65820</v>
+        <v>65231</v>
       </c>
       <c r="D101" s="7">
-        <v>65084</v>
+        <v>64541</v>
       </c>
       <c r="E101" s="3" t="str">
         <f t="shared" si="5"/>
@@ -3986,14 +4033,20 @@
       </c>
       <c r="G101">
         <f t="shared" si="4"/>
-        <v>46</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="7"/>
+      <c r="A102" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="B102" s="7"/>
-      <c r="C102" s="7"/>
-      <c r="D102" s="7"/>
+      <c r="C102" s="7">
+        <v>65820</v>
+      </c>
+      <c r="D102" s="7">
+        <v>65084</v>
+      </c>
       <c r="E102" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4001,6 +4054,10 @@
       <c r="F102" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
+      </c>
+      <c r="G102">
+        <f t="shared" si="4"/>
+        <v>46</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -4223,7 +4280,7 @@
         <v>-</v>
       </c>
       <c r="F118" s="3" t="str">
-        <f t="shared" ref="F118:F121" si="6">IF(D118&lt;&gt;"",IF(B118&lt;&gt;"",D118-B118,"-"), "-")</f>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -4237,7 +4294,7 @@
         <v>-</v>
       </c>
       <c r="F119" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="F119:F122" si="6">IF(D119&lt;&gt;"",IF(B119&lt;&gt;"",D119-B119,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -4278,6 +4335,10 @@
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
+      <c r="F122" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="123" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A123" s="7"/>
@@ -4385,7 +4446,7 @@
       <c r="C133" s="7"/>
       <c r="D133" s="7"/>
       <c r="E133" s="3" t="str">
-        <f t="shared" ref="E133:E137" si="7">IF(C133&lt;&gt;"",IF(B133&lt;&gt;"",C133-B133,"-"), "-")</f>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -4395,7 +4456,7 @@
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
       <c r="E134" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="E134:E138" si="7">IF(C134&lt;&gt;"",IF(B134&lt;&gt;"",C134-B134,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -4435,7 +4496,7 @@
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
       <c r="E138" s="3" t="str">
-        <f t="shared" ref="E138:E139" si="8">IF(C138&lt;&gt;"",IF(B138&lt;&gt;"",B138-C138,"-"), "-")</f>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
     </row>
@@ -4445,7 +4506,7 @@
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
       <c r="E139" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="E139:E140" si="8">IF(C139&lt;&gt;"",IF(B139&lt;&gt;"",B139-C139,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -4454,6 +4515,10 @@
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
+      <c r="E140" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="141" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="7"/>
@@ -4462,6 +4527,7 @@
       <c r="D141" s="7"/>
     </row>
     <row r="142" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A142" s="7"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
@@ -5145,6 +5211,11 @@
       <c r="B278" s="7"/>
       <c r="C278" s="7"/>
       <c r="D278" s="7"/>
+    </row>
+    <row r="279" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B279" s="7"/>
+      <c r="C279" s="7"/>
+      <c r="D279" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11232,10 +11303,10 @@
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="33" t="s">
+      <c r="K1" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="L1" s="34"/>
+      <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
@@ -13087,13 +13158,13 @@
       <c r="G53" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="H53" s="35" t="s">
+      <c r="H53" s="36" t="s">
         <v>165</v>
       </c>
-      <c r="I53" s="36"/>
-      <c r="J53" s="36"/>
-      <c r="K53" s="36"/>
-      <c r="L53" s="37"/>
+      <c r="I53" s="37"/>
+      <c r="J53" s="37"/>
+      <c r="K53" s="37"/>
+      <c r="L53" s="38"/>
     </row>
     <row r="54" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
@@ -13115,11 +13186,11 @@
       <c r="G54" s="27">
         <v>31536</v>
       </c>
-      <c r="H54" s="38"/>
-      <c r="I54" s="39"/>
-      <c r="J54" s="39"/>
-      <c r="K54" s="39"/>
-      <c r="L54" s="40"/>
+      <c r="H54" s="39"/>
+      <c r="I54" s="40"/>
+      <c r="J54" s="40"/>
+      <c r="K54" s="40"/>
+      <c r="L54" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
lode runner v5 - up to level 32, 1255 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF00178-DB2D-4D9D-AAB4-8F821CB0E117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF52CCF-4780-436F-A780-EB80680CD522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45525" yWindow="1620" windowWidth="9060" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="235">
   <si>
     <t>Place</t>
   </si>
@@ -733,6 +733,12 @@
   </si>
   <si>
     <t>ladder</t>
+  </si>
+  <si>
+    <t>fall</t>
+  </si>
+  <si>
+    <t>walk</t>
   </si>
 </sst>
 </file>
@@ -742,12 +748,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1074,120 +1087,121 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -1508,11 +1522,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B3565E-C480-4A10-8524-B7BC06C9B703}">
-  <dimension ref="A1:H279"/>
+  <dimension ref="A1:H282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1608,7 +1622,7 @@
         <v>1764</v>
       </c>
       <c r="E4" s="3">
-        <f t="shared" ref="E4:E69" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
+        <f t="shared" ref="E4:E72" si="0">IF(C4&lt;&gt;"",IF(B4&lt;&gt;"",C4-B4,"-"), "-")</f>
         <v>-37</v>
       </c>
       <c r="F4" s="3">
@@ -1616,7 +1630,7 @@
         <v>30</v>
       </c>
       <c r="G4">
-        <f t="shared" ref="G4:G68" si="2">(C4-C3) - (D4-D3)</f>
+        <f t="shared" ref="G4:G71" si="2">(C4-C3) - (D4-D3)</f>
         <v>-15</v>
       </c>
     </row>
@@ -2693,7 +2707,7 @@
         <v>212</v>
       </c>
       <c r="B46" s="7">
-        <v>27244</v>
+        <v>27241</v>
       </c>
       <c r="C46" s="7">
         <v>28030</v>
@@ -2703,11 +2717,11 @@
       </c>
       <c r="E46" s="3">
         <f t="shared" si="0"/>
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="F46" s="3">
         <f t="shared" si="1"/>
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="G46">
         <f t="shared" si="2"/>
@@ -2744,23 +2758,25 @@
       <c r="A48" s="7" t="s">
         <v>214</v>
       </c>
-      <c r="B48" s="7"/>
+      <c r="B48" s="7">
+        <v>28945</v>
+      </c>
       <c r="C48" s="7">
         <v>29883</v>
       </c>
       <c r="D48" s="7">
         <v>29432</v>
       </c>
-      <c r="E48" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F48" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E48" s="3">
+        <f t="shared" si="0"/>
+        <v>938</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="1"/>
+        <v>487</v>
       </c>
       <c r="G48">
-        <f t="shared" si="2"/>
+        <f>(C48-C47) - (D48-D47)</f>
         <v>171</v>
       </c>
     </row>
@@ -2768,116 +2784,126 @@
       <c r="A49" s="7" t="s">
         <v>215</v>
       </c>
-      <c r="B49" s="7"/>
+      <c r="B49" s="7">
+        <v>29444</v>
+      </c>
       <c r="C49" s="7">
-        <v>30378</v>
+        <v>30382</v>
       </c>
       <c r="D49" s="7">
         <v>29930</v>
       </c>
-      <c r="E49" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F49" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E49" s="3">
+        <f t="shared" si="0"/>
+        <v>938</v>
+      </c>
+      <c r="F49" s="3">
+        <f t="shared" si="1"/>
+        <v>486</v>
       </c>
       <c r="G49">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>216</v>
       </c>
-      <c r="B50" s="7"/>
+      <c r="B50" s="7">
+        <v>29868</v>
+      </c>
       <c r="C50" s="7">
         <v>30809</v>
       </c>
       <c r="D50" s="7">
         <v>30422</v>
       </c>
-      <c r="E50" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F50" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E50" s="3">
+        <f t="shared" si="0"/>
+        <v>941</v>
+      </c>
+      <c r="F50" s="3">
+        <f t="shared" si="1"/>
+        <v>554</v>
       </c>
       <c r="G50">
         <f t="shared" si="2"/>
-        <v>-61</v>
+        <v>-65</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="B51" s="7"/>
+      <c r="B51" s="7">
+        <v>30507</v>
+      </c>
       <c r="C51" s="7">
-        <v>31448</v>
+        <v>31450</v>
       </c>
       <c r="D51" s="7">
         <v>31060</v>
       </c>
-      <c r="E51" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F51" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E51" s="3">
+        <f t="shared" si="0"/>
+        <v>943</v>
+      </c>
+      <c r="F51" s="3">
+        <f t="shared" si="1"/>
+        <v>553</v>
       </c>
       <c r="G51">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="B52" s="7"/>
+      <c r="B52" s="7">
+        <v>31061</v>
+      </c>
       <c r="C52" s="7">
         <v>32009</v>
       </c>
       <c r="D52" s="7">
         <v>31627</v>
       </c>
-      <c r="E52" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F52" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E52" s="3">
+        <f t="shared" si="0"/>
+        <v>948</v>
+      </c>
+      <c r="F52" s="3">
+        <f t="shared" si="1"/>
+        <v>566</v>
       </c>
       <c r="G52">
         <f t="shared" si="2"/>
-        <v>-6</v>
+        <v>-8</v>
       </c>
     </row>
     <row r="53" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>219</v>
       </c>
-      <c r="B53" s="7"/>
+      <c r="B53" s="7">
+        <v>31706</v>
+      </c>
       <c r="C53" s="7">
         <v>32654</v>
       </c>
       <c r="D53" s="7">
         <v>32272</v>
       </c>
-      <c r="E53" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F53" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E53" s="3">
+        <f t="shared" si="0"/>
+        <v>948</v>
+      </c>
+      <c r="F53" s="3">
+        <f t="shared" si="1"/>
+        <v>566</v>
       </c>
       <c r="G53">
         <f t="shared" si="2"/>
@@ -2888,20 +2914,22 @@
       <c r="A54" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="B54" s="7"/>
+      <c r="B54" s="7">
+        <v>32622</v>
+      </c>
       <c r="C54" s="7">
         <v>33576</v>
       </c>
       <c r="D54" s="7">
         <v>33186</v>
       </c>
-      <c r="E54" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F54" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E54" s="3">
+        <f t="shared" si="0"/>
+        <v>954</v>
+      </c>
+      <c r="F54" s="3">
+        <f t="shared" si="1"/>
+        <v>564</v>
       </c>
       <c r="G54">
         <f t="shared" si="2"/>
@@ -2912,20 +2940,22 @@
       <c r="A55" s="7" t="s">
         <v>221</v>
       </c>
-      <c r="B55" s="7"/>
+      <c r="B55" s="7">
+        <v>33269</v>
+      </c>
       <c r="C55" s="7">
         <v>34235</v>
       </c>
       <c r="D55" s="7">
         <v>33845</v>
       </c>
-      <c r="E55" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F55" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E55" s="3">
+        <f t="shared" si="0"/>
+        <v>966</v>
+      </c>
+      <c r="F55" s="3">
+        <f t="shared" si="1"/>
+        <v>576</v>
       </c>
       <c r="G55">
         <f t="shared" si="2"/>
@@ -2936,23 +2966,25 @@
       <c r="A56" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="B56" s="7"/>
+      <c r="B56" s="7">
+        <v>34177</v>
+      </c>
       <c r="C56" s="7">
         <v>35341</v>
       </c>
       <c r="D56" s="7">
         <v>34891</v>
       </c>
-      <c r="E56" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F56" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E56" s="3">
+        <f t="shared" si="0"/>
+        <v>1164</v>
+      </c>
+      <c r="F56" s="3">
+        <f t="shared" si="1"/>
+        <v>714</v>
       </c>
       <c r="G56">
-        <f t="shared" si="2"/>
+        <f>(C56-C55) - (D56-D55)</f>
         <v>60</v>
       </c>
     </row>
@@ -2960,20 +2992,22 @@
       <c r="A57" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="B57" s="7"/>
+      <c r="B57" s="7">
+        <v>34821</v>
+      </c>
       <c r="C57" s="7">
         <v>35986</v>
       </c>
       <c r="D57" s="7">
         <v>35550</v>
       </c>
-      <c r="E57" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F57" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>-</v>
+      <c r="E57" s="3">
+        <f t="shared" si="0"/>
+        <v>1165</v>
+      </c>
+      <c r="F57" s="3">
+        <f t="shared" si="1"/>
+        <v>729</v>
       </c>
       <c r="G57">
         <f t="shared" si="2"/>
@@ -2984,20 +3018,22 @@
       <c r="A58" s="7" t="s">
         <v>224</v>
       </c>
-      <c r="B58" s="7"/>
+      <c r="B58" s="7">
+        <v>35636</v>
+      </c>
       <c r="C58" s="7">
         <v>36861</v>
       </c>
       <c r="D58" s="7">
         <v>36365</v>
       </c>
-      <c r="E58" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F58" s="3" t="str">
-        <f t="shared" ref="F58:F118" si="3">IF(D58&lt;&gt;"",IF(B58&lt;&gt;"",D58-B58,"-"), "-")</f>
-        <v>-</v>
+      <c r="E58" s="3">
+        <f t="shared" si="0"/>
+        <v>1225</v>
+      </c>
+      <c r="F58" s="3">
+        <f t="shared" ref="F58:F121" si="3">IF(D58&lt;&gt;"",IF(B58&lt;&gt;"",D58-B58,"-"), "-")</f>
+        <v>729</v>
       </c>
       <c r="G58">
         <f t="shared" si="2"/>
@@ -3008,20 +3044,22 @@
       <c r="A59" s="7" t="s">
         <v>225</v>
       </c>
-      <c r="B59" s="7"/>
+      <c r="B59" s="7">
+        <v>36237</v>
+      </c>
       <c r="C59" s="7">
         <v>37461</v>
       </c>
       <c r="D59" s="7">
         <v>36977</v>
       </c>
-      <c r="E59" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F59" s="3" t="str">
+      <c r="E59" s="3">
+        <f t="shared" si="0"/>
+        <v>1224</v>
+      </c>
+      <c r="F59" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>740</v>
       </c>
       <c r="G59">
         <f t="shared" si="2"/>
@@ -3032,20 +3070,22 @@
       <c r="A60" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B60" s="7"/>
+      <c r="B60" s="7">
+        <v>37327</v>
+      </c>
       <c r="C60" s="7">
         <v>38564</v>
       </c>
       <c r="D60" s="7">
         <v>38073</v>
       </c>
-      <c r="E60" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F60" s="3" t="str">
+      <c r="E60" s="3">
+        <f t="shared" si="0"/>
+        <v>1237</v>
+      </c>
+      <c r="F60" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>746</v>
       </c>
       <c r="G60">
         <f t="shared" si="2"/>
@@ -3056,20 +3096,22 @@
       <c r="A61" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="B61" s="7"/>
+      <c r="B61" s="7">
+        <v>37819</v>
+      </c>
       <c r="C61" s="7">
         <v>39057</v>
       </c>
       <c r="D61" s="7">
         <v>38571</v>
       </c>
-      <c r="E61" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F61" s="3" t="str">
+      <c r="E61" s="3">
+        <f t="shared" si="0"/>
+        <v>1238</v>
+      </c>
+      <c r="F61" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>752</v>
       </c>
       <c r="G61">
         <f t="shared" si="2"/>
@@ -3077,1029 +3119,1046 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="7" t="s">
+      <c r="A62" s="42" t="s">
+        <v>234</v>
+      </c>
+      <c r="B62" s="7">
+        <v>38071</v>
+      </c>
+      <c r="C62" s="7">
+        <v>39306</v>
+      </c>
+      <c r="D62" s="7"/>
+      <c r="E62" s="3">
+        <f t="shared" si="0"/>
+        <v>1235</v>
+      </c>
+      <c r="F62" s="3"/>
+    </row>
+    <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A63" s="42" t="s">
+        <v>233</v>
+      </c>
+      <c r="B63" s="7">
+        <v>38132</v>
+      </c>
+      <c r="C63" s="7">
+        <v>39350</v>
+      </c>
+      <c r="D63" s="7"/>
+      <c r="E63" s="3">
+        <f t="shared" si="0"/>
+        <v>1218</v>
+      </c>
+      <c r="F63" s="3"/>
+    </row>
+    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="42" t="s">
+        <v>150</v>
+      </c>
+      <c r="B64" s="7">
+        <v>38145</v>
+      </c>
+      <c r="C64" s="7">
+        <v>39398</v>
+      </c>
+      <c r="D64" s="7"/>
+      <c r="E64" s="3">
+        <f t="shared" si="0"/>
+        <v>1253</v>
+      </c>
+      <c r="F64" s="3"/>
+    </row>
+    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A65" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7">
+      <c r="B65" s="7">
+        <v>38527</v>
+      </c>
+      <c r="C65" s="7">
         <v>39781</v>
       </c>
-      <c r="D62" s="7">
+      <c r="D65" s="7">
         <v>39448</v>
       </c>
-      <c r="E62" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F62" s="3" t="str">
+      <c r="E65" s="3">
+        <f t="shared" si="0"/>
+        <v>1254</v>
+      </c>
+      <c r="F65" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G62">
-        <f t="shared" si="2"/>
+        <v>921</v>
+      </c>
+      <c r="G65">
+        <f>(C65-C61) - (D65-D61)</f>
         <v>-153</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="7" t="s">
+    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="B63" s="7"/>
-      <c r="C63" s="7">
+      <c r="B66" s="7">
+        <v>39151</v>
+      </c>
+      <c r="C66" s="7">
         <v>40405</v>
       </c>
-      <c r="D63" s="7">
+      <c r="D66" s="7">
         <v>40072</v>
       </c>
-      <c r="E63" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F63" s="3" t="str">
+      <c r="E66" s="3">
+        <f t="shared" si="0"/>
+        <v>1254</v>
+      </c>
+      <c r="F66" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G63">
+        <v>921</v>
+      </c>
+      <c r="G66">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="7" t="s">
+    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="B64" s="9"/>
-      <c r="C64" s="9">
+      <c r="B67" s="9">
+        <v>39334</v>
+      </c>
+      <c r="C67" s="9">
         <v>40588</v>
       </c>
-      <c r="D64" s="9">
+      <c r="D67" s="9">
         <v>40256</v>
       </c>
-      <c r="E64" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F64" s="3" t="str">
+      <c r="E67" s="3">
+        <f t="shared" si="0"/>
+        <v>1254</v>
+      </c>
+      <c r="F67" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G64">
+        <v>922</v>
+      </c>
+      <c r="G67">
         <f t="shared" si="2"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A65" s="7" t="s">
+    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="7" t="s">
         <v>230</v>
       </c>
-      <c r="B65" s="7"/>
-      <c r="C65" s="7">
+      <c r="B68" s="7">
+        <v>39973</v>
+      </c>
+      <c r="C68" s="7">
         <v>41228</v>
       </c>
-      <c r="D65" s="7">
+      <c r="D68" s="7">
         <v>40894</v>
       </c>
-      <c r="E65" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F65" s="3" t="str">
+      <c r="E68" s="3">
+        <f t="shared" si="0"/>
+        <v>1255</v>
+      </c>
+      <c r="F68" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G65">
+        <v>921</v>
+      </c>
+      <c r="G68">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A66" s="7" t="s">
+    <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="B66" s="9"/>
-      <c r="C66" s="9">
+      <c r="B69" s="9"/>
+      <c r="C69" s="9">
         <v>41865</v>
       </c>
-      <c r="D66" s="9">
+      <c r="D69" s="9">
         <v>41440</v>
       </c>
-      <c r="E66" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F66" s="3" t="str">
+      <c r="E69" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F69" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G66">
+      <c r="G69">
         <f t="shared" si="2"/>
         <v>91</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="7" t="s">
+    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A70" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B67" s="7"/>
-      <c r="C67" s="7">
+      <c r="B70" s="7"/>
+      <c r="C70" s="7">
         <v>42511</v>
       </c>
-      <c r="D67" s="7">
+      <c r="D70" s="7">
         <v>42085</v>
       </c>
-      <c r="E67" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F67" s="3" t="str">
+      <c r="E70" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F70" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G67">
+      <c r="G70">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A68" s="7" t="s">
+    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B68" s="7"/>
-      <c r="C68" s="7">
+      <c r="B71" s="7"/>
+      <c r="C71" s="7">
         <v>43110</v>
       </c>
-      <c r="D68" s="7">
+      <c r="D71" s="7">
         <v>42757</v>
       </c>
-      <c r="E68" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F68" s="3" t="str">
+      <c r="E71" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F71" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G68">
+      <c r="G71">
         <f t="shared" si="2"/>
         <v>-73</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
+    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B69" s="7"/>
-      <c r="C69" s="7">
+      <c r="B72" s="7"/>
+      <c r="C72" s="7">
         <v>43756</v>
       </c>
-      <c r="D69" s="7">
+      <c r="D72" s="7">
         <v>43402</v>
       </c>
-      <c r="E69" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F69" s="3" t="str">
+      <c r="E72" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>-</v>
+      </c>
+      <c r="F72" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G69">
-        <f t="shared" ref="G69:G102" si="4">(C69-C68) - (D69-D68)</f>
+      <c r="G72">
+        <f t="shared" ref="G72:G105" si="4">(C72-C71) - (D72-D71)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="5" t="s">
+    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A73" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B70" s="7"/>
-      <c r="C70" s="7">
+      <c r="B73" s="7"/>
+      <c r="C73" s="7">
         <v>44418</v>
       </c>
-      <c r="D70" s="7">
+      <c r="D73" s="7">
         <v>44061</v>
       </c>
-      <c r="E70" s="3" t="str">
-        <f t="shared" ref="E70:E133" si="5">IF(C70&lt;&gt;"",IF(B70&lt;&gt;"",C70-B70,"-"), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="F70" s="3" t="str">
+      <c r="E73" s="3" t="str">
+        <f t="shared" ref="E73:E136" si="5">IF(C73&lt;&gt;"",IF(B73&lt;&gt;"",C73-B73,"-"), "-")</f>
+        <v>-</v>
+      </c>
+      <c r="F73" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G70">
+      <c r="G73">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="5" t="s">
+    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A74" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B71" s="7"/>
-      <c r="C71" s="7">
+      <c r="B74" s="7"/>
+      <c r="C74" s="7">
         <v>45077</v>
       </c>
-      <c r="D71" s="7">
+      <c r="D74" s="7">
         <v>44720</v>
       </c>
-      <c r="E71" s="3" t="str">
+      <c r="E74" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F71" s="3" t="str">
+      <c r="F74" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G71">
+      <c r="G74">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="5" t="s">
+    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B72" s="7"/>
-      <c r="C72" s="7">
+      <c r="B75" s="7"/>
+      <c r="C75" s="7">
         <v>45719</v>
       </c>
-      <c r="D72" s="7">
+      <c r="D75" s="7">
         <v>45363</v>
       </c>
-      <c r="E72" s="3" t="str">
+      <c r="E75" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F72" s="3" t="str">
+      <c r="F75" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G72">
+      <c r="G75">
         <f t="shared" si="4"/>
         <v>-1</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B73" s="7"/>
-      <c r="C73" s="7">
+      <c r="B76" s="7"/>
+      <c r="C76" s="7">
         <v>46378</v>
       </c>
-      <c r="D73" s="7">
+      <c r="D76" s="7">
         <v>46022</v>
       </c>
-      <c r="E73" s="3" t="str">
+      <c r="E76" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F73" s="3" t="str">
+      <c r="F76" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G73">
+      <c r="G76">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A74" s="5" t="s">
+    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A77" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B74" s="7"/>
-      <c r="C74" s="7">
+      <c r="B77" s="7"/>
+      <c r="C77" s="7">
         <v>46984</v>
       </c>
-      <c r="D74" s="33">
+      <c r="D77" s="33">
         <v>46679</v>
       </c>
-      <c r="E74" s="3" t="str">
+      <c r="E77" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F74" s="3" t="str">
+      <c r="F77" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G74">
+      <c r="G77">
         <f t="shared" si="4"/>
         <v>-51</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A75" s="5" t="s">
+    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A78" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B75" s="7"/>
-      <c r="C75" s="7">
+      <c r="B78" s="7"/>
+      <c r="C78" s="7">
         <v>47629</v>
       </c>
-      <c r="D75" s="7">
+      <c r="D78" s="7">
         <v>47338</v>
       </c>
-      <c r="E75" s="3" t="str">
+      <c r="E78" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F75" s="3" t="str">
+      <c r="F78" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G75">
+      <c r="G78">
         <f t="shared" si="4"/>
         <v>-14</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A76" s="7" t="s">
+    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A79" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B76" s="7"/>
-      <c r="C76" s="7">
+      <c r="B79" s="7"/>
+      <c r="C79" s="7">
         <v>48410</v>
       </c>
-      <c r="D76" s="7">
+      <c r="D79" s="7">
         <v>48121</v>
       </c>
-      <c r="E76" s="3" t="str">
+      <c r="E79" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F76" s="3" t="str">
+      <c r="F79" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G76">
+      <c r="G79">
         <f t="shared" si="4"/>
         <v>-2</v>
       </c>
     </row>
-    <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A77" s="7" t="s">
+    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A80" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7">
+      <c r="B80" s="7"/>
+      <c r="C80" s="7">
         <v>48908</v>
       </c>
-      <c r="D77" s="7">
+      <c r="D80" s="7">
         <v>48619</v>
       </c>
-      <c r="E77" s="3" t="str">
+      <c r="E80" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F77" s="3" t="str">
+      <c r="F80" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G77">
+      <c r="G80">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A78" s="7" t="s">
+    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A81" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B78" s="7"/>
-      <c r="C78" s="7">
+      <c r="B81" s="7"/>
+      <c r="C81" s="7">
         <v>49856</v>
       </c>
-      <c r="D78" s="7">
+      <c r="D81" s="7">
         <v>49502</v>
       </c>
-      <c r="E78" s="3" t="str">
+      <c r="E81" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F78" s="3" t="str">
+      <c r="F81" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G78">
+      <c r="G81">
         <f t="shared" si="4"/>
         <v>65</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
+    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B79" s="7"/>
-      <c r="C79" s="7">
+      <c r="B82" s="7"/>
+      <c r="C82" s="7">
         <v>50516</v>
       </c>
-      <c r="D79" s="7">
+      <c r="D82" s="7">
         <v>50148</v>
       </c>
-      <c r="E79" s="3" t="str">
+      <c r="E82" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F79" s="3" t="str">
+      <c r="F82" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G79">
+      <c r="G82">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A80" s="5" t="s">
+    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B80" s="7"/>
-      <c r="C80" s="7">
+      <c r="B83" s="7"/>
+      <c r="C83" s="7">
         <v>50874</v>
       </c>
-      <c r="D80" s="7">
+      <c r="D83" s="7">
         <v>50417</v>
       </c>
-      <c r="E80" s="3" t="str">
+      <c r="E83" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F80" s="3" t="str">
+      <c r="F83" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G80">
+      <c r="G83">
         <f t="shared" si="4"/>
         <v>89</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="5" t="s">
+    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7">
+      <c r="B84" s="7"/>
+      <c r="C84" s="7">
         <v>51486</v>
       </c>
-      <c r="D81" s="7">
+      <c r="D84" s="7">
         <v>51016</v>
       </c>
-      <c r="E81" s="3" t="str">
+      <c r="E84" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F81" s="3" t="str">
+      <c r="F84" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G81">
+      <c r="G84">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7">
+      <c r="B85" s="7"/>
+      <c r="C85" s="7">
         <v>52507</v>
       </c>
-      <c r="D82" s="7">
+      <c r="D85" s="7">
         <v>52007</v>
       </c>
-      <c r="E82" s="3" t="str">
+      <c r="E85" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F82" s="3" t="str">
+      <c r="F85" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G82">
+      <c r="G85">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
+    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B83" s="7"/>
-      <c r="C83" s="7">
+      <c r="B86" s="7"/>
+      <c r="C86" s="7">
         <v>53153</v>
       </c>
-      <c r="D83" s="7">
+      <c r="D86" s="7">
         <v>52667</v>
       </c>
-      <c r="E83" s="3" t="str">
+      <c r="E86" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F83" s="3" t="str">
+      <c r="F86" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G83">
+      <c r="G86">
         <f t="shared" si="4"/>
         <v>-14</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
+    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B84" s="7"/>
-      <c r="C84" s="7">
+      <c r="B87" s="7"/>
+      <c r="C87" s="7">
         <v>53942</v>
       </c>
-      <c r="D84" s="7">
+      <c r="D87" s="7">
         <v>53473</v>
       </c>
-      <c r="E84" s="3" t="str">
+      <c r="E87" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F84" s="3" t="str">
+      <c r="F87" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G84">
+      <c r="G87">
         <f t="shared" si="4"/>
         <v>-17</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
+    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B85" s="7"/>
-      <c r="C85" s="7">
+      <c r="B88" s="7"/>
+      <c r="C88" s="7">
         <v>54564</v>
       </c>
-      <c r="D85" s="7">
+      <c r="D88" s="7">
         <v>54095</v>
       </c>
-      <c r="E85" s="3" t="str">
+      <c r="E88" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F85" s="3" t="str">
+      <c r="F88" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G85">
+      <c r="G88">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
+    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B86" s="7"/>
-      <c r="C86" s="7">
+      <c r="B89" s="7"/>
+      <c r="C89" s="7">
         <v>55596</v>
       </c>
-      <c r="D86" s="7">
+      <c r="D89" s="7">
         <v>55108</v>
       </c>
-      <c r="E86" s="3" t="str">
+      <c r="E89" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F86" s="3" t="str">
+      <c r="F89" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G86">
+      <c r="G89">
         <f t="shared" si="4"/>
         <v>19</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
+    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A90" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B87" s="7"/>
-      <c r="C87" s="7">
+      <c r="B90" s="7"/>
+      <c r="C90" s="7">
         <v>56185</v>
       </c>
-      <c r="D87" s="7">
+      <c r="D90" s="7">
         <v>55708</v>
       </c>
-      <c r="E87" s="3" t="str">
+      <c r="E90" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F87" s="3" t="str">
+      <c r="F90" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G87">
+      <c r="G90">
         <f t="shared" si="4"/>
         <v>-11</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
+    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B88" s="7"/>
-      <c r="C88" s="7">
+      <c r="B91" s="7"/>
+      <c r="C91" s="7">
         <v>56572</v>
       </c>
-      <c r="D88" s="7">
+      <c r="D91" s="7">
         <v>56104</v>
       </c>
-      <c r="E88" s="3" t="str">
+      <c r="E91" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F88" s="3" t="str">
+      <c r="F91" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G88">
+      <c r="G91">
         <f t="shared" si="4"/>
         <v>-9</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
+    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B89" s="7"/>
-      <c r="C89" s="7">
+      <c r="B92" s="7"/>
+      <c r="C92" s="7">
         <v>57217</v>
       </c>
-      <c r="D89" s="7">
+      <c r="D92" s="7">
         <v>56749</v>
       </c>
-      <c r="E89" s="3" t="str">
+      <c r="E92" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F89" s="3" t="str">
+      <c r="F92" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G89">
+      <c r="G92">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A90" s="5" t="s">
+    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B90" s="7"/>
-      <c r="C90" s="7">
+      <c r="B93" s="7"/>
+      <c r="C93" s="7">
         <v>58008</v>
       </c>
-      <c r="D90" s="7">
+      <c r="D93" s="7">
         <v>57450</v>
       </c>
-      <c r="E90" s="3" t="str">
+      <c r="E93" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F90" s="3" t="str">
+      <c r="F93" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G90">
+      <c r="G93">
         <f t="shared" si="4"/>
         <v>90</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
+    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A94" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7">
+      <c r="B94" s="7"/>
+      <c r="C94" s="7">
         <v>58608</v>
       </c>
-      <c r="D91" s="7">
+      <c r="D94" s="7">
         <v>58050</v>
       </c>
-      <c r="E91" s="3" t="str">
+      <c r="E94" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F91" s="3" t="str">
+      <c r="F94" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G91">
+      <c r="G94">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
+    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B92" s="7"/>
-      <c r="C92" s="7">
+      <c r="B95" s="7"/>
+      <c r="C95" s="7">
         <v>59190</v>
       </c>
-      <c r="D92" s="7">
+      <c r="D95" s="7">
         <v>58612</v>
       </c>
-      <c r="E92" s="3" t="str">
+      <c r="E95" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F92" s="3" t="str">
+      <c r="F95" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G92">
+      <c r="G95">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
+    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B93" s="7"/>
-      <c r="C93" s="7">
+      <c r="B96" s="7"/>
+      <c r="C96" s="7">
         <v>59825</v>
       </c>
-      <c r="D93" s="7">
+      <c r="D96" s="7">
         <v>59247</v>
       </c>
-      <c r="E93" s="3" t="str">
+      <c r="E96" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F93" s="3" t="str">
+      <c r="F96" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G93">
+      <c r="G96">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A94" s="5" t="s">
+    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B94" s="7"/>
-      <c r="C94" s="7">
+      <c r="B97" s="7"/>
+      <c r="C97" s="7">
         <v>60441</v>
       </c>
-      <c r="D94" s="7">
+      <c r="D97" s="7">
         <v>59838</v>
       </c>
-      <c r="E94" s="3" t="str">
+      <c r="E97" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F94" s="3" t="str">
+      <c r="F97" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G94">
+      <c r="G97">
         <f t="shared" si="4"/>
         <v>25</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
+    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B95" s="7"/>
-      <c r="C95" s="7">
+      <c r="B98" s="7"/>
+      <c r="C98" s="7">
         <v>61093</v>
       </c>
-      <c r="D95" s="7">
+      <c r="D98" s="7">
         <v>60490</v>
       </c>
-      <c r="E95" s="3" t="str">
+      <c r="E98" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F95" s="3" t="str">
+      <c r="F98" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G95">
+      <c r="G98">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
+    <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B96" s="10"/>
-      <c r="C96" s="10">
+      <c r="B99" s="10"/>
+      <c r="C99" s="10">
         <v>61914</v>
       </c>
-      <c r="D96" s="10">
+      <c r="D99" s="10">
         <v>61295</v>
       </c>
-      <c r="E96" s="3" t="str">
+      <c r="E99" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F96" s="3" t="str">
+      <c r="F99" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G96">
+      <c r="G99">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
+    <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B97" s="7"/>
-      <c r="C97" s="7">
+      <c r="B100" s="7"/>
+      <c r="C100" s="7">
         <v>62575</v>
       </c>
-      <c r="D97" s="7">
+      <c r="D100" s="7">
         <v>61940</v>
       </c>
-      <c r="E97" s="3" t="str">
+      <c r="E100" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F97" s="3" t="str">
+      <c r="F100" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G97">
+      <c r="G100">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
     </row>
-    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
+    <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B98" s="7"/>
-      <c r="C98" s="7">
+      <c r="B101" s="7"/>
+      <c r="C101" s="7">
         <v>63180</v>
       </c>
-      <c r="D98" s="7">
+      <c r="D101" s="7">
         <v>62513</v>
       </c>
-      <c r="E98" s="3" t="str">
+      <c r="E101" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F98" s="3" t="str">
+      <c r="F101" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G98">
+      <c r="G101">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
+    <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B99" s="7"/>
-      <c r="C99" s="7">
+      <c r="B102" s="7"/>
+      <c r="C102" s="7">
         <v>63825</v>
       </c>
-      <c r="D99" s="7">
+      <c r="D102" s="7">
         <v>63172</v>
       </c>
-      <c r="E99" s="3" t="str">
+      <c r="E102" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F99" s="3" t="str">
+      <c r="F102" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G99">
+      <c r="G102">
         <f t="shared" si="4"/>
         <v>-14</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
+    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B100" s="7"/>
-      <c r="C100" s="7">
+      <c r="B103" s="7"/>
+      <c r="C103" s="7">
         <v>64581</v>
       </c>
-      <c r="D100" s="7">
+      <c r="D103" s="7">
         <v>63896</v>
       </c>
-      <c r="E100" s="3" t="str">
+      <c r="E103" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F100" s="3" t="str">
+      <c r="F103" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G100">
+      <c r="G103">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
+    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B101" s="7"/>
-      <c r="C101" s="7">
+      <c r="B104" s="7"/>
+      <c r="C104" s="7">
         <v>65231</v>
       </c>
-      <c r="D101" s="7">
+      <c r="D104" s="7">
         <v>64541</v>
       </c>
-      <c r="E101" s="3" t="str">
+      <c r="E104" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F101" s="3" t="str">
+      <c r="F104" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G101">
+      <c r="G104">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
+    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B102" s="7"/>
-      <c r="C102" s="7">
+      <c r="B105" s="7"/>
+      <c r="C105" s="7">
         <v>65820</v>
       </c>
-      <c r="D102" s="7">
+      <c r="D105" s="7">
         <v>65084</v>
       </c>
-      <c r="E102" s="3" t="str">
+      <c r="E105" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F102" s="3" t="str">
+      <c r="F105" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G102">
+      <c r="G105">
         <f t="shared" si="4"/>
         <v>46</v>
-      </c>
-    </row>
-    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A103" s="7"/>
-      <c r="B103" s="7"/>
-      <c r="C103" s="7"/>
-      <c r="D103" s="7"/>
-      <c r="E103" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F103" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="7"/>
-      <c r="B104" s="7"/>
-      <c r="C104" s="7"/>
-      <c r="D104" s="7"/>
-      <c r="E104" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F104" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="7"/>
-      <c r="B105" s="7"/>
-      <c r="C105" s="7"/>
-      <c r="D105" s="7"/>
-      <c r="E105" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F105" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -4294,7 +4353,7 @@
         <v>-</v>
       </c>
       <c r="F119" s="3" t="str">
-        <f t="shared" ref="F119:F122" si="6">IF(D119&lt;&gt;"",IF(B119&lt;&gt;"",D119-B119,"-"), "-")</f>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -4308,7 +4367,7 @@
         <v>-</v>
       </c>
       <c r="F120" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -4322,7 +4381,7 @@
         <v>-</v>
       </c>
       <c r="F121" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -4336,7 +4395,7 @@
         <v>-</v>
       </c>
       <c r="F122" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="F122:F125" si="6">IF(D122&lt;&gt;"",IF(B122&lt;&gt;"",D122-B122,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -4349,6 +4408,10 @@
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
+      <c r="F123" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="124" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A124" s="7"/>
@@ -4359,6 +4422,10 @@
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
+      <c r="F124" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="125" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A125" s="7"/>
@@ -4369,6 +4436,10 @@
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
+      <c r="F125" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="126" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A126" s="7"/>
@@ -4456,7 +4527,7 @@
       <c r="C134" s="7"/>
       <c r="D134" s="7"/>
       <c r="E134" s="3" t="str">
-        <f t="shared" ref="E134:E138" si="7">IF(C134&lt;&gt;"",IF(B134&lt;&gt;"",C134-B134,"-"), "-")</f>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -4466,7 +4537,7 @@
       <c r="C135" s="7"/>
       <c r="D135" s="7"/>
       <c r="E135" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -4476,7 +4547,7 @@
       <c r="C136" s="7"/>
       <c r="D136" s="7"/>
       <c r="E136" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -4486,7 +4557,7 @@
       <c r="C137" s="7"/>
       <c r="D137" s="7"/>
       <c r="E137" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="E137:E141" si="7">IF(C137&lt;&gt;"",IF(B137&lt;&gt;"",C137-B137,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -4506,7 +4577,7 @@
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
       <c r="E139" s="3" t="str">
-        <f t="shared" ref="E139:E140" si="8">IF(C139&lt;&gt;"",IF(B139&lt;&gt;"",B139-C139,"-"), "-")</f>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
     </row>
@@ -4516,7 +4587,7 @@
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
       <c r="E140" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
     </row>
@@ -4525,99 +4596,114 @@
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
       <c r="D141" s="7"/>
+      <c r="E141" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="142" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
+      <c r="E142" s="3" t="str">
+        <f t="shared" ref="E142:E143" si="8">IF(C142&lt;&gt;"",IF(B142&lt;&gt;"",B142-C142,"-"), "-")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="143" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
+      <c r="E143" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="144" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
     </row>
-    <row r="145" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
     </row>
-    <row r="146" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
     </row>
-    <row r="147" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
     </row>
-    <row r="148" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
     </row>
-    <row r="149" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
     </row>
-    <row r="150" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
     </row>
-    <row r="151" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
     </row>
-    <row r="152" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
     </row>
-    <row r="153" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
     </row>
-    <row r="154" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
     </row>
-    <row r="157" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
     </row>
-    <row r="158" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
     </row>
-    <row r="159" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
     </row>
-    <row r="160" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
@@ -5216,6 +5302,21 @@
       <c r="B279" s="7"/>
       <c r="C279" s="7"/>
       <c r="D279" s="7"/>
+    </row>
+    <row r="280" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B280" s="7"/>
+      <c r="C280" s="7"/>
+      <c r="D280" s="7"/>
+    </row>
+    <row r="281" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B281" s="7"/>
+      <c r="C281" s="7"/>
+      <c r="D281" s="7"/>
+    </row>
+    <row r="282" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B282" s="7"/>
+      <c r="C282" s="7"/>
+      <c r="D282" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11268,7 +11369,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="14" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
lode runner v5 - up to level 36, 1396 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF52CCF-4780-436F-A780-EB80680CD522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4606D60-AF2F-494D-9B72-3C395DA603E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45525" yWindow="1620" windowWidth="9060" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1525,8 +1525,8 @@
   <dimension ref="A1:H282"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B69" sqref="B69"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3277,20 +3277,22 @@
       <c r="A69" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="B69" s="9"/>
+      <c r="B69" s="9">
+        <v>40494</v>
+      </c>
       <c r="C69" s="9">
         <v>41865</v>
       </c>
       <c r="D69" s="9">
         <v>41440</v>
       </c>
-      <c r="E69" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F69" s="3" t="str">
+      <c r="E69" s="3">
+        <f t="shared" si="0"/>
+        <v>1371</v>
+      </c>
+      <c r="F69" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>946</v>
       </c>
       <c r="G69">
         <f t="shared" si="2"/>
@@ -3301,68 +3303,74 @@
       <c r="A70" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B70" s="7"/>
+      <c r="B70" s="7">
+        <v>41139</v>
+      </c>
       <c r="C70" s="7">
-        <v>42511</v>
+        <v>42512</v>
       </c>
       <c r="D70" s="7">
         <v>42085</v>
       </c>
-      <c r="E70" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F70" s="3" t="str">
+      <c r="E70" s="3">
+        <f t="shared" si="0"/>
+        <v>1373</v>
+      </c>
+      <c r="F70" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>946</v>
       </c>
       <c r="G70">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B71" s="7"/>
+      <c r="B71" s="7">
+        <v>41742</v>
+      </c>
       <c r="C71" s="7">
         <v>43110</v>
       </c>
       <c r="D71" s="7">
         <v>42757</v>
       </c>
-      <c r="E71" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F71" s="3" t="str">
+      <c r="E71" s="3">
+        <f t="shared" si="0"/>
+        <v>1368</v>
+      </c>
+      <c r="F71" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>1015</v>
       </c>
       <c r="G71">
         <f t="shared" si="2"/>
-        <v>-73</v>
+        <v>-74</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B72" s="7"/>
+      <c r="B72" s="7">
+        <v>42387</v>
+      </c>
       <c r="C72" s="7">
         <v>43756</v>
       </c>
       <c r="D72" s="7">
         <v>43402</v>
       </c>
-      <c r="E72" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>-</v>
-      </c>
-      <c r="F72" s="3" t="str">
+      <c r="E72" s="3">
+        <f t="shared" si="0"/>
+        <v>1369</v>
+      </c>
+      <c r="F72" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>1015</v>
       </c>
       <c r="G72">
         <f t="shared" ref="G72:G105" si="4">(C72-C71) - (D72-D71)</f>
@@ -3373,20 +3381,22 @@
       <c r="A73" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B73" s="7"/>
+      <c r="B73" s="7">
+        <v>43033</v>
+      </c>
       <c r="C73" s="7">
         <v>44418</v>
       </c>
       <c r="D73" s="7">
         <v>44061</v>
       </c>
-      <c r="E73" s="3" t="str">
+      <c r="E73" s="3">
         <f t="shared" ref="E73:E136" si="5">IF(C73&lt;&gt;"",IF(B73&lt;&gt;"",C73-B73,"-"), "-")</f>
-        <v>-</v>
-      </c>
-      <c r="F73" s="3" t="str">
+        <v>1385</v>
+      </c>
+      <c r="F73" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>1028</v>
       </c>
       <c r="G73">
         <f t="shared" si="4"/>
@@ -3397,72 +3407,78 @@
       <c r="A74" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B74" s="7"/>
+      <c r="B74" s="7">
+        <v>43693</v>
+      </c>
       <c r="C74" s="7">
-        <v>45077</v>
+        <v>45078</v>
       </c>
       <c r="D74" s="7">
         <v>44720</v>
       </c>
-      <c r="E74" s="3" t="str">
+      <c r="E74" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F74" s="3" t="str">
+        <v>1385</v>
+      </c>
+      <c r="F74" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>1027</v>
       </c>
       <c r="G74">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B75" s="7"/>
+      <c r="B75" s="7">
+        <v>44329</v>
+      </c>
       <c r="C75" s="7">
         <v>45719</v>
       </c>
       <c r="D75" s="7">
         <v>45363</v>
       </c>
-      <c r="E75" s="3" t="str">
+      <c r="E75" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F75" s="3" t="str">
+        <v>1390</v>
+      </c>
+      <c r="F75" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>1034</v>
       </c>
       <c r="G75">
         <f t="shared" si="4"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B76" s="7"/>
+      <c r="B76" s="7">
+        <v>44988</v>
+      </c>
       <c r="C76" s="7">
-        <v>46378</v>
+        <v>46384</v>
       </c>
       <c r="D76" s="7">
         <v>46022</v>
       </c>
-      <c r="E76" s="3" t="str">
+      <c r="E76" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F76" s="3" t="str">
+        <v>1396</v>
+      </c>
+      <c r="F76" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>1034</v>
       </c>
       <c r="G76">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -3486,7 +3502,7 @@
       </c>
       <c r="G77">
         <f t="shared" si="4"/>
-        <v>-51</v>
+        <v>-57</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
lode runner v5 - up to level 47, 1866 frames ahead
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4606D60-AF2F-494D-9B72-3C395DA603E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FC09B1-944D-4AB8-9765-7676B842225C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45525" yWindow="1620" windowWidth="9060" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="46455" yWindow="360" windowWidth="10905" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V5" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="238">
   <si>
     <t>Place</t>
   </si>
@@ -739,6 +739,15 @@
   </si>
   <si>
     <t>walk</t>
+  </si>
+  <si>
+    <t>gold 3</t>
+  </si>
+  <si>
+    <t>gold -1</t>
+  </si>
+  <si>
+    <t>move</t>
   </si>
 </sst>
 </file>
@@ -748,12 +757,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1087,118 +1103,119 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1522,11 +1539,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B3565E-C480-4A10-8524-B7BC06C9B703}">
-  <dimension ref="A1:H282"/>
+  <dimension ref="A1:H285"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B77" sqref="B77"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3032,7 +3049,7 @@
         <v>1225</v>
       </c>
       <c r="F58" s="3">
-        <f t="shared" ref="F58:F121" si="3">IF(D58&lt;&gt;"",IF(B58&lt;&gt;"",D58-B58,"-"), "-")</f>
+        <f t="shared" ref="F58:F124" si="3">IF(D58&lt;&gt;"",IF(B58&lt;&gt;"",D58-B58,"-"), "-")</f>
         <v>729</v>
       </c>
       <c r="G58">
@@ -3119,7 +3136,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="42" t="s">
+      <c r="A62" s="34" t="s">
         <v>234</v>
       </c>
       <c r="B62" s="7">
@@ -3136,7 +3153,7 @@
       <c r="F62" s="3"/>
     </row>
     <row r="63" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A63" s="42" t="s">
+      <c r="A63" s="34" t="s">
         <v>233</v>
       </c>
       <c r="B63" s="7">
@@ -3153,7 +3170,7 @@
       <c r="F63" s="3"/>
     </row>
     <row r="64" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A64" s="42" t="s">
+      <c r="A64" s="34" t="s">
         <v>150</v>
       </c>
       <c r="B64" s="7">
@@ -3373,7 +3390,7 @@
         <v>1015</v>
       </c>
       <c r="G72">
-        <f t="shared" ref="G72:G105" si="4">(C72-C71) - (D72-D71)</f>
+        <f t="shared" ref="G72:G108" si="4">(C72-C71) - (D72-D71)</f>
         <v>1</v>
       </c>
     </row>
@@ -3391,7 +3408,7 @@
         <v>44061</v>
       </c>
       <c r="E73" s="3">
-        <f t="shared" ref="E73:E136" si="5">IF(C73&lt;&gt;"",IF(B73&lt;&gt;"",C73-B73,"-"), "-")</f>
+        <f t="shared" ref="E73:E139" si="5">IF(C73&lt;&gt;"",IF(B73&lt;&gt;"",C73-B73,"-"), "-")</f>
         <v>1385</v>
       </c>
       <c r="F73" s="3">
@@ -3485,20 +3502,22 @@
       <c r="A77" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B77" s="7"/>
+      <c r="B77" s="7">
+        <v>45587</v>
+      </c>
       <c r="C77" s="7">
         <v>46984</v>
       </c>
       <c r="D77" s="33">
         <v>46679</v>
       </c>
-      <c r="E77" s="3" t="str">
+      <c r="E77" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F77" s="3" t="str">
+        <v>1397</v>
+      </c>
+      <c r="F77" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>1092</v>
       </c>
       <c r="G77">
         <f t="shared" si="4"/>
@@ -3509,20 +3528,22 @@
       <c r="A78" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B78" s="7"/>
+      <c r="B78" s="7">
+        <v>46248</v>
+      </c>
       <c r="C78" s="7">
         <v>47629</v>
       </c>
       <c r="D78" s="7">
         <v>47338</v>
       </c>
-      <c r="E78" s="3" t="str">
+      <c r="E78" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F78" s="3" t="str">
+        <v>1381</v>
+      </c>
+      <c r="F78" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>1090</v>
       </c>
       <c r="G78">
         <f t="shared" si="4"/>
@@ -3533,20 +3554,22 @@
       <c r="A79" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B79" s="7"/>
+      <c r="B79" s="7">
+        <v>47029</v>
+      </c>
       <c r="C79" s="7">
         <v>48410</v>
       </c>
       <c r="D79" s="7">
         <v>48121</v>
       </c>
-      <c r="E79" s="3" t="str">
+      <c r="E79" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F79" s="3" t="str">
+        <v>1381</v>
+      </c>
+      <c r="F79" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>1092</v>
       </c>
       <c r="G79">
         <f t="shared" si="4"/>
@@ -3557,20 +3580,22 @@
       <c r="A80" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B80" s="7"/>
+      <c r="B80" s="7">
+        <v>47527</v>
+      </c>
       <c r="C80" s="7">
         <v>48908</v>
       </c>
       <c r="D80" s="7">
         <v>48619</v>
       </c>
-      <c r="E80" s="3" t="str">
+      <c r="E80" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F80" s="3" t="str">
+        <v>1381</v>
+      </c>
+      <c r="F80" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>1092</v>
       </c>
       <c r="G80">
         <f t="shared" si="4"/>
@@ -3578,645 +3603,690 @@
       </c>
     </row>
     <row r="81" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="34" t="s">
+        <v>235</v>
+      </c>
+      <c r="B81" s="7">
+        <v>48010</v>
+      </c>
+      <c r="C81" s="7">
+        <v>48019</v>
+      </c>
+      <c r="D81" s="7"/>
+      <c r="E81" s="3">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="F81" s="3"/>
+    </row>
+    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A82" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B81" s="7"/>
-      <c r="C81" s="7">
+      <c r="B82" s="7">
+        <v>48393</v>
+      </c>
+      <c r="C82" s="7">
         <v>49856</v>
       </c>
-      <c r="D81" s="7">
+      <c r="D82" s="7">
         <v>49502</v>
       </c>
-      <c r="E81" s="3" t="str">
+      <c r="E82" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F81" s="3" t="str">
+        <v>1463</v>
+      </c>
+      <c r="F82" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G81">
-        <f t="shared" si="4"/>
+        <v>1109</v>
+      </c>
+      <c r="G82">
+        <f>(C82-C80) - (D82-D80)</f>
         <v>65</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A82" s="5" t="s">
+    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A83" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B82" s="7"/>
-      <c r="C82" s="7">
+      <c r="B83" s="7">
+        <v>49053</v>
+      </c>
+      <c r="C83" s="7">
         <v>50516</v>
       </c>
-      <c r="D82" s="7">
+      <c r="D83" s="7">
         <v>50148</v>
       </c>
-      <c r="E82" s="3" t="str">
+      <c r="E83" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F82" s="3" t="str">
+        <v>1463</v>
+      </c>
+      <c r="F83" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G82">
+        <v>1095</v>
+      </c>
+      <c r="G83">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A83" s="5" t="s">
+    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A84" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B83" s="7"/>
-      <c r="C83" s="7">
+      <c r="B84" s="7">
+        <v>49311</v>
+      </c>
+      <c r="C84" s="7">
         <v>50874</v>
       </c>
-      <c r="D83" s="7">
+      <c r="D84" s="7">
         <v>50417</v>
       </c>
-      <c r="E83" s="3" t="str">
+      <c r="E84" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F83" s="3" t="str">
+        <v>1563</v>
+      </c>
+      <c r="F84" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G83">
+        <v>1106</v>
+      </c>
+      <c r="G84">
         <f t="shared" si="4"/>
         <v>89</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A84" s="5" t="s">
+    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B84" s="7"/>
-      <c r="C84" s="7">
+      <c r="B85" s="7">
+        <v>49911</v>
+      </c>
+      <c r="C85" s="7">
         <v>51486</v>
       </c>
-      <c r="D84" s="7">
+      <c r="D85" s="7">
         <v>51016</v>
       </c>
-      <c r="E84" s="3" t="str">
+      <c r="E85" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F84" s="3" t="str">
+        <v>1575</v>
+      </c>
+      <c r="F85" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G84">
+        <v>1105</v>
+      </c>
+      <c r="G85">
         <f t="shared" si="4"/>
         <v>13</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A85" s="5" t="s">
+    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B85" s="7"/>
-      <c r="C85" s="7">
+      <c r="B86" s="7">
+        <v>50889</v>
+      </c>
+      <c r="C86" s="7">
         <v>52507</v>
       </c>
-      <c r="D85" s="7">
+      <c r="D86" s="7">
         <v>52007</v>
       </c>
-      <c r="E85" s="3" t="str">
+      <c r="E86" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F85" s="3" t="str">
+        <v>1618</v>
+      </c>
+      <c r="F86" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G85">
+        <v>1118</v>
+      </c>
+      <c r="G86">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A86" s="5" t="s">
+    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B86" s="7"/>
-      <c r="C86" s="7">
+      <c r="B87" s="7">
+        <v>51535</v>
+      </c>
+      <c r="C87" s="7">
         <v>53153</v>
       </c>
-      <c r="D86" s="7">
+      <c r="D87" s="7">
         <v>52667</v>
       </c>
-      <c r="E86" s="3" t="str">
+      <c r="E87" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F86" s="3" t="str">
+        <v>1618</v>
+      </c>
+      <c r="F87" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G86">
+        <v>1132</v>
+      </c>
+      <c r="G87">
         <f t="shared" si="4"/>
         <v>-14</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A87" s="5" t="s">
+    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B87" s="7"/>
-      <c r="C87" s="7">
+      <c r="B88" s="7">
+        <v>52312</v>
+      </c>
+      <c r="C88" s="7">
         <v>53942</v>
       </c>
-      <c r="D87" s="7">
+      <c r="D88" s="7">
         <v>53473</v>
       </c>
-      <c r="E87" s="3" t="str">
+      <c r="E88" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F87" s="3" t="str">
+        <v>1630</v>
+      </c>
+      <c r="F88" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G87">
+        <v>1161</v>
+      </c>
+      <c r="G88">
         <f t="shared" si="4"/>
         <v>-17</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A88" s="5" t="s">
+    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A89" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B88" s="7"/>
-      <c r="C88" s="7">
+      <c r="B89" s="7">
+        <v>52934</v>
+      </c>
+      <c r="C89" s="7">
         <v>54564</v>
       </c>
-      <c r="D88" s="7">
+      <c r="D89" s="7">
         <v>54095</v>
       </c>
-      <c r="E88" s="3" t="str">
+      <c r="E89" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F88" s="3" t="str">
+        <v>1630</v>
+      </c>
+      <c r="F89" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G88">
+        <v>1161</v>
+      </c>
+      <c r="G89">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A89" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B89" s="7"/>
-      <c r="C89" s="7">
-        <v>55596</v>
-      </c>
-      <c r="D89" s="7">
-        <v>55108</v>
-      </c>
-      <c r="E89" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F89" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G89">
-        <f t="shared" si="4"/>
-        <v>19</v>
-      </c>
-    </row>
     <row r="90" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B90" s="7">
+        <v>53936</v>
+      </c>
+      <c r="C90" s="7">
+        <v>55596</v>
+      </c>
+      <c r="D90" s="7">
+        <v>55108</v>
+      </c>
+      <c r="E90" s="3">
+        <f t="shared" si="5"/>
+        <v>1660</v>
+      </c>
+      <c r="F90" s="3">
+        <f t="shared" si="3"/>
+        <v>1172</v>
+      </c>
+      <c r="G90">
+        <f>(C90-C89) - (D90-D89)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A91" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B90" s="7"/>
-      <c r="C90" s="7">
+      <c r="B91" s="7">
+        <v>54526</v>
+      </c>
+      <c r="C91" s="7">
         <v>56185</v>
       </c>
-      <c r="D90" s="7">
+      <c r="D91" s="7">
         <v>55708</v>
       </c>
-      <c r="E90" s="3" t="str">
+      <c r="E91" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F90" s="3" t="str">
+        <v>1659</v>
+      </c>
+      <c r="F91" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G90">
+        <v>1182</v>
+      </c>
+      <c r="G91">
         <f t="shared" si="4"/>
         <v>-11</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A91" s="5" t="s">
+    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A92" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B91" s="7"/>
-      <c r="C91" s="7">
+      <c r="B92" s="7">
+        <v>54878</v>
+      </c>
+      <c r="C92" s="7">
         <v>56572</v>
       </c>
-      <c r="D91" s="7">
+      <c r="D92" s="7">
         <v>56104</v>
       </c>
-      <c r="E91" s="3" t="str">
+      <c r="E92" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F91" s="3" t="str">
+        <v>1694</v>
+      </c>
+      <c r="F92" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G91">
+        <v>1226</v>
+      </c>
+      <c r="G92">
         <f t="shared" si="4"/>
         <v>-9</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A92" s="5" t="s">
+    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A93" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B92" s="7"/>
-      <c r="C92" s="7">
+      <c r="B93" s="7">
+        <v>55524</v>
+      </c>
+      <c r="C93" s="7">
         <v>57217</v>
       </c>
-      <c r="D92" s="7">
+      <c r="D93" s="7">
         <v>56749</v>
       </c>
-      <c r="E92" s="3" t="str">
+      <c r="E93" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F92" s="3" t="str">
+        <v>1693</v>
+      </c>
+      <c r="F93" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G92">
+        <v>1225</v>
+      </c>
+      <c r="G93">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A93" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B93" s="7"/>
-      <c r="C93" s="7">
-        <v>58008</v>
-      </c>
-      <c r="D93" s="7">
-        <v>57450</v>
-      </c>
-      <c r="E93" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F93" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G93">
-        <f t="shared" si="4"/>
-        <v>90</v>
-      </c>
-    </row>
     <row r="94" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A94" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B94" s="7">
+        <v>56204</v>
+      </c>
+      <c r="C94" s="7">
+        <v>58008</v>
+      </c>
+      <c r="D94" s="7">
+        <v>57450</v>
+      </c>
+      <c r="E94" s="3">
+        <f t="shared" si="5"/>
+        <v>1804</v>
+      </c>
+      <c r="F94" s="3">
+        <f t="shared" si="3"/>
+        <v>1246</v>
+      </c>
+      <c r="G94">
+        <f>(C94-C93) - (D94-D93)</f>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A95" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B94" s="7"/>
-      <c r="C94" s="7">
+      <c r="B95" s="7">
+        <v>56804</v>
+      </c>
+      <c r="C95" s="7">
         <v>58608</v>
       </c>
-      <c r="D94" s="7">
+      <c r="D95" s="7">
         <v>58050</v>
       </c>
-      <c r="E94" s="3" t="str">
+      <c r="E95" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F94" s="3" t="str">
+        <v>1804</v>
+      </c>
+      <c r="F95" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G94">
+        <v>1246</v>
+      </c>
+      <c r="G95">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A95" s="5" t="s">
+    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A96" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B95" s="7"/>
-      <c r="C95" s="7">
+      <c r="B96" s="7">
+        <v>57359</v>
+      </c>
+      <c r="C96" s="7">
         <v>59190</v>
       </c>
-      <c r="D95" s="7">
+      <c r="D96" s="7">
         <v>58612</v>
       </c>
-      <c r="E95" s="3" t="str">
+      <c r="E96" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F95" s="3" t="str">
+        <v>1831</v>
+      </c>
+      <c r="F96" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G95">
+        <v>1253</v>
+      </c>
+      <c r="G96">
         <f t="shared" si="4"/>
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A96" s="5" t="s">
+    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A97" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B96" s="7"/>
-      <c r="C96" s="7">
-        <v>59825</v>
-      </c>
-      <c r="D96" s="7">
+      <c r="B97" s="7">
+        <v>57995</v>
+      </c>
+      <c r="C97" s="7">
+        <v>59828</v>
+      </c>
+      <c r="D97" s="7">
         <v>59247</v>
       </c>
-      <c r="E96" s="3" t="str">
+      <c r="E97" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F96" s="3" t="str">
+        <v>1833</v>
+      </c>
+      <c r="F97" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G96">
+        <v>1252</v>
+      </c>
+      <c r="G97">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A98" s="43" t="s">
+        <v>236</v>
+      </c>
+      <c r="B98" s="7">
+        <v>58416</v>
+      </c>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7">
+        <v>59676</v>
+      </c>
+      <c r="E98" s="3"/>
+      <c r="F98" s="3">
+        <f t="shared" si="3"/>
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A99" s="43" t="s">
+        <v>237</v>
+      </c>
+      <c r="B99" s="7">
+        <v>58443</v>
+      </c>
+      <c r="C99" s="7"/>
+      <c r="D99" s="7">
+        <v>59702</v>
+      </c>
+      <c r="E99" s="3"/>
+      <c r="F99" s="3">
+        <f t="shared" si="3"/>
+        <v>1259</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A100" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B100" s="7">
+        <v>58575</v>
+      </c>
+      <c r="C100" s="7">
+        <v>60441</v>
+      </c>
+      <c r="D100" s="7">
+        <v>59838</v>
+      </c>
+      <c r="E100" s="3">
+        <f t="shared" si="5"/>
+        <v>1866</v>
+      </c>
+      <c r="F100" s="3">
+        <f t="shared" si="3"/>
+        <v>1263</v>
+      </c>
+      <c r="G100">
+        <f>(C100-C97) - (D100-D97)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A101" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B101" s="7">
+        <v>59227</v>
+      </c>
+      <c r="C101" s="7">
+        <v>61093</v>
+      </c>
+      <c r="D101" s="7">
+        <v>60490</v>
+      </c>
+      <c r="E101" s="3">
+        <f t="shared" si="5"/>
+        <v>1866</v>
+      </c>
+      <c r="F101" s="3">
+        <f t="shared" si="3"/>
+        <v>1263</v>
+      </c>
+      <c r="G101">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A97" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B97" s="7"/>
-      <c r="C97" s="7">
-        <v>60441</v>
-      </c>
-      <c r="D97" s="7">
-        <v>59838</v>
-      </c>
-      <c r="E97" s="3" t="str">
+    <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A102" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B102" s="10"/>
+      <c r="C102" s="10">
+        <v>61914</v>
+      </c>
+      <c r="D102" s="10">
+        <v>61295</v>
+      </c>
+      <c r="E102" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F97" s="3" t="str">
+      <c r="F102" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G97">
-        <f t="shared" si="4"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B98" s="7"/>
-      <c r="C98" s="7">
-        <v>61093</v>
-      </c>
-      <c r="D98" s="7">
-        <v>60490</v>
-      </c>
-      <c r="E98" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F98" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G98">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B99" s="10"/>
-      <c r="C99" s="10">
-        <v>61914</v>
-      </c>
-      <c r="D99" s="10">
-        <v>61295</v>
-      </c>
-      <c r="E99" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F99" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G99">
+      <c r="G102">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A100" s="5" t="s">
+    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B100" s="7"/>
-      <c r="C100" s="7">
+      <c r="B103" s="7"/>
+      <c r="C103" s="7">
         <v>62575</v>
       </c>
-      <c r="D100" s="7">
+      <c r="D103" s="7">
         <v>61940</v>
       </c>
-      <c r="E100" s="3" t="str">
+      <c r="E103" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F100" s="3" t="str">
+      <c r="F103" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G100">
+      <c r="G103">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A101" s="5" t="s">
+    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B101" s="7"/>
-      <c r="C101" s="7">
+      <c r="B104" s="7"/>
+      <c r="C104" s="7">
         <v>63180</v>
       </c>
-      <c r="D101" s="7">
+      <c r="D104" s="7">
         <v>62513</v>
       </c>
-      <c r="E101" s="3" t="str">
+      <c r="E104" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F101" s="3" t="str">
+      <c r="F104" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G101">
+      <c r="G104">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
     </row>
-    <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
+    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B102" s="7"/>
-      <c r="C102" s="7">
+      <c r="B105" s="7"/>
+      <c r="C105" s="7">
         <v>63825</v>
       </c>
-      <c r="D102" s="7">
+      <c r="D105" s="7">
         <v>63172</v>
       </c>
-      <c r="E102" s="3" t="str">
+      <c r="E105" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F102" s="3" t="str">
+      <c r="F105" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G102">
+      <c r="G105">
         <f t="shared" si="4"/>
         <v>-14</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
+    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B103" s="7"/>
-      <c r="C103" s="7">
+      <c r="B106" s="7"/>
+      <c r="C106" s="7">
         <v>64581</v>
       </c>
-      <c r="D103" s="7">
+      <c r="D106" s="7">
         <v>63896</v>
       </c>
-      <c r="E103" s="3" t="str">
+      <c r="E106" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F103" s="3" t="str">
+      <c r="F106" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G103">
+      <c r="G106">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
     </row>
-    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
+    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B104" s="7"/>
-      <c r="C104" s="7">
+      <c r="B107" s="7"/>
+      <c r="C107" s="7">
         <v>65231</v>
       </c>
-      <c r="D104" s="7">
+      <c r="D107" s="7">
         <v>64541</v>
       </c>
-      <c r="E104" s="3" t="str">
+      <c r="E107" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F104" s="3" t="str">
+      <c r="F107" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G104">
+      <c r="G107">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
-    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
+    <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B105" s="7"/>
-      <c r="C105" s="7">
+      <c r="B108" s="7"/>
+      <c r="C108" s="7">
         <v>65820</v>
       </c>
-      <c r="D105" s="7">
+      <c r="D108" s="7">
         <v>65084</v>
       </c>
-      <c r="E105" s="3" t="str">
+      <c r="E108" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F105" s="3" t="str">
+      <c r="F108" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G105">
+      <c r="G108">
         <f t="shared" si="4"/>
         <v>46</v>
-      </c>
-    </row>
-    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="7"/>
-      <c r="B106" s="7"/>
-      <c r="C106" s="7"/>
-      <c r="D106" s="7"/>
-      <c r="E106" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F106" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="7"/>
-      <c r="B107" s="7"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="7"/>
-      <c r="E107" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F107" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="7"/>
-      <c r="B108" s="7"/>
-      <c r="C108" s="7"/>
-      <c r="D108" s="7"/>
-      <c r="E108" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F108" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -4411,7 +4481,7 @@
         <v>-</v>
       </c>
       <c r="F122" s="3" t="str">
-        <f t="shared" ref="F122:F125" si="6">IF(D122&lt;&gt;"",IF(B122&lt;&gt;"",D122-B122,"-"), "-")</f>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -4425,7 +4495,7 @@
         <v>-</v>
       </c>
       <c r="F123" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -4439,7 +4509,7 @@
         <v>-</v>
       </c>
       <c r="F124" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -4453,7 +4523,7 @@
         <v>-</v>
       </c>
       <c r="F125" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="F125:F128" si="6">IF(D125&lt;&gt;"",IF(B125&lt;&gt;"",D125-B125,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -4466,6 +4536,10 @@
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
+      <c r="F126" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="127" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A127" s="7"/>
@@ -4476,6 +4550,10 @@
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
+      <c r="F127" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="7"/>
@@ -4486,6 +4564,10 @@
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
+      <c r="F128" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
     </row>
     <row r="129" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="7"/>
@@ -4573,7 +4655,7 @@
       <c r="C137" s="7"/>
       <c r="D137" s="7"/>
       <c r="E137" s="3" t="str">
-        <f t="shared" ref="E137:E141" si="7">IF(C137&lt;&gt;"",IF(B137&lt;&gt;"",C137-B137,"-"), "-")</f>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -4583,7 +4665,7 @@
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
       <c r="E138" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -4593,7 +4675,7 @@
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
       <c r="E139" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>-</v>
       </c>
     </row>
@@ -4603,7 +4685,7 @@
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
       <c r="E140" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="E140:E144" si="7">IF(C140&lt;&gt;"",IF(B140&lt;&gt;"",C140-B140,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -4623,7 +4705,7 @@
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
       <c r="E142" s="3" t="str">
-        <f t="shared" ref="E142:E143" si="8">IF(C142&lt;&gt;"",IF(B142&lt;&gt;"",B142-C142,"-"), "-")</f>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
     </row>
@@ -4633,7 +4715,7 @@
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
       <c r="E143" s="3" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
     </row>
@@ -4642,84 +4724,99 @@
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
-    </row>
-    <row r="145" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="E144" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
-    </row>
-    <row r="146" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="E145" s="3" t="str">
+        <f t="shared" ref="E145:E146" si="8">IF(C145&lt;&gt;"",IF(B145&lt;&gt;"",B145-C145,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A146" s="7"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
-    </row>
-    <row r="147" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="E146" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A147" s="7"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
     </row>
-    <row r="148" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A148" s="7"/>
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
     </row>
-    <row r="149" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
     </row>
-    <row r="150" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
     </row>
-    <row r="151" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
     </row>
-    <row r="152" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
     </row>
-    <row r="153" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
     </row>
-    <row r="154" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
     </row>
-    <row r="157" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
     </row>
-    <row r="158" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
     </row>
-    <row r="159" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
     </row>
-    <row r="160" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
@@ -5333,6 +5430,21 @@
       <c r="B282" s="7"/>
       <c r="C282" s="7"/>
       <c r="D282" s="7"/>
+    </row>
+    <row r="283" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B283" s="7"/>
+      <c r="C283" s="7"/>
+      <c r="D283" s="7"/>
+    </row>
+    <row r="284" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B284" s="7"/>
+      <c r="C284" s="7"/>
+      <c r="D284" s="7"/>
+    </row>
+    <row r="285" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B285" s="7"/>
+      <c r="C285" s="7"/>
+      <c r="D285" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11385,7 +11497,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>
@@ -11420,10 +11532,10 @@
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
       <c r="J1" s="15"/>
-      <c r="K1" s="34" t="s">
+      <c r="K1" s="35" t="s">
         <v>158</v>
       </c>
-      <c r="L1" s="35"/>
+      <c r="L1" s="36"/>
     </row>
     <row r="2" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11"/>
@@ -13275,13 +13387,13 @@
       <c r="G53" s="17" t="s">
         <v>158</v>
       </c>
-      <c r="H53" s="36" t="s">
+      <c r="H53" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="I53" s="37"/>
-      <c r="J53" s="37"/>
-      <c r="K53" s="37"/>
-      <c r="L53" s="38"/>
+      <c r="I53" s="38"/>
+      <c r="J53" s="38"/>
+      <c r="K53" s="38"/>
+      <c r="L53" s="39"/>
     </row>
     <row r="54" spans="1:12" ht="26.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
@@ -13303,11 +13415,11 @@
       <c r="G54" s="27">
         <v>31536</v>
       </c>
-      <c r="H54" s="39"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="40"/>
-      <c r="K54" s="40"/>
-      <c r="L54" s="41"/>
+      <c r="H54" s="40"/>
+      <c r="I54" s="41"/>
+      <c r="J54" s="41"/>
+      <c r="K54" s="41"/>
+      <c r="L54" s="42"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
lode runner v5 - up to end of 48, 1929 ahead, still working on optimizing 48
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FC09B1-944D-4AB8-9765-7676B842225C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16815A26-A578-41ED-A0FB-16E7810A7D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="46455" yWindow="360" windowWidth="10905" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="236">
   <si>
     <t>Place</t>
   </si>
@@ -742,12 +742,6 @@
   </si>
   <si>
     <t>gold 3</t>
-  </si>
-  <si>
-    <t>gold -1</t>
-  </si>
-  <si>
-    <t>move</t>
   </si>
 </sst>
 </file>
@@ -757,19 +751,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1103,122 +1090,121 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -1539,11 +1525,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B3565E-C480-4A10-8524-B7BC06C9B703}">
-  <dimension ref="A1:H285"/>
+  <dimension ref="A1:H283"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B102" sqref="B102"/>
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3049,7 +3035,7 @@
         <v>1225</v>
       </c>
       <c r="F58" s="3">
-        <f t="shared" ref="F58:F124" si="3">IF(D58&lt;&gt;"",IF(B58&lt;&gt;"",D58-B58,"-"), "-")</f>
+        <f t="shared" ref="F58:F122" si="3">IF(D58&lt;&gt;"",IF(B58&lt;&gt;"",D58-B58,"-"), "-")</f>
         <v>729</v>
       </c>
       <c r="G58">
@@ -3390,7 +3376,7 @@
         <v>1015</v>
       </c>
       <c r="G72">
-        <f t="shared" ref="G72:G108" si="4">(C72-C71) - (D72-D71)</f>
+        <f t="shared" ref="G72:G106" si="4">(C72-C71) - (D72-D71)</f>
         <v>1</v>
       </c>
     </row>
@@ -3408,7 +3394,7 @@
         <v>44061</v>
       </c>
       <c r="E73" s="3">
-        <f t="shared" ref="E73:E139" si="5">IF(C73&lt;&gt;"",IF(B73&lt;&gt;"",C73-B73,"-"), "-")</f>
+        <f t="shared" ref="E73:E137" si="5">IF(C73&lt;&gt;"",IF(B73&lt;&gt;"",C73-B73,"-"), "-")</f>
         <v>1385</v>
       </c>
       <c r="F73" s="3">
@@ -4036,125 +4022,145 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A98" s="43" t="s">
-        <v>236</v>
+      <c r="A98" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="B98" s="7">
-        <v>58416</v>
-      </c>
-      <c r="C98" s="7"/>
+        <v>58575</v>
+      </c>
+      <c r="C98" s="7">
+        <v>60441</v>
+      </c>
       <c r="D98" s="7">
-        <v>59676</v>
-      </c>
-      <c r="E98" s="3"/>
+        <v>59838</v>
+      </c>
+      <c r="E98" s="3">
+        <f t="shared" si="5"/>
+        <v>1866</v>
+      </c>
       <c r="F98" s="3">
         <f t="shared" si="3"/>
-        <v>1260</v>
+        <v>1263</v>
+      </c>
+      <c r="G98">
+        <f>(C98-C97) - (D98-D97)</f>
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A99" s="43" t="s">
-        <v>237</v>
+      <c r="A99" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="B99" s="7">
-        <v>58443</v>
-      </c>
-      <c r="C99" s="7"/>
+        <v>59227</v>
+      </c>
+      <c r="C99" s="7">
+        <v>61093</v>
+      </c>
       <c r="D99" s="7">
-        <v>59702</v>
-      </c>
-      <c r="E99" s="3"/>
+        <v>60490</v>
+      </c>
+      <c r="E99" s="3">
+        <f t="shared" si="5"/>
+        <v>1866</v>
+      </c>
       <c r="F99" s="3">
         <f t="shared" si="3"/>
-        <v>1259</v>
+        <v>1263</v>
+      </c>
+      <c r="G99">
+        <f t="shared" si="4"/>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A100" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B100" s="7">
-        <v>58575</v>
-      </c>
-      <c r="C100" s="7">
-        <v>60441</v>
-      </c>
-      <c r="D100" s="7">
-        <v>59838</v>
+        <v>42</v>
+      </c>
+      <c r="B100" s="10">
+        <v>60018</v>
+      </c>
+      <c r="C100" s="10">
+        <v>61914</v>
+      </c>
+      <c r="D100" s="10">
+        <v>61295</v>
       </c>
       <c r="E100" s="3">
         <f t="shared" si="5"/>
-        <v>1866</v>
+        <v>1896</v>
       </c>
       <c r="F100" s="3">
         <f t="shared" si="3"/>
-        <v>1263</v>
+        <v>1277</v>
       </c>
       <c r="G100">
-        <f>(C100-C97) - (D100-D97)</f>
-        <v>22</v>
+        <f t="shared" si="4"/>
+        <v>16</v>
       </c>
     </row>
     <row r="101" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A101" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B101" s="7">
-        <v>59227</v>
+        <v>60663</v>
       </c>
       <c r="C101" s="7">
-        <v>61093</v>
+        <v>62575</v>
       </c>
       <c r="D101" s="7">
-        <v>60490</v>
+        <v>61940</v>
       </c>
       <c r="E101" s="3">
         <f t="shared" si="5"/>
-        <v>1866</v>
+        <v>1912</v>
       </c>
       <c r="F101" s="3">
         <f t="shared" si="3"/>
-        <v>1263</v>
+        <v>1277</v>
       </c>
       <c r="G101">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A102" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B102" s="10"/>
-      <c r="C102" s="10">
-        <v>61914</v>
-      </c>
-      <c r="D102" s="10">
-        <v>61295</v>
-      </c>
-      <c r="E102" s="3" t="str">
+        <v>43</v>
+      </c>
+      <c r="B102" s="7">
+        <v>61251</v>
+      </c>
+      <c r="C102" s="7">
+        <v>63180</v>
+      </c>
+      <c r="D102" s="7">
+        <v>62513</v>
+      </c>
+      <c r="E102" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F102" s="3" t="str">
+        <v>1929</v>
+      </c>
+      <c r="F102" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
+        <v>1262</v>
       </c>
       <c r="G102">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A103" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B103" s="7"/>
       <c r="C103" s="7">
-        <v>62575</v>
+        <v>63825</v>
       </c>
       <c r="D103" s="7">
-        <v>61940</v>
+        <v>63172</v>
       </c>
       <c r="E103" s="3" t="str">
         <f t="shared" si="5"/>
@@ -4166,19 +4172,19 @@
       </c>
       <c r="G103">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>-14</v>
       </c>
     </row>
     <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A104" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B104" s="7"/>
       <c r="C104" s="7">
-        <v>63180</v>
+        <v>64581</v>
       </c>
       <c r="D104" s="7">
-        <v>62513</v>
+        <v>63896</v>
       </c>
       <c r="E104" s="3" t="str">
         <f t="shared" si="5"/>
@@ -4195,14 +4201,14 @@
     </row>
     <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A105" s="5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B105" s="7"/>
       <c r="C105" s="7">
-        <v>63825</v>
+        <v>65231</v>
       </c>
       <c r="D105" s="7">
-        <v>63172</v>
+        <v>64541</v>
       </c>
       <c r="E105" s="3" t="str">
         <f t="shared" si="5"/>
@@ -4214,19 +4220,19 @@
       </c>
       <c r="G105">
         <f t="shared" si="4"/>
-        <v>-14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A106" s="5" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="B106" s="7"/>
       <c r="C106" s="7">
-        <v>64581</v>
+        <v>65820</v>
       </c>
       <c r="D106" s="7">
-        <v>63896</v>
+        <v>65084</v>
       </c>
       <c r="E106" s="3" t="str">
         <f t="shared" si="5"/>
@@ -4238,20 +4244,14 @@
       </c>
       <c r="G106">
         <f t="shared" si="4"/>
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="A107" s="7"/>
       <c r="B107" s="7"/>
-      <c r="C107" s="7">
-        <v>65231</v>
-      </c>
-      <c r="D107" s="7">
-        <v>64541</v>
-      </c>
+      <c r="C107" s="7"/>
+      <c r="D107" s="7"/>
       <c r="E107" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4260,22 +4260,12 @@
         <f t="shared" si="3"/>
         <v>-</v>
       </c>
-      <c r="G107">
-        <f t="shared" si="4"/>
-        <v>5</v>
-      </c>
     </row>
     <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="A108" s="7"/>
       <c r="B108" s="7"/>
-      <c r="C108" s="7">
-        <v>65820</v>
-      </c>
-      <c r="D108" s="7">
-        <v>65084</v>
-      </c>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7"/>
       <c r="E108" s="3" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4283,10 +4273,6 @@
       <c r="F108" s="3" t="str">
         <f t="shared" si="3"/>
         <v>-</v>
-      </c>
-      <c r="G108">
-        <f t="shared" si="4"/>
-        <v>46</v>
       </c>
     </row>
     <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -4495,7 +4481,7 @@
         <v>-</v>
       </c>
       <c r="F123" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="F123:F126" si="6">IF(D123&lt;&gt;"",IF(B123&lt;&gt;"",D123-B123,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -4509,7 +4495,7 @@
         <v>-</v>
       </c>
       <c r="F124" s="3" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
     </row>
@@ -4523,7 +4509,7 @@
         <v>-</v>
       </c>
       <c r="F125" s="3" t="str">
-        <f t="shared" ref="F125:F128" si="6">IF(D125&lt;&gt;"",IF(B125&lt;&gt;"",D125-B125,"-"), "-")</f>
+        <f t="shared" si="6"/>
         <v>-</v>
       </c>
     </row>
@@ -4550,10 +4536,6 @@
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F127" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
     </row>
     <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="7"/>
@@ -4564,10 +4546,6 @@
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-      <c r="F128" s="3" t="str">
-        <f t="shared" si="6"/>
-        <v>-</v>
-      </c>
     </row>
     <row r="129" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="7"/>
@@ -4665,7 +4643,7 @@
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
       <c r="E138" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="E138:E142" si="7">IF(C138&lt;&gt;"",IF(B138&lt;&gt;"",C138-B138,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -4675,7 +4653,7 @@
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
       <c r="E139" s="3" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
     </row>
@@ -4685,7 +4663,7 @@
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
       <c r="E140" s="3" t="str">
-        <f t="shared" ref="E140:E144" si="7">IF(C140&lt;&gt;"",IF(B140&lt;&gt;"",C140-B140,"-"), "-")</f>
+        <f t="shared" si="7"/>
         <v>-</v>
       </c>
     </row>
@@ -4715,7 +4693,7 @@
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
       <c r="E143" s="3" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="E143:E144" si="8">IF(C143&lt;&gt;"",IF(B143&lt;&gt;"",B143-C143,"-"), "-")</f>
         <v>-</v>
       </c>
     </row>
@@ -4725,98 +4703,88 @@
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
       <c r="E144" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
-      <c r="E145" s="3" t="str">
-        <f t="shared" ref="E145:E146" si="8">IF(C145&lt;&gt;"",IF(B145&lt;&gt;"",B145-C145,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="146" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
-      <c r="E146" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A147" s="7"/>
+    </row>
+    <row r="147" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
     </row>
-    <row r="148" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A148" s="7"/>
+    <row r="148" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
     </row>
-    <row r="149" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
     </row>
-    <row r="150" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
     </row>
-    <row r="151" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
     </row>
-    <row r="152" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
     </row>
-    <row r="153" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
     </row>
-    <row r="154" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
     </row>
-    <row r="157" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
     </row>
-    <row r="158" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
     </row>
-    <row r="159" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
     </row>
-    <row r="160" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
@@ -5435,16 +5403,6 @@
       <c r="B283" s="7"/>
       <c r="C283" s="7"/>
       <c r="D283" s="7"/>
-    </row>
-    <row r="284" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B284" s="7"/>
-      <c r="C284" s="7"/>
-      <c r="D284" s="7"/>
-    </row>
-    <row r="285" spans="2:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="B285" s="7"/>
-      <c r="C285" s="7"/>
-      <c r="D285" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11497,7 +11455,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="16" type="noConversion"/>
+  <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
lode runner v5 - complete, 2020 frames faster than v4
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16815A26-A578-41ED-A0FB-16E7810A7D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3882081-33E1-42D3-8A7D-9A14D2582A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="46455" yWindow="360" windowWidth="10905" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="236">
   <si>
     <t>Place</t>
   </si>
@@ -751,12 +751,19 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1090,121 +1097,122 @@
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="6" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Accent1" xfId="5" builtinId="29"/>
@@ -1525,11 +1533,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39B3565E-C480-4A10-8524-B7BC06C9B703}">
-  <dimension ref="A1:H283"/>
+  <dimension ref="A1:H287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B103" sqref="B103"/>
+      <selection pane="bottomLeft" activeCell="B111" sqref="B111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3035,7 +3043,7 @@
         <v>1225</v>
       </c>
       <c r="F58" s="3">
-        <f t="shared" ref="F58:F122" si="3">IF(D58&lt;&gt;"",IF(B58&lt;&gt;"",D58-B58,"-"), "-")</f>
+        <f t="shared" ref="F58:F126" si="3">IF(D58&lt;&gt;"",IF(B58&lt;&gt;"",D58-B58,"-"), "-")</f>
         <v>729</v>
       </c>
       <c r="G58">
@@ -3394,7 +3402,7 @@
         <v>44061</v>
       </c>
       <c r="E73" s="3">
-        <f t="shared" ref="E73:E137" si="5">IF(C73&lt;&gt;"",IF(B73&lt;&gt;"",C73-B73,"-"), "-")</f>
+        <f t="shared" ref="E73:E141" si="5">IF(C73&lt;&gt;"",IF(B73&lt;&gt;"",C73-B73,"-"), "-")</f>
         <v>1385</v>
       </c>
       <c r="F73" s="3">
@@ -4126,181 +4134,200 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A102" s="5" t="s">
-        <v>43</v>
+      <c r="A102" s="43" t="s">
+        <v>127</v>
       </c>
       <c r="B102" s="7">
-        <v>61251</v>
+        <v>60822</v>
       </c>
       <c r="C102" s="7">
-        <v>63180</v>
+        <v>62732</v>
       </c>
       <c r="D102" s="7">
-        <v>62513</v>
+        <v>62103</v>
       </c>
       <c r="E102" s="3">
         <f t="shared" si="5"/>
-        <v>1929</v>
+        <v>1910</v>
       </c>
       <c r="F102" s="3">
         <f t="shared" si="3"/>
-        <v>1262</v>
-      </c>
-      <c r="G102">
+        <v>1281</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A103" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B103" s="7">
+        <v>61231</v>
+      </c>
+      <c r="C103" s="7">
+        <v>63180</v>
+      </c>
+      <c r="D103" s="7">
+        <v>62513</v>
+      </c>
+      <c r="E103" s="3">
+        <f t="shared" si="5"/>
+        <v>1949</v>
+      </c>
+      <c r="F103" s="3">
+        <f t="shared" si="3"/>
+        <v>1282</v>
+      </c>
+      <c r="G103">
+        <f>(C103-C101) - (D103-D101)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A104" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B104" s="7">
+        <v>61891</v>
+      </c>
+      <c r="C104" s="7">
+        <v>63825</v>
+      </c>
+      <c r="D104" s="7">
+        <v>63172</v>
+      </c>
+      <c r="E104" s="3">
+        <f t="shared" si="5"/>
+        <v>1934</v>
+      </c>
+      <c r="F104" s="3">
+        <f t="shared" si="3"/>
+        <v>1281</v>
+      </c>
+      <c r="G104">
+        <f t="shared" si="4"/>
+        <v>-14</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A105" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B105" s="7">
+        <v>62598</v>
+      </c>
+      <c r="C105" s="7">
+        <v>64581</v>
+      </c>
+      <c r="D105" s="7">
+        <v>63896</v>
+      </c>
+      <c r="E105" s="3">
+        <f t="shared" si="5"/>
+        <v>1983</v>
+      </c>
+      <c r="F105" s="3">
+        <f t="shared" si="3"/>
+        <v>1298</v>
+      </c>
+      <c r="G105">
         <f t="shared" si="4"/>
         <v>32</v>
       </c>
     </row>
-    <row r="103" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A103" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B103" s="7"/>
-      <c r="C103" s="7">
-        <v>63825</v>
-      </c>
-      <c r="D103" s="7">
-        <v>63172</v>
-      </c>
-      <c r="E103" s="3" t="str">
+    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A106" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B106" s="7">
+        <v>63243</v>
+      </c>
+      <c r="C106" s="7">
+        <v>65231</v>
+      </c>
+      <c r="D106" s="7">
+        <v>64541</v>
+      </c>
+      <c r="E106" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F103" s="3" t="str">
+        <v>1988</v>
+      </c>
+      <c r="F106" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G103">
-        <f t="shared" si="4"/>
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="104" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A104" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B104" s="7"/>
-      <c r="C104" s="7">
-        <v>64581</v>
-      </c>
-      <c r="D104" s="7">
-        <v>63896</v>
-      </c>
-      <c r="E104" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F104" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G104">
-        <f t="shared" si="4"/>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="105" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A105" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B105" s="7"/>
-      <c r="C105" s="7">
-        <v>65231</v>
-      </c>
-      <c r="D105" s="7">
-        <v>64541</v>
-      </c>
-      <c r="E105" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F105" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G105">
+        <v>1298</v>
+      </c>
+      <c r="G106">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
     </row>
-    <row r="106" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A106" s="5" t="s">
+    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A107" s="5"/>
+      <c r="B107" s="7">
+        <v>63497</v>
+      </c>
+      <c r="C107" s="7"/>
+      <c r="D107" s="7">
+        <v>64796</v>
+      </c>
+      <c r="E107" s="3"/>
+      <c r="F107" s="3">
+        <f t="shared" si="3"/>
+        <v>1299</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A108" s="5"/>
+      <c r="B108" s="7">
+        <v>63552</v>
+      </c>
+      <c r="C108" s="7"/>
+      <c r="D108" s="7">
+        <v>64843</v>
+      </c>
+      <c r="E108" s="3"/>
+      <c r="F108" s="3">
+        <f t="shared" si="3"/>
+        <v>1291</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A109" s="5"/>
+      <c r="B109" s="7">
+        <v>63603</v>
+      </c>
+      <c r="C109" s="7"/>
+      <c r="D109" s="7">
+        <v>64877</v>
+      </c>
+      <c r="E109" s="3"/>
+      <c r="F109" s="3">
+        <f t="shared" si="3"/>
+        <v>1274</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A110" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B106" s="7"/>
-      <c r="C106" s="7">
+      <c r="B110" s="7">
+        <v>63800</v>
+      </c>
+      <c r="C110" s="7">
         <v>65820</v>
       </c>
-      <c r="D106" s="7">
+      <c r="D110" s="7">
         <v>65084</v>
       </c>
-      <c r="E106" s="3" t="str">
+      <c r="E110" s="3">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F106" s="3" t="str">
+        <v>2020</v>
+      </c>
+      <c r="F110" s="3">
         <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-      <c r="G106">
-        <f t="shared" si="4"/>
+        <v>1284</v>
+      </c>
+      <c r="G110">
+        <f>(C110-C106) - (D110-D106)</f>
         <v>46</v>
-      </c>
-    </row>
-    <row r="107" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A107" s="7"/>
-      <c r="B107" s="7"/>
-      <c r="C107" s="7"/>
-      <c r="D107" s="7"/>
-      <c r="E107" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F107" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="108" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A108" s="7"/>
-      <c r="B108" s="7"/>
-      <c r="C108" s="7"/>
-      <c r="D108" s="7"/>
-      <c r="E108" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F108" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="109" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A109" s="7"/>
-      <c r="B109" s="7"/>
-      <c r="C109" s="7"/>
-      <c r="D109" s="7"/>
-      <c r="E109" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F109" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="110" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A110" s="7"/>
-      <c r="B110" s="7"/>
-      <c r="C110" s="7"/>
-      <c r="D110" s="7"/>
-      <c r="E110" s="3" t="str">
-        <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="F110" s="3" t="str">
-        <f t="shared" si="3"/>
-        <v>-</v>
       </c>
     </row>
     <row r="111" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -4481,7 +4508,7 @@
         <v>-</v>
       </c>
       <c r="F123" s="3" t="str">
-        <f t="shared" ref="F123:F126" si="6">IF(D123&lt;&gt;"",IF(B123&lt;&gt;"",D123-B123,"-"), "-")</f>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -4495,7 +4522,7 @@
         <v>-</v>
       </c>
       <c r="F124" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -4509,7 +4536,7 @@
         <v>-</v>
       </c>
       <c r="F125" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -4523,7 +4550,7 @@
         <v>-</v>
       </c>
       <c r="F126" s="3" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="3"/>
         <v>-</v>
       </c>
     </row>
@@ -4536,6 +4563,10 @@
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
+      <c r="F127" s="3" t="str">
+        <f t="shared" ref="F127:F130" si="6">IF(D127&lt;&gt;"",IF(B127&lt;&gt;"",D127-B127,"-"), "-")</f>
+        <v>-</v>
+      </c>
     </row>
     <row r="128" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A128" s="7"/>
@@ -4546,8 +4577,12 @@
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="F128" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A129" s="7"/>
       <c r="B129" s="7"/>
       <c r="C129" s="7"/>
@@ -4556,8 +4591,12 @@
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="F129" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A130" s="7"/>
       <c r="B130" s="7"/>
       <c r="C130" s="7"/>
@@ -4566,8 +4605,12 @@
         <f t="shared" si="5"/>
         <v>-</v>
       </c>
-    </row>
-    <row r="131" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="F130" s="3" t="str">
+        <f t="shared" si="6"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A131" s="7"/>
       <c r="B131" s="7"/>
       <c r="C131" s="7"/>
@@ -4577,7 +4620,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A132" s="7"/>
       <c r="B132" s="7"/>
       <c r="C132" s="7"/>
@@ -4587,7 +4630,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="133" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A133" s="7"/>
       <c r="B133" s="7"/>
       <c r="C133" s="7"/>
@@ -4597,7 +4640,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="134" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A134" s="7"/>
       <c r="B134" s="7"/>
       <c r="C134" s="7"/>
@@ -4607,7 +4650,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A135" s="7"/>
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
@@ -4617,7 +4660,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A136" s="7"/>
       <c r="B136" s="7"/>
       <c r="C136" s="7"/>
@@ -4627,7 +4670,7 @@
         <v>-</v>
       </c>
     </row>
-    <row r="137" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A137" s="7"/>
       <c r="B137" s="7"/>
       <c r="C137" s="7"/>
@@ -4637,154 +4680,174 @@
         <v>-</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A138" s="7"/>
       <c r="B138" s="7"/>
       <c r="C138" s="7"/>
       <c r="D138" s="7"/>
       <c r="E138" s="3" t="str">
-        <f t="shared" ref="E138:E142" si="7">IF(C138&lt;&gt;"",IF(B138&lt;&gt;"",C138-B138,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A139" s="7"/>
       <c r="B139" s="7"/>
       <c r="C139" s="7"/>
       <c r="D139" s="7"/>
       <c r="E139" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A140" s="7"/>
       <c r="B140" s="7"/>
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
       <c r="E140" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A141" s="7"/>
       <c r="B141" s="7"/>
       <c r="C141" s="7"/>
       <c r="D141" s="7"/>
       <c r="E141" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="142" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A142" s="7"/>
       <c r="B142" s="7"/>
       <c r="C142" s="7"/>
       <c r="D142" s="7"/>
       <c r="E142" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E142:E146" si="7">IF(C142&lt;&gt;"",IF(B142&lt;&gt;"",C142-B142,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A143" s="7"/>
       <c r="B143" s="7"/>
       <c r="C143" s="7"/>
       <c r="D143" s="7"/>
       <c r="E143" s="3" t="str">
-        <f t="shared" ref="E143:E144" si="8">IF(C143&lt;&gt;"",IF(B143&lt;&gt;"",B143-C143,"-"), "-")</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A144" s="7"/>
       <c r="B144" s="7"/>
       <c r="C144" s="7"/>
       <c r="D144" s="7"/>
       <c r="E144" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="145" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A145" s="7"/>
       <c r="B145" s="7"/>
       <c r="C145" s="7"/>
       <c r="D145" s="7"/>
-    </row>
-    <row r="146" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="E145" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A146" s="7"/>
       <c r="B146" s="7"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
-    </row>
-    <row r="147" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="E146" s="3" t="str">
+        <f t="shared" si="7"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A147" s="7"/>
       <c r="B147" s="7"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
-    </row>
-    <row r="148" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="E147" s="3" t="str">
+        <f t="shared" ref="E147:E148" si="8">IF(C147&lt;&gt;"",IF(B147&lt;&gt;"",B147-C147,"-"), "-")</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A148" s="7"/>
       <c r="B148" s="7"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
-    </row>
-    <row r="149" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="E148" s="3" t="str">
+        <f t="shared" si="8"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A149" s="7"/>
       <c r="B149" s="7"/>
       <c r="C149" s="7"/>
       <c r="D149" s="7"/>
     </row>
-    <row r="150" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="15" x14ac:dyDescent="0.25">
+      <c r="A150" s="7"/>
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
       <c r="D150" s="7"/>
     </row>
-    <row r="151" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B151" s="7"/>
       <c r="C151" s="7"/>
       <c r="D151" s="7"/>
     </row>
-    <row r="152" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B152" s="7"/>
       <c r="C152" s="7"/>
       <c r="D152" s="7"/>
     </row>
-    <row r="153" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B153" s="7"/>
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
     </row>
-    <row r="154" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
     </row>
-    <row r="155" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B155" s="7"/>
       <c r="C155" s="7"/>
       <c r="D155" s="7"/>
     </row>
-    <row r="156" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B156" s="7"/>
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
     </row>
-    <row r="157" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B157" s="7"/>
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
     </row>
-    <row r="158" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B158" s="7"/>
       <c r="C158" s="7"/>
       <c r="D158" s="7"/>
     </row>
-    <row r="159" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B159" s="7"/>
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
     </row>
-    <row r="160" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="B160" s="7"/>
       <c r="C160" s="7"/>
       <c r="D160" s="7"/>
@@ -5403,6 +5466,26 @@
       <c r="B283" s="7"/>
       <c r="C283" s="7"/>
       <c r="D283" s="7"/>
+    </row>
+    <row r="284" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B284" s="7"/>
+      <c r="C284" s="7"/>
+      <c r="D284" s="7"/>
+    </row>
+    <row r="285" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B285" s="7"/>
+      <c r="C285" s="7"/>
+      <c r="D285" s="7"/>
+    </row>
+    <row r="286" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B286" s="7"/>
+      <c r="C286" s="7"/>
+      <c r="D286" s="7"/>
+    </row>
+    <row r="287" spans="2:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="B287" s="7"/>
+      <c r="C287" s="7"/>
+      <c r="D287" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11455,7 +11538,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="15" type="noConversion"/>
+  <phoneticPr fontId="16" type="noConversion"/>
   <pageMargins left="0" right="0" top="0.39410000000000006" bottom="0.39410000000000006" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
lode runner v5 - lv 50 improved, now 2038 faster than v4
</commit_message>
<xml_diff>
--- a/LodeRunner/FrameCompare.xlsx
+++ b/LodeRunner/FrameCompare.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\adelikat-tas\LodeRunner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3882081-33E1-42D3-8A7D-9A14D2582A43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CB2D5B-8B1E-41FE-8C62-D83A7ED1A05C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="46455" yWindow="360" windowWidth="10905" windowHeight="13560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4309,7 +4309,7 @@
         <v>26</v>
       </c>
       <c r="B110" s="7">
-        <v>63800</v>
+        <v>63782</v>
       </c>
       <c r="C110" s="7">
         <v>65820</v>
@@ -4319,11 +4319,11 @@
       </c>
       <c r="E110" s="3">
         <f t="shared" si="5"/>
-        <v>2020</v>
+        <v>2038</v>
       </c>
       <c r="F110" s="3">
         <f t="shared" si="3"/>
-        <v>1284</v>
+        <v>1302</v>
       </c>
       <c r="G110">
         <f>(C110-C106) - (D110-D106)</f>

</xml_diff>